<commit_message>
Latest data: Mon May 23 12:28:34 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA52"/>
+  <dimension ref="A1:AA55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2396,7 +2396,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Altri eventi,Iniziative per bambini</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2406,87 +2406,67 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Viale Jacopo Barozzi, 31</t>
+          <t>Piazza della Manifattura Tabacchi</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2021-05-13T08:16:32+00:00</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Conferenze, eventi per famiglie, serate speciali e visite guidate</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:44+00:00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2021-05-13T08:16:59+00:00</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>info@planetariodimodena.it</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:51+00:00</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2022-05-22T07:00:00+00:00</t>
+          <t>2022-05-25T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2022-05-29T09:11:35+00:00</t>
+          <t>2022-05-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy7_of_le-iniziative-al-planetario/@@images/bce50dab-bfa1-40ef-9085-04f7bab6d51d.jpeg</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>Immagine del pianeta Terra - da unsplash.com</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy6_of_free-walking-tour-visite-guidate-tematiche/@@images/3423aebc-8b5e-4d1d-8f35-b2dce36dab21.jpeg</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2022-05-17T08:44:09+00:00</t>
+          <t>2022-05-23T10:18:25+00:00</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Civico Planetario</t>
+          <t>Ritrovo e partenza: Piazza della Manifattura Tabacchi</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> domenica 22 e domenica 29 maggio ore 15  giovedì 26 maggio ore 21  sabato 28 maggio ore 21</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> a pagamento  vedi costo del biglietto nel programma o sul sito del Planetario: www.planetariodimodena.it </t>
+          <t xml:space="preserve"> Euro 12 a partecipante</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>059 224726</t>
-        </is>
-      </c>
+      <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr">
         <is>
-          <t>Le iniziative al Planetario</t>
+          <t>Free Walking Tour - Visite guidate tematiche</t>
         </is>
       </c>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>https://www.planetariodimodena.it</t>
-        </is>
-      </c>
+      <c r="U19" t="inlineStr"/>
       <c r="V19" t="b">
         <v>0</v>
       </c>
@@ -2495,29 +2475,29 @@
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy7_of_le-iniziative-al-planetario</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy6_of_free-walking-tour-visite-guidate-tematiche</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>44,64907001920466</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>10,917829960080724</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>POINT (10.917829960080724 44.64907001920466)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato,Manifestazioni sportive</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2525,61 +2505,89 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Viale Jacopo Barozzi, 31</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2022-05-17T09:05:44+00:00</t>
+          <t>2021-05-13T08:16:32+00:00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Esibizioni, incontri tematici, esposizioni di auto sono in programma dal 26 al 29 maggio</t>
+          <t>Conferenze, eventi per famiglie, serate speciali e visite guidate</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2022-05-17T09:05:52+00:00</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr"/>
+          <t>2021-05-13T08:16:59+00:00</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>info@planetariodimodena.it</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2022-05-26T08:00:00+00:00</t>
+          <t>2022-05-22T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2022-05-29T09:00:00+00:00</t>
+          <t>2022-05-29T09:11:35+00:00</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/motor-valley-fest-quarta-edizione/@@images/b4ee995e-3238-4045-932b-c7b1819db8ce.jpeg</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy7_of_le-iniziative-al-planetario/@@images/bce50dab-bfa1-40ef-9085-04f7bab6d51d.jpeg</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Immagine del pianeta Terra - da unsplash.com</t>
+        </is>
+      </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2022-05-17T09:05:52+00:00</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr"/>
+          <t>2022-05-17T08:44:09+00:00</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Civico Planetario</t>
+        </is>
+      </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> vedi orari nel programma: motorvalley.it/motorvalleyfest</t>
+          <t xml:space="preserve"> domenica 22 e domenica 29 maggio ore 15  giovedì 26 maggio ore 21  sabato 28 maggio ore 21</t>
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> a pagamento  vedi costo del biglietto nel programma o sul sito del Planetario: www.planetariodimodena.it </t>
+        </is>
+      </c>
       <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>059 224726</t>
+        </is>
+      </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>Motor Valley Fest - Quarta edizione</t>
+          <t>Le iniziative al Planetario</t>
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>https://www.planetariodimodena.it</t>
+        </is>
+      </c>
       <c r="V20" t="b">
         <v>0</v>
       </c>
@@ -2588,29 +2596,29 @@
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/motor-valley-fest-quarta-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy7_of_le-iniziative-al-planetario</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,64907001920466</t>
         </is>
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,917829960080724</t>
         </is>
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.917829960080724 44.64907001920466)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2618,60 +2626,48 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>centro storico</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2022-04-29T10:05:46+00:00</t>
+          <t>2022-05-17T09:05:44+00:00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
+          <t>Esibizioni, incontri tematici, esposizioni di auto sono in programma dal 26 al 29 maggio</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-05-17T09:05:52+00:00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2022-05-01T09:00:00+00:00</t>
+          <t>2022-05-26T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2022-07-17T10:00:00+00:00</t>
+          <t>2022-05-29T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/motor-valley-fest-quarta-edizione/@@images/b4ee995e-3238-4045-932b-c7b1819db8ce.jpeg</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>Piazza Torre</t>
-        </is>
-      </c>
+          <t>2022-05-17T09:05:52+00:00</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
+          <t xml:space="preserve"> vedi orari nel programma: motorvalley.it/motorvalleyfest</t>
         </is>
       </c>
       <c r="O21" t="inlineStr"/>
@@ -2680,7 +2676,7 @@
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, aperture serali</t>
+          <t>Motor Valley Fest - Quarta edizione</t>
         </is>
       </c>
       <c r="T21" t="inlineStr"/>
@@ -2693,7 +2689,7 @@
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/motor-valley-fest-quarta-edizione</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
@@ -2715,7 +2711,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2725,54 +2721,58 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 103</t>
+          <t>centro storico</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2022-05-05T08:41:26+00:00</t>
+          <t>2022-04-29T10:05:46+00:00</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Appuntamenti letterari al femminile</t>
+          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2022-05-05T09:23:17+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2022-05-07T07:00:00+00:00</t>
+          <t>2022-05-01T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2022-05-28T08:00:00+00:00</t>
+          <t>2022-07-17T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/scrittrici-inchiostro/@@images/318772ef-8170-4984-9e11-f2516c109708.jpeg</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2022-05-05T09:23:17+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Chiostro di Palazzo Santa Margherita</t>
+          <t>Piazza Torre</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> i sabati di maggio alle ore 18</t>
+          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
         </is>
       </c>
       <c r="O22" t="inlineStr"/>
@@ -2781,7 +2781,7 @@
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr">
         <is>
-          <t>Scrittrici inChiostro</t>
+          <t>Torre Ghirlandina, aperture serali</t>
         </is>
       </c>
       <c r="T22" t="inlineStr"/>
@@ -2794,7 +2794,7 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/scrittrici-inchiostro</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
@@ -2816,7 +2816,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2826,63 +2826,63 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr"/>
+          <t>2022-05-05T08:41:26+00:00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Appuntamenti letterari al femminile</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-05T09:23:17+00:00</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-05-07T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-05-28T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/scrittrici-inchiostro/@@images/318772ef-8170-4984-9e11-f2516c109708.jpeg</t>
         </is>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2022-05-17T07:27:36+00:00</t>
+          <t>2022-05-05T09:23:17+00:00</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Chiostro di Palazzo Santa Margherita</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> i sabati di maggio alle ore 18</t>
         </is>
       </c>
       <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
-        </is>
-      </c>
+      <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Scrittrici inChiostro</t>
         </is>
       </c>
       <c r="T23" t="inlineStr"/>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/scrittrici-inchiostro</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
@@ -2917,7 +2917,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2927,59 +2927,63 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>via Emilia Centro angolo Piazza Matteotti</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2022-05-13T10:01:30+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2022-05-13T10:03:13+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2022-05-28T09:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2022-06-05T10:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mostra-di-ricamo-e-merletto-da-ieri-a-oggi-la-tradizione-continua/@@images/fecdcb1a-b768-40a7-8809-d18fd2116bab.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
         </is>
       </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2022-05-13T10:03:32+00:00</t>
+          <t>2022-05-17T07:27:36+00:00</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Chiesa S.Giovanni Battista</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal lunedì al venerdì ore 10-18  sabato e domenica ore 10-19</t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr">
         <is>
-          <t>Mostra di ricamo e merletto "Da ieri a oggi.....la tradizione continua"</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T24" t="inlineStr"/>
@@ -2992,7 +2996,7 @@
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mostra-di-ricamo-e-merletto-da-ieri-a-oggi-la-tradizione-continua</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
@@ -3014,7 +3018,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3024,58 +3028,50 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>via Emilia Centro angolo Piazza Matteotti</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
-        </is>
-      </c>
+          <t>2022-05-13T10:01:30+00:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-05-13T10:03:13+00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2022-05-28T13:00:00+00:00</t>
+          <t>2022-05-28T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2022-05-28T14:00:00+00:00</t>
+          <t>2022-06-05T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dai-comacini-ai-maestri-campionesi/@@images/d5218bc2-dc59-43df-b1a3-4f32b072e82f.jpeg</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mostra-di-ricamo-e-merletto-da-ieri-a-oggi-la-tradizione-continua/@@images/fecdcb1a-b768-40a7-8809-d18fd2116bab.jpeg</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2022-02-28T15:10:52+00:00</t>
+          <t>2022-05-13T10:03:32+00:00</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Chiesa S.Giovanni Battista</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> dal lunedì al venerdì ore 10-18  sabato e domenica ore 10-19</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
@@ -3084,7 +3080,7 @@
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>Dai Comacini ai Maestri Campionesi</t>
+          <t>Mostra di ricamo e merletto "Da ieri a oggi.....la tradizione continua"</t>
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
@@ -3097,7 +3093,7 @@
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dai-comacini-ai-maestri-campionesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mostra-di-ricamo-e-merletto-da-ieri-a-oggi-la-tradizione-continua</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
@@ -3129,50 +3125,58 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Piazza Grande</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:44+00:00</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
+          <t>2022-02-25T14:15:15+00:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:51+00:00</t>
+          <t>2022-02-25T14:15:33+00:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2022-03-19T16:00:00+00:00</t>
+          <t>2022-05-28T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2022-05-28T16:00:00+00:00</t>
+          <t>2022-05-28T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/free-walking-tour-visite-guidate-del-centro-storico-di-modena/@@images/26b88750-ac47-44ab-bc5c-66df7933f860.jpeg</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dai-comacini-ai-maestri-campionesi/@@images/d5218bc2-dc59-43df-b1a3-4f32b072e82f.jpeg</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2022-03-23T16:27:28+00:00</t>
+          <t>2022-02-28T15:10:52+00:00</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tutti i sabati dal 19 marzo al 28 maggio alle ore 15.30</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
@@ -3181,7 +3185,7 @@
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr">
         <is>
-          <t>Free Walking Tour - Visite guidate del centro storico di Modena</t>
+          <t>Dai Comacini ai Maestri Campionesi</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
@@ -3194,7 +3198,7 @@
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/free-walking-tour-visite-guidate-del-centro-storico-di-modena</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dai-comacini-ai-maestri-campionesi</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
@@ -3216,7 +3220,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Concerti,Musica</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3226,67 +3230,59 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Largo S.Francesco</t>
+          <t>Piazza Grande</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2022-05-10T10:04:48+00:00</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Diciottesima edizione</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:44+00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2022-05-10T10:08:30+00:00</t>
+          <t>2022-03-23T16:26:51+00:00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2022-05-29T10:00:00+00:00</t>
+          <t>2022-03-19T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2022-05-29T11:00:00+00:00</t>
+          <t>2022-05-28T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-rosa-mistica/@@images/5d666bc9-d035-4acb-9903-21fd8e9003bf.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/free-walking-tour-visite-guidate-del-centro-storico-di-modena/@@images/26b88750-ac47-44ab-bc5c-66df7933f860.jpeg</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-05-10T10:13:42+00:00</t>
+          <t>2022-03-23T16:27:28+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Chiesa di San Francesco</t>
+          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 16.00</t>
+          <t xml:space="preserve"> Tutti i sabati dal 19 marzo al 28 maggio alle ore 15.30</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso libero</t>
-        </is>
-      </c>
+      <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Concerto "Rosa mistica"</t>
+          <t>Free Walking Tour - Visite guidate del centro storico di Modena</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
@@ -3299,7 +3295,7 @@
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-rosa-mistica</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/free-walking-tour-visite-guidate-del-centro-storico-di-modena</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3321,108 +3317,90 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
+          <t>Concerti,Musica</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Montale Rangone</t>
+          <t>Modena</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
+          <t>Largo S.Francesco</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2021-04-26T15:03:43+00:00</t>
+          <t>2022-05-10T10:04:48+00:00</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+          <t>Diciottesima edizione</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2021-04-26T15:06:06+00:00</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>museo@parcomontale.it</t>
-        </is>
-      </c>
+          <t>2022-05-10T10:08:30+00:00</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-04-03T14:00:00+00:00</t>
+          <t>2022-05-29T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-06-19T15:00:00+00:00</t>
+          <t>2022-05-29T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>Parco archeologico della Terramara di Montale</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-rosa-mistica/@@images/5d666bc9-d035-4acb-9903-21fd8e9003bf.jpeg</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-03-28T14:43:35+00:00</t>
+          <t>2022-05-10T10:13:42+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Chiesa di San Francesco</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
+          <t xml:space="preserve"> ore 16.00</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
+          <t xml:space="preserve"> Ingresso libero</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
-        </is>
-      </c>
+      <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Concerto "Rosa mistica"</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>http://www.parcomontale.it/it</t>
-        </is>
-      </c>
+      <c r="U28" t="inlineStr"/>
       <c r="V28" t="b">
         <v>0</v>
       </c>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>41050</t>
-        </is>
+      <c r="W28" t="n">
+        <v>41123</v>
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-rosa-mistica</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3444,122 +3422,130 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Modena</t>
+          <t>Montale Rangone</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Viale Caduti in Guerra, 196</t>
+          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2020-09-17T12:45:54+00:00</t>
+          <t>2021-04-26T15:03:43+00:00</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Gli spettacoli di ERT al Teatro Tempio</t>
+          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2014-09-30T12:50:00+00:00</t>
+          <t>2021-04-26T15:06:06+00:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>info@emiliaromagnateatro.com</t>
+          <t>museo@parcomontale.it</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-05-30T22:00:00+00:00</t>
+          <t>2022-04-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-19T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/kassandra/@@images/29f75f21-a9f0-45e8-8056-8023ce88a666.jpeg</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Parco archeologico della Terramara di Montale</t>
+        </is>
+      </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-03-15T11:11:12+00:00</t>
+          <t>2022-03-28T14:43:35+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Teatro Tempio</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 31 maggio e 1 giugno, 3 giugno e dal 7 al 10 giugno ore 20.30  2, 4, 5, 11 e 12 giugno ore 19.00</t>
+          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
+          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr">
         <is>
-          <t>059/2163021</t>
+          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Kassandra</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr">
         <is>
-          <t>http://www.emiliaromagnateatro.com</t>
+          <t>http://www.parcomontale.it/it</t>
         </is>
       </c>
       <c r="V29" t="b">
         <v>0</v>
       </c>
-      <c r="W29" t="inlineStr"/>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>41050</t>
+        </is>
+      </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/kassandra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
         <is>
-          <t>44,64381951149482</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>10,93139345085676</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>POINT (10.93139345085676 44.64381951149482)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Musica,Spettacoli,Teatro</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3569,83 +3555,67 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 85</t>
+          <t>Piazza Grande</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Spettacolo conclusivo dei corsi di Alta Formazione per cantanti lirici </t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:44+00:00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>info@teatrocomunalemodena.it</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:51+00:00</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-05-31T15:00:00+00:00</t>
+          <t>2022-05-29T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-05-31T16:00:00+00:00</t>
+          <t>2022-05-29T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolceamaro/@@images/2429e532-09b0-41e8-9f85-aa4a21287d10.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche/@@images/bbb27001-b4a3-4ea4-8c8f-b2ea069af5e6.jpeg</t>
         </is>
       </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-03-22T10:17:19+00:00</t>
+          <t>2022-05-23T10:13:30+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> ore 10.00</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> gratuito</t>
+          <t xml:space="preserve"> Euro 12 a partecipante</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>059 2033010</t>
-        </is>
-      </c>
+      <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr">
         <is>
-          <t>DolceAmaro</t>
+          <t>Free Walking Tour - Visite guidate tematiche</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>https://teatrocomunalemodena.it/</t>
-        </is>
-      </c>
+      <c r="U30" t="inlineStr"/>
       <c r="V30" t="b">
         <v>0</v>
       </c>
@@ -3654,7 +3624,7 @@
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolceamaro</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
@@ -3676,7 +3646,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Spettacoli,Concerti,Musica</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3686,110 +3656,112 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 85</t>
+          <t>Viale Caduti in Guerra, 196</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
+          <t>2020-09-17T12:45:54+00:00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Rassegna "L'altro suono festival" del Teatro comunale Pavarotti-Freni</t>
+          <t>Gli spettacoli di ERT al Teatro Tempio</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
+          <t>2014-09-30T12:50:00+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>info@teatrocomunalemodena.it</t>
+          <t>info@emiliaromagnateatro.com</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-06-01T15:00:00+00:00</t>
+          <t>2022-05-30T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-06-01T16:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/vinicio-capossela/@@images/9059bf61-ac70-4134-8ced-4386f5e54ad3.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/kassandra/@@images/29f75f21-a9f0-45e8-8056-8023ce88a666.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-04T10:45:34+00:00</t>
+          <t>2022-03-15T11:11:12+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Teatro Tempio</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> 31 maggio e 1 giugno, 3 giugno e dal 7 al 10 giugno ore 20.30  2, 4, 5, 11 e 12 giugno ore 19.00</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
+        </is>
+      </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr">
         <is>
-          <t>059 2033010</t>
+          <t>059/2163021</t>
         </is>
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Vinicio Capossela</t>
+          <t>Kassandra</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr">
         <is>
-          <t>https://teatrocomunalemodena.it/</t>
+          <t>http://www.emiliaromagnateatro.com</t>
         </is>
       </c>
       <c r="V31" t="b">
         <v>0</v>
       </c>
-      <c r="W31" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W31" t="inlineStr"/>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/vinicio-capossela</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/kassandra</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,64381951149482</t>
         </is>
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,93139345085676</t>
         </is>
       </c>
       <c r="AA31" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.93139345085676 44.64381951149482)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Iniziative per bambini,Manifestazioni sportive</t>
+          <t>Musica,Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3799,63 +3771,83 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
+          <t>Corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2022-05-11T07:00:46+00:00</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>2021-10-04T15:31:48+00:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spettacolo conclusivo dei corsi di Alta Formazione per cantanti lirici </t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr"/>
+          <t>2021-10-04T15:31:55+00:00</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>info@teatrocomunalemodena.it</t>
+        </is>
+      </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-06-02T06:00:00+00:00</t>
+          <t>2022-05-31T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-06-02T07:00:00+00:00</t>
+          <t>2022-05-31T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolceamaro/@@images/2429e532-09b0-41e8-9f85-aa4a21287d10.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
+          <t>2022-03-22T10:17:19+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Autodromo di Modena</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> gratuito</t>
+        </is>
+      </c>
       <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>059 2033010</t>
+        </is>
+      </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Go Kart, go!</t>
+          <t>DolceAmaro</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr"/>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>https://teatrocomunalemodena.it/</t>
+        </is>
+      </c>
       <c r="V32" t="b">
         <v>0</v>
       </c>
@@ -3864,7 +3856,7 @@
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolceamaro</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
@@ -3886,7 +3878,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3896,104 +3888,98 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2021-08-25T12:27:55+00:00</t>
+          <t>2022-03-23T16:26:44+00:00</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2021-08-25T12:28:08+00:00</t>
+          <t>2022-03-23T16:26:51+00:00</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-06-02T12:00:00+00:00</t>
+          <t>2022-06-01T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-05T13:00:00+00:00</t>
+          <t>2022-06-01T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>Immagine di una precedente edizione del mercato</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche/@@images/8e5a5fa0-1d05-41e2-9bd5-115da3e3c5ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-05-21T08:42:42+00:00</t>
+          <t>2022-05-23T10:16:24+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
+          <t>Ritrovo e partenza: Piazza Roma davanti all'Accademia Militare</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Euro 12 a partecipante</t>
+        </is>
+      </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Mercato europeo</t>
+          <t>Free Walking Tour - Visite guidate tematiche</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>http://www.mercatieuropei.com</t>
-        </is>
-      </c>
+      <c r="U33" t="inlineStr"/>
       <c r="V33" t="b">
         <v>0</v>
       </c>
-      <c r="W33" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W33" t="n">
+        <v>41123</v>
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
         <is>
-          <t>44,647524762696584</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>10,925428060260353</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA33" t="inlineStr">
         <is>
-          <t>POINT (10.925428060260353 44.647524762696584)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Altri eventi,Manifestazioni sportive</t>
+          <t>Spettacoli,Concerti,Musica</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -4003,67 +3989,79 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Zona tribune</t>
+          <t>Corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2022-05-11T07:50:51+00:00</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
+          <t>2021-10-04T15:31:48+00:00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Rassegna "L'altro suono festival" del Teatro comunale Pavarotti-Freni</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr"/>
+          <t>2021-10-04T15:31:55+00:00</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>info@teatrocomunalemodena.it</t>
+        </is>
+      </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-06-03T07:00:00+00:00</t>
+          <t>2022-06-01T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-06-03T08:00:00+00:00</t>
+          <t>2022-06-01T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>Immagine presa dal sito della Run 5.30 Modena</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/vinicio-capossela/@@images/9059bf61-ac70-4134-8ced-4386f5e54ad3.jpeg</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-05-04T10:45:34+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 5.30</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr"/>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>059 2033010</t>
+        </is>
+      </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Run 5.30</t>
+          <t>Vinicio Capossela</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr"/>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>https://teatrocomunalemodena.it/</t>
+        </is>
+      </c>
       <c r="V34" t="b">
         <v>0</v>
       </c>
@@ -4072,7 +4070,7 @@
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/vinicio-capossela</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
@@ -4094,7 +4092,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Iniziative per bambini,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4104,90 +4102,72 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
+          <t>2022-05-11T07:00:46+00:00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:01:08+00:00</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-06-02T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-02T07:00:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-11T07:01:08+00:00</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Autodromo di Modena</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
-        </is>
-      </c>
+      <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Go Kart, go!</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>https://www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U35" t="inlineStr"/>
       <c r="V35" t="b">
         <v>0</v>
       </c>
-      <c r="W35" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W35" t="n">
+        <v>41123</v>
       </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
@@ -4209,7 +4189,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4219,98 +4199,104 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
+          <t>2021-08-25T12:27:55+00:00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2021-08-25T12:28:08+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-02T12:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-06-05T13:00:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Immagine di una precedente edizione del mercato</t>
+        </is>
+      </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-21T08:42:42+00:00</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
-        </is>
-      </c>
+      <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Mercato europeo</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>http://www.mercatieuropei.com</t>
+        </is>
+      </c>
       <c r="V36" t="b">
         <v>0</v>
       </c>
-      <c r="W36" t="n">
-        <v>41123</v>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,647524762696584</t>
         </is>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,925428060260353</t>
         </is>
       </c>
       <c r="AA36" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.925428060260353 44.647524762696584)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4320,50 +4306,54 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Zona tribune</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
+          <t>2022-05-11T07:50:51+00:00</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-06-03T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della Run 5.30 Modena</t>
+        </is>
+      </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> ore 5.30</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
@@ -4372,7 +4362,7 @@
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Run 5.30</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
@@ -4385,7 +4375,7 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
@@ -4407,7 +4397,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4417,96 +4407,112 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2021-09-09T10:12:02+00:00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr"/>
+          <t>2022-05-21T09:18:35+00:00</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>FMAV - Palazzina dei Giardini</t>
+        </is>
+      </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr"/>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
+        </is>
+      </c>
       <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr"/>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.fmav.org</t>
         </is>
       </c>
       <c r="V38" t="b">
         <v>0</v>
       </c>
-      <c r="W38" t="inlineStr"/>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
+      </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA38" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4516,75 +4522,67 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U39" t="inlineStr"/>
       <c r="V39" t="b">
         <v>0</v>
       </c>
@@ -4593,7 +4591,7 @@
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
@@ -4615,7 +4613,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4630,45 +4628,45 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
+          <t>2022-05-21T10:32:36+00:00</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-05-21T10:36:00+00:00</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
@@ -4677,7 +4675,7 @@
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
@@ -4690,7 +4688,7 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
@@ -4712,7 +4710,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4722,102 +4720,96 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Commedia brillante</t>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>Teatro Cittadella</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr"/>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V41" t="b">
         <v>0</v>
       </c>
-      <c r="W41" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W41" t="inlineStr"/>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA41" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4827,96 +4819,106 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2021-08-06T11:34:26+00:00</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr"/>
+          <t>2022-02-08T10:09:23+00:00</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>Polisportiva Madonnina</t>
+        </is>
+      </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
-      <c r="R42" t="inlineStr"/>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
         </is>
       </c>
       <c r="V42" t="b">
         <v>0</v>
       </c>
-      <c r="W42" t="inlineStr"/>
+      <c r="W42" t="n">
+        <v>41123</v>
+      </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA42" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4926,54 +4928,50 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
@@ -4982,7 +4980,7 @@
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
@@ -4995,7 +4993,7 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -5037,7 +5035,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Commedia brillante</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5048,23 +5046,23 @@
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
@@ -5074,7 +5072,7 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
@@ -5087,7 +5085,7 @@
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
@@ -5100,7 +5098,7 @@
       </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
@@ -5122,7 +5120,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5132,58 +5130,50 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
@@ -5192,42 +5182,44 @@
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr"/>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V45" t="b">
         <v>0</v>
       </c>
-      <c r="W45" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W45" t="inlineStr"/>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA45" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5237,83 +5229,67 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-03-31T08:55:39+00:00</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U46" t="inlineStr"/>
       <c r="V46" t="b">
         <v>0</v>
       </c>
@@ -5322,7 +5298,7 @@
       </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
@@ -5344,7 +5320,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5354,96 +5330,102 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr"/>
+          <t>2022-03-19T09:28:51+00:00</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Teatro Cittadella</t>
+        </is>
+      </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr"/>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U47" t="inlineStr"/>
       <c r="V47" t="b">
         <v>0</v>
       </c>
-      <c r="W47" t="inlineStr"/>
+      <c r="W47" t="n">
+        <v>41123</v>
+      </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA47" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5453,50 +5435,58 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
+          <t>2022-02-25T14:15:33+00:00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr"/>
+          <t>2022-02-28T15:13:23+00:00</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
@@ -5505,37 +5495,35 @@
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U48" t="inlineStr"/>
       <c r="V48" t="b">
         <v>0</v>
       </c>
-      <c r="W48" t="inlineStr"/>
+      <c r="W48" t="n">
+        <v>41123</v>
+      </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA48" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -5552,54 +5540,62 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr"/>
+          <t>2021-06-10T16:47:55+00:00</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
+          <t>2021-06-10T16:48:45+00:00</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>traborghiecontrade@libero.it</t>
+          <t>anticoinpiazzagrande@gmail.com</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
+          <t>2022-05-06T10:18:45+00:00</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
@@ -5607,18 +5603,18 @@
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr">
         <is>
-          <t>333/9103351</t>
+          <t>340 6059686 oppure 338 2098995</t>
         </is>
       </c>
       <c r="S49" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V49" t="b">
@@ -5629,7 +5625,7 @@
       </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
@@ -5682,23 +5678,23 @@
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
         </is>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
+          <t>2022-05-10T08:24:06+00:00</t>
         </is>
       </c>
       <c r="M50" t="inlineStr"/>
@@ -5728,7 +5724,7 @@
       <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
@@ -5781,23 +5777,23 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
+          <t>2022-05-10T08:26:10+00:00</t>
         </is>
       </c>
       <c r="M51" t="inlineStr"/>
@@ -5827,7 +5823,7 @@
       <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
@@ -5849,7 +5845,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5859,87 +5855,394 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr"/>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V52" t="b">
         <v>0</v>
       </c>
-      <c r="W52" t="inlineStr"/>
+      <c r="W52" t="n">
+        <v>41123</v>
+      </c>
       <c r="X52" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+        </is>
+      </c>
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t>44,64582</t>
+        </is>
+      </c>
+      <c r="Z52" t="inlineStr">
+        <is>
+          <t>10,92572</t>
+        </is>
+      </c>
+      <c r="AA52" t="inlineStr">
+        <is>
+          <t>POINT (10.92572 44.64582)</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2022-09-17T22:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>2022-09-18T21:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:26:55+00:00</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
+      <c r="R53" t="inlineStr"/>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V53" t="b">
+        <v>0</v>
+      </c>
+      <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z53" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA53" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2022-10-15T22:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>2022-10-16T21:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:27:35+00:00</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+      <c r="R54" t="inlineStr"/>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V54" t="b">
+        <v>0</v>
+      </c>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y54" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z54" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA54" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V55" t="b">
+        <v>0</v>
+      </c>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y52" t="inlineStr">
+      <c r="Y55" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z52" t="inlineStr">
+      <c r="Z55" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA52" t="inlineStr">
+      <c r="AA55" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Tue May 24 01:18:44 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA55"/>
+  <dimension ref="A1:AA54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1867,7 +1867,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni</t>
+          <t>Musica,Spettacoli,Concerti</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1877,67 +1877,79 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Via San Carlo, 5</t>
+          <t>Corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2022-05-11T10:57:24+00:00</t>
+          <t>2021-10-04T15:31:48+00:00</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Seminario in presenza e anche online</t>
+          <t>Stagione sinfonica del Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2022-05-11T10:57:31+00:00</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr"/>
+          <t>2021-10-04T15:31:55+00:00</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>info@teatrocomunalemodena.it</t>
+        </is>
+      </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2022-05-23T10:00:00+00:00</t>
+          <t>2022-05-24T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2022-05-23T11:00:00+00:00</t>
+          <t>2022-05-24T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/ripensare-la-scuola-sergio-neri-e-il-tempo-pieno/@@images/ab73114a-4698-40cd-a91c-939e7c30f450.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/spira-mirabilis/@@images/d03f1ad6-ae7f-40b6-908c-bad72cf37db9.jpeg</t>
         </is>
       </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2022-05-12T12:39:29+00:00</t>
+          <t>2022-05-21T07:28:23+00:00</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Sala conferenze Fondazione San Carlo</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 15.30 alle 18.30</t>
+          <t xml:space="preserve"> Alle ore 20.30</t>
         </is>
       </c>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>059 2033010</t>
+        </is>
+      </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>Ripensare la scuola: Sergio Neri e il tempo pieno</t>
+          <t>Spira Mirabilis</t>
         </is>
       </c>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>https://teatrocomunalemodena.it/</t>
+        </is>
+      </c>
       <c r="V14" t="b">
         <v>0</v>
       </c>
@@ -1946,7 +1958,7 @@
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/ripensare-la-scuola-sergio-neri-e-il-tempo-pieno</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/spira-mirabilis</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
@@ -1968,7 +1980,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Altri eventi,Mercati</t>
+          <t>Altri eventi,Musica</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1978,50 +1990,54 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Ingresso da viale Berengario</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2020-12-29T15:02:32+00:00</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
+          <t>2022-05-20T10:02:04+00:00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2020-12-29T15:05:00+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2022-01-03T14:00:00+00:00</t>
+          <t>2022-05-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2022-12-26T14:59:00+00:00</t>
+          <t>2022-06-30T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2021-12-28T10:39:07+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Piazzetta Pomposa</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
+          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
         </is>
       </c>
       <c r="O15" t="inlineStr"/>
@@ -2030,26 +2046,20 @@
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr">
         <is>
-          <t>Mercato settimanale del lunedì</t>
+          <t>Serate in Pomposa - 1° edizione</t>
         </is>
       </c>
       <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.com/</t>
-        </is>
-      </c>
+      <c r="U15" t="inlineStr"/>
       <c r="V15" t="b">
         <v>0</v>
       </c>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W15" t="n">
+        <v>41123</v>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
@@ -2071,7 +2081,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Musica,Spettacoli,Concerti</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2079,60 +2089,56 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Corso Canalgrande, 85</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
+          <t>2021-05-18T13:18:17+00:00</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Stagione sinfonica del Teatro comunale Pavarotti-Freni</t>
+          <t>Quattro iniziative rivolte a bambini e famiglie</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
+          <t>2021-05-18T13:19:13+00:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>info@teatrocomunalemodena.it</t>
+          <t>info@modenamoremio.it</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2022-05-24T15:00:00+00:00</t>
+          <t>2022-05-04T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2022-05-24T16:00:00+00:00</t>
+          <t>2022-05-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/spira-mirabilis/@@images/d03f1ad6-ae7f-40b6-908c-bad72cf37db9.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/i-mercoledi-di-maggio/@@images/9dabb3cb-8df7-4a66-a959-2d9e8db832a9.jpeg</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2022-05-21T07:28:23+00:00</t>
+          <t>2022-04-22T13:36:36+00:00</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Piazze del centro storico, vedi nel programma</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Alle ore 20.30</t>
+          <t xml:space="preserve"> mercoledì 4, 11, 18 e 25 maggio alle ore 17.00</t>
         </is>
       </c>
       <c r="O16" t="inlineStr"/>
@@ -2140,29 +2146,31 @@
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
         <is>
-          <t>059 2033010</t>
+          <t>340 2884443</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>Spira Mirabilis</t>
+          <t>I mercoledì di maggio</t>
         </is>
       </c>
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr">
         <is>
-          <t>https://teatrocomunalemodena.it/</t>
+          <t>www.modenamoremio.it</t>
         </is>
       </c>
       <c r="V16" t="b">
         <v>0</v>
       </c>
-      <c r="W16" t="n">
-        <v>41123</v>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/spira-mirabilis</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/i-mercoledi-di-maggio</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
@@ -2184,7 +2192,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Altri eventi,Musica</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2194,63 +2202,63 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Piazza della Manifattura Tabacchi</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:04+00:00</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:44+00:00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-03-23T16:26:51+00:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2022-05-12T09:00:00+00:00</t>
+          <t>2022-05-25T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2022-06-30T10:00:00+00:00</t>
+          <t>2022-05-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy6_of_free-walking-tour-visite-guidate-tematiche/@@images/3423aebc-8b5e-4d1d-8f35-b2dce36dab21.jpeg</t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-05-23T10:18:25+00:00</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Piazzetta Pomposa</t>
+          <t>Ritrovo e partenza: Piazza della Manifattura Tabacchi</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Euro 12 a partecipante</t>
+        </is>
+      </c>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Serate in Pomposa - 1° edizione</t>
+          <t>Free Walking Tour - Visite guidate tematiche</t>
         </is>
       </c>
       <c r="T17" t="inlineStr"/>
@@ -2263,7 +2271,7 @@
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy6_of_free-walking-tour-visite-guidate-tematiche</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
@@ -2285,7 +2293,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2293,110 +2301,120 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Viale Jacopo Barozzi, 31</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2021-05-18T13:18:17+00:00</t>
+          <t>2021-05-13T08:16:32+00:00</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Quattro iniziative rivolte a bambini e famiglie</t>
+          <t>Conferenze, eventi per famiglie, serate speciali e visite guidate</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2021-05-18T13:19:13+00:00</t>
+          <t>2021-05-13T08:16:59+00:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>info@modenamoremio.it</t>
+          <t>info@planetariodimodena.it</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2022-05-04T13:00:00+00:00</t>
+          <t>2022-05-22T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2022-05-25T14:00:00+00:00</t>
+          <t>2022-05-29T09:11:35+00:00</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/i-mercoledi-di-maggio/@@images/9dabb3cb-8df7-4a66-a959-2d9e8db832a9.jpeg</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy7_of_le-iniziative-al-planetario/@@images/bce50dab-bfa1-40ef-9085-04f7bab6d51d.jpeg</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Immagine del pianeta Terra - da unsplash.com</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2022-04-22T13:36:36+00:00</t>
+          <t>2022-05-17T08:44:09+00:00</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Piazze del centro storico, vedi nel programma</t>
+          <t>Civico Planetario</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> mercoledì 4, 11, 18 e 25 maggio alle ore 17.00</t>
+          <t xml:space="preserve"> domenica 22 e domenica 29 maggio ore 15  giovedì 26 maggio ore 21  sabato 28 maggio ore 21</t>
         </is>
       </c>
       <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> a pagamento  vedi costo del biglietto nel programma o sul sito del Planetario: www.planetariodimodena.it </t>
+        </is>
+      </c>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr">
         <is>
-          <t>340 2884443</t>
+          <t>059 224726</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>I mercoledì di maggio</t>
+          <t>Le iniziative al Planetario</t>
         </is>
       </c>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr">
         <is>
-          <t>www.modenamoremio.it</t>
+          <t>https://www.planetariodimodena.it</t>
         </is>
       </c>
       <c r="V18" t="b">
         <v>0</v>
       </c>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W18" t="n">
+        <v>41123</v>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/i-mercoledi-di-maggio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy7_of_le-iniziative-al-planetario</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,64907001920466</t>
         </is>
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,917829960080724</t>
         </is>
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.917829960080724 44.64907001920466)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2404,65 +2422,57 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Piazza della Manifattura Tabacchi</t>
-        </is>
-      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:44+00:00</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
+          <t>2022-05-17T09:05:44+00:00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Esibizioni, incontri tematici, esposizioni di auto sono in programma dal 26 al 29 maggio</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:51+00:00</t>
+          <t>2022-05-17T09:05:52+00:00</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2022-05-25T15:00:00+00:00</t>
+          <t>2022-05-26T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2022-05-25T16:00:00+00:00</t>
+          <t>2022-05-29T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy6_of_free-walking-tour-visite-guidate-tematiche/@@images/3423aebc-8b5e-4d1d-8f35-b2dce36dab21.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/motor-valley-fest-quarta-edizione/@@images/b4ee995e-3238-4045-932b-c7b1819db8ce.jpeg</t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2022-05-23T10:18:25+00:00</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>Ritrovo e partenza: Piazza della Manifattura Tabacchi</t>
-        </is>
-      </c>
+          <t>2022-05-17T09:05:52+00:00</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> vedi orari nel programma: motorvalley.it/motorvalleyfest</t>
         </is>
       </c>
       <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Euro 12 a partecipante</t>
-        </is>
-      </c>
+      <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr">
         <is>
-          <t>Free Walking Tour - Visite guidate tematiche</t>
+          <t>Motor Valley Fest - Quarta edizione</t>
         </is>
       </c>
       <c r="T19" t="inlineStr"/>
@@ -2475,7 +2485,7 @@
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy6_of_free-walking-tour-visite-guidate-tematiche</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/motor-valley-fest-quarta-edizione</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
@@ -2497,7 +2507,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Altri eventi,Iniziative per bambini</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2507,87 +2517,71 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Viale Jacopo Barozzi, 31</t>
+          <t>centro storico</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2021-05-13T08:16:32+00:00</t>
+          <t>2022-04-29T10:05:46+00:00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Conferenze, eventi per famiglie, serate speciali e visite guidate</t>
+          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2021-05-13T08:16:59+00:00</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>info@planetariodimodena.it</t>
-        </is>
-      </c>
+          <t>2022-04-29T10:06:04+00:00</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2022-05-22T07:00:00+00:00</t>
+          <t>2022-05-01T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2022-05-29T09:11:35+00:00</t>
+          <t>2022-07-17T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy7_of_le-iniziative-al-planetario/@@images/bce50dab-bfa1-40ef-9085-04f7bab6d51d.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Immagine del pianeta Terra - da unsplash.com</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2022-05-17T08:44:09+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Civico Planetario</t>
+          <t>Piazza Torre</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> domenica 22 e domenica 29 maggio ore 15  giovedì 26 maggio ore 21  sabato 28 maggio ore 21</t>
+          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> a pagamento  vedi costo del biglietto nel programma o sul sito del Planetario: www.planetariodimodena.it </t>
-        </is>
-      </c>
+      <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>059 224726</t>
-        </is>
-      </c>
+      <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr">
         <is>
-          <t>Le iniziative al Planetario</t>
+          <t>Torre Ghirlandina, aperture serali</t>
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>https://www.planetariodimodena.it</t>
-        </is>
-      </c>
+      <c r="U20" t="inlineStr"/>
       <c r="V20" t="b">
         <v>0</v>
       </c>
@@ -2596,29 +2590,29 @@
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy7_of_le-iniziative-al-planetario</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>44,64907001920466</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>10,917829960080724</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>POINT (10.917829960080724 44.64907001920466)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato,Manifestazioni sportive</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2626,48 +2620,56 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Corso Canalgrande, 103</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2022-05-17T09:05:44+00:00</t>
+          <t>2022-05-05T08:41:26+00:00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Esibizioni, incontri tematici, esposizioni di auto sono in programma dal 26 al 29 maggio</t>
+          <t>Appuntamenti letterari al femminile</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2022-05-17T09:05:52+00:00</t>
+          <t>2022-05-05T09:23:17+00:00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2022-05-26T08:00:00+00:00</t>
+          <t>2022-05-07T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2022-05-29T09:00:00+00:00</t>
+          <t>2022-05-28T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/motor-valley-fest-quarta-edizione/@@images/b4ee995e-3238-4045-932b-c7b1819db8ce.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/scrittrici-inchiostro/@@images/318772ef-8170-4984-9e11-f2516c109708.jpeg</t>
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2022-05-17T09:05:52+00:00</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr"/>
+          <t>2022-05-05T09:23:17+00:00</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Chiostro di Palazzo Santa Margherita</t>
+        </is>
+      </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> vedi orari nel programma: motorvalley.it/motorvalleyfest</t>
+          <t xml:space="preserve"> i sabati di maggio alle ore 18</t>
         </is>
       </c>
       <c r="O21" t="inlineStr"/>
@@ -2676,7 +2678,7 @@
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr">
         <is>
-          <t>Motor Valley Fest - Quarta edizione</t>
+          <t>Scrittrici inChiostro</t>
         </is>
       </c>
       <c r="T21" t="inlineStr"/>
@@ -2689,7 +2691,7 @@
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/motor-valley-fest-quarta-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/scrittrici-inchiostro</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
@@ -2711,7 +2713,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2721,67 +2723,63 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>centro storico</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2022-04-29T10:05:46+00:00</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:24:22+00:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2022-05-01T09:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2022-07-17T10:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-05-17T07:27:36+00:00</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Piazza Torre</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, aperture serali</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T22" t="inlineStr"/>
@@ -2794,7 +2792,7 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
@@ -2816,7 +2814,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2826,54 +2824,50 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 103</t>
+          <t>via Emilia Centro angolo Piazza Matteotti</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2022-05-05T08:41:26+00:00</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Appuntamenti letterari al femminile</t>
-        </is>
-      </c>
+          <t>2022-05-13T10:01:30+00:00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2022-05-05T09:23:17+00:00</t>
+          <t>2022-05-13T10:03:13+00:00</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2022-05-07T07:00:00+00:00</t>
+          <t>2022-05-28T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2022-05-28T08:00:00+00:00</t>
+          <t>2022-06-05T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/scrittrici-inchiostro/@@images/318772ef-8170-4984-9e11-f2516c109708.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mostra-di-ricamo-e-merletto-da-ieri-a-oggi-la-tradizione-continua/@@images/fecdcb1a-b768-40a7-8809-d18fd2116bab.jpeg</t>
         </is>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2022-05-05T09:23:17+00:00</t>
+          <t>2022-05-13T10:03:32+00:00</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Chiostro di Palazzo Santa Margherita</t>
+          <t>Chiesa S.Giovanni Battista</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> i sabati di maggio alle ore 18</t>
+          <t xml:space="preserve"> dal lunedì al venerdì ore 10-18  sabato e domenica ore 10-19</t>
         </is>
       </c>
       <c r="O23" t="inlineStr"/>
@@ -2882,7 +2876,7 @@
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr">
         <is>
-          <t>Scrittrici inChiostro</t>
+          <t>Mostra di ricamo e merletto "Da ieri a oggi.....la tradizione continua"</t>
         </is>
       </c>
       <c r="T23" t="inlineStr"/>
@@ -2895,7 +2889,7 @@
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/scrittrici-inchiostro</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mostra-di-ricamo-e-merletto-da-ieri-a-oggi-la-tradizione-continua</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
@@ -2917,7 +2911,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2927,63 +2921,67 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
+          <t>2022-02-25T14:15:15+00:00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-02-25T14:15:33+00:00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-05-28T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-05-28T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dai-comacini-ai-maestri-campionesi/@@images/d5218bc2-dc59-43df-b1a3-4f32b072e82f.jpeg</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2022-05-17T07:27:36+00:00</t>
+          <t>2022-02-28T15:10:52+00:00</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
-        </is>
-      </c>
+      <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Dai Comacini ai Maestri Campionesi</t>
         </is>
       </c>
       <c r="T24" t="inlineStr"/>
@@ -2996,7 +2994,7 @@
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dai-comacini-ai-maestri-campionesi</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
@@ -3018,7 +3016,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3028,50 +3026,50 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>via Emilia Centro angolo Piazza Matteotti</t>
+          <t>Piazza Grande</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2022-05-13T10:01:30+00:00</t>
+          <t>2022-03-23T16:26:44+00:00</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2022-05-13T10:03:13+00:00</t>
+          <t>2022-03-23T16:26:51+00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2022-05-28T09:00:00+00:00</t>
+          <t>2022-03-19T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2022-06-05T10:00:00+00:00</t>
+          <t>2022-05-28T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mostra-di-ricamo-e-merletto-da-ieri-a-oggi-la-tradizione-continua/@@images/fecdcb1a-b768-40a7-8809-d18fd2116bab.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/free-walking-tour-visite-guidate-del-centro-storico-di-modena/@@images/26b88750-ac47-44ab-bc5c-66df7933f860.jpeg</t>
         </is>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2022-05-13T10:03:32+00:00</t>
+          <t>2022-03-23T16:27:28+00:00</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Chiesa S.Giovanni Battista</t>
+          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal lunedì al venerdì ore 10-18  sabato e domenica ore 10-19</t>
+          <t xml:space="preserve"> Tutti i sabati dal 19 marzo al 28 maggio alle ore 15.30</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
@@ -3080,7 +3078,7 @@
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>Mostra di ricamo e merletto "Da ieri a oggi.....la tradizione continua"</t>
+          <t>Free Walking Tour - Visite guidate del centro storico di Modena</t>
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
@@ -3093,7 +3091,7 @@
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mostra-di-ricamo-e-merletto-da-ieri-a-oggi-la-tradizione-continua</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/free-walking-tour-visite-guidate-del-centro-storico-di-modena</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
@@ -3115,7 +3113,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Concerti,Musica</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3125,67 +3123,67 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Largo S.Francesco</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-05-10T10:04:48+00:00</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Diciottesima edizione</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-05-10T10:08:30+00:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2022-05-28T13:00:00+00:00</t>
+          <t>2022-05-29T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2022-05-28T14:00:00+00:00</t>
+          <t>2022-05-29T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dai-comacini-ai-maestri-campionesi/@@images/d5218bc2-dc59-43df-b1a3-4f32b072e82f.jpeg</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-rosa-mistica/@@images/5d666bc9-d035-4acb-9903-21fd8e9003bf.jpeg</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2022-02-28T15:10:52+00:00</t>
+          <t>2022-05-10T10:13:42+00:00</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Chiesa di San Francesco</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 16.00</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso libero</t>
+        </is>
+      </c>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr">
         <is>
-          <t>Dai Comacini ai Maestri Campionesi</t>
+          <t>Concerto "Rosa mistica"</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
@@ -3198,7 +3196,7 @@
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dai-comacini-ai-maestri-campionesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-rosa-mistica</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
@@ -3220,82 +3218,108 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Modena</t>
+          <t>Montale Rangone</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Piazza Grande</t>
+          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:44+00:00</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>2021-04-26T15:03:43+00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:51+00:00</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr"/>
+          <t>2021-04-26T15:06:06+00:00</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>museo@parcomontale.it</t>
+        </is>
+      </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2022-03-19T16:00:00+00:00</t>
+          <t>2022-04-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2022-05-28T16:00:00+00:00</t>
+          <t>2022-06-19T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/free-walking-tour-visite-guidate-del-centro-storico-di-modena/@@images/26b88750-ac47-44ab-bc5c-66df7933f860.jpeg</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Parco archeologico della Terramara di Montale</t>
+        </is>
+      </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-03-23T16:27:28+00:00</t>
+          <t>2022-03-28T14:43:35+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tutti i sabati dal 19 marzo al 28 maggio alle ore 15.30</t>
+          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
+        </is>
+      </c>
       <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+        </is>
+      </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Free Walking Tour - Visite guidate del centro storico di Modena</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>http://www.parcomontale.it/it</t>
+        </is>
+      </c>
       <c r="V27" t="b">
         <v>0</v>
       </c>
-      <c r="W27" t="n">
-        <v>41123</v>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>41050</t>
+        </is>
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/free-walking-tour-visite-guidate-del-centro-storico-di-modena</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3317,7 +3341,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Concerti,Musica</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3327,67 +3351,63 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Largo S.Francesco</t>
+          <t>Piazza Grande</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2022-05-10T10:04:48+00:00</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Diciottesima edizione</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:44+00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2022-05-10T10:08:30+00:00</t>
+          <t>2022-03-23T16:26:51+00:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-05-29T10:00:00+00:00</t>
+          <t>2022-05-29T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-05-29T11:00:00+00:00</t>
+          <t>2022-05-29T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-rosa-mistica/@@images/5d666bc9-d035-4acb-9903-21fd8e9003bf.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche/@@images/bbb27001-b4a3-4ea4-8c8f-b2ea069af5e6.jpeg</t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-05-10T10:13:42+00:00</t>
+          <t>2022-05-23T10:13:30+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Chiesa di San Francesco</t>
+          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 16.00</t>
+          <t xml:space="preserve"> ore 10.00</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso libero</t>
+          <t xml:space="preserve"> Euro 12 a partecipante</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Concerto "Rosa mistica"</t>
+          <t>Free Walking Tour - Visite guidate tematiche</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
@@ -3400,7 +3420,7 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-rosa-mistica</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3422,95 +3442,75 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
+          <t>Altri eventi,Mercati</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Montale Rangone</t>
+          <t>Modena</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
+          <t>Ingresso da viale Berengario</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2021-04-26T15:03:43+00:00</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
-        </is>
-      </c>
+          <t>2020-12-29T15:02:32+00:00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2021-04-26T15:06:06+00:00</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>museo@parcomontale.it</t>
-        </is>
-      </c>
+          <t>2020-12-29T15:05:00+00:00</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-04-03T14:00:00+00:00</t>
+          <t>2022-01-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-06-19T15:00:00+00:00</t>
+          <t>2022-12-26T14:59:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>Parco archeologico della Terramara di Montale</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-03-28T14:43:35+00:00</t>
+          <t>2021-12-28T10:39:07+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
+          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
-        </is>
-      </c>
+      <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
-        </is>
-      </c>
+      <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Mercato settimanale del lunedì</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr">
         <is>
-          <t>http://www.parcomontale.it/it</t>
+          <t>http://www.consorzioilmercato.com/</t>
         </is>
       </c>
       <c r="V29" t="b">
@@ -3518,12 +3518,12 @@
       </c>
       <c r="W29" t="inlineStr">
         <is>
-          <t>41050</t>
+          <t>41121</t>
         </is>
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
@@ -3545,7 +3545,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3555,98 +3555,112 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Piazza Grande</t>
+          <t>Viale Caduti in Guerra, 196</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:44+00:00</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr"/>
+          <t>2020-09-17T12:45:54+00:00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Gli spettacoli di ERT al Teatro Tempio</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:51+00:00</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr"/>
+          <t>2014-09-30T12:50:00+00:00</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>info@emiliaromagnateatro.com</t>
+        </is>
+      </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-05-29T15:00:00+00:00</t>
+          <t>2022-05-30T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-05-29T16:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche/@@images/bbb27001-b4a3-4ea4-8c8f-b2ea069af5e6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/kassandra/@@images/29f75f21-a9f0-45e8-8056-8023ce88a666.jpeg</t>
         </is>
       </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-05-23T10:13:30+00:00</t>
+          <t>2022-03-15T11:11:12+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
+          <t>Teatro Tempio</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 10.00</t>
+          <t xml:space="preserve"> 31 maggio e 1 giugno, 3 giugno e dal 7 al 10 giugno ore 20.30  2, 4, 5, 11 e 12 giugno ore 19.00</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Euro 12 a partecipante</t>
+          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>059/2163021</t>
+        </is>
+      </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Free Walking Tour - Visite guidate tematiche</t>
+          <t>Kassandra</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>http://www.emiliaromagnateatro.com</t>
+        </is>
+      </c>
       <c r="V30" t="b">
         <v>0</v>
       </c>
-      <c r="W30" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W30" t="inlineStr"/>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/kassandra</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,64381951149482</t>
         </is>
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,93139345085676</t>
         </is>
       </c>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.93139345085676 44.64381951149482)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Musica,Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3656,112 +3670,114 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Viale Caduti in Guerra, 196</t>
+          <t>Corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2020-09-17T12:45:54+00:00</t>
+          <t>2021-10-04T15:31:48+00:00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Gli spettacoli di ERT al Teatro Tempio</t>
+          <t xml:space="preserve">Spettacolo conclusivo dei corsi di Alta Formazione per cantanti lirici </t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2014-09-30T12:50:00+00:00</t>
+          <t>2021-10-04T15:31:55+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>info@emiliaromagnateatro.com</t>
+          <t>info@teatrocomunalemodena.it</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-05-30T22:00:00+00:00</t>
+          <t>2022-05-31T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-05-31T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/kassandra/@@images/29f75f21-a9f0-45e8-8056-8023ce88a666.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolceamaro/@@images/2429e532-09b0-41e8-9f85-aa4a21287d10.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-03-15T11:11:12+00:00</t>
+          <t>2022-03-22T10:17:19+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Teatro Tempio</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 31 maggio e 1 giugno, 3 giugno e dal 7 al 10 giugno ore 20.30  2, 4, 5, 11 e 12 giugno ore 19.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
+          <t xml:space="preserve"> gratuito</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr">
         <is>
-          <t>059/2163021</t>
+          <t>059 2033010</t>
         </is>
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Kassandra</t>
+          <t>DolceAmaro</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr">
         <is>
-          <t>http://www.emiliaromagnateatro.com</t>
+          <t>https://teatrocomunalemodena.it/</t>
         </is>
       </c>
       <c r="V31" t="b">
         <v>0</v>
       </c>
-      <c r="W31" t="inlineStr"/>
+      <c r="W31" t="n">
+        <v>41123</v>
+      </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/kassandra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolceamaro</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
         <is>
-          <t>44,64381951149482</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>10,93139345085676</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA31" t="inlineStr">
         <is>
-          <t>POINT (10.93139345085676 44.64381951149482)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Musica,Spettacoli,Teatro</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3771,83 +3787,67 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 85</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Spettacolo conclusivo dei corsi di Alta Formazione per cantanti lirici </t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:44+00:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>info@teatrocomunalemodena.it</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:51+00:00</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-05-31T15:00:00+00:00</t>
+          <t>2022-06-01T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-05-31T16:00:00+00:00</t>
+          <t>2022-06-01T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolceamaro/@@images/2429e532-09b0-41e8-9f85-aa4a21287d10.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche/@@images/8e5a5fa0-1d05-41e2-9bd5-115da3e3c5ea.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-03-22T10:17:19+00:00</t>
+          <t>2022-05-23T10:16:24+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Ritrovo e partenza: Piazza Roma davanti all'Accademia Militare</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> gratuito</t>
+          <t xml:space="preserve"> Euro 12 a partecipante</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>059 2033010</t>
-        </is>
-      </c>
+      <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr">
         <is>
-          <t>DolceAmaro</t>
+          <t>Free Walking Tour - Visite guidate tematiche</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr">
-        <is>
-          <t>https://teatrocomunalemodena.it/</t>
-        </is>
-      </c>
+      <c r="U32" t="inlineStr"/>
       <c r="V32" t="b">
         <v>0</v>
       </c>
@@ -3856,7 +3856,7 @@
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolceamaro</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Concerti,Musica</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3888,21 +3888,29 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:44+00:00</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
+          <t>2021-10-04T15:31:48+00:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Rassegna "L'altro suono festival" del Teatro comunale Pavarotti-Freni</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:51+00:00</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr"/>
+          <t>2021-10-04T15:31:55+00:00</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>info@teatrocomunalemodena.it</t>
+        </is>
+      </c>
       <c r="H33" t="inlineStr">
         <is>
           <t>2022-06-01T15:00:00+00:00</t>
@@ -3915,40 +3923,44 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche/@@images/8e5a5fa0-1d05-41e2-9bd5-115da3e3c5ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/vinicio-capossela/@@images/9059bf61-ac70-4134-8ced-4386f5e54ad3.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-05-23T10:16:24+00:00</t>
+          <t>2022-05-04T10:45:34+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Ritrovo e partenza: Piazza Roma davanti all'Accademia Militare</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Euro 12 a partecipante</t>
-        </is>
-      </c>
+      <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>059 2033010</t>
+        </is>
+      </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Free Walking Tour - Visite guidate tematiche</t>
+          <t>Vinicio Capossela</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr"/>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>https://teatrocomunalemodena.it/</t>
+        </is>
+      </c>
       <c r="V33" t="b">
         <v>0</v>
       </c>
@@ -3957,7 +3969,7 @@
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/vinicio-capossela</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
@@ -3979,7 +3991,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Spettacoli,Concerti,Musica</t>
+          <t>Iniziative per bambini,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3989,79 +4001,63 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 85</t>
+          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Rassegna "L'altro suono festival" del Teatro comunale Pavarotti-Freni</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:00:46+00:00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>info@teatrocomunalemodena.it</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:01:08+00:00</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-06-01T15:00:00+00:00</t>
+          <t>2022-06-02T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-06-01T16:00:00+00:00</t>
+          <t>2022-06-02T07:00:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/vinicio-capossela/@@images/9059bf61-ac70-4134-8ced-4386f5e54ad3.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-04T10:45:34+00:00</t>
+          <t>2022-05-11T07:01:08+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Autodromo di Modena</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>059 2033010</t>
-        </is>
-      </c>
+      <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Vinicio Capossela</t>
+          <t>Go Kart, go!</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>https://teatrocomunalemodena.it/</t>
-        </is>
-      </c>
+      <c r="U34" t="inlineStr"/>
       <c r="V34" t="b">
         <v>0</v>
       </c>
@@ -4070,7 +4066,7 @@
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/vinicio-capossela</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
@@ -4092,7 +4088,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Iniziative per bambini,Manifestazioni sportive</t>
+          <t>Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4102,50 +4098,54 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2022-05-11T07:00:46+00:00</t>
+          <t>2021-08-25T12:27:55+00:00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
+          <t>2021-08-25T12:28:08+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-06-02T06:00:00+00:00</t>
+          <t>2022-06-02T12:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-06-02T07:00:00+00:00</t>
+          <t>2022-06-05T13:00:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Immagine di una precedente edizione del mercato</t>
+        </is>
+      </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
+          <t>2022-05-21T08:42:42+00:00</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Autodromo di Modena</t>
+          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
+          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
@@ -4154,42 +4154,48 @@
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Go Kart, go!</t>
+          <t>Mercato europeo</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr"/>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>http://www.mercatieuropei.com</t>
+        </is>
+      </c>
       <c r="V35" t="b">
         <v>0</v>
       </c>
-      <c r="W35" t="n">
-        <v>41123</v>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,647524762696584</t>
         </is>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,925428060260353</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.925428060260353 44.647524762696584)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4199,54 +4205,54 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Zona tribune</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2021-08-25T12:27:55+00:00</t>
+          <t>2022-05-11T07:50:51+00:00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2021-08-25T12:28:08+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-06-02T12:00:00+00:00</t>
+          <t>2022-06-03T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-05T13:00:00+00:00</t>
+          <t>2022-06-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Immagine di una precedente edizione del mercato</t>
+          <t>Immagine presa dal sito della Run 5.30 Modena</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-05-21T08:42:42+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
+          <t xml:space="preserve"> ore 5.30</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
@@ -4255,48 +4261,42 @@
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Mercato europeo</t>
+          <t>Run 5.30</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr">
-        <is>
-          <t>http://www.mercatieuropei.com</t>
-        </is>
-      </c>
+      <c r="U36" t="inlineStr"/>
       <c r="V36" t="b">
         <v>0</v>
       </c>
-      <c r="W36" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W36" t="n">
+        <v>41123</v>
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>44,647524762696584</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>10,925428060260353</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA36" t="inlineStr">
         <is>
-          <t>POINT (10.925428060260353 44.647524762696584)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Altri eventi,Manifestazioni sportive</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4306,76 +4306,90 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Zona tribune</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2022-05-11T07:50:51+00:00</t>
+          <t>2021-09-09T10:12:02+00:00</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-03T07:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-03T08:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>Immagine presa dal sito della Run 5.30 Modena</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 5.30</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr"/>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
+        </is>
+      </c>
       <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr"/>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Run 5.30</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr"/>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V37" t="b">
         <v>0</v>
       </c>
-      <c r="W37" t="n">
-        <v>41123</v>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
@@ -4397,7 +4411,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4407,90 +4421,76 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:25:56+00:00</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
         </is>
       </c>
       <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>https://www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U38" t="inlineStr"/>
       <c r="V38" t="b">
         <v>0</v>
       </c>
-      <c r="W38" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W38" t="n">
+        <v>41123</v>
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
@@ -4512,7 +4512,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4522,63 +4522,59 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
+          <t>2022-05-21T10:32:36+00:00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-21T10:36:00+00:00</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
-        </is>
-      </c>
+      <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
@@ -4591,7 +4587,7 @@
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
@@ -4613,7 +4609,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4623,50 +4619,50 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>Piazza Matteotti</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
@@ -4675,42 +4671,44 @@
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr"/>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V40" t="b">
         <v>0</v>
       </c>
-      <c r="W40" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W40" t="inlineStr"/>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA40" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4720,96 +4718,106 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2021-08-06T11:34:26+00:00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr"/>
+          <t>2022-02-08T10:09:23+00:00</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>Polisportiva Madonnina</t>
+        </is>
+      </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr"/>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
         </is>
       </c>
       <c r="V41" t="b">
         <v>0</v>
       </c>
-      <c r="W41" t="inlineStr"/>
+      <c r="W41" t="n">
+        <v>41123</v>
+      </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA41" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4819,75 +4827,63 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
+          <t>2022-05-06T09:12:13+00:00</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
-      <c r="U42" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U42" t="inlineStr"/>
       <c r="V42" t="b">
         <v>0</v>
       </c>
@@ -4896,7 +4892,7 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
@@ -4918,7 +4914,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4928,59 +4924,67 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr"/>
+          <t>2022-03-19T09:15:00+00:00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Commedia brillante</t>
+        </is>
+      </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
-      <c r="P43" t="inlineStr"/>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
@@ -4993,7 +4997,7 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -5015,7 +5019,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5025,102 +5029,96 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Commedia brillante</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>Teatro Cittadella</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
-      <c r="U44" t="inlineStr"/>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V44" t="b">
         <v>0</v>
       </c>
-      <c r="W44" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W44" t="inlineStr"/>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA44" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5130,50 +5128,54 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr"/>
+          <t>2022-03-31T08:57:09+00:00</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
+        </is>
+      </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
@@ -5182,44 +5184,42 @@
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U45" t="inlineStr"/>
       <c r="V45" t="b">
         <v>0</v>
       </c>
-      <c r="W45" t="inlineStr"/>
+      <c r="W45" t="n">
+        <v>41123</v>
+      </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA45" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5229,63 +5229,67 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
         </is>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr"/>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
@@ -5298,7 +5302,7 @@
       </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
@@ -5320,7 +5324,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5330,67 +5334,67 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-02-25T14:15:33+00:00</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-02-28T15:13:23+00:00</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
@@ -5403,7 +5407,7 @@
       </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
@@ -5425,7 +5429,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5435,71 +5439,83 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-05-06T10:18:45+00:00</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr"/>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S48" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr"/>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>https://www.anticoinpiazzagrande.com/</t>
+        </is>
+      </c>
       <c r="V48" t="b">
         <v>0</v>
       </c>
@@ -5508,7 +5524,7 @@
       </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
@@ -5530,7 +5546,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5540,107 +5556,89 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:24:06+00:00</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr">
         <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V49" t="b">
         <v>0</v>
       </c>
-      <c r="W49" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
@@ -5678,23 +5676,23 @@
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
+          <t>2022-05-10T08:26:10+00:00</t>
         </is>
       </c>
       <c r="M50" t="inlineStr"/>
@@ -5724,7 +5722,7 @@
       <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
@@ -5746,7 +5744,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5756,96 +5754,106 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
-      <c r="R51" t="inlineStr"/>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V51" t="b">
         <v>0</v>
       </c>
-      <c r="W51" t="inlineStr"/>
+      <c r="W51" t="n">
+        <v>41123</v>
+      </c>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA51" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5855,99 +5863,89 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:55+00:00</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V52" t="b">
         <v>0</v>
       </c>
-      <c r="W52" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
@@ -5985,23 +5983,23 @@
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
+          <t>2022-05-10T08:27:35+00:00</t>
         </is>
       </c>
       <c r="M53" t="inlineStr"/>
@@ -6031,7 +6029,7 @@
       <c r="W53" t="inlineStr"/>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
@@ -6084,23 +6082,23 @@
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-11-19T23:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-11-20T22:55:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
+          <t>2022-05-10T08:28:15+00:00</t>
         </is>
       </c>
       <c r="M54" t="inlineStr"/>
@@ -6130,7 +6128,7 @@
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
@@ -6144,105 +6142,6 @@
         </is>
       </c>
       <c r="AA54" t="inlineStr">
-        <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Mercati</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Modena</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>2022-11-19T23:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>2022-11-20T22:55:00+00:00</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr"/>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>2022-05-10T08:28:15+00:00</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr"/>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
-        </is>
-      </c>
-      <c r="O55" t="inlineStr"/>
-      <c r="P55" t="inlineStr"/>
-      <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr"/>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>Mercato straordinario degli ambulanti</t>
-        </is>
-      </c>
-      <c r="T55" t="inlineStr"/>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
-      <c r="V55" t="b">
-        <v>0</v>
-      </c>
-      <c r="W55" t="inlineStr"/>
-      <c r="X55" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
-        </is>
-      </c>
-      <c r="Y55" t="inlineStr">
-        <is>
-          <t>44,65137034620577</t>
-        </is>
-      </c>
-      <c r="Z55" t="inlineStr">
-        <is>
-          <t>10,921029194828652</t>
-        </is>
-      </c>
-      <c r="AA55" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Wed May 25 12:29:44 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA59"/>
+  <dimension ref="A1:AA60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3460,7 +3460,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Concerti,Musica</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3470,67 +3470,71 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Largo S.Francesco</t>
+          <t>piazza Matteotti, 17</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2022-05-10T10:04:48+00:00</t>
+          <t>2022-05-25T09:39:41+00:00</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Diciottesima edizione</t>
+          <t>Spettacolo teatrale per bambini e bambine da 3 a 6 anni</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2022-05-10T10:08:30+00:00</t>
+          <t>2022-05-25T09:43:08+00:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
+          <t>2022-05-29T08:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
           <t>2022-05-29T10:00:00+00:00</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>2022-05-29T11:00:00+00:00</t>
-        </is>
-      </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-rosa-mistica/@@images/5d666bc9-d035-4acb-9903-21fd8e9003bf.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-viaggio-alla-scoperta-della-musica/@@images/c4306e19-428c-42cb-bc32-698e6ea5dd39.jpeg</t>
         </is>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-05-10T10:13:42+00:00</t>
+          <t>2022-05-25T09:43:08+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Chiesa di San Francesco</t>
+          <t>Centro per l'infanzia Mo.Mo</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 16.00</t>
+          <t xml:space="preserve"> Ore 10.00</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso libero</t>
+          <t xml:space="preserve"> Inizia gratuita su prenotazione</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr"/>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>059 235320</t>
+        </is>
+      </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Concerto "Rosa mistica"</t>
+          <t>Un viaggio alla scoperta della musica</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
@@ -3543,130 +3547,112 @@
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-rosa-mistica</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/un-viaggio-alla-scoperta-della-musica</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,648090007085386</t>
         </is>
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,925069996586558</t>
         </is>
       </c>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.925069996586558 44.648090007085386)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
+          <t>Concerti,Musica</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Montale Rangone</t>
+          <t>Modena</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
+          <t>Largo S.Francesco</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2021-04-26T15:03:43+00:00</t>
+          <t>2022-05-10T10:04:48+00:00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+          <t>Diciottesima edizione</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2021-04-26T15:06:06+00:00</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>museo@parcomontale.it</t>
-        </is>
-      </c>
+          <t>2022-05-10T10:08:30+00:00</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-04-03T14:00:00+00:00</t>
+          <t>2022-05-29T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-06-19T15:00:00+00:00</t>
+          <t>2022-05-29T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>Parco archeologico della Terramara di Montale</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-rosa-mistica/@@images/5d666bc9-d035-4acb-9903-21fd8e9003bf.jpeg</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-03-28T14:43:35+00:00</t>
+          <t>2022-05-10T10:13:42+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Chiesa di San Francesco</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
+          <t xml:space="preserve"> ore 16.00</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
+          <t xml:space="preserve"> Ingresso libero</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
-        </is>
-      </c>
+      <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Concerto "Rosa mistica"</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>http://www.parcomontale.it/it</t>
-        </is>
-      </c>
+      <c r="U30" t="inlineStr"/>
       <c r="V30" t="b">
         <v>0</v>
       </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>41050</t>
-        </is>
+      <c r="W30" t="n">
+        <v>41123</v>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-rosa-mistica</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
@@ -3688,86 +3674,108 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Modena</t>
+          <t>Montale Rangone</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Piazza Grande</t>
+          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:44+00:00</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
+          <t>2021-04-26T15:03:43+00:00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:51+00:00</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr"/>
+          <t>2021-04-26T15:06:06+00:00</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>museo@parcomontale.it</t>
+        </is>
+      </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-05-29T15:00:00+00:00</t>
+          <t>2022-04-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-05-29T16:00:00+00:00</t>
+          <t>2022-06-19T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche/@@images/bbb27001-b4a3-4ea4-8c8f-b2ea069af5e6.jpeg</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Parco archeologico della Terramara di Montale</t>
+        </is>
+      </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-23T10:13:30+00:00</t>
+          <t>2022-03-28T14:43:35+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 10.00</t>
+          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Euro 12 a partecipante</t>
+          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr"/>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+        </is>
+      </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Free Walking Tour - Visite guidate tematiche</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr"/>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>http://www.parcomontale.it/it</t>
+        </is>
+      </c>
       <c r="V31" t="b">
         <v>0</v>
       </c>
-      <c r="W31" t="n">
-        <v>41123</v>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>41050</t>
+        </is>
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
@@ -3789,7 +3797,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Altri eventi,Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3799,78 +3807,76 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ingresso da viale Berengario</t>
+          <t>Piazza Grande</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2020-12-29T15:02:32+00:00</t>
+          <t>2022-03-23T16:26:44+00:00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2020-12-29T15:05:00+00:00</t>
+          <t>2022-03-23T16:26:51+00:00</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-01-03T14:00:00+00:00</t>
+          <t>2022-05-29T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-12-26T14:59:00+00:00</t>
+          <t>2022-05-29T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche/@@images/bbb27001-b4a3-4ea4-8c8f-b2ea069af5e6.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2021-12-28T10:39:07+00:00</t>
+          <t>2022-05-23T10:13:30+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
+          <t xml:space="preserve"> ore 10.00</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Euro 12 a partecipante</t>
+        </is>
+      </c>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Mercato settimanale del lunedì</t>
+          <t>Free Walking Tour - Visite guidate tematiche</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.com/</t>
-        </is>
-      </c>
+      <c r="U32" t="inlineStr"/>
       <c r="V32" t="b">
         <v>0</v>
       </c>
-      <c r="W32" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W32" t="n">
+        <v>41123</v>
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
@@ -3892,7 +3898,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Altri eventi,Mercati</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3902,112 +3908,100 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Viale Caduti in Guerra, 196</t>
+          <t>Ingresso da viale Berengario</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2020-09-17T12:45:54+00:00</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Gli spettacoli di ERT al Teatro Tempio</t>
-        </is>
-      </c>
+          <t>2020-12-29T15:02:32+00:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2014-09-30T12:50:00+00:00</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>info@emiliaromagnateatro.com</t>
-        </is>
-      </c>
+          <t>2020-12-29T15:05:00+00:00</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-05-30T22:00:00+00:00</t>
+          <t>2022-01-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-12-26T14:59:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/kassandra/@@images/29f75f21-a9f0-45e8-8056-8023ce88a666.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-03-15T11:11:12+00:00</t>
+          <t>2021-12-28T10:39:07+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Teatro Tempio</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 31 maggio e 1 giugno, 3 giugno e dal 7 al 10 giugno ore 20.30  2, 4, 5, 11 e 12 giugno ore 19.00</t>
+          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
-        </is>
-      </c>
+      <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>059/2163021</t>
-        </is>
-      </c>
+      <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Kassandra</t>
+          <t>Mercato settimanale del lunedì</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr">
         <is>
-          <t>http://www.emiliaromagnateatro.com</t>
+          <t>http://www.consorzioilmercato.com/</t>
         </is>
       </c>
       <c r="V33" t="b">
         <v>0</v>
       </c>
-      <c r="W33" t="inlineStr"/>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
+      </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/kassandra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
         <is>
-          <t>44,64381951149482</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>10,93139345085676</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA33" t="inlineStr">
         <is>
-          <t>POINT (10.93139345085676 44.64381951149482)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -4017,112 +4011,112 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>via degli Adelardi, 4</t>
+          <t>Viale Caduti in Guerra, 196</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:25+00:00</t>
+          <t>2020-09-17T12:45:54+00:00</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Proiezione del film di Francesco Conversano e Nene Grignaffini</t>
+          <t>Gli spettacoli di ERT al Teatro Tempio</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:52+00:00</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr"/>
+          <t>2014-09-30T12:50:00+00:00</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>info@emiliaromagnateatro.com</t>
+        </is>
+      </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-05-31T06:00:00+00:00</t>
+          <t>2022-05-30T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-05-31T06:44:31+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/paisan-ciao/@@images/00f14156-0e06-4604-8c79-4aa96ada1a7a.jpeg</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>Immagine della locandina del film</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/kassandra/@@images/29f75f21-a9f0-45e8-8056-8023ce88a666.jpeg</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-24T07:41:04+00:00</t>
+          <t>2022-03-15T11:11:12+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Sala Truffaut</t>
+          <t>Teatro Tempio</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.15</t>
+          <t xml:space="preserve"> 31 maggio e 1 giugno, 3 giugno e dal 7 al 10 giugno ore 20.30  2, 4, 5, 11 e 12 giugno ore 19.00</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
+        </is>
+      </c>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr">
         <is>
-          <t>059 236288</t>
+          <t>059/2163021</t>
         </is>
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Paisan, Ciao</t>
+          <t>Kassandra</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr">
         <is>
-          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
+          <t>http://www.emiliaromagnateatro.com</t>
         </is>
       </c>
       <c r="V34" t="b">
         <v>0</v>
       </c>
-      <c r="W34" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
-      </c>
+      <c r="W34" t="inlineStr"/>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/paisan-ciao</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/kassandra</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
         <is>
-          <t>44,6456499931615</t>
+          <t>44,64381951149482</t>
         </is>
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>10,921599972490952</t>
+          <t>10,93139345085676</t>
         </is>
       </c>
       <c r="AA34" t="inlineStr">
         <is>
-          <t>POINT (10.921599972490952 44.6456499931615)</t>
+          <t>POINT (10.93139345085676 44.64381951149482)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Musica,Spettacoli,Teatro</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4132,114 +4126,112 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 85</t>
+          <t>via degli Adelardi, 4</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
+          <t>2021-04-28T06:30:25+00:00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Spettacolo conclusivo dei corsi di Alta Formazione per cantanti lirici </t>
+          <t>Proiezione del film di Francesco Conversano e Nene Grignaffini</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>info@teatrocomunalemodena.it</t>
-        </is>
-      </c>
+          <t>2021-04-28T06:30:52+00:00</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-05-31T15:00:00+00:00</t>
+          <t>2022-05-31T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-05-31T16:00:00+00:00</t>
+          <t>2022-05-31T06:44:31+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolceamaro/@@images/2429e532-09b0-41e8-9f85-aa4a21287d10.jpeg</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/paisan-ciao/@@images/00f14156-0e06-4604-8c79-4aa96ada1a7a.jpeg</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Immagine della locandina del film</t>
+        </is>
+      </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-03-22T10:17:19+00:00</t>
+          <t>2022-05-24T07:41:04+00:00</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Sala Truffaut</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> ore 21.15</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> gratuito</t>
-        </is>
-      </c>
+      <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr">
         <is>
-          <t>059 2033010</t>
+          <t>059 236288</t>
         </is>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>DolceAmaro</t>
+          <t>Paisan, Ciao</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr">
         <is>
-          <t>https://teatrocomunalemodena.it/</t>
+          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
         </is>
       </c>
       <c r="V35" t="b">
         <v>0</v>
       </c>
-      <c r="W35" t="n">
-        <v>41123</v>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolceamaro</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/paisan-ciao</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,6456499931615</t>
         </is>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921599972490952</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921599972490952 44.6456499931615)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Musica,Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4249,67 +4241,83 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:44+00:00</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr"/>
+          <t>2021-10-04T15:31:48+00:00</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spettacolo conclusivo dei corsi di Alta Formazione per cantanti lirici </t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:51+00:00</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr"/>
+          <t>2021-10-04T15:31:55+00:00</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>info@teatrocomunalemodena.it</t>
+        </is>
+      </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-06-01T15:00:00+00:00</t>
+          <t>2022-05-31T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-01T16:00:00+00:00</t>
+          <t>2022-05-31T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche/@@images/8e5a5fa0-1d05-41e2-9bd5-115da3e3c5ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolceamaro/@@images/2429e532-09b0-41e8-9f85-aa4a21287d10.jpeg</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-05-23T10:16:24+00:00</t>
+          <t>2022-03-22T10:17:19+00:00</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Ritrovo e partenza: Piazza Roma davanti all'Accademia Militare</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Euro 12 a partecipante</t>
+          <t xml:space="preserve"> gratuito</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr"/>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>059 2033010</t>
+        </is>
+      </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Free Walking Tour - Visite guidate tematiche</t>
+          <t>DolceAmaro</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>https://teatrocomunalemodena.it/</t>
+        </is>
+      </c>
       <c r="V36" t="b">
         <v>0</v>
       </c>
@@ -4318,7 +4326,7 @@
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolceamaro</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
@@ -4340,7 +4348,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Spettacoli,Concerti,Musica</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4350,29 +4358,21 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 85</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Rassegna "L'altro suono festival" del Teatro comunale Pavarotti-Freni</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:44+00:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>info@teatrocomunalemodena.it</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:51+00:00</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
           <t>2022-06-01T15:00:00+00:00</t>
@@ -4385,44 +4385,40 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/vinicio-capossela/@@images/9059bf61-ac70-4134-8ced-4386f5e54ad3.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche/@@images/8e5a5fa0-1d05-41e2-9bd5-115da3e3c5ea.jpeg</t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-05-04T10:45:34+00:00</t>
+          <t>2022-05-23T10:16:24+00:00</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Ritrovo e partenza: Piazza Roma davanti all'Accademia Militare</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr"/>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Euro 12 a partecipante</t>
+        </is>
+      </c>
       <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>059 2033010</t>
-        </is>
-      </c>
+      <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Vinicio Capossela</t>
+          <t>Free Walking Tour - Visite guidate tematiche</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>https://teatrocomunalemodena.it/</t>
-        </is>
-      </c>
+      <c r="U37" t="inlineStr"/>
       <c r="V37" t="b">
         <v>0</v>
       </c>
@@ -4431,7 +4427,7 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/vinicio-capossela</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
@@ -4453,7 +4449,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Iniziative per bambini,Manifestazioni sportive</t>
+          <t>Spettacoli,Concerti,Musica</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4463,63 +4459,79 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
+          <t>Corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2022-05-11T07:00:46+00:00</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr"/>
+          <t>2021-10-04T15:31:48+00:00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Rassegna "L'altro suono festival" del Teatro comunale Pavarotti-Freni</t>
+        </is>
+      </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr"/>
+          <t>2021-10-04T15:31:55+00:00</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>info@teatrocomunalemodena.it</t>
+        </is>
+      </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-02T06:00:00+00:00</t>
+          <t>2022-06-01T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-02T07:00:00+00:00</t>
+          <t>2022-06-01T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/vinicio-capossela/@@images/9059bf61-ac70-4134-8ced-4386f5e54ad3.jpeg</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
+          <t>2022-05-04T10:45:34+00:00</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>Autodromo di Modena</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr"/>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>059 2033010</t>
+        </is>
+      </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Go Kart, go!</t>
+          <t>Vinicio Capossela</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>https://teatrocomunalemodena.it/</t>
+        </is>
+      </c>
       <c r="V38" t="b">
         <v>0</v>
       </c>
@@ -4528,7 +4540,7 @@
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/vinicio-capossela</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
@@ -4550,7 +4562,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Iniziative per bambini,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4560,54 +4572,50 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2021-08-25T12:27:55+00:00</t>
+          <t>2022-05-11T07:00:46+00:00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2021-08-25T12:28:08+00:00</t>
+          <t>2022-05-11T07:01:08+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-02T12:00:00+00:00</t>
+          <t>2022-06-02T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-05T13:00:00+00:00</t>
+          <t>2022-06-02T07:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>Immagine di una precedente edizione del mercato</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-05-21T08:42:42+00:00</t>
+          <t>2022-05-11T07:01:08+00:00</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
+          <t>Autodromo di Modena</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
@@ -4616,48 +4624,42 @@
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Mercato europeo</t>
+          <t>Go Kart, go!</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>http://www.mercatieuropei.com</t>
-        </is>
-      </c>
+      <c r="U39" t="inlineStr"/>
       <c r="V39" t="b">
         <v>0</v>
       </c>
-      <c r="W39" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W39" t="n">
+        <v>41123</v>
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
         <is>
-          <t>44,647524762696584</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>10,925428060260353</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA39" t="inlineStr">
         <is>
-          <t>POINT (10.925428060260353 44.647524762696584)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Altri eventi,Manifestazioni sportive</t>
+          <t>Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4667,54 +4669,54 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Zona tribune</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-05-11T07:50:51+00:00</t>
+          <t>2021-08-25T12:27:55+00:00</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2021-08-25T12:28:08+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-03T07:00:00+00:00</t>
+          <t>2022-06-02T12:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-03T08:00:00+00:00</t>
+          <t>2022-06-05T13:00:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della Run 5.30 Modena</t>
+          <t>Immagine di una precedente edizione del mercato</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-05-21T08:42:42+00:00</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 5.30</t>
+          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
@@ -4723,42 +4725,48 @@
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Run 5.30</t>
+          <t>Mercato europeo</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr"/>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>http://www.mercatieuropei.com</t>
+        </is>
+      </c>
       <c r="V40" t="b">
         <v>0</v>
       </c>
-      <c r="W40" t="n">
-        <v>41123</v>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,647524762696584</t>
         </is>
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,925428060260353</t>
         </is>
       </c>
       <c r="AA40" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.925428060260353 44.647524762696584)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Altri eventi,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4768,112 +4776,98 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>via degli Adelardi, 4</t>
+          <t>Zona tribune</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:25+00:00</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Proiezione del film di Marco Pollini</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:50:51+00:00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:52+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-04T06:00:00+00:00</t>
+          <t>2022-06-03T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-04T06:44:31+00:00</t>
+          <t>2022-06-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-grande-guerra-del-salento/@@images/b18d66e7-4b46-4875-9d8e-b70050efe202.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Immagine della locandina del film</t>
+          <t>Immagine presa dal sito della Run 5.30 Modena</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-05-24T07:43:55+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Sala Truffaut</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.15</t>
+          <t xml:space="preserve"> ore 5.30</t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>059 236288</t>
-        </is>
-      </c>
+      <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>La grande guerra del Salento</t>
+          <t>Run 5.30</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr">
-        <is>
-          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
-        </is>
-      </c>
+      <c r="U41" t="inlineStr"/>
       <c r="V41" t="b">
         <v>0</v>
       </c>
-      <c r="W41" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W41" t="n">
+        <v>41123</v>
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-grande-guerra-del-salento</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
         <is>
-          <t>44,6456499931615</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>10,921599972490952</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA41" t="inlineStr">
         <is>
-          <t>POINT (10.921599972490952 44.6456499931615)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4883,77 +4877,77 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>via degli Adelardi, 4</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr"/>
+          <t>2021-04-28T06:30:25+00:00</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Proiezione del film di Marco Pollini</t>
+        </is>
+      </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2021-04-28T06:30:52+00:00</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-06-04T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-04T06:44:31+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-grande-guerra-del-salento/@@images/b18d66e7-4b46-4875-9d8e-b70050efe202.jpeg</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Immagine della locandina del film</t>
+        </is>
+      </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-24T07:43:55+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Sala Truffaut</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> ore 21.15</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
-        </is>
-      </c>
+      <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr">
         <is>
-          <t>059 2033166</t>
+          <t>059 236288</t>
         </is>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>La grande guerra del Salento</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr">
         <is>
-          <t>https://www.fmav.org</t>
+          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
         </is>
       </c>
       <c r="V42" t="b">
@@ -4966,29 +4960,29 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-grande-guerra-del-salento</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,6456499931615</t>
         </is>
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921599972490952</t>
         </is>
       </c>
       <c r="AA42" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921599972490952 44.6456499931615)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4998,76 +4992,90 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
+          <t>2021-09-09T10:12:02+00:00</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-05-25T07:44:29+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
         </is>
       </c>
       <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr"/>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V43" t="b">
         <v>0</v>
       </c>
-      <c r="W43" t="n">
-        <v>41123</v>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -5089,7 +5097,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5099,59 +5107,63 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-05-25T07:44:29+00:00</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr"/>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
@@ -5164,7 +5176,7 @@
       </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
@@ -5186,7 +5198,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5196,50 +5208,50 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr"/>
+          <t>2022-05-21T10:36:00+00:00</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti</t>
+        </is>
+      </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
@@ -5248,44 +5260,42 @@
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U45" t="inlineStr"/>
       <c r="V45" t="b">
         <v>0</v>
       </c>
-      <c r="W45" t="inlineStr"/>
+      <c r="W45" t="n">
+        <v>41123</v>
+      </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA45" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5295,106 +5305,96 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Polisportiva Madonnina</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V46" t="b">
         <v>0</v>
       </c>
-      <c r="W46" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA46" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5404,63 +5404,75 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
+          <t>2021-08-06T11:34:26+00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr"/>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S47" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr"/>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+        </is>
+      </c>
       <c r="V47" t="b">
         <v>0</v>
       </c>
@@ -5469,7 +5481,7 @@
       </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
@@ -5491,7 +5503,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5501,67 +5513,59 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>Commedia brillante</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
@@ -5574,7 +5578,7 @@
       </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
@@ -5596,7 +5600,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5606,96 +5610,102 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t>Commedia brillante</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr"/>
+          <t>2022-03-19T09:32:45+00:00</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>Teatro Cittadella</t>
+        </is>
+      </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr"/>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
-      <c r="U49" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U49" t="inlineStr"/>
       <c r="V49" t="b">
         <v>0</v>
       </c>
-      <c r="W49" t="inlineStr"/>
+      <c r="W49" t="n">
+        <v>41123</v>
+      </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5705,54 +5715,50 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr"/>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
@@ -5761,42 +5767,44 @@
       <c r="R50" t="inlineStr"/>
       <c r="S50" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
-      <c r="U50" t="inlineStr"/>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V50" t="b">
         <v>0</v>
       </c>
-      <c r="W50" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA50" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5806,67 +5814,63 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
@@ -5879,7 +5883,7 @@
       </c>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
@@ -5901,7 +5905,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5911,67 +5915,67 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q52" t="inlineStr"/>
       <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
@@ -5984,7 +5988,7 @@
       </c>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
@@ -6006,7 +6010,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -6016,83 +6020,71 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-02-25T14:15:33+00:00</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-02-28T15:13:23+00:00</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R53" t="inlineStr"/>
       <c r="S53" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
-      <c r="U53" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U53" t="inlineStr"/>
       <c r="V53" t="b">
         <v>0</v>
       </c>
@@ -6101,7 +6093,7 @@
       </c>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
@@ -6123,7 +6115,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -6133,89 +6125,107 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr"/>
+          <t>2022-05-06T10:18:45+00:00</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+        </is>
+      </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O54" t="inlineStr"/>
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr"/>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S54" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V54" t="b">
         <v>0</v>
       </c>
-      <c r="W54" t="inlineStr"/>
+      <c r="W54" t="n">
+        <v>41123</v>
+      </c>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA54" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6253,23 +6263,23 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
         </is>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
+          <t>2022-05-10T08:24:06+00:00</t>
         </is>
       </c>
       <c r="M55" t="inlineStr"/>
@@ -6299,7 +6309,7 @@
       <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr">
@@ -6321,7 +6331,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -6331,106 +6341,96 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:10+00:00</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr"/>
       <c r="N56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="inlineStr"/>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R56" t="inlineStr"/>
       <c r="S56" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V56" t="b">
         <v>0</v>
       </c>
-      <c r="W56" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W56" t="inlineStr"/>
       <c r="X56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y56" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z56" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA56" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -6440,89 +6440,99 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O57" t="inlineStr"/>
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr"/>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S57" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V57" t="b">
         <v>0</v>
       </c>
-      <c r="W57" t="inlineStr"/>
+      <c r="W57" t="n">
+        <v>41123</v>
+      </c>
       <c r="X57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y57" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z57" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA57" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6560,23 +6570,23 @@
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M58" t="inlineStr"/>
@@ -6606,7 +6616,7 @@
       <c r="W58" t="inlineStr"/>
       <c r="X58" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y58" t="inlineStr">
@@ -6659,23 +6669,23 @@
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:27:35+00:00</t>
         </is>
       </c>
       <c r="M59" t="inlineStr"/>
@@ -6705,20 +6715,119 @@
       <c r="W59" t="inlineStr"/>
       <c r="X59" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z59" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA59" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="inlineStr"/>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T60" t="inlineStr"/>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V60" t="b">
+        <v>0</v>
+      </c>
+      <c r="W60" t="inlineStr"/>
+      <c r="X60" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y59" t="inlineStr">
+      <c r="Y60" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z59" t="inlineStr">
+      <c r="Z60" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA59" t="inlineStr">
+      <c r="AA60" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Thu May 26 16:22:46 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA62"/>
+  <dimension ref="A1:AA63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5164,7 +5164,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5174,90 +5174,80 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>ingresso da Strada S.Faustino, 172</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr"/>
+          <t>2022-05-26T14:09:48+00:00</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Spettacolo di danza</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-05-26T14:09:58+00:00</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-06-04T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-04T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-giro-del-mondo-in-90-minuti/@@images/c6bc9831-404e-402b-9e60-623bc0a2ba80.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-26T14:11:15+00:00</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Parco Ferrari</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> ore 20.00</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
+          <t xml:space="preserve"> ingresso libero</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Il giro del mondo in 90 minuti</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr">
-        <is>
-          <t>https://www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U45" t="inlineStr"/>
       <c r="V45" t="b">
         <v>0</v>
       </c>
-      <c r="W45" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W45" t="n">
+        <v>41123</v>
       </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-giro-del-mondo-in-90-minuti</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
@@ -5279,7 +5269,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5289,76 +5279,90 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
+          <t>2021-09-09T10:12:02+00:00</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
         </is>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-05-26T07:16:41+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
         </is>
       </c>
       <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr"/>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr"/>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V46" t="b">
         <v>0</v>
       </c>
-      <c r="W46" t="n">
-        <v>41123</v>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
@@ -5380,7 +5384,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5390,59 +5394,63 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-05-26T07:16:41+00:00</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr"/>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
@@ -5455,7 +5463,7 @@
       </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
@@ -5477,7 +5485,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5487,50 +5495,50 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr"/>
+          <t>2022-05-21T10:36:00+00:00</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti</t>
+        </is>
+      </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
@@ -5539,44 +5547,42 @@
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U48" t="inlineStr"/>
       <c r="V48" t="b">
         <v>0</v>
       </c>
-      <c r="W48" t="inlineStr"/>
+      <c r="W48" t="n">
+        <v>41123</v>
+      </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA48" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5586,106 +5592,96 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>Polisportiva Madonnina</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V49" t="b">
         <v>0</v>
       </c>
-      <c r="W49" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5695,63 +5691,75 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
+          <t>2021-08-06T11:34:26+00:00</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr"/>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
-      <c r="U50" t="inlineStr"/>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+        </is>
+      </c>
       <c r="V50" t="b">
         <v>0</v>
       </c>
@@ -5760,7 +5768,7 @@
       </c>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
@@ -5782,7 +5790,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5792,67 +5800,59 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Commedia brillante</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
@@ -5887,7 +5887,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5897,96 +5897,102 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t>Commedia brillante</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr"/>
+          <t>2022-03-19T09:32:45+00:00</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Teatro Cittadella</t>
+        </is>
+      </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q52" t="inlineStr"/>
       <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
-      <c r="U52" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U52" t="inlineStr"/>
       <c r="V52" t="b">
         <v>0</v>
       </c>
-      <c r="W52" t="inlineStr"/>
+      <c r="W52" t="n">
+        <v>41123</v>
+      </c>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5996,54 +6002,50 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O53" t="inlineStr"/>
@@ -6052,42 +6054,44 @@
       <c r="R53" t="inlineStr"/>
       <c r="S53" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
-      <c r="U53" t="inlineStr"/>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V53" t="b">
         <v>0</v>
       </c>
-      <c r="W53" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W53" t="inlineStr"/>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA53" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -6097,67 +6101,63 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P54" t="inlineStr"/>
       <c r="Q54" t="inlineStr"/>
       <c r="R54" t="inlineStr"/>
       <c r="S54" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T54" t="inlineStr"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
@@ -6192,7 +6192,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -6202,67 +6202,67 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O55" t="inlineStr"/>
-      <c r="P55" t="inlineStr"/>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="inlineStr"/>
       <c r="S55" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T55" t="inlineStr"/>
@@ -6275,7 +6275,7 @@
       </c>
       <c r="X55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr">
@@ -6297,7 +6297,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -6307,83 +6307,71 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-02-25T14:15:33+00:00</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-02-28T15:13:23+00:00</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="inlineStr"/>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R56" t="inlineStr"/>
       <c r="S56" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T56" t="inlineStr"/>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U56" t="inlineStr"/>
       <c r="V56" t="b">
         <v>0</v>
       </c>
@@ -6392,7 +6380,7 @@
       </c>
       <c r="X56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y56" t="inlineStr">
@@ -6414,7 +6402,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -6424,89 +6412,107 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr"/>
+          <t>2022-05-06T10:18:45+00:00</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+        </is>
+      </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O57" t="inlineStr"/>
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr"/>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S57" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V57" t="b">
         <v>0</v>
       </c>
-      <c r="W57" t="inlineStr"/>
+      <c r="W57" t="n">
+        <v>41123</v>
+      </c>
       <c r="X57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y57" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z57" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA57" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6544,23 +6550,23 @@
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
         </is>
       </c>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
+          <t>2022-05-10T08:24:06+00:00</t>
         </is>
       </c>
       <c r="M58" t="inlineStr"/>
@@ -6590,7 +6596,7 @@
       <c r="W58" t="inlineStr"/>
       <c r="X58" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y58" t="inlineStr">
@@ -6612,7 +6618,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -6622,106 +6628,96 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:10+00:00</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr"/>
       <c r="N59" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr"/>
       <c r="Q59" t="inlineStr"/>
-      <c r="R59" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R59" t="inlineStr"/>
       <c r="S59" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T59" t="inlineStr"/>
       <c r="U59" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V59" t="b">
         <v>0</v>
       </c>
-      <c r="W59" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W59" t="inlineStr"/>
       <c r="X59" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y59" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z59" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA59" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -6731,89 +6727,99 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
-        </is>
-      </c>
-      <c r="M60" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr"/>
       <c r="Q60" t="inlineStr"/>
-      <c r="R60" t="inlineStr"/>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S60" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T60" t="inlineStr"/>
       <c r="U60" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V60" t="b">
         <v>0</v>
       </c>
-      <c r="W60" t="inlineStr"/>
+      <c r="W60" t="n">
+        <v>41123</v>
+      </c>
       <c r="X60" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y60" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z60" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA60" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6851,23 +6857,23 @@
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M61" t="inlineStr"/>
@@ -6897,7 +6903,7 @@
       <c r="W61" t="inlineStr"/>
       <c r="X61" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y61" t="inlineStr">
@@ -6950,23 +6956,23 @@
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K62" t="inlineStr"/>
       <c r="L62" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:27:35+00:00</t>
         </is>
       </c>
       <c r="M62" t="inlineStr"/>
@@ -6996,20 +7002,119 @@
       <c r="W62" t="inlineStr"/>
       <c r="X62" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y62" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z62" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA62" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
+      <c r="R63" t="inlineStr"/>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T63" t="inlineStr"/>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V63" t="b">
+        <v>0</v>
+      </c>
+      <c r="W63" t="inlineStr"/>
+      <c r="X63" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y62" t="inlineStr">
+      <c r="Y63" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z62" t="inlineStr">
+      <c r="Z63" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA62" t="inlineStr">
+      <c r="AA63" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Fri May 27 08:19:31 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -4950,7 +4950,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ingresso da Strada S.Faustino, 172</t>
+          <t>ingresso da Strada S.Faustino, 182</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -4987,7 +4987,7 @@
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-05-26T14:11:15+00:00</t>
+          <t>2022-05-27T06:18:12+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">

</xml_diff>

<commit_message>
Latest data: Fri May 27 16:22:08 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA61"/>
+  <dimension ref="A1:AA63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1898,7 +1898,7 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2022-05-26T07:55:24+00:00</t>
+          <t>2022-05-27T14:17:16+00:00</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -3220,7 +3220,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3230,50 +3230,54 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Piazza Grande</t>
+          <t>Via F. Selmi, 67</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:44+00:00</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>2022-05-27T13:32:13+00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Esposizione a tema a cura degli studenti della classe 3G dell'IIS A.Venturi di Modena</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:51+00:00</t>
+          <t>2022-05-27T13:32:23+00:00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2022-03-19T16:00:00+00:00</t>
+          <t>2022-05-28T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2022-05-28T16:00:00+00:00</t>
+          <t>2022-06-05T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/free-walking-tour-visite-guidate-del-centro-storico-di-modena/@@images/26b88750-ac47-44ab-bc5c-66df7933f860.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/201cle-ferite201d-per-i-50-anni-di-medici-senza-frontiere/@@images/8d3225be-145b-4570-8501-7c691ae317e4.jpeg</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-03-23T16:27:28+00:00</t>
+          <t>2022-05-27T14:11:04+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
+          <t>Complesso San Paolo, Cortile del Leccio</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tutti i sabati dal 19 marzo al 28 maggio alle ore 15.30</t>
+          <t xml:space="preserve"> sabato e feriali ore 9.00-19.00  domenica e festivi ore 9.00-13.00 </t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
@@ -3282,7 +3286,7 @@
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Free Walking Tour - Visite guidate del centro storico di Modena</t>
+          <t>“Le Ferite” per i 50 anni di Medici Senza Frontiere</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
@@ -3295,7 +3299,7 @@
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/free-walking-tour-visite-guidate-del-centro-storico-di-modena</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/201cle-ferite201d-per-i-50-anni-di-medici-senza-frontiere</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3317,7 +3321,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3327,71 +3331,63 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>piazza Matteotti, 17</t>
+          <t>Via F. Selmi, 67</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2022-05-25T09:39:41+00:00</t>
+          <t>2022-05-27T13:32:13+00:00</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale per bambini e bambine da 3 a 6 anni</t>
+          <t>Presentazione del libro ed esposizione a tema a cura degli studenti della classe 3G dell'IIS A.Venturi di Modena</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2022-05-25T09:43:08+00:00</t>
+          <t>2022-05-27T13:32:23+00:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-05-29T08:00:00+00:00</t>
+          <t>2022-05-28T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-05-29T10:00:00+00:00</t>
+          <t>2022-05-28T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-viaggio-alla-scoperta-della-musica/@@images/c4306e19-428c-42cb-bc32-698e6ea5dd39.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_201cle-ferite201d-per-i-50-anni-di-medici-senza-frontiere/@@images/c8a46615-786c-4007-9ec5-18ab3716c26a.jpeg</t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-05-25T09:43:08+00:00</t>
+          <t>2022-05-27T14:10:34+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Centro per l'infanzia Mo.Mo</t>
+          <t>Complesso San Paolo, Cortile del Leccio</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ore 10.00</t>
+          <t xml:space="preserve"> ore 16.30</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Inizia gratuita su prenotazione</t>
-        </is>
-      </c>
+      <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>059 235320</t>
-        </is>
-      </c>
+      <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Un viaggio alla scoperta della musica</t>
+          <t>“Le Ferite” per i 50 anni di Medici Senza Frontiere</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
@@ -3404,29 +3400,29 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/un-viaggio-alla-scoperta-della-musica</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_201cle-ferite201d-per-i-50-anni-di-medici-senza-frontiere</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
         <is>
-          <t>44,648090007085386</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>10,925069996586558</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA28" t="inlineStr">
         <is>
-          <t>POINT (10.925069996586558 44.648090007085386)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Concerti,Musica</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3436,67 +3432,59 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Largo S.Francesco</t>
+          <t>Piazza Grande</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2022-05-10T10:04:48+00:00</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Diciottesima edizione</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:44+00:00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2022-05-10T10:08:30+00:00</t>
+          <t>2022-03-23T16:26:51+00:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-05-29T10:00:00+00:00</t>
+          <t>2022-03-19T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-05-29T11:00:00+00:00</t>
+          <t>2022-05-28T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-rosa-mistica/@@images/5d666bc9-d035-4acb-9903-21fd8e9003bf.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/free-walking-tour-visite-guidate-del-centro-storico-di-modena/@@images/26b88750-ac47-44ab-bc5c-66df7933f860.jpeg</t>
         </is>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-05-10T10:13:42+00:00</t>
+          <t>2022-03-23T16:27:28+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Chiesa di San Francesco</t>
+          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 16.00</t>
+          <t xml:space="preserve"> Tutti i sabati dal 19 marzo al 28 maggio alle ore 15.30</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso libero</t>
-        </is>
-      </c>
+      <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Concerto "Rosa mistica"</t>
+          <t>Free Walking Tour - Visite guidate del centro storico di Modena</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
@@ -3509,7 +3497,7 @@
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-rosa-mistica</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/free-walking-tour-visite-guidate-del-centro-storico-di-modena</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
@@ -3531,130 +3519,116 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Montale Rangone</t>
+          <t>Modena</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
+          <t>piazza Matteotti, 17</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2021-04-26T15:03:43+00:00</t>
+          <t>2022-05-25T09:39:41+00:00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+          <t>Spettacolo teatrale per bambini e bambine da 3 a 6 anni</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2021-04-26T15:06:06+00:00</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>museo@parcomontale.it</t>
-        </is>
-      </c>
+          <t>2022-05-25T09:43:08+00:00</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-04-03T14:00:00+00:00</t>
+          <t>2022-05-29T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-06-19T15:00:00+00:00</t>
+          <t>2022-05-29T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>Parco archeologico della Terramara di Montale</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-viaggio-alla-scoperta-della-musica/@@images/c4306e19-428c-42cb-bc32-698e6ea5dd39.jpeg</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-03-28T14:43:35+00:00</t>
+          <t>2022-05-25T09:43:08+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Centro per l'infanzia Mo.Mo</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
+          <t xml:space="preserve"> Ore 10.00</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
+          <t xml:space="preserve"> Inizia gratuita su prenotazione</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr">
         <is>
-          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+          <t>059 235320</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Un viaggio alla scoperta della musica</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>http://www.parcomontale.it/it</t>
-        </is>
-      </c>
+      <c r="U30" t="inlineStr"/>
       <c r="V30" t="b">
         <v>0</v>
       </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>41050</t>
-        </is>
+      <c r="W30" t="n">
+        <v>41123</v>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/un-viaggio-alla-scoperta-della-musica</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,648090007085386</t>
         </is>
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,925069996586558</t>
         </is>
       </c>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.925069996586558 44.648090007085386)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Concerti,Musica</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3664,63 +3638,67 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Piazza Grande</t>
+          <t>Largo S.Francesco</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:44+00:00</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
+          <t>2022-05-10T10:04:48+00:00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Diciottesima edizione</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:51+00:00</t>
+          <t>2022-05-10T10:08:30+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-05-29T15:00:00+00:00</t>
+          <t>2022-05-29T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-05-29T16:00:00+00:00</t>
+          <t>2022-05-29T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche/@@images/bbb27001-b4a3-4ea4-8c8f-b2ea069af5e6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-rosa-mistica/@@images/5d666bc9-d035-4acb-9903-21fd8e9003bf.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-23T10:13:30+00:00</t>
+          <t>2022-05-10T10:13:42+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
+          <t>Chiesa di San Francesco</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 10.00</t>
+          <t xml:space="preserve"> ore 16.00</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Euro 12 a partecipante</t>
+          <t xml:space="preserve"> Ingresso libero</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Free Walking Tour - Visite guidate tematiche</t>
+          <t>Concerto "Rosa mistica"</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
@@ -3733,7 +3711,7 @@
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-rosa-mistica</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
@@ -3755,75 +3733,95 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Altri eventi,Mercati</t>
+          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Modena</t>
+          <t>Montale Rangone</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ingresso da viale Berengario</t>
+          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2020-12-29T15:02:32+00:00</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>2021-04-26T15:03:43+00:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2020-12-29T15:05:00+00:00</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr"/>
+          <t>2021-04-26T15:06:06+00:00</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>museo@parcomontale.it</t>
+        </is>
+      </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-01-03T14:00:00+00:00</t>
+          <t>2022-04-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-12-26T14:59:00+00:00</t>
+          <t>2022-06-19T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Parco archeologico della Terramara di Montale</t>
+        </is>
+      </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2021-12-28T10:39:07+00:00</t>
+          <t>2022-03-28T14:43:35+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
+          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
+        </is>
+      </c>
       <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+        </is>
+      </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Mercato settimanale del lunedì</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.com/</t>
+          <t>http://www.parcomontale.it/it</t>
         </is>
       </c>
       <c r="V32" t="b">
@@ -3831,12 +3829,12 @@
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>41121</t>
+          <t>41050</t>
         </is>
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
@@ -3858,7 +3856,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3868,112 +3866,98 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Viale Caduti in Guerra, 196</t>
+          <t>Piazza Grande</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2020-09-17T12:45:54+00:00</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Gli spettacoli di ERT al Teatro Tempio</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:44+00:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2014-09-30T12:50:00+00:00</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>info@emiliaromagnateatro.com</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:51+00:00</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-05-30T22:00:00+00:00</t>
+          <t>2022-05-29T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-05-29T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/kassandra/@@images/29f75f21-a9f0-45e8-8056-8023ce88a666.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche/@@images/bbb27001-b4a3-4ea4-8c8f-b2ea069af5e6.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-03-15T11:11:12+00:00</t>
+          <t>2022-05-23T10:13:30+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Teatro Tempio</t>
+          <t>Ritrovo e partenza: Piazza Grande, Pietra Ringadora</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 31 maggio e 1 giugno, 3 giugno e dal 7 al 10 giugno ore 20.30  2, 4, 5, 11 e 12 giugno ore 19.00</t>
+          <t xml:space="preserve"> ore 10.00</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
+          <t xml:space="preserve"> Euro 12 a partecipante</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>059/2163021</t>
-        </is>
-      </c>
+      <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Kassandra</t>
+          <t>Free Walking Tour - Visite guidate tematiche</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>http://www.emiliaromagnateatro.com</t>
-        </is>
-      </c>
+      <c r="U33" t="inlineStr"/>
       <c r="V33" t="b">
         <v>0</v>
       </c>
-      <c r="W33" t="inlineStr"/>
+      <c r="W33" t="n">
+        <v>41123</v>
+      </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/kassandra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_free-walking-tour-visite-guidate-tematiche</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
         <is>
-          <t>44,64381951149482</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>10,93139345085676</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA33" t="inlineStr">
         <is>
-          <t>POINT (10.93139345085676 44.64381951149482)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Altri eventi,Mercati</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3983,77 +3967,65 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>via degli Adelardi, 4</t>
+          <t>Ingresso da viale Berengario</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:25+00:00</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Proiezione del film di Francesco Conversano e Nene Grignaffini</t>
-        </is>
-      </c>
+          <t>2020-12-29T15:02:32+00:00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:52+00:00</t>
+          <t>2020-12-29T15:05:00+00:00</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-05-31T06:00:00+00:00</t>
+          <t>2022-01-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-05-31T06:44:31+00:00</t>
+          <t>2022-12-26T14:59:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/paisan-ciao/@@images/00f14156-0e06-4604-8c79-4aa96ada1a7a.jpeg</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>Immagine della locandina del film</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-24T07:41:04+00:00</t>
+          <t>2021-12-28T10:39:07+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Sala Truffaut</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.15</t>
+          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>059 236288</t>
-        </is>
-      </c>
+      <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Paisan, Ciao</t>
+          <t>Mercato settimanale del lunedì</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr">
         <is>
-          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
+          <t>http://www.consorzioilmercato.com/</t>
         </is>
       </c>
       <c r="V34" t="b">
@@ -4066,29 +4038,29 @@
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/paisan-ciao</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
         <is>
-          <t>44,6456499931615</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>10,921599972490952</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA34" t="inlineStr">
         <is>
-          <t>POINT (10.921599972490952 44.6456499931615)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Musica,Spettacoli,Teatro</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4098,114 +4070,112 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 85</t>
+          <t>Viale Caduti in Guerra, 196</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
+          <t>2020-09-17T12:45:54+00:00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Spettacolo conclusivo dei corsi di Alta Formazione per cantanti lirici </t>
+          <t>Gli spettacoli di ERT al Teatro Tempio</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
+          <t>2014-09-30T12:50:00+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>info@teatrocomunalemodena.it</t>
+          <t>info@emiliaromagnateatro.com</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-05-31T15:00:00+00:00</t>
+          <t>2022-05-30T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-05-31T16:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolceamaro/@@images/2429e532-09b0-41e8-9f85-aa4a21287d10.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/kassandra/@@images/29f75f21-a9f0-45e8-8056-8023ce88a666.jpeg</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-03-22T10:17:19+00:00</t>
+          <t>2022-03-15T11:11:12+00:00</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Teatro Tempio</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> 31 maggio e 1 giugno, 3 giugno e dal 7 al 10 giugno ore 20.30  2, 4, 5, 11 e 12 giugno ore 19.00</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> gratuito</t>
+          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr">
         <is>
-          <t>059 2033010</t>
+          <t>059/2163021</t>
         </is>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>DolceAmaro</t>
+          <t>Kassandra</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr">
         <is>
-          <t>https://teatrocomunalemodena.it/</t>
+          <t>http://www.emiliaromagnateatro.com</t>
         </is>
       </c>
       <c r="V35" t="b">
         <v>0</v>
       </c>
-      <c r="W35" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W35" t="inlineStr"/>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolceamaro</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/kassandra</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,64381951149482</t>
         </is>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,93139345085676</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.93139345085676 44.64381951149482)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Altri eventi,Musica</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4215,98 +4185,112 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via degli Adelardi, 4</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:04+00:00</t>
+          <t>2021-04-28T06:30:25+00:00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
+          <t>Proiezione del film di Francesco Conversano e Nene Grignaffini</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2021-04-28T06:30:52+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-05-12T09:00:00+00:00</t>
+          <t>2022-05-31T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-30T10:00:00+00:00</t>
+          <t>2022-05-31T06:44:31+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/paisan-ciao/@@images/00f14156-0e06-4604-8c79-4aa96ada1a7a.jpeg</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Immagine della locandina del film</t>
+        </is>
+      </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-05-24T07:41:04+00:00</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Piazzetta Pomposa</t>
+          <t>Sala Truffaut</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
+          <t xml:space="preserve"> ore 21.15</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr"/>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>059 236288</t>
+        </is>
+      </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Serate in Pomposa - 1° edizione</t>
+          <t>Paisan, Ciao</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
+        </is>
+      </c>
       <c r="V36" t="b">
         <v>0</v>
       </c>
-      <c r="W36" t="n">
-        <v>41123</v>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/paisan-ciao</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,6456499931615</t>
         </is>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921599972490952</t>
         </is>
       </c>
       <c r="AA36" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921599972490952 44.6456499931615)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Musica,Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4316,67 +4300,83 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:44+00:00</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr"/>
+          <t>2021-10-04T15:31:48+00:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spettacolo conclusivo dei corsi di Alta Formazione per cantanti lirici </t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:51+00:00</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr"/>
+          <t>2021-10-04T15:31:55+00:00</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>info@teatrocomunalemodena.it</t>
+        </is>
+      </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-01T15:00:00+00:00</t>
+          <t>2022-05-31T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-01T16:00:00+00:00</t>
+          <t>2022-05-31T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche/@@images/8e5a5fa0-1d05-41e2-9bd5-115da3e3c5ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolceamaro/@@images/2429e532-09b0-41e8-9f85-aa4a21287d10.jpeg</t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-05-23T10:16:24+00:00</t>
+          <t>2022-03-22T10:17:19+00:00</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Ritrovo e partenza: Piazza Roma davanti all'Accademia Militare</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Euro 12 a partecipante</t>
+          <t xml:space="preserve"> gratuito</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr"/>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>059 2033010</t>
+        </is>
+      </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Free Walking Tour - Visite guidate tematiche</t>
+          <t>DolceAmaro</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr"/>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>https://teatrocomunalemodena.it/</t>
+        </is>
+      </c>
       <c r="V37" t="b">
         <v>0</v>
       </c>
@@ -4385,7 +4385,7 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolceamaro</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
@@ -4407,7 +4407,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Spettacoli,Concerti,Musica</t>
+          <t>Altri eventi,Musica</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4417,79 +4417,67 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 85</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
+          <t>2022-05-20T10:02:04+00:00</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Rassegna "L'altro suono festival" del Teatro comunale Pavarotti-Freni</t>
+          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>info@teatrocomunalemodena.it</t>
-        </is>
-      </c>
+          <t>2022-05-20T10:02:34+00:00</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-01T15:00:00+00:00</t>
+          <t>2022-05-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-01T16:00:00+00:00</t>
+          <t>2022-06-30T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/vinicio-capossela/@@images/9059bf61-ac70-4134-8ced-4386f5e54ad3.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-05-04T10:45:34+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Piazzetta Pomposa</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>059 2033010</t>
-        </is>
-      </c>
+      <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Vinicio Capossela</t>
+          <t>Serate in Pomposa - 1° edizione</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>https://teatrocomunalemodena.it/</t>
-        </is>
-      </c>
+      <c r="U38" t="inlineStr"/>
       <c r="V38" t="b">
         <v>0</v>
       </c>
@@ -4498,7 +4486,7 @@
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/vinicio-capossela</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
@@ -4520,7 +4508,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Iniziative per bambini,Manifestazioni sportive</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4530,59 +4518,63 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2022-05-11T07:00:46+00:00</t>
+          <t>2022-03-23T16:26:44+00:00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
+          <t>2022-03-23T16:26:51+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-02T06:00:00+00:00</t>
+          <t>2022-06-01T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-02T07:00:00+00:00</t>
+          <t>2022-06-01T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche/@@images/8e5a5fa0-1d05-41e2-9bd5-115da3e3c5ea.jpeg</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
+          <t>2022-05-23T10:16:24+00:00</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Autodromo di Modena</t>
+          <t>Ritrovo e partenza: Piazza Roma davanti all'Accademia Militare</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Euro 12 a partecipante</t>
+        </is>
+      </c>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Go Kart, go!</t>
+          <t>Free Walking Tour - Visite guidate tematiche</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
@@ -4595,7 +4587,7 @@
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
@@ -4617,7 +4609,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Spettacoli,Concerti,Musica</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4627,104 +4619,110 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2021-08-25T12:27:55+00:00</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr"/>
+          <t>2021-10-04T15:31:48+00:00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Rassegna "L'altro suono festival" del Teatro comunale Pavarotti-Freni</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2021-08-25T12:28:08+00:00</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr"/>
+          <t>2021-10-04T15:31:55+00:00</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>info@teatrocomunalemodena.it</t>
+        </is>
+      </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-02T12:00:00+00:00</t>
+          <t>2022-06-01T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-05T13:00:00+00:00</t>
+          <t>2022-06-01T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>Immagine di una precedente edizione del mercato</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/vinicio-capossela/@@images/9059bf61-ac70-4134-8ced-4386f5e54ad3.jpeg</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-05-21T08:42:42+00:00</t>
+          <t>2022-05-04T10:45:34+00:00</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr"/>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>059 2033010</t>
+        </is>
+      </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Mercato europeo</t>
+          <t>Vinicio Capossela</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="inlineStr">
         <is>
-          <t>http://www.mercatieuropei.com</t>
+          <t>https://teatrocomunalemodena.it/</t>
         </is>
       </c>
       <c r="V40" t="b">
         <v>0</v>
       </c>
-      <c r="W40" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W40" t="n">
+        <v>41123</v>
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/vinicio-capossela</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
         <is>
-          <t>44,647524762696584</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>10,925428060260353</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA40" t="inlineStr">
         <is>
-          <t>POINT (10.925428060260353 44.647524762696584)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Altri eventi,Manifestazioni sportive</t>
+          <t>Iniziative per bambini,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4734,54 +4732,50 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Zona tribune</t>
+          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-05-11T07:50:51+00:00</t>
+          <t>2022-05-11T07:00:46+00:00</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-05-11T07:01:08+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-03T07:00:00+00:00</t>
+          <t>2022-06-02T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-03T08:00:00+00:00</t>
+          <t>2022-06-02T07:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>Immagine presa dal sito della Run 5.30 Modena</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-05-11T07:01:08+00:00</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Autodromo di Modena</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 5.30</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
@@ -4790,7 +4784,7 @@
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>Run 5.30</t>
+          <t>Go Kart, go!</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
@@ -4803,7 +4797,7 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
@@ -4825,7 +4819,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4835,77 +4829,69 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>via degli Adelardi, 4</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:25+00:00</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Proiezione del film di Marco Pollini</t>
-        </is>
-      </c>
+          <t>2021-08-25T12:27:55+00:00</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:52+00:00</t>
+          <t>2021-08-25T12:28:08+00:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-04T06:00:00+00:00</t>
+          <t>2022-06-02T12:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-06-04T06:44:31+00:00</t>
+          <t>2022-06-05T13:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-grande-guerra-del-salento/@@images/b18d66e7-4b46-4875-9d8e-b70050efe202.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Immagine della locandina del film</t>
+          <t>Immagine di una precedente edizione del mercato</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-05-24T07:43:55+00:00</t>
+          <t>2022-05-21T08:42:42+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Sala Truffaut</t>
+          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.15</t>
+          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>059 236288</t>
-        </is>
-      </c>
+      <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>La grande guerra del Salento</t>
+          <t>Mercato europeo</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr">
         <is>
-          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
+          <t>http://www.mercatieuropei.com</t>
         </is>
       </c>
       <c r="V42" t="b">
@@ -4918,29 +4904,29 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-grande-guerra-del-salento</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
         <is>
-          <t>44,6456499931615</t>
+          <t>44,647524762696584</t>
         </is>
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>10,921599972490952</t>
+          <t>10,925428060260353</t>
         </is>
       </c>
       <c r="AA42" t="inlineStr">
         <is>
-          <t>POINT (10.921599972490952 44.6456499931615)</t>
+          <t>POINT (10.925428060260353 44.647524762696584)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Altri eventi,Spettacoli</t>
+          <t>Altri eventi,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4950,67 +4936,63 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ingresso da Strada S.Faustino, 182</t>
+          <t>Zona tribune</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2022-05-26T14:09:48+00:00</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Spettacolo di danza</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:50:51+00:00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2022-05-26T14:09:58+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-04T14:00:00+00:00</t>
+          <t>2022-06-03T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-06-04T15:00:00+00:00</t>
+          <t>2022-06-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-giro-del-mondo-in-90-minuti/@@images/c6bc9831-404e-402b-9e60-623bc0a2ba80.jpeg</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della Run 5.30 Modena</t>
+        </is>
+      </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-05-27T06:18:12+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Parco Ferrari</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 20.00</t>
+          <t xml:space="preserve"> ore 5.30</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ingresso libero</t>
-        </is>
-      </c>
+      <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Il giro del mondo in 90 minuti</t>
+          <t>Run 5.30</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
@@ -5023,7 +5005,7 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-giro-del-mondo-in-90-minuti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -5045,7 +5027,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5055,77 +5037,77 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>via degli Adelardi, 4</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
+          <t>2021-04-28T06:30:25+00:00</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Proiezione del film di Marco Pollini</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2021-04-28T06:30:52+00:00</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-06-04T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-04T06:44:31+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-grande-guerra-del-salento/@@images/b18d66e7-4b46-4875-9d8e-b70050efe202.jpeg</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Immagine della locandina del film</t>
+        </is>
+      </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-24T07:43:55+00:00</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Sala Truffaut</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> ore 21.15</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
-        </is>
-      </c>
+      <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr">
         <is>
-          <t>059 2033166</t>
+          <t>059 236288</t>
         </is>
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>La grande guerra del Salento</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr">
         <is>
-          <t>https://www.fmav.org</t>
+          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
         </is>
       </c>
       <c r="V44" t="b">
@@ -5138,29 +5120,29 @@
       </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-grande-guerra-del-salento</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,6456499931615</t>
         </is>
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921599972490952</t>
         </is>
       </c>
       <c r="AA44" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921599972490952 44.6456499931615)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5170,63 +5152,67 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>ingresso da Strada S.Faustino, 182</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr"/>
+          <t>2022-05-26T14:09:48+00:00</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Spettacolo di danza</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-26T14:09:58+00:00</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-04T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-06-04T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-giro-del-mondo-in-90-minuti/@@images/c6bc9831-404e-402b-9e60-623bc0a2ba80.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-05-26T07:16:41+00:00</t>
+          <t>2022-05-27T06:18:12+00:00</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Parco Ferrari</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> ore 20.00</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> ingresso libero</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Il giro del mondo in 90 minuti</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
@@ -5239,7 +5225,7 @@
       </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-giro-del-mondo-in-90-minuti</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
@@ -5261,7 +5247,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5271,72 +5257,90 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
+          <t>2021-09-09T10:12:02+00:00</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
         </is>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr"/>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
+        </is>
+      </c>
       <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr"/>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr"/>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V46" t="b">
         <v>0</v>
       </c>
-      <c r="W46" t="n">
-        <v>41123</v>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
@@ -5358,7 +5362,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5368,96 +5372,98 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:24:22+00:00</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr"/>
+          <t>2022-05-26T07:16:41+00:00</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Complesso San Paolo</t>
+        </is>
+      </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr"/>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U47" t="inlineStr"/>
       <c r="V47" t="b">
         <v>0</v>
       </c>
-      <c r="W47" t="inlineStr"/>
+      <c r="W47" t="n">
+        <v>41123</v>
+      </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA47" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5467,75 +5473,63 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
+          <t>2022-05-21T10:32:36+00:00</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
+          <t>2022-06-11T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
           <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>2022-06-12T12:00:00+00:00</t>
-        </is>
-      </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-05-21T10:36:00+00:00</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U48" t="inlineStr"/>
       <c r="V48" t="b">
         <v>0</v>
       </c>
@@ -5544,7 +5538,7 @@
       </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
@@ -5566,7 +5560,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5576,50 +5570,50 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>Piazza Roma</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
@@ -5628,42 +5622,44 @@
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
-      <c r="U49" t="inlineStr"/>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V49" t="b">
         <v>0</v>
       </c>
-      <c r="W49" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5673,71 +5669,75 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>Commedia brillante</t>
-        </is>
-      </c>
+          <t>2021-08-06T11:34:26+00:00</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr"/>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
-      <c r="U50" t="inlineStr"/>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+        </is>
+      </c>
       <c r="V50" t="b">
         <v>0</v>
       </c>
@@ -5746,7 +5746,7 @@
       </c>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
@@ -5768,7 +5768,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5778,50 +5778,50 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr"/>
+          <t>2022-05-06T09:12:25+00:00</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>Piazza Roma</t>
+        </is>
+      </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
@@ -5830,44 +5830,42 @@
       <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
-      <c r="U51" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U51" t="inlineStr"/>
       <c r="V51" t="b">
         <v>0</v>
       </c>
-      <c r="W51" t="inlineStr"/>
+      <c r="W51" t="n">
+        <v>41123</v>
+      </c>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA51" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5877,28 +5875,28 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Commedia brillante</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -5908,32 +5906,36 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q52" t="inlineStr"/>
       <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
@@ -5946,7 +5948,7 @@
       </c>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
@@ -5968,7 +5970,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5978,102 +5980,96 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>Teatro Cittadella</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr"/>
       <c r="R53" t="inlineStr"/>
       <c r="S53" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
-      <c r="U53" t="inlineStr"/>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V53" t="b">
         <v>0</v>
       </c>
-      <c r="W53" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W53" t="inlineStr"/>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA53" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -6083,58 +6079,54 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O54" t="inlineStr"/>
@@ -6143,7 +6135,7 @@
       <c r="R54" t="inlineStr"/>
       <c r="S54" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T54" t="inlineStr"/>
@@ -6156,7 +6148,7 @@
       </c>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
@@ -6178,7 +6170,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -6188,83 +6180,71 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-03-19T09:19:36+00:00</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O55" t="inlineStr"/>
-      <c r="P55" t="inlineStr"/>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R55" t="inlineStr"/>
       <c r="S55" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T55" t="inlineStr"/>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U55" t="inlineStr"/>
       <c r="V55" t="b">
         <v>0</v>
       </c>
@@ -6273,7 +6253,7 @@
       </c>
       <c r="X55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr">
@@ -6295,7 +6275,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -6305,50 +6285,58 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
+          <t>2022-02-25T14:15:33+00:00</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr"/>
+          <t>2022-02-28T15:13:23+00:00</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O56" t="inlineStr"/>
@@ -6357,44 +6345,42 @@
       <c r="R56" t="inlineStr"/>
       <c r="S56" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T56" t="inlineStr"/>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U56" t="inlineStr"/>
       <c r="V56" t="b">
         <v>0</v>
       </c>
-      <c r="W56" t="inlineStr"/>
+      <c r="W56" t="n">
+        <v>41123</v>
+      </c>
       <c r="X56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y56" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z56" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA56" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -6404,96 +6390,114 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr"/>
+          <t>2022-05-06T10:18:45+00:00</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+        </is>
+      </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O57" t="inlineStr"/>
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr"/>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S57" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V57" t="b">
         <v>0</v>
       </c>
-      <c r="W57" t="inlineStr"/>
+      <c r="W57" t="n">
+        <v>41123</v>
+      </c>
       <c r="X57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y57" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z57" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA57" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -6503,99 +6507,89 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
         </is>
       </c>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:24:06+00:00</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr"/>
       <c r="N58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O58" t="inlineStr"/>
       <c r="P58" t="inlineStr"/>
       <c r="Q58" t="inlineStr"/>
-      <c r="R58" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R58" t="inlineStr"/>
       <c r="S58" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T58" t="inlineStr"/>
       <c r="U58" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V58" t="b">
         <v>0</v>
       </c>
-      <c r="W58" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W58" t="inlineStr"/>
       <c r="X58" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y58" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z58" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA58" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
@@ -6633,23 +6627,23 @@
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
+          <t>2022-05-10T08:26:10+00:00</t>
         </is>
       </c>
       <c r="M59" t="inlineStr"/>
@@ -6679,7 +6673,7 @@
       <c r="W59" t="inlineStr"/>
       <c r="X59" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y59" t="inlineStr">
@@ -6701,7 +6695,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -6711,89 +6705,99 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
-        </is>
-      </c>
-      <c r="M60" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr"/>
       <c r="Q60" t="inlineStr"/>
-      <c r="R60" t="inlineStr"/>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S60" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T60" t="inlineStr"/>
       <c r="U60" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V60" t="b">
         <v>0</v>
       </c>
-      <c r="W60" t="inlineStr"/>
+      <c r="W60" t="n">
+        <v>41123</v>
+      </c>
       <c r="X60" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y60" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z60" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA60" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6831,23 +6835,23 @@
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M61" t="inlineStr"/>
@@ -6877,20 +6881,218 @@
       <c r="W61" t="inlineStr"/>
       <c r="X61" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y61" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z61" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA61" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2022-10-15T22:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>2022-10-16T21:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:27:35+00:00</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
+      <c r="R62" t="inlineStr"/>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T62" t="inlineStr"/>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V62" t="b">
+        <v>0</v>
+      </c>
+      <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y62" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z62" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA62" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
+      <c r="R63" t="inlineStr"/>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T63" t="inlineStr"/>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V63" t="b">
+        <v>0</v>
+      </c>
+      <c r="W63" t="inlineStr"/>
+      <c r="X63" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y61" t="inlineStr">
+      <c r="Y63" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z61" t="inlineStr">
+      <c r="Z63" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA61" t="inlineStr">
+      <c r="AA63" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Mon May 30 09:21:27 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA49"/>
+  <dimension ref="A1:AA50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3020,7 +3020,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Concerti,Musica</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3030,192 +3030,178 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2021-08-25T12:27:55+00:00</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
+          <t>2022-05-30T09:17:47+00:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>In occasione della Festa della Repubblica</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2021-08-25T12:28:08+00:00</t>
+          <t>2022-05-30T09:20:03+00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2022-06-02T12:00:00+00:00</t>
+          <t>2022-06-02T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2022-06-05T13:00:00+00:00</t>
+          <t>2022-06-02T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-della-banda-cittadina-a-ferri/@@images/eaeaa0eb-f871-4bc3-885d-dd19e1c86208.jpeg</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Immagine di una precedente edizione del mercato</t>
+          <t>Palazzo Ducale sede dell'Accademia Militare</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2022-05-21T08:42:42+00:00</t>
+          <t>2022-05-30T09:20:03+00:00</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
+          <t>Cortile d'onore del Palazzo Ducale - Accedemia Miliatre</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ingresso libero</t>
+        </is>
+      </c>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>Mercato europeo</t>
+          <t>Concerto della Banda cittadina A.Ferri</t>
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>http://www.mercatieuropei.com</t>
-        </is>
-      </c>
+      <c r="U25" t="inlineStr"/>
       <c r="V25" t="b">
         <v>0</v>
       </c>
-      <c r="W25" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W25" t="n">
+        <v>41123</v>
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-della-banda-cittadina-a-ferri</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>44,647524762696584</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>10,925428060260353</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>POINT (10.925428060260353 44.647524762696584)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
+          <t>Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Montale Rangone</t>
+          <t>Modena</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2021-04-26T15:03:43+00:00</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
-        </is>
-      </c>
+          <t>2021-08-25T12:27:55+00:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2021-04-26T15:06:06+00:00</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>museo@parcomontale.it</t>
-        </is>
-      </c>
+          <t>2021-08-25T12:28:08+00:00</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2022-04-03T14:00:00+00:00</t>
+          <t>2022-06-02T12:00:00+00:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2022-06-19T15:00:00+00:00</t>
+          <t>2022-06-05T13:00:00+00:00</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Immagine di una precedente edizione del mercato</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2022-03-28T14:43:35+00:00</t>
+          <t>2022-05-21T08:42:42+00:00</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
+          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
-        </is>
-      </c>
+      <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
-        </is>
-      </c>
+      <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Mercato europeo</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr">
         <is>
-          <t>http://www.parcomontale.it/it</t>
+          <t>http://www.mercatieuropei.com</t>
         </is>
       </c>
       <c r="V26" t="b">
@@ -3223,113 +3209,135 @@
       </c>
       <c r="W26" t="inlineStr">
         <is>
-          <t>41050</t>
+          <t>41121</t>
         </is>
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,647524762696584</t>
         </is>
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,925428060260353</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.925428060260353 44.647524762696584)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Altri eventi,Manifestazioni sportive</t>
+          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Modena</t>
+          <t>Montale Rangone</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Zona tribune</t>
+          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2022-05-11T07:50:51+00:00</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>2021-04-26T15:03:43+00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr"/>
+          <t>2021-04-26T15:06:06+00:00</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>museo@parcomontale.it</t>
+        </is>
+      </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2022-06-03T07:00:00+00:00</t>
+          <t>2022-04-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2022-06-03T08:00:00+00:00</t>
+          <t>2022-06-19T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della Run 5.30 Modena</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-03-28T14:43:35+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 5.30</t>
+          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
+        </is>
+      </c>
       <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+        </is>
+      </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Run 5.30</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>http://www.parcomontale.it/it</t>
+        </is>
+      </c>
       <c r="V27" t="b">
         <v>0</v>
       </c>
-      <c r="W27" t="n">
-        <v>41123</v>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>41050</t>
+        </is>
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3351,7 +3359,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Altri eventi,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3361,58 +3369,54 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>centro storico</t>
+          <t>Zona tribune</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2022-04-29T10:05:46+00:00</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:50:51+00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-05-01T09:00:00+00:00</t>
+          <t>2022-06-03T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-07-17T10:00:00+00:00</t>
+          <t>2022-06-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Immagine presa dal sito della Run 5.30 Modena</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Piazza Torre</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
+          <t xml:space="preserve"> ore 5.30</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
@@ -3421,7 +3425,7 @@
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, aperture serali</t>
+          <t>Run 5.30</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
@@ -3434,7 +3438,7 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3456,7 +3460,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3466,112 +3470,102 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>via degli Adelardi, 4</t>
+          <t>centro storico</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:25+00:00</t>
+          <t>2022-04-29T10:05:46+00:00</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Proiezione del film di Marco Pollini</t>
+          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:52+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-06-04T06:00:00+00:00</t>
+          <t>2022-05-01T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-06-04T06:44:31+00:00</t>
+          <t>2022-07-17T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-grande-guerra-del-salento/@@images/b18d66e7-4b46-4875-9d8e-b70050efe202.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Immagine della locandina del film</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-05-24T07:43:55+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Sala Truffaut</t>
+          <t>Piazza Torre</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.15</t>
+          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>059 236288</t>
-        </is>
-      </c>
+      <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr">
         <is>
-          <t>La grande guerra del Salento</t>
+          <t>Torre Ghirlandina, aperture serali</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
-        </is>
-      </c>
+      <c r="U29" t="inlineStr"/>
       <c r="V29" t="b">
         <v>0</v>
       </c>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W29" t="n">
+        <v>41123</v>
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-grande-guerra-del-salento</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
         <is>
-          <t>44,6456499931615</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>10,921599972490952</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>POINT (10.921599972490952 44.6456499931615)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Altri eventi,Spettacoli</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3581,102 +3575,112 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ingresso da Strada S.Faustino, 182</t>
+          <t>via degli Adelardi, 4</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2022-05-26T14:09:48+00:00</t>
+          <t>2021-04-28T06:30:25+00:00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Spettacolo di danza</t>
+          <t>Proiezione del film di Marco Pollini</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2022-05-26T14:09:58+00:00</t>
+          <t>2021-04-28T06:30:52+00:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-06-04T14:00:00+00:00</t>
+          <t>2022-06-04T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-06-04T15:00:00+00:00</t>
+          <t>2022-06-04T06:44:31+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-giro-del-mondo-in-90-minuti/@@images/c6bc9831-404e-402b-9e60-623bc0a2ba80.jpeg</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-grande-guerra-del-salento/@@images/b18d66e7-4b46-4875-9d8e-b70050efe202.jpeg</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Immagine della locandina del film</t>
+        </is>
+      </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-05-27T06:18:12+00:00</t>
+          <t>2022-05-24T07:43:55+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Parco Ferrari</t>
+          <t>Sala Truffaut</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 20.00</t>
+          <t xml:space="preserve"> ore 21.15</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ingresso libero</t>
-        </is>
-      </c>
+      <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>059 236288</t>
+        </is>
+      </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Il giro del mondo in 90 minuti</t>
+          <t>La grande guerra del Salento</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
+        </is>
+      </c>
       <c r="V30" t="b">
         <v>0</v>
       </c>
-      <c r="W30" t="n">
-        <v>41123</v>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-giro-del-mondo-in-90-minuti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-grande-guerra-del-salento</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,6456499931615</t>
         </is>
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921599972490952</t>
         </is>
       </c>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921599972490952 44.6456499931615)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3686,90 +3690,80 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>ingresso da Strada S.Faustino, 182</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
+          <t>2022-05-26T14:09:48+00:00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Spettacolo di danza</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-05-26T14:09:58+00:00</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-06-04T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-04T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-giro-del-mondo-in-90-minuti/@@images/c6bc9831-404e-402b-9e60-623bc0a2ba80.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-27T06:18:12+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Parco Ferrari</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> ore 20.00</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
+          <t xml:space="preserve"> ingresso libero</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Il giro del mondo in 90 minuti</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>https://www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U31" t="inlineStr"/>
       <c r="V31" t="b">
         <v>0</v>
       </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W31" t="n">
+        <v>41123</v>
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-giro-del-mondo-in-90-minuti</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
@@ -3791,7 +3785,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3801,76 +3795,90 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
+          <t>2021-09-09T10:12:02+00:00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-05-26T07:16:41+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
         </is>
       </c>
       <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr"/>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V32" t="b">
         <v>0</v>
       </c>
-      <c r="W32" t="n">
-        <v>41123</v>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
@@ -3919,23 +3927,23 @@
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-05-26T07:20:15+00:00</t>
+          <t>2022-05-26T07:16:41+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
@@ -3945,7 +3953,7 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
@@ -3971,7 +3979,7 @@
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
@@ -3993,7 +4001,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -4003,59 +4011,63 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-05-26T07:20:15+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
@@ -4068,7 +4080,7 @@
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
@@ -4090,7 +4102,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4100,50 +4112,50 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr"/>
+          <t>2022-05-21T10:36:00+00:00</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti</t>
+        </is>
+      </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
@@ -4152,44 +4164,42 @@
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U35" t="inlineStr"/>
       <c r="V35" t="b">
         <v>0</v>
       </c>
-      <c r="W35" t="inlineStr"/>
+      <c r="W35" t="n">
+        <v>41123</v>
+      </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4199,106 +4209,96 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>Polisportiva Madonnina</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V36" t="b">
         <v>0</v>
       </c>
-      <c r="W36" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W36" t="inlineStr"/>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA36" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4308,63 +4308,75 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
+          <t>2021-08-06T11:34:26+00:00</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr"/>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr"/>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+        </is>
+      </c>
       <c r="V37" t="b">
         <v>0</v>
       </c>
@@ -4373,7 +4385,7 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
@@ -4395,7 +4407,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4405,67 +4417,59 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>Commedia brillante</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
@@ -4478,7 +4482,7 @@
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
@@ -4500,7 +4504,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4510,96 +4514,102 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t>Commedia brillante</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr"/>
+          <t>2022-03-19T09:32:45+00:00</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>Teatro Cittadella</t>
+        </is>
+      </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U39" t="inlineStr"/>
       <c r="V39" t="b">
         <v>0</v>
       </c>
-      <c r="W39" t="inlineStr"/>
+      <c r="W39" t="n">
+        <v>41123</v>
+      </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA39" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4609,54 +4619,50 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
@@ -4665,42 +4671,44 @@
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr"/>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V40" t="b">
         <v>0</v>
       </c>
-      <c r="W40" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W40" t="inlineStr"/>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA40" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4710,67 +4718,63 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
@@ -4783,7 +4787,7 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
@@ -4805,7 +4809,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4815,67 +4819,67 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr"/>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
@@ -4888,7 +4892,7 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
@@ -4910,7 +4914,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4920,83 +4924,71 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-02-25T14:15:33+00:00</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-02-28T15:13:23+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U43" t="inlineStr"/>
       <c r="V43" t="b">
         <v>0</v>
       </c>
@@ -5005,7 +4997,7 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -5027,7 +5019,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5037,89 +5029,107 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr"/>
+          <t>2022-05-06T10:18:45+00:00</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+        </is>
+      </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr"/>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V44" t="b">
         <v>0</v>
       </c>
-      <c r="W44" t="inlineStr"/>
+      <c r="W44" t="n">
+        <v>41123</v>
+      </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA44" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -5157,23 +5167,23 @@
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
+          <t>2022-05-10T08:24:06+00:00</t>
         </is>
       </c>
       <c r="M45" t="inlineStr"/>
@@ -5203,7 +5213,7 @@
       <c r="W45" t="inlineStr"/>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
@@ -5225,7 +5235,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5235,106 +5245,96 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:10+00:00</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V46" t="b">
         <v>0</v>
       </c>
-      <c r="W46" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA46" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5344,89 +5344,99 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr"/>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S47" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V47" t="b">
         <v>0</v>
       </c>
-      <c r="W47" t="inlineStr"/>
+      <c r="W47" t="n">
+        <v>41123</v>
+      </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA47" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -5464,23 +5474,23 @@
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M48" t="inlineStr"/>
@@ -5510,7 +5520,7 @@
       <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
@@ -5563,23 +5573,23 @@
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:27:35+00:00</t>
         </is>
       </c>
       <c r="M49" t="inlineStr"/>
@@ -5609,20 +5619,119 @@
       <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z49" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA49" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="inlineStr"/>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V50" t="b">
+        <v>0</v>
+      </c>
+      <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y49" t="inlineStr">
+      <c r="Y50" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z49" t="inlineStr">
+      <c r="Z50" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA49" t="inlineStr">
+      <c r="AA50" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Tue May 31 01:17:05 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -2049,7 +2049,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2057,88 +2057,114 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Viale Caduti in Guerra, 196</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2022-05-26T09:12:46+00:00</t>
+          <t>2020-09-17T12:45:54+00:00</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Giovedì 2 giugno, celebrazioni con alzabandiera e sfilata della banda cittadina. Iniziative in programma già dal 30 maggio</t>
+          <t>Gli spettacoli di ERT al Teatro Tempio</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2022-05-30T09:29:45+00:00</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr"/>
+          <t>2014-09-30T12:50:00+00:00</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>info@emiliaromagnateatro.com</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2022-05-30T09:00:00+00:00</t>
+          <t>2022-05-30T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2022-06-02T10:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/festa-della-repubblica/@@images/0031a2b2-623b-4b21-8316-cfd065155db6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/kassandra/@@images/29f75f21-a9f0-45e8-8056-8023ce88a666.jpeg</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2022-05-30T09:29:45+00:00</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
+          <t>2022-03-15T11:11:12+00:00</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Teatro Tempio</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 31 maggio e 1 giugno, 3 giugno e dal 7 al 10 giugno ore 20.30  2, 4, 5, 11 e 12 giugno ore 19.00</t>
+        </is>
+      </c>
       <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
+        </is>
+      </c>
       <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>059/2163021</t>
+        </is>
+      </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>Festa della Repubblica</t>
+          <t>Kassandra</t>
         </is>
       </c>
       <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>http://www.emiliaromagnateatro.com</t>
+        </is>
+      </c>
       <c r="V16" t="b">
         <v>0</v>
       </c>
-      <c r="W16" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/festa-della-repubblica</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/kassandra</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,64381951149482</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,93139345085676</t>
         </is>
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.93139345085676 44.64381951149482)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2148,106 +2174,112 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Largo Garibaldi, 15</t>
+          <t>via degli Adelardi, 4</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2022-05-26T10:41:07+00:00</t>
+          <t>2021-04-28T06:30:25+00:00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Rassegna degli spettacoli degli studenti degli istituti scolastici superiori di Modena</t>
+          <t>Proiezione del film di Francesco Conversano e Nene Grignaffini</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2022-05-26T10:43:09+00:00</t>
+          <t>2021-04-28T06:30:52+00:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2022-05-25T10:00:00+00:00</t>
+          <t>2022-05-31T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2022-05-31T11:00:00+00:00</t>
+          <t>2022-05-31T06:44:31+00:00</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/teatro-di-classe/@@images/e2c8fdee-bd18-4665-a203-859f06d4c9ae.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/paisan-ciao/@@images/00f14156-0e06-4604-8c79-4aa96ada1a7a.jpeg</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Teatro Storchi</t>
+          <t>Immagine della locandina del film</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2022-05-26T10:43:09+00:00</t>
+          <t>2022-05-24T07:41:04+00:00</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Teatro Storchi</t>
+          <t>Sala Truffaut</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> ore 21.15</t>
         </is>
       </c>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Prezzi dei biglietti € 8 </t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>059 236288</t>
+        </is>
+      </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Teatro di classe</t>
+          <t>Paisan, Ciao</t>
         </is>
       </c>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
+        </is>
+      </c>
       <c r="V17" t="b">
         <v>0</v>
       </c>
-      <c r="W17" t="n">
-        <v>41123</v>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/teatro-di-classe</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/paisan-ciao</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,6456499931615</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921599972490952</t>
         </is>
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921599972490952 44.6456499931615)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Altri eventi,Mercati</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2255,80 +2287,66 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Ingresso da viale Berengario</t>
-        </is>
-      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2020-12-29T15:02:32+00:00</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
+          <t>2022-05-26T09:12:46+00:00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Giovedì 2 giugno, celebrazioni con alzabandiera e sfilata della banda cittadina. Iniziative in programma già dal 30 maggio</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2020-12-29T15:05:00+00:00</t>
+          <t>2022-05-30T09:29:45+00:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2022-01-03T14:00:00+00:00</t>
+          <t>2022-05-30T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2022-12-26T14:59:00+00:00</t>
+          <t>2022-06-02T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/festa-della-repubblica/@@images/0031a2b2-623b-4b21-8316-cfd065155db6.jpeg</t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2021-12-28T10:39:07+00:00</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>Parco Novi Sad</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
-        </is>
-      </c>
+          <t>2022-05-30T09:29:45+00:00</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr">
         <is>
-          <t>Mercato settimanale del lunedì</t>
+          <t>Festa della Repubblica</t>
         </is>
       </c>
       <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.com/</t>
-        </is>
-      </c>
+      <c r="U18" t="inlineStr"/>
       <c r="V18" t="b">
         <v>0</v>
       </c>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W18" t="n">
+        <v>41123</v>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/festa-della-repubblica</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
@@ -2360,112 +2378,106 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Viale Caduti in Guerra, 196</t>
+          <t>Largo Garibaldi, 15</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2020-09-17T12:45:54+00:00</t>
+          <t>2022-05-26T10:41:07+00:00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Gli spettacoli di ERT al Teatro Tempio</t>
+          <t>Rassegna degli spettacoli degli studenti degli istituti scolastici superiori di Modena</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2014-09-30T12:50:00+00:00</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>info@emiliaromagnateatro.com</t>
-        </is>
-      </c>
+          <t>2022-05-26T10:43:09+00:00</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2022-05-30T22:00:00+00:00</t>
+          <t>2022-05-25T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-05-31T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/kassandra/@@images/29f75f21-a9f0-45e8-8056-8023ce88a666.jpeg</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/teatro-di-classe/@@images/e2c8fdee-bd18-4665-a203-859f06d4c9ae.jpeg</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Teatro Storchi</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2022-03-15T11:11:12+00:00</t>
+          <t>2022-05-26T10:43:09+00:00</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Teatro Tempio</t>
+          <t>Teatro Storchi</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 31 maggio e 1 giugno, 3 giugno e dal 7 al 10 giugno ore 20.30  2, 4, 5, 11 e 12 giugno ore 19.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
+          <t xml:space="preserve"> Prezzi dei biglietti € 8 </t>
         </is>
       </c>
       <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>059/2163021</t>
-        </is>
-      </c>
+      <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr">
         <is>
-          <t>Kassandra</t>
+          <t>Teatro di classe</t>
         </is>
       </c>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>http://www.emiliaromagnateatro.com</t>
-        </is>
-      </c>
+      <c r="U19" t="inlineStr"/>
       <c r="V19" t="b">
         <v>0</v>
       </c>
-      <c r="W19" t="inlineStr"/>
+      <c r="W19" t="n">
+        <v>41123</v>
+      </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/kassandra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/teatro-di-classe</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>44,64381951149482</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>10,93139345085676</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>POINT (10.93139345085676 44.64381951149482)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Musica,Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2475,112 +2487,114 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>via degli Adelardi, 4</t>
+          <t>Corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:25+00:00</t>
+          <t>2021-10-04T15:31:48+00:00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Proiezione del film di Francesco Conversano e Nene Grignaffini</t>
+          <t>Spettacolo lirico sinfonico in forma semiscenica</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:52+00:00</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr"/>
+          <t>2021-10-04T15:31:55+00:00</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>info@teatrocomunalemodena.it</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2022-05-31T06:00:00+00:00</t>
+          <t>2022-05-31T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2022-05-31T06:44:31+00:00</t>
+          <t>2022-05-31T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/paisan-ciao/@@images/00f14156-0e06-4604-8c79-4aa96ada1a7a.jpeg</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>Immagine della locandina del film</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolceamaro-il-gioco-delle-coppie/@@images/2429e532-09b0-41e8-9f85-aa4a21287d10.jpeg</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2022-05-24T07:41:04+00:00</t>
+          <t>2022-05-30T10:13:58+00:00</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Sala Truffaut</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.15</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> gratuito</t>
+        </is>
+      </c>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr">
         <is>
-          <t>059 236288</t>
+          <t>059 2033010</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>Paisan, Ciao</t>
+          <t>DolceAmaro: "Il gioco delle coppie"</t>
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr">
         <is>
-          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
+          <t>https://teatrocomunalemodena.it/</t>
         </is>
       </c>
       <c r="V20" t="b">
         <v>0</v>
       </c>
-      <c r="W20" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W20" t="n">
+        <v>41123</v>
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/paisan-ciao</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolceamaro-il-gioco-delle-coppie</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>44,6456499931615</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>10,921599972490952</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>POINT (10.921599972490952 44.6456499931615)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Musica,Spettacoli,Teatro</t>
+          <t>Altri eventi,Musica</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2590,83 +2604,67 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 85</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
+          <t>2022-05-20T10:02:04+00:00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Spettacolo lirico sinfonico in forma semiscenica</t>
+          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>info@teatrocomunalemodena.it</t>
-        </is>
-      </c>
+          <t>2022-05-20T10:02:34+00:00</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2022-05-31T15:00:00+00:00</t>
+          <t>2022-05-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2022-05-31T16:00:00+00:00</t>
+          <t>2022-06-30T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolceamaro-il-gioco-delle-coppie/@@images/2429e532-09b0-41e8-9f85-aa4a21287d10.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2022-05-30T10:13:58+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Piazzetta Pomposa</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
         </is>
       </c>
       <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> gratuito</t>
-        </is>
-      </c>
+      <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>059 2033010</t>
-        </is>
-      </c>
+      <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr">
         <is>
-          <t>DolceAmaro: "Il gioco delle coppie"</t>
+          <t>Serate in Pomposa - 1° edizione</t>
         </is>
       </c>
       <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>https://teatrocomunalemodena.it/</t>
-        </is>
-      </c>
+      <c r="U21" t="inlineStr"/>
       <c r="V21" t="b">
         <v>0</v>
       </c>
@@ -2675,7 +2673,7 @@
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolceamaro-il-gioco-delle-coppie</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
@@ -2697,7 +2695,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Altri eventi,Musica</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2707,63 +2705,63 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:04+00:00</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:44+00:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-03-23T16:26:51+00:00</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2022-05-12T09:00:00+00:00</t>
+          <t>2022-06-01T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2022-06-30T10:00:00+00:00</t>
+          <t>2022-06-01T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche/@@images/8e5a5fa0-1d05-41e2-9bd5-115da3e3c5ea.jpeg</t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-05-23T10:16:24+00:00</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Piazzetta Pomposa</t>
+          <t>Ritrovo e partenza: Piazza Roma davanti all'Accademia Militare</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Euro 12 a partecipante</t>
+        </is>
+      </c>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr">
         <is>
-          <t>Serate in Pomposa - 1° edizione</t>
+          <t>Free Walking Tour - Visite guidate tematiche</t>
         </is>
       </c>
       <c r="T22" t="inlineStr"/>
@@ -2776,7 +2774,7 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
@@ -2798,7 +2796,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Concerti,Musica</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2808,21 +2806,29 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:44+00:00</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr"/>
+          <t>2021-10-04T15:31:48+00:00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Rassegna "L'altro suono festival" del Teatro comunale Pavarotti-Freni</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:51+00:00</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr"/>
+          <t>2021-10-04T15:31:55+00:00</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>info@teatrocomunalemodena.it</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr">
         <is>
           <t>2022-06-01T15:00:00+00:00</t>
@@ -2835,40 +2841,44 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche/@@images/8e5a5fa0-1d05-41e2-9bd5-115da3e3c5ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/vinicio-capossela/@@images/9059bf61-ac70-4134-8ced-4386f5e54ad3.jpeg</t>
         </is>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2022-05-23T10:16:24+00:00</t>
+          <t>2022-05-04T10:45:34+00:00</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Ritrovo e partenza: Piazza Roma davanti all'Accademia Militare</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Euro 12 a partecipante</t>
-        </is>
-      </c>
+      <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>059 2033010</t>
+        </is>
+      </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>Free Walking Tour - Visite guidate tematiche</t>
+          <t>Vinicio Capossela</t>
         </is>
       </c>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>https://teatrocomunalemodena.it/</t>
+        </is>
+      </c>
       <c r="V23" t="b">
         <v>0</v>
       </c>
@@ -2877,7 +2887,7 @@
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/vinicio-capossela</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
@@ -2899,7 +2909,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Spettacoli,Concerti,Musica</t>
+          <t>Iniziative per bambini,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2909,79 +2919,63 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 85</t>
+          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Rassegna "L'altro suono festival" del Teatro comunale Pavarotti-Freni</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:00:46+00:00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>info@teatrocomunalemodena.it</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:01:08+00:00</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2022-06-01T15:00:00+00:00</t>
+          <t>2022-06-02T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2022-06-01T16:00:00+00:00</t>
+          <t>2022-06-02T07:00:00+00:00</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/vinicio-capossela/@@images/9059bf61-ac70-4134-8ced-4386f5e54ad3.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
         </is>
       </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2022-05-04T10:45:34+00:00</t>
+          <t>2022-05-11T07:01:08+00:00</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Autodromo di Modena</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
         </is>
       </c>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>059 2033010</t>
-        </is>
-      </c>
+      <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr">
         <is>
-          <t>Vinicio Capossela</t>
+          <t>Go Kart, go!</t>
         </is>
       </c>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>https://teatrocomunalemodena.it/</t>
-        </is>
-      </c>
+      <c r="U24" t="inlineStr"/>
       <c r="V24" t="b">
         <v>0</v>
       </c>
@@ -2990,7 +2984,7 @@
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/vinicio-capossela</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
@@ -3012,7 +3006,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Iniziative per bambini,Manifestazioni sportive</t>
+          <t>Concerti,Musica</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3022,59 +3016,71 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2022-05-11T07:00:46+00:00</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
+          <t>2022-05-30T09:17:47+00:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>In occasione della Festa della Repubblica</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
+          <t>2022-05-30T09:20:03+00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2022-06-02T06:00:00+00:00</t>
+          <t>2022-06-02T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2022-06-02T07:00:00+00:00</t>
+          <t>2022-06-02T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-della-banda-cittadina-a-ferri/@@images/eaeaa0eb-f871-4bc3-885d-dd19e1c86208.jpeg</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Palazzo Ducale sede dell'Accademia Militare</t>
+        </is>
+      </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
+          <t>2022-05-30T09:32:43+00:00</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Autodromo di Modena</t>
+          <t>Cortile d'onore del Palazzo Ducale - Accedemia Miliatre</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ingresso libero</t>
+        </is>
+      </c>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>Go Kart, go!</t>
+          <t>Concerto della Banda cittadina A.Ferri</t>
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
@@ -3087,7 +3093,7 @@
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-della-banda-cittadina-a-ferri</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
@@ -3109,7 +3115,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Concerti,Musica</t>
+          <t>Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3119,178 +3125,192 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2022-05-30T09:17:47+00:00</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>In occasione della Festa della Repubblica</t>
-        </is>
-      </c>
+          <t>2021-08-25T12:27:55+00:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2022-05-30T09:20:03+00:00</t>
+          <t>2021-08-25T12:28:08+00:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2022-06-02T09:00:00+00:00</t>
+          <t>2022-06-02T12:00:00+00:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2022-06-02T10:00:00+00:00</t>
+          <t>2022-06-05T13:00:00+00:00</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-della-banda-cittadina-a-ferri/@@images/eaeaa0eb-f871-4bc3-885d-dd19e1c86208.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Palazzo Ducale sede dell'Accademia Militare</t>
+          <t>Immagine di una precedente edizione del mercato</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2022-05-30T09:32:43+00:00</t>
+          <t>2022-05-21T08:42:42+00:00</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Cortile d'onore del Palazzo Ducale - Accedemia Miliatre</t>
+          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ingresso libero</t>
-        </is>
-      </c>
+      <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr">
         <is>
-          <t>Concerto della Banda cittadina A.Ferri</t>
+          <t>Mercato europeo</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr"/>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>http://www.mercatieuropei.com</t>
+        </is>
+      </c>
       <c r="V26" t="b">
         <v>0</v>
       </c>
-      <c r="W26" t="n">
-        <v>41123</v>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-della-banda-cittadina-a-ferri</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,647524762696584</t>
         </is>
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,925428060260353</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.925428060260353 44.647524762696584)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Modena</t>
+          <t>Montale Rangone</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2021-08-25T12:27:55+00:00</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>2021-04-26T15:03:43+00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2021-08-25T12:28:08+00:00</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr"/>
+          <t>2021-04-26T15:06:06+00:00</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>museo@parcomontale.it</t>
+        </is>
+      </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2022-06-02T12:00:00+00:00</t>
+          <t>2022-04-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2022-06-05T13:00:00+00:00</t>
+          <t>2022-06-19T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Immagine di una precedente edizione del mercato</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-05-21T08:42:42+00:00</t>
+          <t>2022-03-28T14:43:35+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
+          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
+        </is>
+      </c>
       <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+        </is>
+      </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Mercato europeo</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr">
         <is>
-          <t>http://www.mercatieuropei.com</t>
+          <t>http://www.parcomontale.it/it</t>
         </is>
       </c>
       <c r="V27" t="b">
@@ -3298,135 +3318,113 @@
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>41121</t>
+          <t>41050</t>
         </is>
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>44,647524762696584</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>10,925428060260353</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA27" t="inlineStr">
         <is>
-          <t>POINT (10.925428060260353 44.647524762696584)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
+          <t>Altri eventi,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Montale Rangone</t>
+          <t>Modena</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
+          <t>Zona tribune</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2021-04-26T15:03:43+00:00</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:50:51+00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2021-04-26T15:06:06+00:00</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>museo@parcomontale.it</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:51:19+00:00</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-04-03T14:00:00+00:00</t>
+          <t>2022-06-03T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-06-19T15:00:00+00:00</t>
+          <t>2022-06-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Immagine presa dal sito della Run 5.30 Modena</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-03-28T14:43:35+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
+          <t xml:space="preserve"> ore 5.30</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
-        </is>
-      </c>
+      <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
-        </is>
-      </c>
+      <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Run 5.30</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>http://www.parcomontale.it/it</t>
-        </is>
-      </c>
+      <c r="U28" t="inlineStr"/>
       <c r="V28" t="b">
         <v>0</v>
       </c>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>41050</t>
-        </is>
+      <c r="W28" t="n">
+        <v>41123</v>
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3448,7 +3446,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Altri eventi,Manifestazioni sportive</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3458,54 +3456,58 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Zona tribune</t>
+          <t>centro storico</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2022-05-11T07:50:51+00:00</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
+          <t>2022-04-29T10:05:46+00:00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-06-03T07:00:00+00:00</t>
+          <t>2022-05-01T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-06-03T08:00:00+00:00</t>
+          <t>2022-07-17T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della Run 5.30 Modena</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Piazza Torre</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 5.30</t>
+          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
@@ -3514,7 +3516,7 @@
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Run 5.30</t>
+          <t>Torre Ghirlandina, aperture serali</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
@@ -3527,7 +3529,7 @@
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
@@ -3549,7 +3551,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3559,102 +3561,112 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>centro storico</t>
+          <t>via degli Adelardi, 4</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2022-04-29T10:05:46+00:00</t>
+          <t>2021-04-28T06:30:25+00:00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
+          <t>Proiezione del film di Marco Pollini</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2021-04-28T06:30:52+00:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-05-01T09:00:00+00:00</t>
+          <t>2022-06-04T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-07-17T10:00:00+00:00</t>
+          <t>2022-06-04T06:44:31+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-grande-guerra-del-salento/@@images/b18d66e7-4b46-4875-9d8e-b70050efe202.jpeg</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Immagine della locandina del film</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-05-24T07:43:55+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Piazza Torre</t>
+          <t>Sala Truffaut</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
+          <t xml:space="preserve"> ore 21.15</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>059 236288</t>
+        </is>
+      </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, aperture serali</t>
+          <t>La grande guerra del Salento</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
+        </is>
+      </c>
       <c r="V30" t="b">
         <v>0</v>
       </c>
-      <c r="W30" t="n">
-        <v>41123</v>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-grande-guerra-del-salento</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,6456499931615</t>
         </is>
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921599972490952</t>
         </is>
       </c>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921599972490952 44.6456499931615)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3664,112 +3676,102 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>via degli Adelardi, 4</t>
+          <t>centro storico</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:25+00:00</t>
+          <t>2022-05-30T09:44:00+00:00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Proiezione del film di Marco Pollini</t>
+          <t xml:space="preserve">Evneto dedicato alle famiglie, che fa divertire grandi e piccini </t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:52+00:00</t>
+          <t>2022-05-30T09:44:15+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-06-04T06:00:00+00:00</t>
+          <t>2022-06-04T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-06-04T06:44:31+00:00</t>
+          <t>2022-06-05T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-grande-guerra-del-salento/@@images/b18d66e7-4b46-4875-9d8e-b70050efe202.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/modenagioca/@@images/b0abc4c6-5a49-4d8e-aa9f-0fd608824e22.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Immagine della locandina del film</t>
+          <t>immagine dal sito modenagioca.it</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-24T07:43:55+00:00</t>
+          <t>2022-05-30T10:12:24+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Sala Truffaut</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.15</t>
+          <t xml:space="preserve"> dalle ore 9 alle 20</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>059 236288</t>
-        </is>
-      </c>
+      <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>La grande guerra del Salento</t>
+          <t>ModenaGioca</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
-        </is>
-      </c>
+      <c r="U31" t="inlineStr"/>
       <c r="V31" t="b">
         <v>0</v>
       </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W31" t="n">
+        <v>41123</v>
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-grande-guerra-del-salento</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/modenagioca</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
         <is>
-          <t>44,6456499931615</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>10,921599972490952</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA31" t="inlineStr">
         <is>
-          <t>POINT (10.921599972490952 44.6456499931615)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3779,67 +3781,67 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>centro storico</t>
+          <t>ingresso da Strada S.Faustino, 182</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:44:00+00:00</t>
+          <t>2022-05-26T14:09:48+00:00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Evneto dedicato alle famiglie, che fa divertire grandi e piccini </t>
+          <t>Spettacolo di danza</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:44:15+00:00</t>
+          <t>2022-05-26T14:09:58+00:00</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-06-04T09:00:00+00:00</t>
+          <t>2022-06-04T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-06-05T10:00:00+00:00</t>
+          <t>2022-06-04T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/modenagioca/@@images/b0abc4c6-5a49-4d8e-aa9f-0fd608824e22.jpeg</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>immagine dal sito modenagioca.it</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-giro-del-mondo-in-90-minuti/@@images/c6bc9831-404e-402b-9e60-623bc0a2ba80.jpeg</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-05-30T10:12:24+00:00</t>
+          <t>2022-05-27T06:18:12+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Parco Ferrari</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 20</t>
+          <t xml:space="preserve"> ore 20.00</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ingresso libero</t>
+        </is>
+      </c>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr">
         <is>
-          <t>ModenaGioca</t>
+          <t>Il giro del mondo in 90 minuti</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
@@ -3852,7 +3854,7 @@
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/modenagioca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-giro-del-mondo-in-90-minuti</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
@@ -3874,7 +3876,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Altri eventi,Spettacoli</t>
+          <t>Altri eventi,Mercati</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3884,80 +3886,78 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ingresso da Strada S.Faustino, 182</t>
+          <t>Ingresso da viale Berengario</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2022-05-26T14:09:48+00:00</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Spettacolo di danza</t>
-        </is>
-      </c>
+          <t>2020-12-29T15:02:32+00:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2022-05-26T14:09:58+00:00</t>
+          <t>2020-12-29T15:05:00+00:00</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-06-04T14:00:00+00:00</t>
+          <t>2022-01-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-04T15:00:00+00:00</t>
+          <t>2022-12-26T14:59:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-giro-del-mondo-in-90-minuti/@@images/c6bc9831-404e-402b-9e60-623bc0a2ba80.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-05-27T06:18:12+00:00</t>
+          <t>2021-12-28T10:39:07+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Parco Ferrari</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 20.00</t>
+          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ingresso libero</t>
-        </is>
-      </c>
+      <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Il giro del mondo in 90 minuti</t>
+          <t>Mercato settimanale del lunedì</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr"/>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.com/</t>
+        </is>
+      </c>
       <c r="V33" t="b">
         <v>0</v>
       </c>
-      <c r="W33" t="n">
-        <v>41123</v>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-giro-del-mondo-in-90-minuti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">

</xml_diff>

<commit_message>
Latest data: Wed Jun  1 01:26:41 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA59"/>
+  <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2164,7 +2164,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Altri eventi,Musica</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2174,112 +2174,98 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>via degli Adelardi, 4</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:25+00:00</t>
+          <t>2022-05-20T10:02:04+00:00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Proiezione del film di Francesco Conversano e Nene Grignaffini</t>
+          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:52+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2022-05-31T06:00:00+00:00</t>
+          <t>2022-05-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2022-05-31T06:44:31+00:00</t>
+          <t>2022-06-30T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/paisan-ciao/@@images/00f14156-0e06-4604-8c79-4aa96ada1a7a.jpeg</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>Immagine della locandina del film</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2022-05-24T07:41:04+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Sala Truffaut</t>
+          <t>Piazzetta Pomposa</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.15</t>
+          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
         </is>
       </c>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>059 236288</t>
-        </is>
-      </c>
+      <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Paisan, Ciao</t>
+          <t>Serate in Pomposa - 1° edizione</t>
         </is>
       </c>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
-        </is>
-      </c>
+      <c r="U17" t="inlineStr"/>
       <c r="V17" t="b">
         <v>0</v>
       </c>
-      <c r="W17" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W17" t="n">
+        <v>41123</v>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/paisan-ciao</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>44,6456499931615</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>10,921599972490952</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>POINT (10.921599972490952 44.6456499931615)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2287,53 +2273,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Piazza Roma</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2022-05-26T09:12:46+00:00</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Giovedì 2 giugno, celebrazioni con alzabandiera e sfilata della banda cittadina. Iniziative in programma già dal 30 maggio</t>
-        </is>
-      </c>
+          <t>2022-03-23T16:26:44+00:00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2022-05-30T09:29:45+00:00</t>
+          <t>2022-03-23T16:26:51+00:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2022-05-30T09:00:00+00:00</t>
+          <t>2022-06-01T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2022-06-02T10:00:00+00:00</t>
+          <t>2022-06-01T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/festa-della-repubblica/@@images/0031a2b2-623b-4b21-8316-cfd065155db6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche/@@images/8e5a5fa0-1d05-41e2-9bd5-115da3e3c5ea.jpeg</t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2022-05-30T09:29:45+00:00</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
+          <t>2022-05-23T10:16:24+00:00</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Ritrovo e partenza: Piazza Roma davanti all'Accademia Militare</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ore 19.00</t>
+        </is>
+      </c>
       <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Euro 12 a partecipante</t>
+        </is>
+      </c>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr">
         <is>
-          <t>Festa della Repubblica</t>
+          <t>Free Walking Tour - Visite guidate tematiche</t>
         </is>
       </c>
       <c r="T18" t="inlineStr"/>
@@ -2346,7 +2344,7 @@
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/festa-della-repubblica</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
@@ -2368,7 +2366,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Spettacoli,Concerti,Musica</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2378,53 +2376,53 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Largo Garibaldi, 15</t>
+          <t>Corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2022-05-26T10:41:07+00:00</t>
+          <t>2021-10-04T15:31:48+00:00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Rassegna degli spettacoli degli studenti degli istituti scolastici superiori di Modena</t>
+          <t>Rassegna "L'altro suono festival" del Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2022-05-26T10:43:09+00:00</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr"/>
+          <t>2021-10-04T15:31:55+00:00</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>info@teatrocomunalemodena.it</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2022-05-25T10:00:00+00:00</t>
+          <t>2022-06-01T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2022-05-31T11:00:00+00:00</t>
+          <t>2022-06-01T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/teatro-di-classe/@@images/e2c8fdee-bd18-4665-a203-859f06d4c9ae.jpeg</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>Teatro Storchi</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/vinicio-capossela/@@images/9059bf61-ac70-4134-8ced-4386f5e54ad3.jpeg</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2022-05-26T10:43:09+00:00</t>
+          <t>2022-05-04T10:45:34+00:00</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Teatro Storchi</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -2433,20 +2431,24 @@
         </is>
       </c>
       <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Prezzi dei biglietti € 8 </t>
-        </is>
-      </c>
+      <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr"/>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>059 2033010</t>
+        </is>
+      </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>Teatro di classe</t>
+          <t>Vinicio Capossela</t>
         </is>
       </c>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>https://teatrocomunalemodena.it/</t>
+        </is>
+      </c>
       <c r="V19" t="b">
         <v>0</v>
       </c>
@@ -2455,7 +2457,7 @@
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/teatro-di-classe</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/vinicio-capossela</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
@@ -2477,7 +2479,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Musica,Spettacoli,Teatro</t>
+          <t>Iniziative per bambini,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2487,83 +2489,63 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 85</t>
+          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Spettacolo lirico sinfonico in forma semiscenica</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:00:46+00:00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>info@teatrocomunalemodena.it</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:01:08+00:00</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2022-05-31T15:00:00+00:00</t>
+          <t>2022-06-02T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2022-05-31T16:00:00+00:00</t>
+          <t>2022-06-02T07:00:00+00:00</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolceamaro-il-gioco-delle-coppie/@@images/2429e532-09b0-41e8-9f85-aa4a21287d10.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2022-05-30T10:13:58+00:00</t>
+          <t>2022-05-11T07:01:08+00:00</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Autodromo di Modena</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> gratuito</t>
-        </is>
-      </c>
+      <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>059 2033010</t>
-        </is>
-      </c>
+      <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr">
         <is>
-          <t>DolceAmaro: "Il gioco delle coppie"</t>
+          <t>Go Kart, go!</t>
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>https://teatrocomunalemodena.it/</t>
-        </is>
-      </c>
+      <c r="U20" t="inlineStr"/>
       <c r="V20" t="b">
         <v>0</v>
       </c>
@@ -2572,7 +2554,7 @@
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolceamaro-il-gioco-delle-coppie</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
@@ -2594,7 +2576,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Altri eventi,Musica</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2602,65 +2584,53 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Centro storico</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:04+00:00</t>
+          <t>2022-05-26T09:12:46+00:00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
+          <t>Giovedì 2 giugno, celebrazioni con alzabandiera e sfilata della banda cittadina. Iniziative in programma già dal 30 maggio</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-05-30T09:29:45+00:00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2022-05-12T09:00:00+00:00</t>
+          <t>2022-05-30T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2022-06-30T10:00:00+00:00</t>
+          <t>2022-06-02T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/festa-della-repubblica/@@images/0031a2b2-623b-4b21-8316-cfd065155db6.jpeg</t>
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>Piazzetta Pomposa</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
-        </is>
-      </c>
+          <t>2022-05-30T09:29:45+00:00</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr">
         <is>
-          <t>Serate in Pomposa - 1° edizione</t>
+          <t>Festa della Repubblica</t>
         </is>
       </c>
       <c r="T21" t="inlineStr"/>
@@ -2673,7 +2643,7 @@
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/festa-della-repubblica</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
@@ -2695,7 +2665,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Concerti,Musica</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2710,58 +2680,66 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:44+00:00</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
+          <t>2022-05-30T09:17:47+00:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>In occasione della Festa della Repubblica</t>
+        </is>
+      </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2022-03-23T16:26:51+00:00</t>
+          <t>2022-05-30T09:20:03+00:00</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2022-06-01T15:00:00+00:00</t>
+          <t>2022-06-02T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2022-06-01T16:00:00+00:00</t>
+          <t>2022-06-02T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche/@@images/8e5a5fa0-1d05-41e2-9bd5-115da3e3c5ea.jpeg</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-della-banda-cittadina-a-ferri/@@images/eaeaa0eb-f871-4bc3-885d-dd19e1c86208.jpeg</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Palazzo Ducale sede dell'Accademia Militare</t>
+        </is>
+      </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2022-05-23T10:16:24+00:00</t>
+          <t>2022-05-30T09:32:43+00:00</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Ritrovo e partenza: Piazza Roma davanti all'Accademia Militare</t>
+          <t>Cortile d'onore del Palazzo Ducale - Accedemia Miliatre</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Euro 12 a partecipante</t>
+          <t xml:space="preserve"> ingresso libero</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr">
         <is>
-          <t>Free Walking Tour - Visite guidate tematiche</t>
+          <t>Concerto della Banda cittadina A.Ferri</t>
         </is>
       </c>
       <c r="T22" t="inlineStr"/>
@@ -2774,7 +2752,7 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy5_of_free-walking-tour-visite-guidate-tematiche</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-della-banda-cittadina-a-ferri</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
@@ -2796,7 +2774,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Spettacoli,Concerti,Musica</t>
+          <t>Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2806,185 +2784,205 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Corso Canalgrande, 85</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:48+00:00</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Rassegna "L'altro suono festival" del Teatro comunale Pavarotti-Freni</t>
-        </is>
-      </c>
+          <t>2021-08-25T12:27:55+00:00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2021-10-04T15:31:55+00:00</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>info@teatrocomunalemodena.it</t>
-        </is>
-      </c>
+          <t>2021-08-25T12:28:08+00:00</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2022-06-01T15:00:00+00:00</t>
+          <t>2022-06-02T12:00:00+00:00</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2022-06-01T16:00:00+00:00</t>
+          <t>2022-06-05T13:00:00+00:00</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/vinicio-capossela/@@images/9059bf61-ac70-4134-8ced-4386f5e54ad3.jpeg</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Immagine di una precedente edizione del mercato</t>
+        </is>
+      </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2022-05-04T10:45:34+00:00</t>
+          <t>2022-05-21T08:42:42+00:00</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
         </is>
       </c>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>059 2033010</t>
-        </is>
-      </c>
+      <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr">
         <is>
-          <t>Vinicio Capossela</t>
+          <t>Mercato europeo</t>
         </is>
       </c>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr">
         <is>
-          <t>https://teatrocomunalemodena.it/</t>
+          <t>http://www.mercatieuropei.com</t>
         </is>
       </c>
       <c r="V23" t="b">
         <v>0</v>
       </c>
-      <c r="W23" t="n">
-        <v>41123</v>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/vinicio-capossela</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,647524762696584</t>
         </is>
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,925428060260353</t>
         </is>
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.925428060260353 44.647524762696584)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Iniziative per bambini,Manifestazioni sportive</t>
+          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Modena</t>
+          <t>Montale Rangone</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
+          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2022-05-11T07:00:46+00:00</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
+          <t>2021-04-26T15:03:43+00:00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
+          <t>2021-04-26T15:06:06+00:00</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>museo@parcomontale.it</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2022-06-02T06:00:00+00:00</t>
+          <t>2022-04-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2022-06-02T07:00:00+00:00</t>
+          <t>2022-06-19T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Parco archeologico della Terramara di Montale</t>
+        </is>
+      </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
+          <t>2022-03-28T14:43:35+00:00</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Autodromo di Modena</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
+          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
         </is>
       </c>
       <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
+        </is>
+      </c>
       <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="inlineStr"/>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+        </is>
+      </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>Go Kart, go!</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr"/>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>http://www.parcomontale.it/it</t>
+        </is>
+      </c>
       <c r="V24" t="b">
         <v>0</v>
       </c>
-      <c r="W24" t="n">
-        <v>41123</v>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>41050</t>
+        </is>
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
@@ -3006,7 +3004,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Concerti,Musica</t>
+          <t>Altri eventi,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3016,71 +3014,63 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Zona tribune</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2022-05-30T09:17:47+00:00</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>In occasione della Festa della Repubblica</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:50:51+00:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2022-05-30T09:20:03+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2022-06-02T09:00:00+00:00</t>
+          <t>2022-06-03T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2022-06-02T10:00:00+00:00</t>
+          <t>2022-06-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-della-banda-cittadina-a-ferri/@@images/eaeaa0eb-f871-4bc3-885d-dd19e1c86208.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Palazzo Ducale sede dell'Accademia Militare</t>
+          <t>Immagine presa dal sito della Run 5.30 Modena</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2022-05-30T09:32:43+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Cortile d'onore del Palazzo Ducale - Accedemia Miliatre</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> ore 5.30</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ingresso libero</t>
-        </is>
-      </c>
+      <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>Concerto della Banda cittadina A.Ferri</t>
+          <t>Run 5.30</t>
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
@@ -3093,7 +3083,7 @@
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-della-banda-cittadina-a-ferri</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
@@ -3115,7 +3105,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3125,54 +3115,58 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>centro storico</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2021-08-25T12:27:55+00:00</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
+          <t>2022-04-29T10:05:46+00:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2021-08-25T12:28:08+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2022-06-02T12:00:00+00:00</t>
+          <t>2022-05-01T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2022-06-05T13:00:00+00:00</t>
+          <t>2022-07-17T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Immagine di una precedente edizione del mercato</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2022-05-21T08:42:42+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
+          <t>Piazza Torre</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
+          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
@@ -3181,136 +3175,122 @@
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr">
         <is>
-          <t>Mercato europeo</t>
+          <t>Torre Ghirlandina, aperture serali</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>http://www.mercatieuropei.com</t>
-        </is>
-      </c>
+      <c r="U26" t="inlineStr"/>
       <c r="V26" t="b">
         <v>0</v>
       </c>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W26" t="n">
+        <v>41123</v>
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>44,647524762696584</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>10,925428060260353</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>POINT (10.925428060260353 44.647524762696584)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Montale Rangone</t>
+          <t>Modena</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
+          <t>via degli Adelardi, 4</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2021-04-26T15:03:43+00:00</t>
+          <t>2021-04-28T06:30:25+00:00</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+          <t>Proiezione del film di Marco Pollini</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2021-04-26T15:06:06+00:00</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>museo@parcomontale.it</t>
-        </is>
-      </c>
+          <t>2021-04-28T06:30:52+00:00</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2022-04-03T14:00:00+00:00</t>
+          <t>2022-06-04T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2022-06-19T15:00:00+00:00</t>
+          <t>2022-06-04T06:44:31+00:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-grande-guerra-del-salento/@@images/b18d66e7-4b46-4875-9d8e-b70050efe202.jpeg</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Immagine della locandina del film</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-03-28T14:43:35+00:00</t>
+          <t>2022-05-24T07:43:55+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Sala Truffaut</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
+          <t xml:space="preserve"> ore 21.15</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
-        </is>
-      </c>
+      <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr">
         <is>
-          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+          <t>059 236288</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>La grande guerra del Salento</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr">
         <is>
-          <t>http://www.parcomontale.it/it</t>
+          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
         </is>
       </c>
       <c r="V27" t="b">
@@ -3318,34 +3298,34 @@
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>41050</t>
+          <t>41121</t>
         </is>
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-grande-guerra-del-salento</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,6456499931615</t>
         </is>
       </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921599972490952</t>
         </is>
       </c>
       <c r="AA27" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921599972490952 44.6456499931615)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Altri eventi,Manifestazioni sportive</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3355,54 +3335,58 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Zona tribune</t>
+          <t>centro storico</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2022-05-11T07:50:51+00:00</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr"/>
+          <t>2022-05-30T09:44:00+00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Evneto dedicato alle famiglie, che fa divertire grandi e piccini </t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-05-30T09:44:15+00:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-06-03T07:00:00+00:00</t>
+          <t>2022-06-04T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-06-03T08:00:00+00:00</t>
+          <t>2022-06-05T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/modenagioca/@@images/b0abc4c6-5a49-4d8e-aa9f-0fd608824e22.jpeg</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della Run 5.30 Modena</t>
+          <t>immagine dal sito modenagioca.it</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-05-30T10:12:24+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 5.30</t>
+          <t xml:space="preserve"> dalle ore 9 alle 20</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
@@ -3411,7 +3395,7 @@
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Run 5.30</t>
+          <t>ModenaGioca</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
@@ -3424,7 +3408,7 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/modenagioca</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3446,7 +3430,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3456,67 +3440,67 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>centro storico</t>
+          <t>ingresso da Strada S.Faustino, 182</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2022-04-29T10:05:46+00:00</t>
+          <t>2022-05-26T14:09:48+00:00</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
+          <t>Spettacolo di danza</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-05-26T14:09:58+00:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-05-01T09:00:00+00:00</t>
+          <t>2022-06-04T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-07-17T10:00:00+00:00</t>
+          <t>2022-06-04T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-giro-del-mondo-in-90-minuti/@@images/c6bc9831-404e-402b-9e60-623bc0a2ba80.jpeg</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-05-27T06:18:12+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Piazza Torre</t>
+          <t>Parco Ferrari</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
+          <t xml:space="preserve"> ore 20.00</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ingresso libero</t>
+        </is>
+      </c>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, aperture serali</t>
+          <t>Il giro del mondo in 90 minuti</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
@@ -3529,7 +3513,7 @@
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-giro-del-mondo-in-90-minuti</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
@@ -3551,7 +3535,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Altri eventi,Mercati</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3561,77 +3545,65 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>via degli Adelardi, 4</t>
+          <t>Ingresso da viale Berengario</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:25+00:00</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Proiezione del film di Marco Pollini</t>
-        </is>
-      </c>
+          <t>2020-12-29T15:02:32+00:00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:52+00:00</t>
+          <t>2020-12-29T15:05:00+00:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-06-04T06:00:00+00:00</t>
+          <t>2022-01-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-06-04T06:44:31+00:00</t>
+          <t>2022-12-26T14:59:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-grande-guerra-del-salento/@@images/b18d66e7-4b46-4875-9d8e-b70050efe202.jpeg</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>Immagine della locandina del film</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-05-24T07:43:55+00:00</t>
+          <t>2021-12-28T10:39:07+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Sala Truffaut</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.15</t>
+          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>059 236288</t>
-        </is>
-      </c>
+      <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr">
         <is>
-          <t>La grande guerra del Salento</t>
+          <t>Mercato settimanale del lunedì</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr">
         <is>
-          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
+          <t>http://www.consorzioilmercato.com/</t>
         </is>
       </c>
       <c r="V30" t="b">
@@ -3644,29 +3616,29 @@
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-grande-guerra-del-salento</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>44,6456499931615</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>10,921599972490952</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>POINT (10.921599972490952 44.6456499931615)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3676,80 +3648,90 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>centro storico</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2022-05-30T09:44:00+00:00</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Evneto dedicato alle famiglie, che fa divertire grandi e piccini </t>
-        </is>
-      </c>
+          <t>2021-09-09T10:12:02+00:00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2022-05-30T09:44:15+00:00</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-06-04T09:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-06-05T10:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/modenagioca/@@images/b0abc4c6-5a49-4d8e-aa9f-0fd608824e22.jpeg</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>immagine dal sito modenagioca.it</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-30T10:12:24+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 20</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
+        </is>
+      </c>
       <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr"/>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>ModenaGioca</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr"/>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V31" t="b">
         <v>0</v>
       </c>
-      <c r="W31" t="n">
-        <v>41123</v>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/modenagioca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
@@ -3771,7 +3753,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Altri eventi,Spettacoli</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3781,67 +3763,63 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ingresso da Strada S.Faustino, 182</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2022-05-26T14:09:48+00:00</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Spettacolo di danza</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:24:22+00:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2022-05-26T14:09:58+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-06-04T14:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-06-04T15:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-giro-del-mondo-in-90-minuti/@@images/c6bc9831-404e-402b-9e60-623bc0a2ba80.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-05-27T06:18:12+00:00</t>
+          <t>2022-05-26T07:16:41+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Parco Ferrari</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 20.00</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ingresso libero</t>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
         </is>
       </c>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Il giro del mondo in 90 minuti</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
@@ -3854,7 +3832,7 @@
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-giro-del-mondo-in-90-minuti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
@@ -3876,7 +3854,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Altri eventi,Mercati</t>
+          <t>Visite guidate,Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3884,80 +3862,78 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Ingresso da viale Berengario</t>
-        </is>
-      </c>
+      <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2020-12-29T15:02:32+00:00</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
+          <t>2022-05-30T09:56:40+00:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2020-12-29T15:05:00+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-01-03T14:00:00+00:00</t>
+          <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-12-26T14:59:00+00:00</t>
+          <t>2022-06-10T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2021-12-28T10:39:07+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Duomo di Modena</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
+          <t xml:space="preserve"> dalle ore 20.30</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gratuito</t>
+        </is>
+      </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Mercato settimanale del lunedì</t>
+          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.com/</t>
-        </is>
-      </c>
+      <c r="U33" t="inlineStr"/>
       <c r="V33" t="b">
         <v>0</v>
       </c>
-      <c r="W33" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W33" t="n">
+        <v>41123</v>
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
@@ -3979,7 +3955,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Concerti,Spettacoli,Altri eventi</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3989,90 +3965,76 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
+          <t>2022-05-30T11:40:24+00:00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-05-30T11:41:23+00:00</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-06-10T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-10T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-30T11:42:41+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
-        </is>
-      </c>
+      <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>https://www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U34" t="inlineStr"/>
       <c r="V34" t="b">
         <v>0</v>
       </c>
-      <c r="W34" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W34" t="n">
+        <v>41123</v>
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
@@ -4094,7 +4056,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Concerti</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4104,98 +4066,112 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Strada Pomposiana 292</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr"/>
+          <t>2022-05-30T09:03:14+00:00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-10T19:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-06-10T21:00:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-05-26T07:16:41+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Fattoria Centofiori</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> Ore 21.00</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
         </is>
       </c>
       <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="inlineStr"/>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>Whatsapp 3293357131</t>
+        </is>
+      </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Marco Ferri Quartet</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr"/>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>www.fattoriacentofiori.it</t>
+        </is>
+      </c>
       <c r="V35" t="b">
         <v>0</v>
       </c>
-      <c r="W35" t="n">
-        <v>41123</v>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>41123</t>
+        </is>
       </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,63693000592147</t>
         </is>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,81076003183179</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.81076003183179 44.63693000592147)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Visite guidate,Altri eventi,Spettacoli</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4203,65 +4179,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>via Selmi, 63</t>
+        </is>
+      </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2022-05-30T09:56:40+00:00</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:24:22+00:00</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-06-10T09:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-10T10:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-05-26T07:20:15+00:00</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Duomo di Modena</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 20.30</t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gratuito</t>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
         </is>
       </c>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
@@ -4274,7 +4250,7 @@
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
@@ -4296,7 +4272,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Altri eventi</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4306,54 +4282,50 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 85</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-10T11:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-10T12:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-05-30T11:42:41+00:00</t>
+          <t>2022-05-21T10:36:00+00:00</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
@@ -4362,7 +4334,7 @@
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
@@ -4375,7 +4347,7 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
@@ -4397,7 +4369,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Concerti</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4407,112 +4379,96 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Strada Pomposiana 292</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2022-05-30T09:03:14+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-10T19:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-10T21:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>Fattoria Centofiori</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ore 21.00</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
-        </is>
-      </c>
+      <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>Whatsapp 3293357131</t>
-        </is>
-      </c>
+      <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Marco Ferri Quartet</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr">
         <is>
-          <t>www.fattoriacentofiori.it</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V38" t="b">
         <v>0</v>
       </c>
-      <c r="W38" t="inlineStr">
-        <is>
-          <t>41123</t>
-        </is>
-      </c>
+      <c r="W38" t="inlineStr"/>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
         <is>
-          <t>44,63693000592147</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>10,81076003183179</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA38" t="inlineStr">
         <is>
-          <t>POINT (10.81076003183179 44.63693000592147)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4522,63 +4478,63 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>via S.Pietro, 1</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr"/>
+          <t>2022-05-30T10:02:38+00:00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-06-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-06-12T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-05-26T07:20:15+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Chiostro di San Pietro</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> ore 15.00</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
-        </is>
-      </c>
+      <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Contro la guerra</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
@@ -4591,7 +4547,7 @@
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
@@ -4613,7 +4569,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4623,63 +4579,75 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
+          <t>2021-08-06T11:34:26+00:00</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr"/>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr"/>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+        </is>
+      </c>
       <c r="V40" t="b">
         <v>0</v>
       </c>
@@ -4688,7 +4656,7 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
@@ -4710,7 +4678,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4720,50 +4688,50 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr"/>
+          <t>2022-05-06T09:12:25+00:00</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>Piazza Roma</t>
+        </is>
+      </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
@@ -4772,44 +4740,42 @@
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U41" t="inlineStr"/>
       <c r="V41" t="b">
         <v>0</v>
       </c>
-      <c r="W41" t="inlineStr"/>
+      <c r="W41" t="n">
+        <v>41123</v>
+      </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA41" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4819,63 +4785,67 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>via S.Pietro, 1</t>
+          <t>ingresso da corso Cavour, 2</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:38+00:00</t>
+          <t>2022-05-30T11:14:00+00:00</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Presentazione del libro</t>
+          <t>Laboratorio per bambini 6-10 anni</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-12T09:00:00+00:00</t>
+          <t>2022-06-16T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-06-12T10:00:00+00:00</t>
+          <t>2022-06-16T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Chiostro di San Pietro</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.00</t>
+          <t xml:space="preserve"> ore 17.00</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr"/>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
+        </is>
+      </c>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>Contro la guerra</t>
+          <t>Un percorso ad arte: il mio giardino blu</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
@@ -4888,7 +4858,7 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
@@ -4910,7 +4880,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4920,75 +4890,71 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr"/>
+          <t>2022-03-19T09:15:00+00:00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Commedia brillante</t>
+        </is>
+      </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
-      <c r="P43" t="inlineStr"/>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U43" t="inlineStr"/>
       <c r="V43" t="b">
         <v>0</v>
       </c>
@@ -4997,7 +4963,7 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -5019,7 +4985,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5029,63 +4995,79 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
+          <t>2022-05-30T10:57:49+00:00</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-05-30T11:00:13+00:00</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>FMAV - Museo della Figurina</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr"/>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+        </is>
+      </c>
       <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr"/>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
-      <c r="U44" t="inlineStr"/>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>www.fmav.org</t>
+        </is>
+      </c>
       <c r="V44" t="b">
         <v>0</v>
       </c>
@@ -5094,7 +5076,7 @@
       </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
@@ -5116,7 +5098,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Iniziative per bambini</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5126,71 +5108,79 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ingresso da corso Cavour, 2</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:00+00:00</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>Laboratorio per bambini 6-10 anni</t>
-        </is>
-      </c>
+          <t>2022-05-30T10:57:49+00:00</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-06-16T11:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-06-16T12:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-30T11:06:40+00:00</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>FMAV - Museo della Figurina</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 17.00</t>
+          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
+          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
         </is>
       </c>
       <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="inlineStr"/>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>Un percorso ad arte: il mio giardino blu</t>
+          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr"/>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>www.fmav.org</t>
+        </is>
+      </c>
       <c r="V45" t="b">
         <v>0</v>
       </c>
@@ -5199,7 +5189,7 @@
       </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
@@ -5221,7 +5211,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5231,102 +5221,96 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Commedia brillante</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Teatro Cittadella</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr"/>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V46" t="b">
         <v>0</v>
       </c>
-      <c r="W46" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA46" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5336,79 +5320,67 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
+          <t>2022-03-31T08:53:45+00:00</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+        </is>
+      </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-03-31T08:55:39+00:00</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-05-30T11:00:13+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>FMAV - Museo della Figurina</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
-        </is>
-      </c>
+      <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr">
-        <is>
-          <t>www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U47" t="inlineStr"/>
       <c r="V47" t="b">
         <v>0</v>
       </c>
@@ -5417,7 +5389,7 @@
       </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
@@ -5439,7 +5411,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5449,79 +5421,71 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr"/>
+          <t>2022-03-19T09:15:00+00:00</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Spettacolo teatrale</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-03-19T09:19:36+00:00</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
         </is>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-05-30T11:06:40+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>FMAV - Museo della Figurina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
         </is>
       </c>
       <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U48" t="inlineStr"/>
       <c r="V48" t="b">
         <v>0</v>
       </c>
@@ -5530,7 +5494,7 @@
       </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
@@ -5552,7 +5516,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5562,50 +5526,58 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
+          <t>2022-02-25T14:15:33+00:00</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr"/>
+          <t>2022-02-28T15:13:23+00:00</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
@@ -5614,44 +5586,42 @@
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
-      <c r="U49" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U49" t="inlineStr"/>
       <c r="V49" t="b">
         <v>0</v>
       </c>
-      <c r="W49" t="inlineStr"/>
+      <c r="W49" t="n">
+        <v>41123</v>
+      </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5661,67 +5631,83 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
+          <t>2022-05-06T10:18:45+00:00</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr"/>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
-      <c r="U50" t="inlineStr"/>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>https://www.anticoinpiazzagrande.com/</t>
+        </is>
+      </c>
       <c r="V50" t="b">
         <v>0</v>
       </c>
@@ -5730,7 +5716,7 @@
       </c>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
@@ -5752,7 +5738,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5762,102 +5748,96 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
         </is>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>Teatro Cittadella</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:24:06+00:00</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
-      <c r="U51" t="inlineStr"/>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V51" t="b">
         <v>0</v>
       </c>
-      <c r="W51" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA51" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5867,58 +5847,50 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:10+00:00</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
@@ -5927,35 +5899,37 @@
       <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
-      <c r="U52" t="inlineStr"/>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V52" t="b">
         <v>0</v>
       </c>
-      <c r="W52" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
@@ -5972,62 +5946,54 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
+          <t>2022-04-07T09:06:38+00:00</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
+          <t>traborghiecontrade@libero.it</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-04-07T09:10:43+00:00</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O53" t="inlineStr"/>
@@ -6035,18 +6001,18 @@
       <c r="Q53" t="inlineStr"/>
       <c r="R53" t="inlineStr">
         <is>
-          <t>340 6059686 oppure 338 2098995</t>
+          <t>333/9103351</t>
         </is>
       </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr">
         <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V53" t="b">
@@ -6057,7 +6023,7 @@
       </c>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
@@ -6110,23 +6076,23 @@
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M54" t="inlineStr"/>
@@ -6156,7 +6122,7 @@
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
@@ -6209,23 +6175,23 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
+          <t>2022-05-10T08:27:35+00:00</t>
         </is>
       </c>
       <c r="M55" t="inlineStr"/>
@@ -6255,7 +6221,7 @@
       <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr">
@@ -6277,7 +6243,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -6287,394 +6253,87 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-11-19T23:00:00+00:00</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-11-20T22:55:00+00:00</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
         </is>
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr"/>
       <c r="N56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="inlineStr"/>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R56" t="inlineStr"/>
       <c r="S56" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V56" t="b">
         <v>0</v>
       </c>
-      <c r="W56" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W56" t="inlineStr"/>
       <c r="X56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y56" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z56" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA56" t="inlineStr">
-        <is>
-          <t>POINT (10.92572 44.64582)</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Mercati</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Modena</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>2022-09-17T22:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>2022-09-18T21:55:00+00:00</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr"/>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>2022-05-10T08:26:55+00:00</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr"/>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
-        </is>
-      </c>
-      <c r="O57" t="inlineStr"/>
-      <c r="P57" t="inlineStr"/>
-      <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr"/>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>Mercato straordinario degli ambulanti</t>
-        </is>
-      </c>
-      <c r="T57" t="inlineStr"/>
-      <c r="U57" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
-      <c r="V57" t="b">
-        <v>0</v>
-      </c>
-      <c r="W57" t="inlineStr"/>
-      <c r="X57" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
-        </is>
-      </c>
-      <c r="Y57" t="inlineStr">
-        <is>
-          <t>44,65137034620577</t>
-        </is>
-      </c>
-      <c r="Z57" t="inlineStr">
-        <is>
-          <t>10,921029194828652</t>
-        </is>
-      </c>
-      <c r="AA57" t="inlineStr">
-        <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Mercati</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Modena</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>2022-10-15T22:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>2022-10-16T21:55:00+00:00</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr"/>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>2022-05-10T08:27:35+00:00</t>
-        </is>
-      </c>
-      <c r="M58" t="inlineStr"/>
-      <c r="N58" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
-        </is>
-      </c>
-      <c r="O58" t="inlineStr"/>
-      <c r="P58" t="inlineStr"/>
-      <c r="Q58" t="inlineStr"/>
-      <c r="R58" t="inlineStr"/>
-      <c r="S58" t="inlineStr">
-        <is>
-          <t>Mercato straordinario degli ambulanti</t>
-        </is>
-      </c>
-      <c r="T58" t="inlineStr"/>
-      <c r="U58" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
-      <c r="V58" t="b">
-        <v>0</v>
-      </c>
-      <c r="W58" t="inlineStr"/>
-      <c r="X58" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
-        </is>
-      </c>
-      <c r="Y58" t="inlineStr">
-        <is>
-          <t>44,65137034620577</t>
-        </is>
-      </c>
-      <c r="Z58" t="inlineStr">
-        <is>
-          <t>10,921029194828652</t>
-        </is>
-      </c>
-      <c r="AA58" t="inlineStr">
-        <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Mercati</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Modena</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr"/>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>2022-11-19T23:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>2022-11-20T22:55:00+00:00</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr"/>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>2022-05-10T08:28:15+00:00</t>
-        </is>
-      </c>
-      <c r="M59" t="inlineStr"/>
-      <c r="N59" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
-        </is>
-      </c>
-      <c r="O59" t="inlineStr"/>
-      <c r="P59" t="inlineStr"/>
-      <c r="Q59" t="inlineStr"/>
-      <c r="R59" t="inlineStr"/>
-      <c r="S59" t="inlineStr">
-        <is>
-          <t>Mercato straordinario degli ambulanti</t>
-        </is>
-      </c>
-      <c r="T59" t="inlineStr"/>
-      <c r="U59" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
-      <c r="V59" t="b">
-        <v>0</v>
-      </c>
-      <c r="W59" t="inlineStr"/>
-      <c r="X59" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
-        </is>
-      </c>
-      <c r="Y59" t="inlineStr">
-        <is>
-          <t>44,65137034620577</t>
-        </is>
-      </c>
-      <c r="Z59" t="inlineStr">
-        <is>
-          <t>10,921029194828652</t>
-        </is>
-      </c>
-      <c r="AA59" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Wed Jun  1 12:33:47 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA56"/>
+  <dimension ref="A1:AA58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2774,79 +2774,95 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Modena</t>
+          <t>Montale Rangone</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2021-08-25T12:27:55+00:00</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr"/>
+          <t>2021-04-26T15:03:43+00:00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2021-08-25T12:28:08+00:00</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr"/>
+          <t>2021-04-26T15:06:06+00:00</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>museo@parcomontale.it</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2022-06-02T12:00:00+00:00</t>
+          <t>2022-04-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2022-06-05T13:00:00+00:00</t>
+          <t>2022-06-19T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/95eee6fe-2dc5-49a1-8611-3f5329c0af16.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Immagine di una precedente edizione del mercato</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2022-05-21T08:42:42+00:00</t>
+          <t>2022-03-28T14:43:35+00:00</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
+          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
         </is>
       </c>
       <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
+        </is>
+      </c>
       <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+        </is>
+      </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>Mercato europeo</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr">
         <is>
-          <t>http://www.mercatieuropei.com</t>
+          <t>http://www.parcomontale.it/it</t>
         </is>
       </c>
       <c r="V23" t="b">
@@ -2854,135 +2870,113 @@
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>41121</t>
+          <t>41050</t>
         </is>
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>44,647524762696584</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>10,925428060260353</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>POINT (10.925428060260353 44.647524762696584)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
+          <t>Altri eventi,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Montale Rangone</t>
+          <t>Modena</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
+          <t>Zona tribune</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2021-04-26T15:03:43+00:00</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:50:51+00:00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2021-04-26T15:06:06+00:00</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>museo@parcomontale.it</t>
-        </is>
-      </c>
+          <t>2022-05-11T07:51:19+00:00</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2022-04-03T14:00:00+00:00</t>
+          <t>2022-06-03T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2022-06-19T15:00:00+00:00</t>
+          <t>2022-06-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Immagine presa dal sito della Run 5.30 Modena</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2022-03-28T14:43:35+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
+          <t xml:space="preserve"> ore 5.30</t>
         </is>
       </c>
       <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
-        </is>
-      </c>
+      <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
-        </is>
-      </c>
+      <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Run 5.30</t>
         </is>
       </c>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>http://www.parcomontale.it/it</t>
-        </is>
-      </c>
+      <c r="U24" t="inlineStr"/>
       <c r="V24" t="b">
         <v>0</v>
       </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>41050</t>
-        </is>
+      <c r="W24" t="n">
+        <v>41123</v>
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
@@ -3004,7 +2998,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Altri eventi,Manifestazioni sportive</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3014,54 +3008,58 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Zona tribune</t>
+          <t>centro storico</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2022-05-11T07:50:51+00:00</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
+          <t>2022-04-29T10:05:46+00:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2022-06-03T07:00:00+00:00</t>
+          <t>2022-05-01T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2022-06-03T08:00:00+00:00</t>
+          <t>2022-07-17T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della Run 5.30 Modena</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Piazza Torre</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 5.30</t>
+          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
@@ -3070,7 +3068,7 @@
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>Run 5.30</t>
+          <t>Torre Ghirlandina, aperture serali</t>
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
@@ -3083,7 +3081,7 @@
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
@@ -3105,7 +3103,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3115,58 +3113,54 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>centro storico</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2022-04-29T10:05:46+00:00</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
-        </is>
-      </c>
+          <t>2021-08-25T12:27:55+00:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2021-08-25T12:28:08+00:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2022-05-01T09:00:00+00:00</t>
+          <t>2022-06-03T12:00:00+00:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2022-07-17T10:00:00+00:00</t>
+          <t>2022-06-05T13:00:00+00:00</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/e4443673-2e50-47eb-bc7e-424d7cb9cc58.jpeg</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Immagine di una precedente edizione del mercato</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-06-01T10:17:30+00:00</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Piazza Torre</t>
+          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
+          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
@@ -3175,35 +3169,41 @@
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, aperture serali</t>
+          <t>Mercato europeo</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr"/>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>http://www.mercatieuropei.com</t>
+        </is>
+      </c>
       <c r="V26" t="b">
         <v>0</v>
       </c>
-      <c r="W26" t="n">
-        <v>41123</v>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,647524762696584</t>
         </is>
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,925428060260353</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.925428060260353 44.647524762696584)</t>
         </is>
       </c>
     </row>
@@ -5837,7 +5837,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5847,96 +5847,118 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-06-01T09:27:21+00:00</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr"/>
+          <t>2022-06-01T09:27:29+00:00</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>mundus@ater.emr.it</t>
+        </is>
+      </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-07-26T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-07-26T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Grupo Compay Segundo</t>
+        </is>
+      </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr"/>
+          <t>2022-06-01T09:27:29+00:00</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Giardini Ducali</t>
+        </is>
+      </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr"/>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>059 340221</t>
+        </is>
+      </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V52" t="b">
         <v>0</v>
       </c>
-      <c r="W52" t="inlineStr"/>
+      <c r="W52" t="n">
+        <v>41123</v>
+      </c>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5946,73 +5968,85 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr"/>
+          <t>2022-06-01T09:27:21+00:00</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
+        </is>
+      </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
+          <t>2022-06-01T09:27:29+00:00</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>traborghiecontrade@libero.it</t>
+          <t>mundus@ater.emr.it</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-08-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-08-03T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Mauro Ottolini</t>
+        </is>
+      </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
+          <t>2022-06-01T09:48:07+00:00</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+          <t>Giardini Ducali</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr"/>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q53" t="inlineStr"/>
       <c r="R53" t="inlineStr">
         <is>
-          <t>333/9103351</t>
+          <t>059 340221</t>
         </is>
       </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Nada màs fuerte</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V53" t="b">
@@ -6023,7 +6057,7 @@
       </c>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
@@ -6076,23 +6110,23 @@
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
+          <t>2022-05-10T08:26:10+00:00</t>
         </is>
       </c>
       <c r="M54" t="inlineStr"/>
@@ -6122,7 +6156,7 @@
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
@@ -6144,7 +6178,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -6154,89 +6188,99 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr"/>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S55" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V55" t="b">
         <v>0</v>
       </c>
-      <c r="W55" t="inlineStr"/>
+      <c r="W55" t="n">
+        <v>41123</v>
+      </c>
       <c r="X55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA55" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6274,23 +6318,23 @@
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M56" t="inlineStr"/>
@@ -6320,20 +6364,218 @@
       <c r="W56" t="inlineStr"/>
       <c r="X56" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z56" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA56" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2022-10-15T22:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>2022-10-16T21:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:27:35+00:00</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V57" t="b">
+        <v>0</v>
+      </c>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z57" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA57" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="inlineStr"/>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T58" t="inlineStr"/>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V58" t="b">
+        <v>0</v>
+      </c>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y56" t="inlineStr">
+      <c r="Y58" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z56" t="inlineStr">
+      <c r="Z58" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA56" t="inlineStr">
+      <c r="AA58" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Wed Jun  1 13:34:37 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA58"/>
+  <dimension ref="A1:AA59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3535,7 +3535,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Altri eventi,Mercati</t>
+          <t>Concerti,Spettacoli,Musica</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3545,78 +3545,80 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Ingresso da viale Berengario</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2020-12-29T15:02:32+00:00</t>
+          <t>2022-05-30T11:40:24+00:00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2020-12-29T15:05:00+00:00</t>
+          <t>2022-05-30T11:41:23+00:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-01-03T14:00:00+00:00</t>
+          <t>2022-06-06T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-12-26T14:59:00+00:00</t>
+          <t>2022-06-06T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-inaugurale-della-nuova-filarmonica-del-teatro-comunale/@@images/bd0aa52a-489c-4715-b957-8a4551ed5f95.jpeg</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Dmitry Masleev</t>
+        </is>
+      </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2021-12-28T10:39:07+00:00</t>
+          <t>2022-06-01T12:46:07+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr"/>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingressio con biglietto gratuito. I biglietti sono disponibili presso la biglietteria del Teatro o telefonando allo 059  2033010</t>
+        </is>
+      </c>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Mercato settimanale del lunedì</t>
+          <t>Concerto inaugurale della nuova Filarmonica del Teatro comunale</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.com/</t>
-        </is>
-      </c>
+      <c r="U30" t="inlineStr"/>
       <c r="V30" t="b">
         <v>0</v>
       </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W30" t="n">
+        <v>41123</v>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-inaugurale-della-nuova-filarmonica-del-teatro-comunale</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
@@ -3638,7 +3640,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi,Mercati</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3648,77 +3650,65 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>Ingresso da viale Berengario</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
+          <t>2020-12-29T15:02:32+00:00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2020-12-29T15:05:00+00:00</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-01-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-12-26T14:59:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2021-12-28T10:39:07+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
-        </is>
-      </c>
+      <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Mercato settimanale del lunedì</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr">
         <is>
-          <t>https://www.fmav.org</t>
+          <t>http://www.consorzioilmercato.com/</t>
         </is>
       </c>
       <c r="V31" t="b">
@@ -3731,7 +3721,7 @@
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
@@ -3753,7 +3743,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3763,76 +3753,90 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
+          <t>2021-09-09T10:12:02+00:00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-05-26T07:16:41+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
         </is>
       </c>
       <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr"/>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V32" t="b">
         <v>0</v>
       </c>
-      <c r="W32" t="n">
-        <v>41123</v>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
@@ -3854,7 +3858,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Visite guidate,Altri eventi,Spettacoli</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3862,65 +3866,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>via Selmi, 63</t>
+        </is>
+      </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2022-05-30T09:56:40+00:00</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:24:22+00:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-06-10T09:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-10T10:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-05-26T07:16:41+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Duomo di Modena</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 20.30</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gratuito</t>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
         </is>
       </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
@@ -3933,7 +3937,7 @@
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
@@ -3955,7 +3959,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Altri eventi</t>
+          <t>Visite guidate,Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3963,65 +3967,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>corso Canalgrande, 85</t>
-        </is>
-      </c>
+      <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
+          <t>2022-05-30T09:56:40+00:00</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
+          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-06-10T11:00:00+00:00</t>
+          <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-06-10T12:00:00+00:00</t>
+          <t>2022-06-10T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-30T11:42:41+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Duomo di Modena</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> dalle ore 20.30</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gratuito</t>
+        </is>
+      </c>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
+          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
@@ -4034,7 +4038,7 @@
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
@@ -4056,7 +4060,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Concerti</t>
+          <t>Concerti,Spettacoli,Altri eventi</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4066,112 +4070,98 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Strada Pomposiana 292</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2022-05-30T09:03:14+00:00</t>
+          <t>2022-05-30T11:40:24+00:00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:41:23+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-06-10T19:00:00+00:00</t>
+          <t>2022-06-10T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-06-10T21:00:00+00:00</t>
+          <t>2022-06-10T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:42:41+00:00</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Fattoria Centofiori</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ore 21.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
-        </is>
-      </c>
+      <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>Whatsapp 3293357131</t>
-        </is>
-      </c>
+      <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Marco Ferri Quartet</t>
+          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>www.fattoriacentofiori.it</t>
-        </is>
-      </c>
+      <c r="U35" t="inlineStr"/>
       <c r="V35" t="b">
         <v>0</v>
       </c>
-      <c r="W35" t="inlineStr">
-        <is>
-          <t>41123</t>
-        </is>
+      <c r="W35" t="n">
+        <v>41123</v>
       </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>44,63693000592147</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>10,81076003183179</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>POINT (10.81076003183179 44.63693000592147)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Concerti</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4181,98 +4171,112 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Strada Pomposiana 292</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr"/>
+          <t>2022-05-30T09:03:14+00:00</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-06-10T19:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-06-10T21:00:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-05-26T07:20:15+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Fattoria Centofiori</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> Ore 21.00</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
         </is>
       </c>
       <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr"/>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>Whatsapp 3293357131</t>
+        </is>
+      </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Marco Ferri Quartet</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>www.fattoriacentofiori.it</t>
+        </is>
+      </c>
       <c r="V36" t="b">
         <v>0</v>
       </c>
-      <c r="W36" t="n">
-        <v>41123</v>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>41123</t>
+        </is>
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,63693000592147</t>
         </is>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,81076003183179</t>
         </is>
       </c>
       <c r="AA36" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.81076003183179 44.63693000592147)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4282,59 +4286,63 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-05-26T07:20:15+00:00</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr"/>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
@@ -4347,7 +4355,7 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
@@ -4369,7 +4377,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4379,50 +4387,50 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr"/>
+          <t>2022-05-21T10:36:00+00:00</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti</t>
+        </is>
+      </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
@@ -4431,44 +4439,42 @@
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U38" t="inlineStr"/>
       <c r="V38" t="b">
         <v>0</v>
       </c>
-      <c r="W38" t="inlineStr"/>
+      <c r="W38" t="n">
+        <v>41123</v>
+      </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA38" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4478,54 +4484,50 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>via S.Pietro, 1</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:38+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Presentazione del libro</t>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-12T09:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-12T10:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>Chiostro di San Pietro</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.00</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
@@ -4534,42 +4536,44 @@
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Contro la guerra</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr"/>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V39" t="b">
         <v>0</v>
       </c>
-      <c r="W39" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W39" t="inlineStr"/>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA39" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4579,75 +4583,67 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>via S.Pietro, 1</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr"/>
+          <t>2022-05-30T10:02:38+00:00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-12T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>Chiostro di San Pietro</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> ore 15.00</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Contro la guerra</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U40" t="inlineStr"/>
       <c r="V40" t="b">
         <v>0</v>
       </c>
@@ -4656,7 +4652,7 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
@@ -4678,7 +4674,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4688,63 +4684,75 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
+          <t>2021-08-06T11:34:26+00:00</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr"/>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr"/>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+        </is>
+      </c>
       <c r="V41" t="b">
         <v>0</v>
       </c>
@@ -4753,7 +4761,7 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
@@ -4775,7 +4783,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Iniziative per bambini</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4785,67 +4793,59 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ingresso da corso Cavour, 2</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:00+00:00</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Laboratorio per bambini 6-10 anni</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-16T11:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-06-16T12:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 17.00</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
-        </is>
-      </c>
+      <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>Un percorso ad arte: il mio giardino blu</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
@@ -4858,7 +4858,7 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
@@ -4880,7 +4880,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4890,67 +4890,67 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>ingresso da corso Cavour, 2</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-05-30T11:14:00+00:00</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Commedia brillante</t>
+          <t>Laboratorio per bambini 6-10 anni</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-16T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-16T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> ore 17.00</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
         </is>
       </c>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Un percorso ad arte: il mio giardino blu</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -4985,7 +4985,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -4995,79 +4995,71 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
+          <t>2022-03-19T09:15:00+00:00</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Commedia brillante</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-03-19T09:19:36+00:00</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-05-30T11:00:13+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>FMAV - Museo della Figurina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
-      <c r="U44" t="inlineStr">
-        <is>
-          <t>www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U44" t="inlineStr"/>
       <c r="V44" t="b">
         <v>0</v>
       </c>
@@ -5076,7 +5068,7 @@
       </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
@@ -5098,7 +5090,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5139,13 +5131,13 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-05-30T11:06:40+00:00</t>
+          <t>2022-05-30T11:00:13+00:00</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
@@ -5155,13 +5147,13 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
         </is>
       </c>
       <c r="Q45" t="inlineStr"/>
@@ -5172,7 +5164,7 @@
       </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
+          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
@@ -5189,7 +5181,7 @@
       </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
@@ -5211,7 +5203,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5221,96 +5213,110 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-30T10:57:49+00:00</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
         </is>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr"/>
+          <t>2022-05-30T11:06:40+00:00</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>FMAV - Museo della Figurina</t>
+        </is>
+      </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr"/>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+        </is>
+      </c>
       <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr"/>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>www.fmav.org</t>
         </is>
       </c>
       <c r="V46" t="b">
         <v>0</v>
       </c>
-      <c r="W46" t="inlineStr"/>
+      <c r="W46" t="n">
+        <v>41123</v>
+      </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA46" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5320,54 +5326,50 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr"/>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
@@ -5376,42 +5378,44 @@
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr"/>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V47" t="b">
         <v>0</v>
       </c>
-      <c r="W47" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA47" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5421,67 +5425,63 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
@@ -5494,7 +5494,7 @@
       </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5526,67 +5526,67 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr"/>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
@@ -5599,7 +5599,7 @@
       </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
@@ -5621,7 +5621,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5631,83 +5631,71 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-02-25T14:15:33+00:00</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-02-28T15:13:23+00:00</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R50" t="inlineStr"/>
       <c r="S50" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
-      <c r="U50" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U50" t="inlineStr"/>
       <c r="V50" t="b">
         <v>0</v>
       </c>
@@ -5716,7 +5704,7 @@
       </c>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
@@ -5738,7 +5726,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5748,96 +5736,114 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr"/>
+          <t>2022-05-06T10:18:45+00:00</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+        </is>
+      </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
-      <c r="R51" t="inlineStr"/>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V51" t="b">
         <v>0</v>
       </c>
-      <c r="W51" t="inlineStr"/>
+      <c r="W51" t="n">
+        <v>41123</v>
+      </c>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA51" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Concerti,Musica,Spettacoli</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5847,111 +5853,89 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ingresso da Corso Cavour, 2</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:21+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>mundus@ater.emr.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-07-26T08:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-07-26T09:00:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>Grupo Compay Segundo</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>Giardini Ducali</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:24:06+00:00</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.30</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
-        </is>
-      </c>
+      <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>059 340221</t>
-        </is>
-      </c>
+      <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr">
         <is>
-          <t>https://www.ater.emr.it/it</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V52" t="b">
         <v>0</v>
       </c>
-      <c r="W52" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
@@ -5993,27 +5977,27 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-08-03T08:00:00+00:00</t>
+          <t>2022-07-26T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-08-03T09:00:00+00:00</t>
+          <t>2022-07-26T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Mauro Ottolini</t>
+          <t>Grupo Compay Segundo</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-06-01T09:48:07+00:00</t>
+          <t>2022-06-01T09:27:29+00:00</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
@@ -6040,7 +6024,7 @@
       </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>Nada màs fuerte</t>
+          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
@@ -6057,7 +6041,7 @@
       </c>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
@@ -6079,7 +6063,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -6089,96 +6073,118 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-06-01T09:27:21+00:00</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr"/>
+          <t>2022-06-01T09:27:29+00:00</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>mundus@ater.emr.it</t>
+        </is>
+      </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-08-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-08-03T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Mauro Ottolini</t>
+        </is>
+      </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr"/>
+          <t>2022-06-01T09:48:07+00:00</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>Giardini Ducali</t>
+        </is>
+      </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr"/>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>059 340221</t>
+        </is>
+      </c>
       <c r="S54" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Nada màs fuerte</t>
         </is>
       </c>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V54" t="b">
         <v>0</v>
       </c>
-      <c r="W54" t="inlineStr"/>
+      <c r="W54" t="n">
+        <v>41123</v>
+      </c>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA54" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -6188,106 +6194,96 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:10+00:00</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr"/>
       <c r="N55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R55" t="inlineStr"/>
       <c r="S55" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V55" t="b">
         <v>0</v>
       </c>
-      <c r="W55" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA55" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -6297,89 +6293,99 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="inlineStr"/>
-      <c r="R56" t="inlineStr"/>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S56" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V56" t="b">
         <v>0</v>
       </c>
-      <c r="W56" t="inlineStr"/>
+      <c r="W56" t="n">
+        <v>41123</v>
+      </c>
       <c r="X56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y56" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z56" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA56" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6417,23 +6423,23 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M57" t="inlineStr"/>
@@ -6463,7 +6469,7 @@
       <c r="W57" t="inlineStr"/>
       <c r="X57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y57" t="inlineStr">
@@ -6516,23 +6522,23 @@
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:27:35+00:00</t>
         </is>
       </c>
       <c r="M58" t="inlineStr"/>
@@ -6562,20 +6568,119 @@
       <c r="W58" t="inlineStr"/>
       <c r="X58" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z58" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA58" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
+      <c r="R59" t="inlineStr"/>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T59" t="inlineStr"/>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V59" t="b">
+        <v>0</v>
+      </c>
+      <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y58" t="inlineStr">
+      <c r="Y59" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z58" t="inlineStr">
+      <c r="Z59" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA58" t="inlineStr">
+      <c r="AA59" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Fri Jun  3 01:05:41 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA57"/>
+  <dimension ref="A1:AA55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2164,7 +2164,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Iniziative per bambini,Manifestazioni sportive</t>
+          <t>Altri eventi,Manifestazioni sportive</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2174,50 +2174,54 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Strada Pomposiana n. 255/A - Loc. Marzaglia</t>
+          <t>Zona tribune</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2022-05-11T07:00:46+00:00</t>
+          <t>2022-05-11T07:50:51+00:00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2022-06-02T06:00:00+00:00</t>
+          <t>2022-06-03T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2022-06-02T07:00:00+00:00</t>
+          <t>2022-06-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/go-kart-go/@@images/ae9c72c5-09fb-4387-a0c6-e72a157b01d6.jpeg</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della Run 5.30 Modena</t>
+        </is>
+      </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2022-05-11T07:01:08+00:00</t>
+          <t>2022-05-11T07:51:19+00:00</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Autodromo di Modena</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13 e dalle 14 alle 18</t>
+          <t xml:space="preserve"> ore 5.30</t>
         </is>
       </c>
       <c r="O17" t="inlineStr"/>
@@ -2226,7 +2230,7 @@
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Go Kart, go!</t>
+          <t>Run 5.30</t>
         </is>
       </c>
       <c r="T17" t="inlineStr"/>
@@ -2239,7 +2243,7 @@
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/go-kart-go</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
@@ -2261,7 +2265,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Altri eventi,Musica</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2271,54 +2275,58 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>centro storico</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:04+00:00</t>
+          <t>2022-04-29T10:05:46+00:00</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
+          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2022-05-12T09:00:00+00:00</t>
+          <t>2022-05-01T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2022-06-30T10:00:00+00:00</t>
+          <t>2022-07-17T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Piazzetta Pomposa</t>
+          <t>Piazza Torre</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
+          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
         </is>
       </c>
       <c r="O18" t="inlineStr"/>
@@ -2327,7 +2335,7 @@
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr">
         <is>
-          <t>Serate in Pomposa - 1° edizione</t>
+          <t>Torre Ghirlandina, aperture serali</t>
         </is>
       </c>
       <c r="T18" t="inlineStr"/>
@@ -2340,7 +2348,7 @@
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
@@ -2362,7 +2370,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2370,88 +2378,106 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti</t>
+        </is>
+      </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2022-05-26T09:12:46+00:00</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Giovedì 2 giugno, celebrazioni con alzabandiera e sfilata della banda cittadina. Iniziative in programma già dal 30 maggio</t>
-        </is>
-      </c>
+          <t>2021-08-25T12:27:55+00:00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2022-05-30T09:29:45+00:00</t>
+          <t>2021-08-25T12:28:08+00:00</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2022-05-30T09:00:00+00:00</t>
+          <t>2022-06-03T12:00:00+00:00</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2022-06-02T10:00:00+00:00</t>
+          <t>2022-06-05T13:00:00+00:00</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/festa-della-repubblica/@@images/0031a2b2-623b-4b21-8316-cfd065155db6.jpeg</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/e4443673-2e50-47eb-bc7e-424d7cb9cc58.jpeg</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Immagine di una precedente edizione del mercato</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2022-05-30T09:29:45+00:00</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
+          <t>2022-06-01T10:17:30+00:00</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
+        </is>
+      </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr">
         <is>
-          <t>Festa della Repubblica</t>
+          <t>Mercato europeo</t>
         </is>
       </c>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>http://www.mercatieuropei.com</t>
+        </is>
+      </c>
       <c r="V19" t="b">
         <v>0</v>
       </c>
-      <c r="W19" t="n">
-        <v>41123</v>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/festa-della-repubblica</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,647524762696584</t>
         </is>
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,925428060260353</t>
         </is>
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.925428060260353 44.647524762696584)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Concerti,Musica</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2461,207 +2487,195 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>via degli Adelardi, 4</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2022-05-30T09:17:47+00:00</t>
+          <t>2021-04-28T06:30:25+00:00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>In occasione della Festa della Repubblica</t>
+          <t>Proiezione del film di Marco Pollini</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2022-05-30T09:20:03+00:00</t>
+          <t>2021-04-28T06:30:52+00:00</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2022-06-02T09:00:00+00:00</t>
+          <t>2022-06-04T06:00:00+00:00</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2022-06-02T10:00:00+00:00</t>
+          <t>2022-06-04T06:44:31+00:00</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-della-banda-cittadina-a-ferri/@@images/eaeaa0eb-f871-4bc3-885d-dd19e1c86208.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-grande-guerra-del-salento/@@images/b18d66e7-4b46-4875-9d8e-b70050efe202.jpeg</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Palazzo Ducale sede dell'Accademia Militare</t>
+          <t>Immagine della locandina del film</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2022-05-30T09:32:43+00:00</t>
+          <t>2022-05-24T07:43:55+00:00</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Cortile d'onore del Palazzo Ducale - Accedemia Miliatre</t>
+          <t>Sala Truffaut</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> ore 21.15</t>
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ingresso libero</t>
-        </is>
-      </c>
+      <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>059 236288</t>
+        </is>
+      </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>Concerto della Banda cittadina A.Ferri</t>
+          <t>La grande guerra del Salento</t>
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
+        </is>
+      </c>
       <c r="V20" t="b">
         <v>0</v>
       </c>
-      <c r="W20" t="n">
-        <v>41123</v>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-della-banda-cittadina-a-ferri</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-grande-guerra-del-salento</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,6456499931615</t>
         </is>
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921599972490952</t>
         </is>
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921599972490952 44.6456499931615)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Montale Rangone</t>
+          <t>Modena</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
+          <t>centro storico</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2021-04-26T15:03:43+00:00</t>
+          <t>2022-05-30T09:44:00+00:00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+          <t xml:space="preserve">Evneto dedicato alle famiglie, che fa divertire grandi e piccini </t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2021-04-26T15:06:06+00:00</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>museo@parcomontale.it</t>
-        </is>
-      </c>
+          <t>2022-05-30T09:44:15+00:00</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2022-04-03T14:00:00+00:00</t>
+          <t>2022-06-04T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2022-06-19T15:00:00+00:00</t>
+          <t>2022-06-05T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/modenagioca/@@images/b0abc4c6-5a49-4d8e-aa9f-0fd608824e22.jpeg</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>immagine dal sito modenagioca.it</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2022-03-28T14:43:35+00:00</t>
+          <t>2022-05-30T10:12:24+00:00</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
+          <t xml:space="preserve"> dalle ore 9 alle 20</t>
         </is>
       </c>
       <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
-        </is>
-      </c>
+      <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
-        </is>
-      </c>
+      <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>ModenaGioca</t>
         </is>
       </c>
       <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>http://www.parcomontale.it/it</t>
-        </is>
-      </c>
+      <c r="U21" t="inlineStr"/>
       <c r="V21" t="b">
         <v>0</v>
       </c>
-      <c r="W21" t="inlineStr">
-        <is>
-          <t>41050</t>
-        </is>
+      <c r="W21" t="n">
+        <v>41123</v>
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/modenagioca</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
@@ -2683,7 +2697,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Altri eventi,Manifestazioni sportive</t>
+          <t>Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2693,63 +2707,67 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Zona tribune</t>
+          <t>ingresso da Strada S.Faustino, 182</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2022-05-11T07:50:51+00:00</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
+          <t>2022-05-26T14:09:48+00:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Spettacolo di danza</t>
+        </is>
+      </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-05-26T14:09:58+00:00</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2022-06-03T07:00:00+00:00</t>
+          <t>2022-06-04T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2022-06-03T08:00:00+00:00</t>
+          <t>2022-06-04T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/run-5.30/@@images/24b6a680-9979-4ba1-8fe1-9af5096da63e.jpeg</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>Immagine presa dal sito della Run 5.30 Modena</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-giro-del-mondo-in-90-minuti/@@images/c6bc9831-404e-402b-9e60-623bc0a2ba80.jpeg</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2022-05-11T07:51:19+00:00</t>
+          <t>2022-05-27T06:18:12+00:00</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Parco Ferrari</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 5.30</t>
+          <t xml:space="preserve"> ore 20.00</t>
         </is>
       </c>
       <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ingresso libero</t>
+        </is>
+      </c>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr">
         <is>
-          <t>Run 5.30</t>
+          <t>Il giro del mondo in 90 minuti</t>
         </is>
       </c>
       <c r="T22" t="inlineStr"/>
@@ -2762,7 +2780,7 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/run-5.30</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-giro-del-mondo-in-90-minuti</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
@@ -2784,90 +2802,108 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Modena</t>
+          <t>Montale Rangone</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>centro storico</t>
+          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2022-04-29T10:05:46+00:00</t>
+          <t>2021-04-26T15:03:43+00:00</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
+          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr"/>
+          <t>2021-04-26T15:06:06+00:00</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>museo@parcomontale.it</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2022-05-01T09:00:00+00:00</t>
+          <t>2022-04-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2022-07-17T10:00:00+00:00</t>
+          <t>2022-06-19T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-03-28T14:43:35+00:00</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Piazza Torre</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
+          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
         </is>
       </c>
       <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
+        </is>
+      </c>
       <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+        </is>
+      </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, aperture serali</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>http://www.parcomontale.it/it</t>
+        </is>
+      </c>
       <c r="V23" t="b">
         <v>0</v>
       </c>
-      <c r="W23" t="n">
-        <v>41123</v>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>41050</t>
+        </is>
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
@@ -2889,7 +2925,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2897,106 +2933,88 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Piazza Matteotti</t>
-        </is>
-      </c>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2021-08-25T12:27:55+00:00</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
+          <t>2022-05-26T09:12:46+00:00</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Giovedì 2 giugno, celebrazioni con alzabandiera e sfilata della banda cittadina. Iniziative in programma già dal 30 maggio</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2021-08-25T12:28:08+00:00</t>
+          <t>2022-05-30T09:29:45+00:00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2022-06-03T12:00:00+00:00</t>
+          <t>2022-05-30T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2022-06-05T13:00:00+00:00</t>
+          <t>2022-06-02T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-europeo/@@images/e4443673-2e50-47eb-bc7e-424d7cb9cc58.jpeg</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>Immagine di una precedente edizione del mercato</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/festa-della-repubblica/@@images/0031a2b2-623b-4b21-8316-cfd065155db6.jpeg</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2022-06-01T10:17:30+00:00</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>Piazza Matteotti, Via Emilia Centro, Largo Porta Bologna</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Dalle 9.00 alle 23.00</t>
-        </is>
-      </c>
+          <t>2022-05-30T09:29:45+00:00</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr">
         <is>
-          <t>Mercato europeo</t>
+          <t>Festa della Repubblica</t>
         </is>
       </c>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>http://www.mercatieuropei.com</t>
-        </is>
-      </c>
+      <c r="U24" t="inlineStr"/>
       <c r="V24" t="b">
         <v>0</v>
       </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W24" t="n">
+        <v>41123</v>
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-europeo</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/festa-della-repubblica</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
         <is>
-          <t>44,647524762696584</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>10,925428060260353</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>POINT (10.925428060260353 44.647524762696584)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Concerti,Spettacoli,Musica</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3006,112 +3024,102 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>via degli Adelardi, 4</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:25+00:00</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Proiezione del film di Marco Pollini</t>
-        </is>
-      </c>
+          <t>2022-05-30T11:40:24+00:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2021-04-28T06:30:52+00:00</t>
+          <t>2022-05-30T11:41:23+00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2022-06-04T06:00:00+00:00</t>
+          <t>2022-06-06T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2022-06-04T06:44:31+00:00</t>
+          <t>2022-06-06T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-grande-guerra-del-salento/@@images/b18d66e7-4b46-4875-9d8e-b70050efe202.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-inaugurale-della-nuova-filarmonica-del-teatro-comunale/@@images/bd0aa52a-489c-4715-b957-8a4551ed5f95.jpeg</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Immagine della locandina del film</t>
+          <t>Dmitry Masleev</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2022-05-24T07:43:55+00:00</t>
+          <t>2022-06-01T12:46:07+00:00</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Sala Truffaut</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.15</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingressio con biglietto gratuito. I biglietti sono disponibili presso la biglietteria del Teatro o telefonando allo 059  2033010</t>
+        </is>
+      </c>
       <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>059 236288</t>
-        </is>
-      </c>
+      <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>La grande guerra del Salento</t>
+          <t>Concerto inaugurale della nuova Filarmonica del Teatro comunale</t>
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>https://www.circuitocinema.mo.it/sala-truffaut/</t>
-        </is>
-      </c>
+      <c r="U25" t="inlineStr"/>
       <c r="V25" t="b">
         <v>0</v>
       </c>
-      <c r="W25" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W25" t="n">
+        <v>41123</v>
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-grande-guerra-del-salento</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-inaugurale-della-nuova-filarmonica-del-teatro-comunale</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>44,6456499931615</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>10,921599972490952</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>POINT (10.921599972490952 44.6456499931615)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Altri eventi,Mercati</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3121,58 +3129,50 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>centro storico</t>
+          <t>Ingresso da viale Berengario</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2022-05-30T09:44:00+00:00</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Evneto dedicato alle famiglie, che fa divertire grandi e piccini </t>
-        </is>
-      </c>
+          <t>2020-12-29T15:02:32+00:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2022-05-30T09:44:15+00:00</t>
+          <t>2020-12-29T15:05:00+00:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2022-06-04T09:00:00+00:00</t>
+          <t>2022-01-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2022-06-05T10:00:00+00:00</t>
+          <t>2022-12-26T14:59:00+00:00</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/modenagioca/@@images/b0abc4c6-5a49-4d8e-aa9f-0fd608824e22.jpeg</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>immagine dal sito modenagioca.it</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2022-05-30T10:12:24+00:00</t>
+          <t>2021-12-28T10:39:07+00:00</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 20</t>
+          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
@@ -3181,20 +3181,26 @@
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr">
         <is>
-          <t>ModenaGioca</t>
+          <t>Mercato settimanale del lunedì</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr"/>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.com/</t>
+        </is>
+      </c>
       <c r="V26" t="b">
         <v>0</v>
       </c>
-      <c r="W26" t="n">
-        <v>41123</v>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/modenagioca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
@@ -3216,7 +3222,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Altri eventi,Spettacoli</t>
+          <t>Altri eventi,Musica</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3226,67 +3232,63 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ingresso da Strada S.Faustino, 182</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2022-05-26T14:09:48+00:00</t>
+          <t>2022-05-20T10:02:04+00:00</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Spettacolo di danza</t>
+          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2022-05-26T14:09:58+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2022-06-04T14:00:00+00:00</t>
+          <t>2022-05-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2022-06-04T15:00:00+00:00</t>
+          <t>2022-06-30T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-giro-del-mondo-in-90-minuti/@@images/c6bc9831-404e-402b-9e60-623bc0a2ba80.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-05-27T06:18:12+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Parco Ferrari</t>
+          <t>Piazzetta Pomposa</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 20.00</t>
+          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ingresso libero</t>
-        </is>
-      </c>
+      <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Il giro del mondo in 90 minuti</t>
+          <t>Serate in Pomposa - 1° edizione</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
@@ -3299,7 +3301,7 @@
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-giro-del-mondo-in-90-minuti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3321,7 +3323,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Musica</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3331,80 +3333,90 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 85</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
+          <t>2021-09-09T10:12:02+00:00</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-06-06T11:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-06-06T12:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-inaugurale-della-nuova-filarmonica-del-teatro-comunale/@@images/bd0aa52a-489c-4715-b957-8a4551ed5f95.jpeg</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>Dmitry Masleev</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-06-01T12:46:07+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingressio con biglietto gratuito. I biglietti sono disponibili presso la biglietteria del Teatro o telefonando allo 059  2033010</t>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
         </is>
       </c>
       <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr"/>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Concerto inaugurale della nuova Filarmonica del Teatro comunale</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr"/>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V28" t="b">
         <v>0</v>
       </c>
-      <c r="W28" t="n">
-        <v>41123</v>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-inaugurale-della-nuova-filarmonica-del-teatro-comunale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3426,7 +3438,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Altri eventi,Mercati</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3436,78 +3448,76 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ingresso da viale Berengario</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2020-12-29T15:02:32+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2020-12-29T15:05:00+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-01-03T14:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-12-26T14:59:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2021-12-28T10:39:07+00:00</t>
+          <t>2022-05-26T07:16:41+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Mercato settimanale del lunedì</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.com/</t>
-        </is>
-      </c>
+      <c r="U29" t="inlineStr"/>
       <c r="V29" t="b">
         <v>0</v>
       </c>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W29" t="n">
+        <v>41123</v>
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
@@ -3529,7 +3539,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Visite guidate,Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3537,92 +3547,78 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
-        </is>
-      </c>
+      <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr"/>
+          <t>2022-05-30T09:56:40+00:00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
+        </is>
+      </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-05-30T09:57:07+00:00</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-10T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
         </is>
       </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Duomo di Modena</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> dalle ore 20.30</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
+          <t xml:space="preserve"> Gratuito</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>https://www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U30" t="inlineStr"/>
       <c r="V30" t="b">
         <v>0</v>
       </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W30" t="n">
+        <v>41123</v>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
@@ -3644,7 +3640,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Concerti,Spettacoli,Altri eventi</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3654,63 +3650,63 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
+          <t>2022-05-30T11:40:24+00:00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-30T11:41:23+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-10T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-06-10T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-26T07:16:41+00:00</t>
+          <t>2022-05-30T11:42:41+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
-        </is>
-      </c>
+      <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
@@ -3723,7 +3719,7 @@
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
@@ -3745,7 +3741,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Visite guidate,Altri eventi,Spettacoli</t>
+          <t>Concerti</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3753,100 +3749,114 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Strada Pomposiana 292</t>
+        </is>
+      </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:56:40+00:00</t>
+          <t>2022-05-30T09:03:14+00:00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
+          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-06-10T09:00:00+00:00</t>
+          <t>2022-06-10T19:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-06-10T10:00:00+00:00</t>
+          <t>2022-06-10T21:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Duomo di Modena</t>
+          <t>Fattoria Centofiori</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 20.30</t>
+          <t xml:space="preserve"> Ore 21.00</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gratuito</t>
+          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
         </is>
       </c>
       <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>Whatsapp 3293357131</t>
+        </is>
+      </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
+          <t>Marco Ferri Quartet</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr"/>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>www.fattoriacentofiori.it</t>
+        </is>
+      </c>
       <c r="V32" t="b">
         <v>0</v>
       </c>
-      <c r="W32" t="n">
-        <v>41123</v>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>41123</t>
+        </is>
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,63693000592147</t>
         </is>
       </c>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,81076003183179</t>
         </is>
       </c>
       <c r="AA32" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.81076003183179 44.63693000592147)</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Altri eventi</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3856,63 +3866,63 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 85</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:24:22+00:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-06-10T11:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-10T12:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-05-30T11:42:41+00:00</t>
+          <t>2022-05-26T07:20:15+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
@@ -3925,7 +3935,7 @@
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
@@ -3947,7 +3957,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Concerti</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3957,112 +3967,94 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Strada Pomposiana 292</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2022-05-30T09:03:14+00:00</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-06-10T19:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-06-10T21:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-21T10:36:00+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Fattoria Centofiori</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ore 21.00</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
-        </is>
-      </c>
+      <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>Whatsapp 3293357131</t>
-        </is>
-      </c>
+      <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Marco Ferri Quartet</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>www.fattoriacentofiori.it</t>
-        </is>
-      </c>
+      <c r="U34" t="inlineStr"/>
       <c r="V34" t="b">
         <v>0</v>
       </c>
-      <c r="W34" t="inlineStr">
-        <is>
-          <t>41123</t>
-        </is>
+      <c r="W34" t="n">
+        <v>41123</v>
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
         <is>
-          <t>44,63693000592147</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>10,81076003183179</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA34" t="inlineStr">
         <is>
-          <t>POINT (10.81076003183179 44.63693000592147)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4072,98 +4064,96 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-05-26T07:20:15+00:00</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>Complesso San Paolo</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
-        </is>
-      </c>
+      <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr"/>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V35" t="b">
         <v>0</v>
       </c>
-      <c r="W35" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W35" t="inlineStr"/>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4173,50 +4163,54 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via S.Pietro, 1</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr"/>
+          <t>2022-05-30T10:02:38+00:00</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-06-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-12T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Chiostro di San Pietro</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> ore 15.00</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
@@ -4225,7 +4219,7 @@
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Contro la guerra</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
@@ -4238,7 +4232,7 @@
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
@@ -4260,7 +4254,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4270,96 +4264,106 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2021-08-06T11:34:26+00:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr"/>
+          <t>2022-02-08T10:09:23+00:00</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>Polisportiva Madonnina</t>
+        </is>
+      </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr"/>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
         </is>
       </c>
       <c r="V37" t="b">
         <v>0</v>
       </c>
-      <c r="W37" t="inlineStr"/>
+      <c r="W37" t="n">
+        <v>41123</v>
+      </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA37" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4369,54 +4373,50 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>via S.Pietro, 1</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:38+00:00</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>Presentazione del libro</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-12T09:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-12T10:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>Chiostro di San Pietro</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.00</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
@@ -4425,7 +4425,7 @@
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Contro la guerra</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
@@ -4438,7 +4438,7 @@
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
@@ -4460,7 +4460,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4470,75 +4470,71 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>ingresso da corso Cavour, 2</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr"/>
+          <t>2022-05-30T11:14:00+00:00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Laboratorio per bambini 6-10 anni</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-16T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-16T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> ore 17.00</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
+        </is>
+      </c>
       <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Un percorso ad arte: il mio giardino blu</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U39" t="inlineStr"/>
       <c r="V39" t="b">
         <v>0</v>
       </c>
@@ -4547,7 +4543,7 @@
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
@@ -4569,7 +4565,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4579,59 +4575,67 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr"/>
+          <t>2022-03-19T09:15:00+00:00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Commedia brillante</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
-      <c r="P40" t="inlineStr"/>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
@@ -4644,7 +4648,7 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
@@ -4666,7 +4670,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Iniziative per bambini</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4676,71 +4680,79 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ingresso da corso Cavour, 2</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:00+00:00</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Laboratorio per bambini 6-10 anni</t>
-        </is>
-      </c>
+          <t>2022-05-30T10:57:49+00:00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-16T11:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-16T12:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-30T11:00:13+00:00</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>FMAV - Museo della Figurina</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 17.00</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
+          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
         </is>
       </c>
       <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr"/>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>Un percorso ad arte: il mio giardino blu</t>
+          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr"/>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>www.fmav.org</t>
+        </is>
+      </c>
       <c r="V41" t="b">
         <v>0</v>
       </c>
@@ -4749,7 +4761,7 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
@@ -4771,7 +4783,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4781,71 +4793,79 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Commedia brillante</t>
-        </is>
-      </c>
+          <t>2022-05-30T10:57:49+00:00</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-05-30T11:06:40+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>FMAV - Museo della Figurina</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
         </is>
       </c>
       <c r="Q42" t="inlineStr"/>
-      <c r="R42" t="inlineStr"/>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
-      <c r="U42" t="inlineStr"/>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>www.fmav.org</t>
+        </is>
+      </c>
       <c r="V42" t="b">
         <v>0</v>
       </c>
@@ -4854,7 +4874,7 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
@@ -4876,7 +4896,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4886,110 +4906,96 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-05-30T11:00:13+00:00</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>FMAV - Museo della Figurina</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
-        </is>
-      </c>
+      <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
       <c r="U43" t="inlineStr">
         <is>
-          <t>www.fmav.org</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V43" t="b">
         <v>0</v>
       </c>
-      <c r="W43" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W43" t="inlineStr"/>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA43" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -4999,79 +5005,67 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
+          <t>2022-03-31T08:53:45+00:00</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-03-31T08:55:39+00:00</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-05-30T11:06:40+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>FMAV - Museo della Figurina</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
-        </is>
-      </c>
+      <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
-      <c r="U44" t="inlineStr">
-        <is>
-          <t>www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U44" t="inlineStr"/>
       <c r="V44" t="b">
         <v>0</v>
       </c>
@@ -5080,7 +5074,7 @@
       </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
@@ -5102,7 +5096,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5112,96 +5106,102 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr"/>
+          <t>2022-03-19T09:28:51+00:00</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>Teatro Cittadella</t>
+        </is>
+      </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
-      <c r="P45" t="inlineStr"/>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U45" t="inlineStr"/>
       <c r="V45" t="b">
         <v>0</v>
       </c>
-      <c r="W45" t="inlineStr"/>
+      <c r="W45" t="n">
+        <v>41123</v>
+      </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA45" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5211,54 +5211,58 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2022-02-25T14:15:33+00:00</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
+          <t>2022-02-28T15:13:23+00:00</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
@@ -5267,7 +5271,7 @@
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
@@ -5280,7 +5284,7 @@
       </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
@@ -5302,7 +5306,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5312,71 +5316,83 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-05-06T10:18:45+00:00</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr"/>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S47" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr"/>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>https://www.anticoinpiazzagrande.com/</t>
+        </is>
+      </c>
       <c r="V47" t="b">
         <v>0</v>
       </c>
@@ -5385,7 +5401,7 @@
       </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
@@ -5407,7 +5423,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5417,58 +5433,50 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:24:06+00:00</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr"/>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
@@ -5477,42 +5485,44 @@
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr"/>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V48" t="b">
         <v>0</v>
       </c>
-      <c r="W48" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA48" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5522,81 +5532,85 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-06-01T09:27:21+00:00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
+          <t>2022-06-01T09:27:29+00:00</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
+          <t>mundus@ater.emr.it</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-07-26T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-07-26T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+          <t>Grupo Compay Segundo</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-06-01T09:27:29+00:00</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Giardini Ducali</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr"/>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr">
         <is>
-          <t>340 6059686 oppure 338 2098995</t>
+          <t>059 340221</t>
         </is>
       </c>
       <c r="S49" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr">
         <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V49" t="b">
@@ -5607,7 +5621,7 @@
       </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
@@ -5629,7 +5643,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5639,96 +5653,118 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-06-01T09:27:21+00:00</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr"/>
+          <t>2022-06-01T09:27:29+00:00</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>mundus@ater.emr.it</t>
+        </is>
+      </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-08-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-08-03T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Mauro Ottolini</t>
+        </is>
+      </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr"/>
+          <t>2022-06-01T09:48:07+00:00</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>Giardini Ducali</t>
+        </is>
+      </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr"/>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr"/>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>059 340221</t>
+        </is>
+      </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Nada màs fuerte</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V50" t="b">
         <v>0</v>
       </c>
-      <c r="W50" t="inlineStr"/>
+      <c r="W50" t="n">
+        <v>41123</v>
+      </c>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA50" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Concerti,Musica,Spettacoli</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5738,118 +5774,96 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ingresso da Corso Cavour, 2</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:21+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>mundus@ater.emr.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-07-26T08:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-07-26T09:00:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>Grupo Compay Segundo</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>Giardini Ducali</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:10+00:00</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.30</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
-        </is>
-      </c>
+      <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
-      <c r="R51" t="inlineStr">
-        <is>
-          <t>059 340221</t>
-        </is>
-      </c>
+      <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr">
         <is>
-          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr">
         <is>
-          <t>https://www.ater.emr.it/it</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V51" t="b">
         <v>0</v>
       </c>
-      <c r="W51" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA51" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Concerti,Musica,Spettacoli</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5859,85 +5873,73 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ingresso da Corso Cavour, 2</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:21+00:00</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
+          <t>2022-04-07T09:06:38+00:00</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>mundus@ater.emr.it</t>
+          <t>traborghiecontrade@libero.it</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-08-03T08:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-08-03T09:00:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>Mauro Ottolini</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-06-01T09:48:07+00:00</t>
+          <t>2022-04-07T09:10:43+00:00</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>Giardini Ducali</t>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.30</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
-        </is>
-      </c>
+      <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
       <c r="R52" t="inlineStr">
         <is>
-          <t>059 340221</t>
+          <t>333/9103351</t>
         </is>
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Nada màs fuerte</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr">
         <is>
-          <t>https://www.ater.emr.it/it</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V52" t="b">
@@ -5948,7 +5950,7 @@
       </c>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
@@ -6001,23 +6003,23 @@
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M53" t="inlineStr"/>
@@ -6047,7 +6049,7 @@
       <c r="W53" t="inlineStr"/>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
@@ -6069,7 +6071,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -6079,99 +6081,89 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:27:35+00:00</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O54" t="inlineStr"/>
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R54" t="inlineStr"/>
       <c r="S54" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V54" t="b">
         <v>0</v>
       </c>
-      <c r="W54" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA54" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
@@ -6209,23 +6201,23 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-11-19T23:00:00+00:00</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-11-20T22:55:00+00:00</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
         </is>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
+          <t>2022-05-10T08:28:15+00:00</t>
         </is>
       </c>
       <c r="M55" t="inlineStr"/>
@@ -6255,7 +6247,7 @@
       <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr">
@@ -6269,204 +6261,6 @@
         </is>
       </c>
       <c r="AA55" t="inlineStr">
-        <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Mercati</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Modena</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>2022-10-15T22:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>2022-10-16T21:55:00+00:00</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr"/>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>2022-05-10T08:27:35+00:00</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr"/>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
-        </is>
-      </c>
-      <c r="O56" t="inlineStr"/>
-      <c r="P56" t="inlineStr"/>
-      <c r="Q56" t="inlineStr"/>
-      <c r="R56" t="inlineStr"/>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>Mercato straordinario degli ambulanti</t>
-        </is>
-      </c>
-      <c r="T56" t="inlineStr"/>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
-      <c r="V56" t="b">
-        <v>0</v>
-      </c>
-      <c r="W56" t="inlineStr"/>
-      <c r="X56" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
-        </is>
-      </c>
-      <c r="Y56" t="inlineStr">
-        <is>
-          <t>44,65137034620577</t>
-        </is>
-      </c>
-      <c r="Z56" t="inlineStr">
-        <is>
-          <t>10,921029194828652</t>
-        </is>
-      </c>
-      <c r="AA56" t="inlineStr">
-        <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Mercati</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Modena</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>2022-11-19T23:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>2022-11-20T22:55:00+00:00</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr"/>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>2022-05-10T08:28:15+00:00</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr"/>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
-        </is>
-      </c>
-      <c r="O57" t="inlineStr"/>
-      <c r="P57" t="inlineStr"/>
-      <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr"/>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>Mercato straordinario degli ambulanti</t>
-        </is>
-      </c>
-      <c r="T57" t="inlineStr"/>
-      <c r="U57" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
-      <c r="V57" t="b">
-        <v>0</v>
-      </c>
-      <c r="W57" t="inlineStr"/>
-      <c r="X57" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
-        </is>
-      </c>
-      <c r="Y57" t="inlineStr">
-        <is>
-          <t>44,65137034620577</t>
-        </is>
-      </c>
-      <c r="Z57" t="inlineStr">
-        <is>
-          <t>10,921029194828652</t>
-        </is>
-      </c>
-      <c r="AA57" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Fri Jun  3 16:20:10 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA55"/>
+  <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3222,7 +3222,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Altri eventi,Musica</t>
+          <t>Altri eventi,Spettacoli,Musica</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3237,49 +3237,49 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:04+00:00</t>
+          <t>2022-06-03T15:42:40+00:00</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
+          <t>Rassegna di spettacoli in Piazza XX Settembre</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-06-03T15:43:48+00:00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2022-05-12T09:00:00+00:00</t>
+          <t>2022-06-07T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2022-06-30T10:00:00+00:00</t>
+          <t>2022-06-28T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/note-di-stelle/@@images/78120e75-8036-4a4c-b46e-10cc1ff7fe4c.jpeg</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-06-03T15:43:48+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Piazzetta Pomposa</t>
+          <t>Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
+          <t xml:space="preserve"> 7, 14, 21 e 28 giugno alle ore 21.00</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
@@ -3288,7 +3288,7 @@
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Serate in Pomposa - 1° edizione</t>
+          <t>Note di Stelle</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/note-di-stelle</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3323,7 +3323,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi,Musica</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3333,90 +3333,76 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr"/>
+          <t>2022-05-20T10:02:04+00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-05-20T10:02:34+00:00</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-05-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-30T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazzetta Pomposa</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
-        </is>
-      </c>
+      <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Serate in Pomposa - 1° edizione</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>https://www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U28" t="inlineStr"/>
       <c r="V28" t="b">
         <v>0</v>
       </c>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W28" t="n">
+        <v>41123</v>
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3438,7 +3424,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3448,76 +3434,90 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
+          <t>2021-09-09T10:12:02+00:00</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
         </is>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-05-26T07:16:41+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
         </is>
       </c>
       <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr"/>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V29" t="b">
         <v>0</v>
       </c>
-      <c r="W29" t="n">
-        <v>41123</v>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
@@ -3539,7 +3539,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Visite guidate,Altri eventi,Spettacoli</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3547,65 +3547,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>via Selmi, 63</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2022-05-30T09:56:40+00:00</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:24:22+00:00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-06-10T09:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-06-10T10:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-05-26T07:16:41+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Duomo di Modena</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 20.30</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gratuito</t>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
         </is>
       </c>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
@@ -3618,7 +3618,7 @@
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
@@ -3640,7 +3640,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Altri eventi</t>
+          <t>Visite guidate,Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3648,65 +3648,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>corso Canalgrande, 85</t>
-        </is>
-      </c>
+      <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
+          <t>2022-05-30T09:56:40+00:00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
+          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-06-10T11:00:00+00:00</t>
+          <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-06-10T12:00:00+00:00</t>
+          <t>2022-06-10T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-30T11:42:41+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Duomo di Modena</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> dalle ore 20.30</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gratuito</t>
+        </is>
+      </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
+          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
@@ -3741,7 +3741,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Concerti</t>
+          <t>Concerti,Spettacoli,Altri eventi</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3751,112 +3751,98 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Strada Pomposiana 292</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:03:14+00:00</t>
+          <t>2022-05-30T11:40:24+00:00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:41:23+00:00</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-06-10T19:00:00+00:00</t>
+          <t>2022-06-10T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-06-10T21:00:00+00:00</t>
+          <t>2022-06-10T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:42:41+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Fattoria Centofiori</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ore 21.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
-        </is>
-      </c>
+      <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>Whatsapp 3293357131</t>
-        </is>
-      </c>
+      <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Marco Ferri Quartet</t>
+          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr">
-        <is>
-          <t>www.fattoriacentofiori.it</t>
-        </is>
-      </c>
+      <c r="U32" t="inlineStr"/>
       <c r="V32" t="b">
         <v>0</v>
       </c>
-      <c r="W32" t="inlineStr">
-        <is>
-          <t>41123</t>
-        </is>
+      <c r="W32" t="n">
+        <v>41123</v>
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
         <is>
-          <t>44,63693000592147</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>10,81076003183179</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA32" t="inlineStr">
         <is>
-          <t>POINT (10.81076003183179 44.63693000592147)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Concerti</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3866,98 +3852,112 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Strada Pomposiana 292</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
+          <t>2022-05-30T09:03:14+00:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-06-10T19:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-06-10T21:00:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-05-26T07:20:15+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Fattoria Centofiori</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> Ore 21.00</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
         </is>
       </c>
       <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>Whatsapp 3293357131</t>
+        </is>
+      </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Marco Ferri Quartet</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr"/>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>www.fattoriacentofiori.it</t>
+        </is>
+      </c>
       <c r="V33" t="b">
         <v>0</v>
       </c>
-      <c r="W33" t="n">
-        <v>41123</v>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>41123</t>
+        </is>
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,63693000592147</t>
         </is>
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,81076003183179</t>
         </is>
       </c>
       <c r="AA33" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.81076003183179 44.63693000592147)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3967,59 +3967,63 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-05-26T07:20:15+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
@@ -4032,7 +4036,7 @@
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
@@ -4054,7 +4058,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4064,50 +4068,50 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr"/>
+          <t>2022-05-21T10:36:00+00:00</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti</t>
+        </is>
+      </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
@@ -4116,44 +4120,42 @@
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U35" t="inlineStr"/>
       <c r="V35" t="b">
         <v>0</v>
       </c>
-      <c r="W35" t="inlineStr"/>
+      <c r="W35" t="n">
+        <v>41123</v>
+      </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4163,54 +4165,50 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>via S.Pietro, 1</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:38+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Presentazione del libro</t>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-06-12T09:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-12T10:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>Chiostro di San Pietro</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.00</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
@@ -4219,42 +4217,44 @@
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Contro la guerra</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V36" t="b">
         <v>0</v>
       </c>
-      <c r="W36" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W36" t="inlineStr"/>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA36" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4264,75 +4264,67 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>via S.Pietro, 1</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr"/>
+          <t>2022-05-30T10:02:38+00:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-12T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>Chiostro di San Pietro</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> ore 15.00</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Contro la guerra</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U37" t="inlineStr"/>
       <c r="V37" t="b">
         <v>0</v>
       </c>
@@ -4341,7 +4333,7 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
@@ -4363,7 +4355,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4373,63 +4365,75 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
+          <t>2021-08-06T11:34:26+00:00</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr"/>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+        </is>
+      </c>
       <c r="V38" t="b">
         <v>0</v>
       </c>
@@ -4438,7 +4442,7 @@
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
@@ -4460,7 +4464,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Iniziative per bambini</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4470,67 +4474,59 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ingresso da corso Cavour, 2</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:00+00:00</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>Laboratorio per bambini 6-10 anni</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-16T11:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-16T12:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 17.00</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
-        </is>
-      </c>
+      <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Un percorso ad arte: il mio giardino blu</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
@@ -4543,7 +4539,7 @@
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
@@ -4565,7 +4561,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4575,67 +4571,67 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>ingresso da corso Cavour, 2</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-05-30T11:14:00+00:00</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Commedia brillante</t>
+          <t>Laboratorio per bambini 6-10 anni</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-16T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-16T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> ore 17.00</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
         </is>
       </c>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Un percorso ad arte: il mio giardino blu</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
@@ -4648,7 +4644,7 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
@@ -4670,7 +4666,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4680,79 +4676,71 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr"/>
+          <t>2022-03-19T09:15:00+00:00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Commedia brillante</t>
+        </is>
+      </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-03-19T09:19:36+00:00</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-05-30T11:00:13+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>FMAV - Museo della Figurina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr">
-        <is>
-          <t>www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U41" t="inlineStr"/>
       <c r="V41" t="b">
         <v>0</v>
       </c>
@@ -4761,7 +4749,7 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
@@ -4783,7 +4771,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4824,13 +4812,13 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-05-30T11:06:40+00:00</t>
+          <t>2022-05-30T11:00:13+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
@@ -4840,13 +4828,13 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
         </is>
       </c>
       <c r="Q42" t="inlineStr"/>
@@ -4857,7 +4845,7 @@
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
+          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
@@ -4874,7 +4862,7 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
@@ -4896,7 +4884,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4906,96 +4894,110 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-30T10:57:49+00:00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr"/>
+          <t>2022-05-30T11:06:40+00:00</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>FMAV - Museo della Figurina</t>
+        </is>
+      </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
-      <c r="P43" t="inlineStr"/>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+        </is>
+      </c>
       <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr"/>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
       <c r="U43" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>www.fmav.org</t>
         </is>
       </c>
       <c r="V43" t="b">
         <v>0</v>
       </c>
-      <c r="W43" t="inlineStr"/>
+      <c r="W43" t="n">
+        <v>41123</v>
+      </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA43" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5005,54 +5007,50 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
@@ -5061,42 +5059,44 @@
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
-      <c r="U44" t="inlineStr"/>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V44" t="b">
         <v>0</v>
       </c>
-      <c r="W44" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W44" t="inlineStr"/>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA44" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5106,67 +5106,63 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
-      <c r="P45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
@@ -5179,7 +5175,7 @@
       </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
@@ -5201,7 +5197,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5211,67 +5207,67 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr"/>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
@@ -5284,7 +5280,7 @@
       </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
@@ -5306,7 +5302,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5316,83 +5312,71 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-02-25T14:15:33+00:00</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-02-28T15:13:23+00:00</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U47" t="inlineStr"/>
       <c r="V47" t="b">
         <v>0</v>
       </c>
@@ -5401,7 +5385,7 @@
       </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
@@ -5423,7 +5407,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5433,96 +5417,114 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr"/>
+          <t>2022-05-06T10:18:45+00:00</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+        </is>
+      </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr"/>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S48" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
       <c r="U48" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V48" t="b">
         <v>0</v>
       </c>
-      <c r="W48" t="inlineStr"/>
+      <c r="W48" t="n">
+        <v>41123</v>
+      </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA48" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Concerti,Musica,Spettacoli</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5532,111 +5534,89 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ingresso da Corso Cavour, 2</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:21+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>mundus@ater.emr.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-07-26T08:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-07-26T09:00:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>Grupo Compay Segundo</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>Giardini Ducali</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:24:06+00:00</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.30</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
-        </is>
-      </c>
+      <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>059 340221</t>
-        </is>
-      </c>
+      <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr">
         <is>
-          <t>https://www.ater.emr.it/it</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V49" t="b">
         <v>0</v>
       </c>
-      <c r="W49" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
@@ -5678,27 +5658,27 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-08-03T08:00:00+00:00</t>
+          <t>2022-07-26T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-08-03T09:00:00+00:00</t>
+          <t>2022-07-26T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Mauro Ottolini</t>
+          <t>Grupo Compay Segundo</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-06-01T09:48:07+00:00</t>
+          <t>2022-06-01T09:27:29+00:00</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
@@ -5725,7 +5705,7 @@
       </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>Nada màs fuerte</t>
+          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
@@ -5742,7 +5722,7 @@
       </c>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
@@ -5764,7 +5744,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5774,96 +5754,118 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-06-01T09:27:21+00:00</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr"/>
+          <t>2022-06-01T09:27:29+00:00</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>mundus@ater.emr.it</t>
+        </is>
+      </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-08-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-08-03T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Mauro Ottolini</t>
+        </is>
+      </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr"/>
+          <t>2022-06-01T09:48:07+00:00</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>Giardini Ducali</t>
+        </is>
+      </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr"/>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q51" t="inlineStr"/>
-      <c r="R51" t="inlineStr"/>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>059 340221</t>
+        </is>
+      </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Nada màs fuerte</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V51" t="b">
         <v>0</v>
       </c>
-      <c r="W51" t="inlineStr"/>
+      <c r="W51" t="n">
+        <v>41123</v>
+      </c>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA51" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5873,106 +5875,96 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:10+00:00</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V52" t="b">
         <v>0</v>
       </c>
-      <c r="W52" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5982,89 +5974,99 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr"/>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V53" t="b">
         <v>0</v>
       </c>
-      <c r="W53" t="inlineStr"/>
+      <c r="W53" t="n">
+        <v>41123</v>
+      </c>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA53" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6102,23 +6104,23 @@
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M54" t="inlineStr"/>
@@ -6148,7 +6150,7 @@
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
@@ -6201,23 +6203,23 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:27:35+00:00</t>
         </is>
       </c>
       <c r="M55" t="inlineStr"/>
@@ -6247,20 +6249,119 @@
       <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y55" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z55" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA55" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V56" t="b">
+        <v>0</v>
+      </c>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y55" t="inlineStr">
+      <c r="Y56" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z55" t="inlineStr">
+      <c r="Z56" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA55" t="inlineStr">
+      <c r="AA56" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Sat Jun  4 08:16:41 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA54"/>
+  <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3024,7 +3024,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Altri eventi,Spettacoli,Musica</t>
+          <t>Altri eventi,Spettacoli,Musica,Libri</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3044,7 +3044,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Rassegna di spettacoli in Piazza XX Settembre</t>
+          <t>Rassegna di eventi culturali in Piazza XX Settembre</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3071,7 +3071,7 @@
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2022-06-03T15:43:48+00:00</t>
+          <t>2022-06-04T06:35:10+00:00</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 7, 14, 21 e 28 giugno alle ore 21.00</t>
+          <t xml:space="preserve"> 7, 14, 21 e 28 giugno alle ore 19 presentazione di libri  alle ore 21 spettacoli</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
@@ -3125,7 +3125,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Altri eventi,Musica</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3135,67 +3135,79 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Corso Vittorio Emanuele, 59</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:04+00:00</t>
+          <t>2022-06-04T07:59:44+00:00</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
+          <t>Presentazione del libro</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr"/>
+          <t>2022-06-04T07:59:52+00:00</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>​info@accademiasla-mo.it</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2022-05-12T09:00:00+00:00</t>
+          <t>2022-06-08T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2022-06-30T10:00:00+00:00</t>
+          <t>2022-06-08T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione/@@images/1a4df534-f8d8-4ac6-87d4-3d9176cd882c.jpeg</t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-06-04T07:59:52+00:00</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Piazzetta Pomposa</t>
+          <t>Accademia Nazionale di Scienze Lettere e Arti di Modena</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
+          <t xml:space="preserve"> ore 15.30</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr"/>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>059 225566</t>
+        </is>
+      </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>Serate in Pomposa - 1° edizione</t>
+          <t>"Delitti in prima pagina. La giustizia nella società dell’informazione"</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr"/>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>www.accademiasla-mo.it</t>
+        </is>
+      </c>
       <c r="V26" t="b">
         <v>0</v>
       </c>
@@ -3204,7 +3216,7 @@
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
@@ -3226,7 +3238,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi,Musica</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3236,90 +3248,76 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>2022-05-20T10:02:04+00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-05-20T10:02:34+00:00</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-05-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-30T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazzetta Pomposa</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
-        </is>
-      </c>
+      <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Serate in Pomposa - 1° edizione</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>https://www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U27" t="inlineStr"/>
       <c r="V27" t="b">
         <v>0</v>
       </c>
-      <c r="W27" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W27" t="n">
+        <v>41123</v>
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3341,7 +3339,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3351,76 +3349,90 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
+          <t>2021-09-09T10:12:02+00:00</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-05-26T07:16:41+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
         </is>
       </c>
       <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr"/>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr"/>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V28" t="b">
         <v>0</v>
       </c>
-      <c r="W28" t="n">
-        <v>41123</v>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3442,7 +3454,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Visite guidate,Altri eventi,Spettacoli</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3450,65 +3462,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>via Selmi, 63</t>
+        </is>
+      </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2022-05-30T09:56:40+00:00</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:24:22+00:00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-06-10T09:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-06-10T10:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-05-26T07:16:41+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Duomo di Modena</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 20.30</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gratuito</t>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
         </is>
       </c>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
@@ -3521,7 +3533,7 @@
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
@@ -3543,7 +3555,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Altri eventi</t>
+          <t>Visite guidate,Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3551,65 +3563,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>corso Canalgrande, 85</t>
-        </is>
-      </c>
+      <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
+          <t>2022-05-30T09:56:40+00:00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
+          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-06-10T11:00:00+00:00</t>
+          <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-06-10T12:00:00+00:00</t>
+          <t>2022-06-10T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
         </is>
       </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-05-30T11:42:41+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Duomo di Modena</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> dalle ore 20.30</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr"/>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gratuito</t>
+        </is>
+      </c>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
+          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
@@ -3622,7 +3634,7 @@
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
@@ -3644,7 +3656,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Concerti</t>
+          <t>Concerti,Spettacoli,Altri eventi</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3654,112 +3666,98 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Strada Pomposiana 292</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2022-05-30T09:03:14+00:00</t>
+          <t>2022-05-30T11:40:24+00:00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:41:23+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-06-10T19:00:00+00:00</t>
+          <t>2022-06-10T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-06-10T21:00:00+00:00</t>
+          <t>2022-06-10T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:42:41+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Fattoria Centofiori</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ore 21.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
-        </is>
-      </c>
+      <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>Whatsapp 3293357131</t>
-        </is>
-      </c>
+      <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Marco Ferri Quartet</t>
+          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>www.fattoriacentofiori.it</t>
-        </is>
-      </c>
+      <c r="U31" t="inlineStr"/>
       <c r="V31" t="b">
         <v>0</v>
       </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>41123</t>
-        </is>
+      <c r="W31" t="n">
+        <v>41123</v>
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
         <is>
-          <t>44,63693000592147</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>10,81076003183179</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA31" t="inlineStr">
         <is>
-          <t>POINT (10.81076003183179 44.63693000592147)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Concerti</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3769,98 +3767,112 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Strada Pomposiana 292</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>2022-05-30T09:03:14+00:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-06-10T19:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-06-10T21:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-05-26T07:20:15+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Fattoria Centofiori</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> Ore 21.00</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
         </is>
       </c>
       <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>Whatsapp 3293357131</t>
+        </is>
+      </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Marco Ferri Quartet</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr"/>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>www.fattoriacentofiori.it</t>
+        </is>
+      </c>
       <c r="V32" t="b">
         <v>0</v>
       </c>
-      <c r="W32" t="n">
-        <v>41123</v>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>41123</t>
+        </is>
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,63693000592147</t>
         </is>
       </c>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,81076003183179</t>
         </is>
       </c>
       <c r="AA32" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.81076003183179 44.63693000592147)</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3870,59 +3882,63 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-05-26T07:20:15+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
@@ -3935,7 +3951,7 @@
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
@@ -3957,7 +3973,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3967,50 +3983,50 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr"/>
+          <t>2022-05-21T10:36:00+00:00</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti</t>
+        </is>
+      </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
@@ -4019,44 +4035,42 @@
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U34" t="inlineStr"/>
       <c r="V34" t="b">
         <v>0</v>
       </c>
-      <c r="W34" t="inlineStr"/>
+      <c r="W34" t="n">
+        <v>41123</v>
+      </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA34" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4066,54 +4080,50 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>via S.Pietro, 1</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:38+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Presentazione del libro</t>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-06-12T09:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-06-12T10:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>Chiostro di San Pietro</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.00</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
@@ -4122,42 +4132,44 @@
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Contro la guerra</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr"/>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V35" t="b">
         <v>0</v>
       </c>
-      <c r="W35" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W35" t="inlineStr"/>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4167,75 +4179,67 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>via S.Pietro, 1</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr"/>
+          <t>2022-05-30T10:02:38+00:00</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-12T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>Chiostro di San Pietro</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> ore 15.00</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Contro la guerra</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U36" t="inlineStr"/>
       <c r="V36" t="b">
         <v>0</v>
       </c>
@@ -4244,7 +4248,7 @@
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
@@ -4266,7 +4270,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4276,63 +4280,75 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
+          <t>2021-08-06T11:34:26+00:00</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr"/>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr"/>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+        </is>
+      </c>
       <c r="V37" t="b">
         <v>0</v>
       </c>
@@ -4341,7 +4357,7 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
@@ -4363,7 +4379,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Iniziative per bambini</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4373,67 +4389,59 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ingresso da corso Cavour, 2</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:00+00:00</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>Laboratorio per bambini 6-10 anni</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-16T11:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-16T12:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 17.00</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
-        </is>
-      </c>
+      <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Un percorso ad arte: il mio giardino blu</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
@@ -4446,7 +4454,7 @@
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
@@ -4468,7 +4476,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4478,67 +4486,67 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>ingresso da corso Cavour, 2</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-05-30T11:14:00+00:00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Commedia brillante</t>
+          <t>Laboratorio per bambini 6-10 anni</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-16T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-16T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> ore 17.00</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
         </is>
       </c>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Un percorso ad arte: il mio giardino blu</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
@@ -4551,7 +4559,7 @@
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
@@ -4573,7 +4581,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4583,79 +4591,67 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr"/>
+          <t>2022-06-03T15:42:40+00:00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Il ricavato sarà devoluto allassociazione Porta Aperta </t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-06-03T15:43:48+00:00</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-16T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-16T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio/@@images/c0ad8cb1-5f1a-4d1b-83ff-c7132036d15c.jpeg</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-05-30T11:00:13+00:00</t>
+          <t>2022-06-04T06:39:39+00:00</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>FMAV - Museo della Figurina</t>
+          <t>Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
+          <t xml:space="preserve"> ore 20.30</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
-      <c r="P40" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
-        </is>
-      </c>
+      <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
+          <t>Cena solidale per i 20 anni di Modenamoremio</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr">
-        <is>
-          <t>www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U40" t="inlineStr"/>
       <c r="V40" t="b">
         <v>0</v>
       </c>
@@ -4664,7 +4660,7 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
@@ -4686,7 +4682,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4696,79 +4692,71 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr"/>
+          <t>2022-03-19T09:15:00+00:00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Commedia brillante</t>
+        </is>
+      </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-03-19T09:19:36+00:00</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-05-30T11:06:40+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>FMAV - Museo della Figurina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr">
-        <is>
-          <t>www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U41" t="inlineStr"/>
       <c r="V41" t="b">
         <v>0</v>
       </c>
@@ -4777,7 +4765,7 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
@@ -4799,7 +4787,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4809,96 +4797,110 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-30T10:57:49+00:00</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr"/>
+          <t>2022-05-30T11:00:13+00:00</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>FMAV - Museo della Figurina</t>
+        </is>
+      </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr"/>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+        </is>
+      </c>
       <c r="Q42" t="inlineStr"/>
-      <c r="R42" t="inlineStr"/>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>www.fmav.org</t>
         </is>
       </c>
       <c r="V42" t="b">
         <v>0</v>
       </c>
-      <c r="W42" t="inlineStr"/>
+      <c r="W42" t="n">
+        <v>41123</v>
+      </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA42" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4908,67 +4910,79 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
-        </is>
-      </c>
+          <t>2022-05-30T10:57:49+00:00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
+          <t>2022-05-30T11:06:40+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
+          <t>FMAV - Museo della Figurina</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
-      <c r="P43" t="inlineStr"/>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+        </is>
+      </c>
       <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr"/>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>www.fmav.org</t>
+        </is>
+      </c>
       <c r="V43" t="b">
         <v>0</v>
       </c>
@@ -4977,7 +4991,7 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -4999,7 +5013,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5009,102 +5023,96 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>Teatro Cittadella</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
-      <c r="U44" t="inlineStr"/>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V44" t="b">
         <v>0</v>
       </c>
-      <c r="W44" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W44" t="inlineStr"/>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA44" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5114,58 +5122,54 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
@@ -5174,7 +5178,7 @@
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
@@ -5187,7 +5191,7 @@
       </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
@@ -5209,7 +5213,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5219,83 +5223,71 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-03-19T09:19:36+00:00</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr"/>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U46" t="inlineStr"/>
       <c r="V46" t="b">
         <v>0</v>
       </c>
@@ -5304,7 +5296,7 @@
       </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
@@ -5326,7 +5318,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5336,50 +5328,58 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
+          <t>2022-02-25T14:15:33+00:00</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr"/>
+          <t>2022-02-28T15:13:23+00:00</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
@@ -5388,44 +5388,42 @@
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U47" t="inlineStr"/>
       <c r="V47" t="b">
         <v>0</v>
       </c>
-      <c r="W47" t="inlineStr"/>
+      <c r="W47" t="n">
+        <v>41123</v>
+      </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA47" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Concerti,Musica,Spettacoli</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5435,85 +5433,81 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ingresso da Corso Cavour, 2</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:21+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
+          <t>2021-06-10T16:48:45+00:00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>mundus@ater.emr.it</t>
+          <t>anticoinpiazzagrande@gmail.com</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-07-26T08:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-07-26T09:00:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Grupo Compay Segundo</t>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
+          <t>2022-05-06T10:18:45+00:00</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Giardini Ducali</t>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.30</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
-        </is>
-      </c>
+      <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr">
         <is>
-          <t>059 340221</t>
+          <t>340 6059686 oppure 338 2098995</t>
         </is>
       </c>
       <c r="S48" t="inlineStr">
         <is>
-          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
       <c r="U48" t="inlineStr">
         <is>
-          <t>https://www.ater.emr.it/it</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V48" t="b">
@@ -5524,7 +5518,7 @@
       </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
@@ -5546,7 +5540,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Concerti,Musica,Spettacoli</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5556,118 +5550,96 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ingresso da Corso Cavour, 2</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:21+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>mundus@ater.emr.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-08-03T08:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-08-03T09:00:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>Mauro Ottolini</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-06-01T09:48:07+00:00</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>Giardini Ducali</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:24:06+00:00</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.30</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
-        </is>
-      </c>
+      <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>059 340221</t>
-        </is>
-      </c>
+      <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>Nada màs fuerte</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr">
         <is>
-          <t>https://www.ater.emr.it/it</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V49" t="b">
         <v>0</v>
       </c>
-      <c r="W49" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5677,96 +5649,118 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-06-01T09:27:21+00:00</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr"/>
+          <t>2022-06-01T09:27:29+00:00</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>mundus@ater.emr.it</t>
+        </is>
+      </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-07-26T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-07-26T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Grupo Compay Segundo</t>
+        </is>
+      </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr"/>
+          <t>2022-06-01T09:27:29+00:00</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>Giardini Ducali</t>
+        </is>
+      </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr"/>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr"/>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>059 340221</t>
+        </is>
+      </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V50" t="b">
         <v>0</v>
       </c>
-      <c r="W50" t="inlineStr"/>
+      <c r="W50" t="n">
+        <v>41123</v>
+      </c>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA50" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5776,73 +5770,85 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr"/>
+          <t>2022-06-01T09:27:21+00:00</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
+        </is>
+      </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
+          <t>2022-06-01T09:27:29+00:00</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>traborghiecontrade@libero.it</t>
+          <t>mundus@ater.emr.it</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-08-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-08-03T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Mauro Ottolini</t>
+        </is>
+      </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
+          <t>2022-06-01T09:48:07+00:00</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+          <t>Giardini Ducali</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr"/>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr">
         <is>
-          <t>333/9103351</t>
+          <t>059 340221</t>
         </is>
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Nada màs fuerte</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V51" t="b">
@@ -5853,7 +5859,7 @@
       </c>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
@@ -5906,23 +5912,23 @@
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
+          <t>2022-05-10T08:26:10+00:00</t>
         </is>
       </c>
       <c r="M52" t="inlineStr"/>
@@ -5952,7 +5958,7 @@
       <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
@@ -5974,7 +5980,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5984,89 +5990,99 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr"/>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V53" t="b">
         <v>0</v>
       </c>
-      <c r="W53" t="inlineStr"/>
+      <c r="W53" t="n">
+        <v>41123</v>
+      </c>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA53" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6104,23 +6120,23 @@
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M54" t="inlineStr"/>
@@ -6150,20 +6166,218 @@
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y54" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z54" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA54" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2022-10-15T22:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>2022-10-16T21:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:27:35+00:00</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V55" t="b">
+        <v>0</v>
+      </c>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y55" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z55" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA55" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V56" t="b">
+        <v>0</v>
+      </c>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y54" t="inlineStr">
+      <c r="Y56" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z54" t="inlineStr">
+      <c r="Z56" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA54" t="inlineStr">
+      <c r="AA56" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Sat Jun  4 08:36:27 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA56"/>
+  <dimension ref="A1:AA57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3238,7 +3238,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Altri eventi,Musica</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3248,63 +3248,63 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Strada Vaciglio Nord, 6</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:04+00:00</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
-        </is>
-      </c>
+          <t>2022-06-04T08:30:34+00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-06-04T08:30:59+00:00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2022-05-12T09:00:00+00:00</t>
+          <t>2022-06-08T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2022-06-30T10:00:00+00:00</t>
+          <t>2022-07-08T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo/@@images/04c6eef6-5450-4d2e-a11b-c353a7bdb6b0.jpeg</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-06-04T08:30:59+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Piazzetta Pomposa</t>
+          <t>Sala Renata Bergonzoni della Casa delle Donne</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
+          <t xml:space="preserve"> Inaugurazione mercoledì 8 giugno ore 18.30  mostra aperta dal 10 giugno nei seguenti orari:  venerdì e sabato dalle 10 alle 13 (ad esclusione di venerdì 17 giugno) </t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ingresso libero</t>
+        </is>
+      </c>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Serate in Pomposa - 1° edizione</t>
+          <t>Oro rosso. Fragole, pomodori, molestie e sfruttamento nel Mediterraneo</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
@@ -3317,7 +3317,7 @@
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3339,7 +3339,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi,Musica</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3349,90 +3349,76 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr"/>
+          <t>2022-05-20T10:02:04+00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-05-20T10:02:34+00:00</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-05-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-30T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazzetta Pomposa</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
-        </is>
-      </c>
+      <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Serate in Pomposa - 1° edizione</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>https://www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U28" t="inlineStr"/>
       <c r="V28" t="b">
         <v>0</v>
       </c>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W28" t="n">
+        <v>41123</v>
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3454,7 +3440,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3464,76 +3450,90 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
+          <t>2021-09-09T10:12:02+00:00</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
         </is>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-05-26T07:16:41+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
         </is>
       </c>
       <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr"/>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V29" t="b">
         <v>0</v>
       </c>
-      <c r="W29" t="n">
-        <v>41123</v>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
@@ -3555,7 +3555,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Visite guidate,Altri eventi,Spettacoli</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3563,65 +3563,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>via Selmi, 63</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2022-05-30T09:56:40+00:00</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:24:22+00:00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-06-10T09:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-06-10T10:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-05-26T07:16:41+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Duomo di Modena</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 20.30</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gratuito</t>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
         </is>
       </c>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
@@ -3634,7 +3634,7 @@
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
@@ -3656,7 +3656,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Altri eventi</t>
+          <t>Visite guidate,Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3664,65 +3664,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>corso Canalgrande, 85</t>
-        </is>
-      </c>
+      <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
+          <t>2022-05-30T09:56:40+00:00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
+          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-06-10T11:00:00+00:00</t>
+          <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-06-10T12:00:00+00:00</t>
+          <t>2022-06-10T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-30T11:42:41+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Duomo di Modena</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> dalle ore 20.30</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gratuito</t>
+        </is>
+      </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
+          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
@@ -3735,7 +3735,7 @@
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
@@ -3757,7 +3757,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Concerti</t>
+          <t>Concerti,Spettacoli,Altri eventi</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3767,112 +3767,98 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Strada Pomposiana 292</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:03:14+00:00</t>
+          <t>2022-05-30T11:40:24+00:00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:41:23+00:00</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-06-10T19:00:00+00:00</t>
+          <t>2022-06-10T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-06-10T21:00:00+00:00</t>
+          <t>2022-06-10T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:42:41+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Fattoria Centofiori</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ore 21.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
-        </is>
-      </c>
+      <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>Whatsapp 3293357131</t>
-        </is>
-      </c>
+      <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Marco Ferri Quartet</t>
+          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr">
-        <is>
-          <t>www.fattoriacentofiori.it</t>
-        </is>
-      </c>
+      <c r="U32" t="inlineStr"/>
       <c r="V32" t="b">
         <v>0</v>
       </c>
-      <c r="W32" t="inlineStr">
-        <is>
-          <t>41123</t>
-        </is>
+      <c r="W32" t="n">
+        <v>41123</v>
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
         <is>
-          <t>44,63693000592147</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>10,81076003183179</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA32" t="inlineStr">
         <is>
-          <t>POINT (10.81076003183179 44.63693000592147)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Concerti</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3882,98 +3868,112 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Strada Pomposiana 292</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
+          <t>2022-05-30T09:03:14+00:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-06-10T19:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-06-10T21:00:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-05-26T07:20:15+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Fattoria Centofiori</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> Ore 21.00</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
         </is>
       </c>
       <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>Whatsapp 3293357131</t>
+        </is>
+      </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Marco Ferri Quartet</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr"/>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>www.fattoriacentofiori.it</t>
+        </is>
+      </c>
       <c r="V33" t="b">
         <v>0</v>
       </c>
-      <c r="W33" t="n">
-        <v>41123</v>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>41123</t>
+        </is>
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,63693000592147</t>
         </is>
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,81076003183179</t>
         </is>
       </c>
       <c r="AA33" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.81076003183179 44.63693000592147)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3983,59 +3983,63 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-05-26T07:20:15+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
@@ -4048,7 +4052,7 @@
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
@@ -4070,7 +4074,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4080,50 +4084,50 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr"/>
+          <t>2022-05-21T10:36:00+00:00</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti</t>
+        </is>
+      </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
@@ -4132,44 +4136,42 @@
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U35" t="inlineStr"/>
       <c r="V35" t="b">
         <v>0</v>
       </c>
-      <c r="W35" t="inlineStr"/>
+      <c r="W35" t="n">
+        <v>41123</v>
+      </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4179,54 +4181,50 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>via S.Pietro, 1</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:38+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Presentazione del libro</t>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-06-12T09:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-12T10:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>Chiostro di San Pietro</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.00</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
@@ -4235,42 +4233,44 @@
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Contro la guerra</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V36" t="b">
         <v>0</v>
       </c>
-      <c r="W36" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W36" t="inlineStr"/>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA36" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4280,75 +4280,67 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>via S.Pietro, 1</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr"/>
+          <t>2022-05-30T10:02:38+00:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-12T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>Chiostro di San Pietro</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> ore 15.00</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Contro la guerra</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U37" t="inlineStr"/>
       <c r="V37" t="b">
         <v>0</v>
       </c>
@@ -4357,7 +4349,7 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
@@ -4379,7 +4371,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4389,63 +4381,75 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
+          <t>2021-08-06T11:34:26+00:00</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr"/>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+        </is>
+      </c>
       <c r="V38" t="b">
         <v>0</v>
       </c>
@@ -4454,7 +4458,7 @@
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
@@ -4476,7 +4480,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Iniziative per bambini</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4486,67 +4490,59 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ingresso da corso Cavour, 2</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:00+00:00</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>Laboratorio per bambini 6-10 anni</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-16T11:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-16T12:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 17.00</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
-        </is>
-      </c>
+      <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Un percorso ad arte: il mio giardino blu</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
@@ -4559,7 +4555,7 @@
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
@@ -4581,7 +4577,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4591,63 +4587,67 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ingresso da corso Cavour, 2</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-06-03T15:42:40+00:00</t>
+          <t>2022-05-30T11:14:00+00:00</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Il ricavato sarà devoluto allassociazione Porta Aperta </t>
+          <t>Laboratorio per bambini 6-10 anni</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-06-03T15:43:48+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-16T15:00:00+00:00</t>
+          <t>2022-06-16T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-16T16:00:00+00:00</t>
+          <t>2022-06-16T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio/@@images/c0ad8cb1-5f1a-4d1b-83ff-c7132036d15c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-06-04T06:39:39+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Piazza XX Settembre</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 20.30</t>
+          <t xml:space="preserve"> ore 17.00</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
-      <c r="P40" t="inlineStr"/>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
+        </is>
+      </c>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Cena solidale per i 20 anni di Modenamoremio</t>
+          <t>Un percorso ad arte: il mio giardino blu</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
@@ -4660,7 +4660,7 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
@@ -4682,7 +4682,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4692,67 +4692,63 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-06-03T15:42:40+00:00</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Commedia brillante</t>
+          <t xml:space="preserve">Il ricavato sarà devoluto allassociazione Porta Aperta </t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-06-03T15:43:48+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-16T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-16T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio/@@images/c0ad8cb1-5f1a-4d1b-83ff-c7132036d15c.jpeg</t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-06-04T06:39:39+00:00</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> ore 20.30</t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Cena solidale per i 20 anni di Modenamoremio</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
@@ -4765,7 +4761,7 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
@@ -4787,7 +4783,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4797,79 +4793,71 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr"/>
+          <t>2022-03-19T09:15:00+00:00</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Commedia brillante</t>
+        </is>
+      </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-03-19T09:19:36+00:00</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-05-30T11:00:13+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>FMAV - Museo della Figurina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr"/>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
-      <c r="U42" t="inlineStr">
-        <is>
-          <t>www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U42" t="inlineStr"/>
       <c r="V42" t="b">
         <v>0</v>
       </c>
@@ -4878,7 +4866,7 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
@@ -4900,7 +4888,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4941,13 +4929,13 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-05-30T11:06:40+00:00</t>
+          <t>2022-05-30T11:00:13+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
@@ -4957,13 +4945,13 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
         </is>
       </c>
       <c r="Q43" t="inlineStr"/>
@@ -4974,7 +4962,7 @@
       </c>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
+          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
@@ -4991,7 +4979,7 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -5013,7 +5001,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5023,96 +5011,110 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-30T10:57:49+00:00</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr"/>
+          <t>2022-05-30T11:06:40+00:00</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>FMAV - Museo della Figurina</t>
+        </is>
+      </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr"/>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+        </is>
+      </c>
       <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr"/>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>www.fmav.org</t>
         </is>
       </c>
       <c r="V44" t="b">
         <v>0</v>
       </c>
-      <c r="W44" t="inlineStr"/>
+      <c r="W44" t="n">
+        <v>41123</v>
+      </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA44" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5122,54 +5124,50 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
@@ -5178,42 +5176,44 @@
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr"/>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V45" t="b">
         <v>0</v>
       </c>
-      <c r="W45" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W45" t="inlineStr"/>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA45" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5223,67 +5223,63 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
@@ -5296,7 +5292,7 @@
       </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
@@ -5318,7 +5314,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5328,67 +5324,67 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr"/>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
@@ -5401,7 +5397,7 @@
       </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
@@ -5423,7 +5419,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5433,83 +5429,71 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-02-25T14:15:33+00:00</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-02-28T15:13:23+00:00</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U48" t="inlineStr"/>
       <c r="V48" t="b">
         <v>0</v>
       </c>
@@ -5518,7 +5502,7 @@
       </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
@@ -5540,7 +5524,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5550,96 +5534,114 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr"/>
+          <t>2022-05-06T10:18:45+00:00</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+        </is>
+      </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
-      <c r="R49" t="inlineStr"/>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S49" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V49" t="b">
         <v>0</v>
       </c>
-      <c r="W49" t="inlineStr"/>
+      <c r="W49" t="n">
+        <v>41123</v>
+      </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Concerti,Musica,Spettacoli</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5649,111 +5651,89 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ingresso da Corso Cavour, 2</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:21+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>mundus@ater.emr.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-07-26T08:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-07-26T09:00:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>Grupo Compay Segundo</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>Giardini Ducali</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:24:06+00:00</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr"/>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.30</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
-        </is>
-      </c>
+      <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr">
-        <is>
-          <t>059 340221</t>
-        </is>
-      </c>
+      <c r="R50" t="inlineStr"/>
       <c r="S50" t="inlineStr">
         <is>
-          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr">
         <is>
-          <t>https://www.ater.emr.it/it</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V50" t="b">
         <v>0</v>
       </c>
-      <c r="W50" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA50" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
@@ -5795,27 +5775,27 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-08-03T08:00:00+00:00</t>
+          <t>2022-07-26T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-08-03T09:00:00+00:00</t>
+          <t>2022-07-26T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Mauro Ottolini</t>
+          <t>Grupo Compay Segundo</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-06-01T09:48:07+00:00</t>
+          <t>2022-06-01T09:27:29+00:00</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
@@ -5842,7 +5822,7 @@
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>Nada màs fuerte</t>
+          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
@@ -5859,7 +5839,7 @@
       </c>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
@@ -5881,7 +5861,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5891,96 +5871,118 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-06-01T09:27:21+00:00</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr"/>
+          <t>2022-06-01T09:27:29+00:00</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>mundus@ater.emr.it</t>
+        </is>
+      </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-08-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-08-03T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Mauro Ottolini</t>
+        </is>
+      </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr"/>
+          <t>2022-06-01T09:48:07+00:00</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Giardini Ducali</t>
+        </is>
+      </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr"/>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>059 340221</t>
+        </is>
+      </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Nada màs fuerte</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V52" t="b">
         <v>0</v>
       </c>
-      <c r="W52" t="inlineStr"/>
+      <c r="W52" t="n">
+        <v>41123</v>
+      </c>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5990,106 +5992,96 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:10+00:00</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R53" t="inlineStr"/>
       <c r="S53" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V53" t="b">
         <v>0</v>
       </c>
-      <c r="W53" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W53" t="inlineStr"/>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA53" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -6099,89 +6091,99 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O54" t="inlineStr"/>
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr"/>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S54" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V54" t="b">
         <v>0</v>
       </c>
-      <c r="W54" t="inlineStr"/>
+      <c r="W54" t="n">
+        <v>41123</v>
+      </c>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA54" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6219,23 +6221,23 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M55" t="inlineStr"/>
@@ -6265,7 +6267,7 @@
       <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr">
@@ -6318,23 +6320,23 @@
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:27:35+00:00</t>
         </is>
       </c>
       <c r="M56" t="inlineStr"/>
@@ -6364,20 +6366,119 @@
       <c r="W56" t="inlineStr"/>
       <c r="X56" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z56" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA56" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V57" t="b">
+        <v>0</v>
+      </c>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y56" t="inlineStr">
+      <c r="Y57" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z56" t="inlineStr">
+      <c r="Z57" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA56" t="inlineStr">
+      <c r="AA57" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Sat Jun  4 08:56:33 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA57"/>
+  <dimension ref="A1:AA58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3656,7 +3656,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Visite guidate,Altri eventi,Spettacoli</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3664,65 +3664,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Strada Vaciglio Nord, 6</t>
+        </is>
+      </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2022-05-30T09:56:40+00:00</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
-        </is>
-      </c>
+          <t>2022-06-04T08:30:34+00:00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-06-04T08:30:59+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
+          <t>2022-06-10T08:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
           <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>2022-06-10T10:00:00+00:00</t>
-        </is>
-      </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie/@@images/9a9f2a19-02f6-4cd6-a272-5cac5ae7adbd.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-06-04T08:52:51+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Duomo di Modena</t>
+          <t>Sala Renata Bergonzoni della Casa delle Donne</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 20.30</t>
+          <t xml:space="preserve"> ore 18.30</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gratuito</t>
+          <t xml:space="preserve"> ingresso libero</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
+          <t>Da suddite a cittadine. Gabriella Degli Esposti e le partigiane modenesi nelle fonti documentarie e nelle memorie</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
@@ -3735,7 +3735,7 @@
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
@@ -3757,7 +3757,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Altri eventi</t>
+          <t>Visite guidate,Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3765,65 +3765,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>corso Canalgrande, 85</t>
-        </is>
-      </c>
+      <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
+          <t>2022-05-30T09:56:40+00:00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
+          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-06-10T11:00:00+00:00</t>
+          <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-06-10T12:00:00+00:00</t>
+          <t>2022-06-10T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-05-30T11:42:41+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Duomo di Modena</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> dalle ore 20.30</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gratuito</t>
+        </is>
+      </c>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
+          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
@@ -3836,7 +3836,7 @@
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
@@ -3858,7 +3858,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Concerti</t>
+          <t>Concerti,Spettacoli,Altri eventi</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3868,112 +3868,98 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Strada Pomposiana 292</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2022-05-30T09:03:14+00:00</t>
+          <t>2022-05-30T11:40:24+00:00</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:41:23+00:00</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-06-10T19:00:00+00:00</t>
+          <t>2022-06-10T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-10T21:00:00+00:00</t>
+          <t>2022-06-10T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:42:41+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Fattoria Centofiori</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ore 21.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
-        </is>
-      </c>
+      <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>Whatsapp 3293357131</t>
-        </is>
-      </c>
+      <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Marco Ferri Quartet</t>
+          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>www.fattoriacentofiori.it</t>
-        </is>
-      </c>
+      <c r="U33" t="inlineStr"/>
       <c r="V33" t="b">
         <v>0</v>
       </c>
-      <c r="W33" t="inlineStr">
-        <is>
-          <t>41123</t>
-        </is>
+      <c r="W33" t="n">
+        <v>41123</v>
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
         <is>
-          <t>44,63693000592147</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>10,81076003183179</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA33" t="inlineStr">
         <is>
-          <t>POINT (10.81076003183179 44.63693000592147)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Concerti</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3983,98 +3969,112 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Strada Pomposiana 292</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
+          <t>2022-05-30T09:03:14+00:00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-06-10T19:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-06-10T21:00:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-26T07:20:15+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Fattoria Centofiori</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> Ore 21.00</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
         </is>
       </c>
       <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr"/>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>Whatsapp 3293357131</t>
+        </is>
+      </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Marco Ferri Quartet</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr"/>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>www.fattoriacentofiori.it</t>
+        </is>
+      </c>
       <c r="V34" t="b">
         <v>0</v>
       </c>
-      <c r="W34" t="n">
-        <v>41123</v>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>41123</t>
+        </is>
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,63693000592147</t>
         </is>
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,81076003183179</t>
         </is>
       </c>
       <c r="AA34" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.81076003183179 44.63693000592147)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4084,59 +4084,63 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-05-26T07:20:15+00:00</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr"/>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
@@ -4149,7 +4153,7 @@
       </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
@@ -4171,7 +4175,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4181,50 +4185,50 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr"/>
+          <t>2022-05-21T10:36:00+00:00</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti</t>
+        </is>
+      </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
@@ -4233,44 +4237,42 @@
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U36" t="inlineStr"/>
       <c r="V36" t="b">
         <v>0</v>
       </c>
-      <c r="W36" t="inlineStr"/>
+      <c r="W36" t="n">
+        <v>41123</v>
+      </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA36" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4280,54 +4282,50 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>via S.Pietro, 1</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:38+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Presentazione del libro</t>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-12T09:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-12T10:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>Chiostro di San Pietro</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.00</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
@@ -4336,42 +4334,44 @@
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Contro la guerra</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr"/>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V37" t="b">
         <v>0</v>
       </c>
-      <c r="W37" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W37" t="inlineStr"/>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA37" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4381,75 +4381,67 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>via S.Pietro, 1</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr"/>
+          <t>2022-05-30T10:02:38+00:00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-12T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>Chiostro di San Pietro</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> ore 15.00</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Contro la guerra</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U38" t="inlineStr"/>
       <c r="V38" t="b">
         <v>0</v>
       </c>
@@ -4458,7 +4450,7 @@
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
@@ -4480,7 +4472,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4490,63 +4482,75 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
+          <t>2021-08-06T11:34:26+00:00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="inlineStr"/>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr"/>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+        </is>
+      </c>
       <c r="V39" t="b">
         <v>0</v>
       </c>
@@ -4555,7 +4559,7 @@
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
@@ -4577,7 +4581,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Iniziative per bambini</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4587,67 +4591,59 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ingresso da corso Cavour, 2</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:00+00:00</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>Laboratorio per bambini 6-10 anni</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-16T11:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-16T12:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 17.00</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
-      <c r="P40" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
-        </is>
-      </c>
+      <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Un percorso ad arte: il mio giardino blu</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
@@ -4660,7 +4656,7 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
@@ -4682,7 +4678,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4692,63 +4688,67 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ingresso da corso Cavour, 2</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-06-03T15:42:40+00:00</t>
+          <t>2022-05-30T11:14:00+00:00</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Il ricavato sarà devoluto allassociazione Porta Aperta </t>
+          <t>Laboratorio per bambini 6-10 anni</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-06-03T15:43:48+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-16T15:00:00+00:00</t>
+          <t>2022-06-16T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-16T16:00:00+00:00</t>
+          <t>2022-06-16T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio/@@images/c0ad8cb1-5f1a-4d1b-83ff-c7132036d15c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-06-04T06:39:39+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Piazza XX Settembre</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 20.30</t>
+          <t xml:space="preserve"> ore 17.00</t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr"/>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
+        </is>
+      </c>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>Cena solidale per i 20 anni di Modenamoremio</t>
+          <t>Un percorso ad arte: il mio giardino blu</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
@@ -4761,7 +4761,7 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
@@ -4783,7 +4783,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4793,67 +4793,63 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-06-03T15:42:40+00:00</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Commedia brillante</t>
+          <t xml:space="preserve">Il ricavato sarà devoluto allassociazione Porta Aperta </t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-06-03T15:43:48+00:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-16T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-16T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio/@@images/c0ad8cb1-5f1a-4d1b-83ff-c7132036d15c.jpeg</t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-06-04T06:39:39+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> ore 20.30</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Cena solidale per i 20 anni di Modenamoremio</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
@@ -4866,7 +4862,7 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
@@ -4888,7 +4884,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4898,79 +4894,71 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr"/>
+          <t>2022-03-19T09:15:00+00:00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Commedia brillante</t>
+        </is>
+      </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-03-19T09:19:36+00:00</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-05-30T11:00:13+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>FMAV - Museo della Figurina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U43" t="inlineStr"/>
       <c r="V43" t="b">
         <v>0</v>
       </c>
@@ -4979,7 +4967,7 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -5001,7 +4989,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5042,13 +5030,13 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-05-30T11:06:40+00:00</t>
+          <t>2022-05-30T11:00:13+00:00</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
@@ -5058,13 +5046,13 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
         </is>
       </c>
       <c r="Q44" t="inlineStr"/>
@@ -5075,7 +5063,7 @@
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
+          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
@@ -5092,7 +5080,7 @@
       </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
@@ -5114,7 +5102,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5124,96 +5112,110 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-30T10:57:49+00:00</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr"/>
+          <t>2022-05-30T11:06:40+00:00</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>FMAV - Museo della Figurina</t>
+        </is>
+      </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
-      <c r="P45" t="inlineStr"/>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+        </is>
+      </c>
       <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="inlineStr"/>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>www.fmav.org</t>
         </is>
       </c>
       <c r="V45" t="b">
         <v>0</v>
       </c>
-      <c r="W45" t="inlineStr"/>
+      <c r="W45" t="n">
+        <v>41123</v>
+      </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA45" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5223,54 +5225,50 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
@@ -5279,42 +5277,44 @@
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr"/>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V46" t="b">
         <v>0</v>
       </c>
-      <c r="W46" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA46" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5324,67 +5324,63 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
@@ -5397,7 +5393,7 @@
       </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
@@ -5419,7 +5415,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5429,67 +5425,67 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
-      <c r="P48" t="inlineStr"/>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
@@ -5502,7 +5498,7 @@
       </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
@@ -5524,7 +5520,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5534,83 +5530,71 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-02-25T14:15:33+00:00</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-02-28T15:13:23+00:00</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
-      <c r="U49" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U49" t="inlineStr"/>
       <c r="V49" t="b">
         <v>0</v>
       </c>
@@ -5619,7 +5603,7 @@
       </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
@@ -5641,7 +5625,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5651,96 +5635,114 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr"/>
+          <t>2022-05-06T10:18:45+00:00</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+        </is>
+      </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr"/>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V50" t="b">
         <v>0</v>
       </c>
-      <c r="W50" t="inlineStr"/>
+      <c r="W50" t="n">
+        <v>41123</v>
+      </c>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA50" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Concerti,Musica,Spettacoli</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5750,111 +5752,89 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ingresso da Corso Cavour, 2</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:21+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>mundus@ater.emr.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-07-26T08:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-07-26T09:00:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>Grupo Compay Segundo</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>Giardini Ducali</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:24:06+00:00</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.30</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
-        </is>
-      </c>
+      <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
-      <c r="R51" t="inlineStr">
-        <is>
-          <t>059 340221</t>
-        </is>
-      </c>
+      <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr">
         <is>
-          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr">
         <is>
-          <t>https://www.ater.emr.it/it</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V51" t="b">
         <v>0</v>
       </c>
-      <c r="W51" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA51" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
@@ -5896,27 +5876,27 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-08-03T08:00:00+00:00</t>
+          <t>2022-07-26T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-08-03T09:00:00+00:00</t>
+          <t>2022-07-26T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Mauro Ottolini</t>
+          <t>Grupo Compay Segundo</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-06-01T09:48:07+00:00</t>
+          <t>2022-06-01T09:27:29+00:00</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
@@ -5943,7 +5923,7 @@
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Nada màs fuerte</t>
+          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
@@ -5960,7 +5940,7 @@
       </c>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
@@ -5982,7 +5962,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5992,96 +5972,118 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-06-01T09:27:21+00:00</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr"/>
+          <t>2022-06-01T09:27:29+00:00</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>mundus@ater.emr.it</t>
+        </is>
+      </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-08-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-08-03T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Mauro Ottolini</t>
+        </is>
+      </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr"/>
+          <t>2022-06-01T09:48:07+00:00</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>Giardini Ducali</t>
+        </is>
+      </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr"/>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr"/>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>059 340221</t>
+        </is>
+      </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Nada màs fuerte</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V53" t="b">
         <v>0</v>
       </c>
-      <c r="W53" t="inlineStr"/>
+      <c r="W53" t="n">
+        <v>41123</v>
+      </c>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA53" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -6091,106 +6093,96 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:10+00:00</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O54" t="inlineStr"/>
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R54" t="inlineStr"/>
       <c r="S54" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V54" t="b">
         <v>0</v>
       </c>
-      <c r="W54" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA54" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -6200,89 +6192,99 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr"/>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S55" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V55" t="b">
         <v>0</v>
       </c>
-      <c r="W55" t="inlineStr"/>
+      <c r="W55" t="n">
+        <v>41123</v>
+      </c>
       <c r="X55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA55" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6320,23 +6322,23 @@
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M56" t="inlineStr"/>
@@ -6366,7 +6368,7 @@
       <c r="W56" t="inlineStr"/>
       <c r="X56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y56" t="inlineStr">
@@ -6419,23 +6421,23 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:27:35+00:00</t>
         </is>
       </c>
       <c r="M57" t="inlineStr"/>
@@ -6465,20 +6467,119 @@
       <c r="W57" t="inlineStr"/>
       <c r="X57" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z57" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA57" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="inlineStr"/>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T58" t="inlineStr"/>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V58" t="b">
+        <v>0</v>
+      </c>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y57" t="inlineStr">
+      <c r="Y58" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z57" t="inlineStr">
+      <c r="Z58" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA57" t="inlineStr">
+      <c r="AA58" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Sat Jun  4 09:16:03 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA58"/>
+  <dimension ref="A1:AA59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2727,7 +2727,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Concerti,Musica</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2735,66 +2735,92 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>viale Monte Kosica, amgolo viale Molza</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2022-05-26T09:12:46+00:00</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Giovedì 2 giugno, celebrazioni con alzabandiera e sfilata della banda cittadina. Iniziative in programma già dal 30 maggio</t>
-        </is>
-      </c>
+          <t>2021-06-24T13:52:45+00:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2022-05-30T09:29:45+00:00</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr"/>
+          <t>2021-06-24T13:52:57+00:00</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>latenda@comune.modena.it</t>
+        </is>
+      </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2022-05-30T09:00:00+00:00</t>
+          <t>2022-06-06T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2022-06-02T10:00:00+00:00</t>
+          <t>2022-06-06T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/festa-della-repubblica/@@images/0031a2b2-623b-4b21-8316-cfd065155db6.jpeg</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/a-la-tenda-il-rock-dei-delta/@@images/e89ce1ee-1337-48c0-8eeb-d60c0b9187d9.jpeg</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Delta Sleep</t>
+        </is>
+      </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2022-05-30T09:29:45+00:00</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
+          <t>2022-06-04T09:03:06+00:00</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>La Tenda</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ore 21.00</t>
+        </is>
+      </c>
       <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr">
         <is>
-          <t>Festa della Repubblica</t>
+          <t>A La Tenda, il rock dei Delta</t>
         </is>
       </c>
       <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/latenda</t>
+        </is>
+      </c>
       <c r="V22" t="b">
         <v>0</v>
       </c>
-      <c r="W22" t="n">
-        <v>41123</v>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/festa-della-repubblica</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/a-la-tenda-il-rock-dei-delta</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
@@ -2816,7 +2842,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Musica</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2824,69 +2850,53 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>corso Canalgrande, 85</t>
-        </is>
-      </c>
+      <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr"/>
+          <t>2022-05-26T09:12:46+00:00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Giovedì 2 giugno, celebrazioni con alzabandiera e sfilata della banda cittadina. Iniziative in programma già dal 30 maggio</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
+          <t>2022-05-30T09:29:45+00:00</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2022-06-06T11:00:00+00:00</t>
+          <t>2022-05-30T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2022-06-06T12:00:00+00:00</t>
+          <t>2022-06-02T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-inaugurale-della-nuova-filarmonica-del-teatro-comunale/@@images/bd0aa52a-489c-4715-b957-8a4551ed5f95.jpeg</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>Dmitry Masleev</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/festa-della-repubblica/@@images/0031a2b2-623b-4b21-8316-cfd065155db6.jpeg</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2022-06-01T12:46:07+00:00</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
-        </is>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ore 21.00</t>
-        </is>
-      </c>
+          <t>2022-05-30T09:29:45+00:00</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingressio con biglietto gratuito. I biglietti sono disponibili presso la biglietteria del Teatro o telefonando allo 059  2033010</t>
-        </is>
-      </c>
+      <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr">
         <is>
-          <t>Concerto inaugurale della nuova Filarmonica del Teatro comunale</t>
+          <t>Festa della Repubblica</t>
         </is>
       </c>
       <c r="T23" t="inlineStr"/>
@@ -2899,7 +2909,7 @@
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-inaugurale-della-nuova-filarmonica-del-teatro-comunale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/festa-della-repubblica</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
@@ -2921,7 +2931,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Altri eventi,Mercati</t>
+          <t>Concerti,Spettacoli,Musica</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2931,78 +2941,80 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Ingresso da viale Berengario</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2020-12-29T15:02:32+00:00</t>
+          <t>2022-05-30T11:40:24+00:00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2020-12-29T15:05:00+00:00</t>
+          <t>2022-05-30T11:41:23+00:00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2022-01-03T14:00:00+00:00</t>
+          <t>2022-06-06T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2022-12-26T14:59:00+00:00</t>
+          <t>2022-06-06T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-inaugurale-della-nuova-filarmonica-del-teatro-comunale/@@images/bd0aa52a-489c-4715-b957-8a4551ed5f95.jpeg</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Dmitry Masleev</t>
+        </is>
+      </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2021-12-28T10:39:07+00:00</t>
+          <t>2022-06-01T12:46:07+00:00</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingressio con biglietto gratuito. I biglietti sono disponibili presso la biglietteria del Teatro o telefonando allo 059  2033010</t>
+        </is>
+      </c>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr">
         <is>
-          <t>Mercato settimanale del lunedì</t>
+          <t>Concerto inaugurale della nuova Filarmonica del Teatro comunale</t>
         </is>
       </c>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.com/</t>
-        </is>
-      </c>
+      <c r="U24" t="inlineStr"/>
       <c r="V24" t="b">
         <v>0</v>
       </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W24" t="n">
+        <v>41123</v>
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-inaugurale-della-nuova-filarmonica-del-teatro-comunale</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
@@ -3024,7 +3036,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Altri eventi,Spettacoli,Musica,Libri</t>
+          <t>Altri eventi,Mercati</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3034,54 +3046,50 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Ingresso da viale Berengario</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2022-06-03T15:42:40+00:00</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Rassegna di eventi culturali in Piazza XX Settembre</t>
-        </is>
-      </c>
+          <t>2020-12-29T15:02:32+00:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2022-06-03T15:43:48+00:00</t>
+          <t>2020-12-29T15:05:00+00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2022-06-07T15:00:00+00:00</t>
+          <t>2022-01-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2022-06-28T16:00:00+00:00</t>
+          <t>2022-12-26T14:59:00+00:00</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/note-di-stelle/@@images/78120e75-8036-4a4c-b46e-10cc1ff7fe4c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
         </is>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2022-06-04T06:35:10+00:00</t>
+          <t>2021-12-28T10:39:07+00:00</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Piazza XX Settembre</t>
+          <t>Parco Novi Sad</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 7, 14, 21 e 28 giugno alle ore 19 presentazione di libri  alle ore 21 spettacoli</t>
+          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
@@ -3090,20 +3098,26 @@
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>Note di Stelle</t>
+          <t>Mercato settimanale del lunedì</t>
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
-      <c r="U25" t="inlineStr"/>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.com/</t>
+        </is>
+      </c>
       <c r="V25" t="b">
         <v>0</v>
       </c>
-      <c r="W25" t="n">
-        <v>41123</v>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/note-di-stelle</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
@@ -3125,7 +3139,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Altri eventi,Spettacoli,Musica,Libri</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3135,79 +3149,67 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Corso Vittorio Emanuele, 59</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2022-06-04T07:59:44+00:00</t>
+          <t>2022-06-03T15:42:40+00:00</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Presentazione del libro</t>
+          <t>Rassegna di eventi culturali in Piazza XX Settembre</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2022-06-04T07:59:52+00:00</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>​info@accademiasla-mo.it</t>
-        </is>
-      </c>
+          <t>2022-06-03T15:43:48+00:00</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2022-06-08T07:00:00+00:00</t>
+          <t>2022-06-07T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2022-06-08T08:00:00+00:00</t>
+          <t>2022-06-28T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione/@@images/1a4df534-f8d8-4ac6-87d4-3d9176cd882c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/note-di-stelle/@@images/78120e75-8036-4a4c-b46e-10cc1ff7fe4c.jpeg</t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2022-06-04T07:59:52+00:00</t>
+          <t>2022-06-04T06:35:10+00:00</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Accademia Nazionale di Scienze Lettere e Arti di Modena</t>
+          <t>Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.30</t>
+          <t xml:space="preserve"> 7, 14, 21 e 28 giugno alle ore 19 presentazione di libri  alle ore 21 spettacoli</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>059 225566</t>
-        </is>
-      </c>
+      <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr">
         <is>
-          <t>"Delitti in prima pagina. La giustizia nella società dell’informazione"</t>
+          <t>Note di Stelle</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>www.accademiasla-mo.it</t>
-        </is>
-      </c>
+      <c r="U26" t="inlineStr"/>
       <c r="V26" t="b">
         <v>0</v>
       </c>
@@ -3216,7 +3218,7 @@
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/note-di-stelle</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
@@ -3238,7 +3240,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3248,67 +3250,79 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Strada Vaciglio Nord, 6</t>
+          <t>Corso Vittorio Emanuele, 59</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2022-06-04T08:30:34+00:00</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>2022-06-04T07:59:44+00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2022-06-04T08:30:59+00:00</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr"/>
+          <t>2022-06-04T07:59:52+00:00</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>​info@accademiasla-mo.it</t>
+        </is>
+      </c>
       <c r="H27" t="inlineStr">
         <is>
+          <t>2022-06-08T07:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
           <t>2022-06-08T08:00:00+00:00</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>2022-07-08T09:00:00+00:00</t>
-        </is>
-      </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo/@@images/04c6eef6-5450-4d2e-a11b-c353a7bdb6b0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione/@@images/1a4df534-f8d8-4ac6-87d4-3d9176cd882c.jpeg</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-06-04T08:30:59+00:00</t>
+          <t>2022-06-04T07:59:52+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Sala Renata Bergonzoni della Casa delle Donne</t>
+          <t>Accademia Nazionale di Scienze Lettere e Arti di Modena</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Inaugurazione mercoledì 8 giugno ore 18.30  mostra aperta dal 10 giugno nei seguenti orari:  venerdì e sabato dalle 10 alle 13 (ad esclusione di venerdì 17 giugno) </t>
+          <t xml:space="preserve"> ore 15.30</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ingresso libero</t>
-        </is>
-      </c>
+      <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>059 225566</t>
+        </is>
+      </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Oro rosso. Fragole, pomodori, molestie e sfruttamento nel Mediterraneo</t>
+          <t>"Delitti in prima pagina. La giustizia nella società dell’informazione"</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>www.accademiasla-mo.it</t>
+        </is>
+      </c>
       <c r="V27" t="b">
         <v>0</v>
       </c>
@@ -3317,7 +3331,7 @@
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3339,7 +3353,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Altri eventi,Musica</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3349,63 +3363,63 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Strada Vaciglio Nord, 6</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:04+00:00</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
-        </is>
-      </c>
+          <t>2022-06-04T08:30:34+00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-06-04T08:30:59+00:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-05-12T09:00:00+00:00</t>
+          <t>2022-06-08T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-06-30T10:00:00+00:00</t>
+          <t>2022-07-08T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo/@@images/04c6eef6-5450-4d2e-a11b-c353a7bdb6b0.jpeg</t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-06-04T08:30:59+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Piazzetta Pomposa</t>
+          <t>Sala Renata Bergonzoni della Casa delle Donne</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
+          <t xml:space="preserve"> Inaugurazione mercoledì 8 giugno ore 18.30  mostra aperta dal 10 giugno nei seguenti orari:  venerdì e sabato dalle 10 alle 13 (ad esclusione di venerdì 17 giugno) </t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ingresso libero</t>
+        </is>
+      </c>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Serate in Pomposa - 1° edizione</t>
+          <t>Oro rosso. Fragole, pomodori, molestie e sfruttamento nel Mediterraneo</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
@@ -3418,7 +3432,7 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3440,7 +3454,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi,Musica</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3450,90 +3464,76 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
+          <t>2022-05-20T10:02:04+00:00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-05-20T10:02:34+00:00</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-05-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-30T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
         </is>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazzetta Pomposa</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
-        </is>
-      </c>
+      <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Serate in Pomposa - 1° edizione</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>https://www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U29" t="inlineStr"/>
       <c r="V29" t="b">
         <v>0</v>
       </c>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W29" t="n">
+        <v>41123</v>
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
@@ -3555,7 +3555,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3565,76 +3565,90 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
+          <t>2021-09-09T10:12:02+00:00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
         </is>
       </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-05-26T07:16:41+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
         </is>
       </c>
       <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V30" t="b">
         <v>0</v>
       </c>
-      <c r="W30" t="n">
-        <v>41123</v>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
@@ -3656,7 +3670,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3666,63 +3680,63 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Strada Vaciglio Nord, 6</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2022-06-04T08:30:34+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2022-06-04T08:30:59+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
+          <t>2022-06-10T07:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
           <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>2022-06-10T09:00:00+00:00</t>
-        </is>
-      </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie/@@images/9a9f2a19-02f6-4cd6-a272-5cac5ae7adbd.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-06-04T08:52:51+00:00</t>
+          <t>2022-05-26T07:16:41+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Sala Renata Bergonzoni della Casa delle Donne</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 18.30</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ingresso libero</t>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
         </is>
       </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Da suddite a cittadine. Gabriella Degli Esposti e le partigiane modenesi nelle fonti documentarie e nelle memorie</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
@@ -3735,7 +3749,7 @@
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
@@ -3757,7 +3771,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Visite guidate,Altri eventi,Spettacoli</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3765,65 +3779,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Strada Vaciglio Nord, 6</t>
+        </is>
+      </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:56:40+00:00</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
-        </is>
-      </c>
+          <t>2022-06-04T08:30:34+00:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-06-04T08:30:59+00:00</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
+          <t>2022-06-10T08:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
           <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>2022-06-10T10:00:00+00:00</t>
-        </is>
-      </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie/@@images/9a9f2a19-02f6-4cd6-a272-5cac5ae7adbd.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-06-04T08:52:51+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Duomo di Modena</t>
+          <t>Sala Renata Bergonzoni della Casa delle Donne</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 20.30</t>
+          <t xml:space="preserve"> ore 18.30</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gratuito</t>
+          <t xml:space="preserve"> ingresso libero</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
+          <t>Da suddite a cittadine. Gabriella Degli Esposti e le partigiane modenesi nelle fonti documentarie e nelle memorie</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
@@ -3836,7 +3850,7 @@
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
@@ -3858,7 +3872,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Altri eventi</t>
+          <t>Visite guidate,Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3866,65 +3880,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>corso Canalgrande, 85</t>
-        </is>
-      </c>
+      <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
+          <t>2022-05-30T09:56:40+00:00</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
+          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-06-10T11:00:00+00:00</t>
+          <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-10T12:00:00+00:00</t>
+          <t>2022-06-10T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-05-30T11:42:41+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Duomo di Modena</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> dalle ore 20.30</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gratuito</t>
+        </is>
+      </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
+          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
@@ -3937,7 +3951,7 @@
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
@@ -3959,7 +3973,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Concerti</t>
+          <t>Concerti,Spettacoli,Altri eventi</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3969,112 +3983,98 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Strada Pomposiana 292</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2022-05-30T09:03:14+00:00</t>
+          <t>2022-05-30T11:40:24+00:00</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:41:23+00:00</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-06-10T19:00:00+00:00</t>
+          <t>2022-06-10T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-06-10T21:00:00+00:00</t>
+          <t>2022-06-10T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:42:41+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>Fattoria Centofiori</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ore 21.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
-        </is>
-      </c>
+      <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>Whatsapp 3293357131</t>
-        </is>
-      </c>
+      <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Marco Ferri Quartet</t>
+          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>www.fattoriacentofiori.it</t>
-        </is>
-      </c>
+      <c r="U34" t="inlineStr"/>
       <c r="V34" t="b">
         <v>0</v>
       </c>
-      <c r="W34" t="inlineStr">
-        <is>
-          <t>41123</t>
-        </is>
+      <c r="W34" t="n">
+        <v>41123</v>
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
         <is>
-          <t>44,63693000592147</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>10,81076003183179</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA34" t="inlineStr">
         <is>
-          <t>POINT (10.81076003183179 44.63693000592147)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Concerti</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4084,98 +4084,112 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Strada Pomposiana 292</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr"/>
+          <t>2022-05-30T09:03:14+00:00</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-06-10T19:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-06-10T21:00:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-05-26T07:20:15+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Fattoria Centofiori</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> Ore 21.00</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
         </is>
       </c>
       <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="inlineStr"/>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>Whatsapp 3293357131</t>
+        </is>
+      </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Marco Ferri Quartet</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr"/>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>www.fattoriacentofiori.it</t>
+        </is>
+      </c>
       <c r="V35" t="b">
         <v>0</v>
       </c>
-      <c r="W35" t="n">
-        <v>41123</v>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>41123</t>
+        </is>
       </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,63693000592147</t>
         </is>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,81076003183179</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.81076003183179 44.63693000592147)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4185,59 +4199,63 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-05-26T07:20:15+00:00</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
@@ -4250,7 +4268,7 @@
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
@@ -4272,7 +4290,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4282,50 +4300,50 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr"/>
+          <t>2022-05-21T10:36:00+00:00</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti</t>
+        </is>
+      </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
@@ -4334,44 +4352,42 @@
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U37" t="inlineStr"/>
       <c r="V37" t="b">
         <v>0</v>
       </c>
-      <c r="W37" t="inlineStr"/>
+      <c r="W37" t="n">
+        <v>41123</v>
+      </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA37" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4381,54 +4397,50 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>via S.Pietro, 1</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:38+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Presentazione del libro</t>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-12T09:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-12T10:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>Chiostro di San Pietro</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.00</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
@@ -4437,42 +4449,44 @@
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Contro la guerra</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V38" t="b">
         <v>0</v>
       </c>
-      <c r="W38" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W38" t="inlineStr"/>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA38" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4482,75 +4496,67 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>via S.Pietro, 1</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr"/>
+          <t>2022-05-30T10:02:38+00:00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-12T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>Chiostro di San Pietro</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> ore 15.00</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Contro la guerra</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U39" t="inlineStr"/>
       <c r="V39" t="b">
         <v>0</v>
       </c>
@@ -4559,7 +4565,7 @@
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
@@ -4581,7 +4587,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4591,63 +4597,75 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
+          <t>2021-08-06T11:34:26+00:00</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr"/>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr"/>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+        </is>
+      </c>
       <c r="V40" t="b">
         <v>0</v>
       </c>
@@ -4656,7 +4674,7 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
@@ -4678,7 +4696,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Iniziative per bambini</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4688,67 +4706,59 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ingresso da corso Cavour, 2</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:00+00:00</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Laboratorio per bambini 6-10 anni</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-16T11:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-16T12:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 17.00</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
-        </is>
-      </c>
+      <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>Un percorso ad arte: il mio giardino blu</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
@@ -4761,7 +4771,7 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
@@ -4783,7 +4793,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4793,63 +4803,67 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ingresso da corso Cavour, 2</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2022-06-03T15:42:40+00:00</t>
+          <t>2022-05-30T11:14:00+00:00</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Il ricavato sarà devoluto allassociazione Porta Aperta </t>
+          <t>Laboratorio per bambini 6-10 anni</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2022-06-03T15:43:48+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-16T15:00:00+00:00</t>
+          <t>2022-06-16T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-06-16T16:00:00+00:00</t>
+          <t>2022-06-16T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio/@@images/c0ad8cb1-5f1a-4d1b-83ff-c7132036d15c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-06-04T06:39:39+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Piazza XX Settembre</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 20.30</t>
+          <t xml:space="preserve"> ore 17.00</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr"/>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
+        </is>
+      </c>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>Cena solidale per i 20 anni di Modenamoremio</t>
+          <t>Un percorso ad arte: il mio giardino blu</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
@@ -4862,7 +4876,7 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
@@ -4884,7 +4898,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4894,67 +4908,63 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-06-03T15:42:40+00:00</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Commedia brillante</t>
+          <t xml:space="preserve">Il ricavato sarà devoluto allassociazione Porta Aperta </t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-06-03T15:43:48+00:00</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-16T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-16T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio/@@images/c0ad8cb1-5f1a-4d1b-83ff-c7132036d15c.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-06-04T06:39:39+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> ore 20.30</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Cena solidale per i 20 anni di Modenamoremio</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
@@ -4967,7 +4977,7 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -4989,7 +4999,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -4999,79 +5009,71 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
+          <t>2022-03-19T09:15:00+00:00</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Commedia brillante</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-03-19T09:19:36+00:00</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-05-30T11:00:13+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>FMAV - Museo della Figurina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
-      <c r="U44" t="inlineStr">
-        <is>
-          <t>www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U44" t="inlineStr"/>
       <c r="V44" t="b">
         <v>0</v>
       </c>
@@ -5080,7 +5082,7 @@
       </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
@@ -5102,7 +5104,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5143,13 +5145,13 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-05-30T11:06:40+00:00</t>
+          <t>2022-05-30T11:00:13+00:00</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
@@ -5159,13 +5161,13 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
         </is>
       </c>
       <c r="Q45" t="inlineStr"/>
@@ -5176,7 +5178,7 @@
       </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
+          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
@@ -5193,7 +5195,7 @@
       </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
@@ -5215,7 +5217,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5225,96 +5227,110 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-30T10:57:49+00:00</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
         </is>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr"/>
+          <t>2022-05-30T11:06:40+00:00</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>FMAV - Museo della Figurina</t>
+        </is>
+      </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr"/>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+        </is>
+      </c>
       <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr"/>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>www.fmav.org</t>
         </is>
       </c>
       <c r="V46" t="b">
         <v>0</v>
       </c>
-      <c r="W46" t="inlineStr"/>
+      <c r="W46" t="n">
+        <v>41123</v>
+      </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA46" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5324,54 +5340,50 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr"/>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
@@ -5380,42 +5392,44 @@
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr"/>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V47" t="b">
         <v>0</v>
       </c>
-      <c r="W47" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA47" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5425,67 +5439,63 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
@@ -5498,7 +5508,7 @@
       </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
@@ -5520,7 +5530,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5530,67 +5540,67 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr"/>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
@@ -5603,7 +5613,7 @@
       </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
@@ -5625,7 +5635,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5635,83 +5645,71 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-02-25T14:15:33+00:00</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-02-28T15:13:23+00:00</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R50" t="inlineStr"/>
       <c r="S50" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
-      <c r="U50" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U50" t="inlineStr"/>
       <c r="V50" t="b">
         <v>0</v>
       </c>
@@ -5720,7 +5718,7 @@
       </c>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
@@ -5742,7 +5740,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5752,96 +5750,114 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr"/>
+          <t>2022-05-06T10:18:45+00:00</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+        </is>
+      </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
-      <c r="R51" t="inlineStr"/>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V51" t="b">
         <v>0</v>
       </c>
-      <c r="W51" t="inlineStr"/>
+      <c r="W51" t="n">
+        <v>41123</v>
+      </c>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA51" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Concerti,Musica,Spettacoli</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5851,111 +5867,89 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ingresso da Corso Cavour, 2</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:21+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>mundus@ater.emr.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-07-26T08:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-07-26T09:00:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>Grupo Compay Segundo</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>Giardini Ducali</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:24:06+00:00</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.30</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
-        </is>
-      </c>
+      <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>059 340221</t>
-        </is>
-      </c>
+      <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr">
         <is>
-          <t>https://www.ater.emr.it/it</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V52" t="b">
         <v>0</v>
       </c>
-      <c r="W52" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
@@ -5997,27 +5991,27 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-08-03T08:00:00+00:00</t>
+          <t>2022-07-26T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-08-03T09:00:00+00:00</t>
+          <t>2022-07-26T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Mauro Ottolini</t>
+          <t>Grupo Compay Segundo</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-06-01T09:48:07+00:00</t>
+          <t>2022-06-01T09:27:29+00:00</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
@@ -6044,7 +6038,7 @@
       </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>Nada màs fuerte</t>
+          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
@@ -6061,7 +6055,7 @@
       </c>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
@@ -6083,7 +6077,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -6093,96 +6087,118 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-06-01T09:27:21+00:00</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr"/>
+          <t>2022-06-01T09:27:29+00:00</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>mundus@ater.emr.it</t>
+        </is>
+      </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-08-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-08-03T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Mauro Ottolini</t>
+        </is>
+      </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr"/>
+          <t>2022-06-01T09:48:07+00:00</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>Giardini Ducali</t>
+        </is>
+      </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr"/>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>059 340221</t>
+        </is>
+      </c>
       <c r="S54" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Nada màs fuerte</t>
         </is>
       </c>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V54" t="b">
         <v>0</v>
       </c>
-      <c r="W54" t="inlineStr"/>
+      <c r="W54" t="n">
+        <v>41123</v>
+      </c>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA54" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -6192,106 +6208,96 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:10+00:00</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr"/>
       <c r="N55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R55" t="inlineStr"/>
       <c r="S55" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V55" t="b">
         <v>0</v>
       </c>
-      <c r="W55" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA55" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -6301,89 +6307,99 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="inlineStr"/>
-      <c r="R56" t="inlineStr"/>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S56" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V56" t="b">
         <v>0</v>
       </c>
-      <c r="W56" t="inlineStr"/>
+      <c r="W56" t="n">
+        <v>41123</v>
+      </c>
       <c r="X56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y56" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z56" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA56" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6421,23 +6437,23 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M57" t="inlineStr"/>
@@ -6467,7 +6483,7 @@
       <c r="W57" t="inlineStr"/>
       <c r="X57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y57" t="inlineStr">
@@ -6520,23 +6536,23 @@
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:27:35+00:00</t>
         </is>
       </c>
       <c r="M58" t="inlineStr"/>
@@ -6566,20 +6582,119 @@
       <c r="W58" t="inlineStr"/>
       <c r="X58" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z58" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA58" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
+      <c r="R59" t="inlineStr"/>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T59" t="inlineStr"/>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V59" t="b">
+        <v>0</v>
+      </c>
+      <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y58" t="inlineStr">
+      <c r="Y59" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z58" t="inlineStr">
+      <c r="Z59" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA58" t="inlineStr">
+      <c r="AA59" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Sat Jun  4 12:22:32 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA59"/>
+  <dimension ref="A1:AA60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4290,7 +4290,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4300,50 +4300,62 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Largo Porta Sant’Agostino, 228</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr"/>
+          <t>2022-06-04T09:45:49+00:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>mostra fotografica di Francesco Jodice</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr"/>
+          <t>2022-06-04T09:46:06+00:00</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>info@agomodena.it</t>
+        </is>
+      </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-06-11T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-08-28T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/ritratti-di-classe/@@images/3dba106b-6f95-4190-991d-b13abf85501a.jpeg</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Ritratti di classe</t>
+        </is>
+      </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-06-04T09:47:46+00:00</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>AGO Modena Fabbriche culturali</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> vedi sul sito dell'evento</t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
@@ -4352,11 +4364,15 @@
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Ritratti di Classe</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr"/>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>www.agomodena.it</t>
+        </is>
+      </c>
       <c r="V37" t="b">
         <v>0</v>
       </c>
@@ -4365,7 +4381,7 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/ritratti-di-classe</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
@@ -4387,7 +4403,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4397,50 +4413,50 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr"/>
+          <t>2022-05-21T10:36:00+00:00</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti</t>
+        </is>
+      </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
@@ -4449,44 +4465,42 @@
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U38" t="inlineStr"/>
       <c r="V38" t="b">
         <v>0</v>
       </c>
-      <c r="W38" t="inlineStr"/>
+      <c r="W38" t="n">
+        <v>41123</v>
+      </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA38" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4496,54 +4510,50 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>via S.Pietro, 1</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:38+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Presentazione del libro</t>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-12T09:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-12T10:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>Chiostro di San Pietro</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.00</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
@@ -4552,42 +4562,44 @@
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Contro la guerra</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr"/>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V39" t="b">
         <v>0</v>
       </c>
-      <c r="W39" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W39" t="inlineStr"/>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA39" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4597,75 +4609,67 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>via S.Pietro, 1</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr"/>
+          <t>2022-05-30T10:02:38+00:00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-12T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>Chiostro di San Pietro</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> ore 15.00</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Contro la guerra</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U40" t="inlineStr"/>
       <c r="V40" t="b">
         <v>0</v>
       </c>
@@ -4674,7 +4678,7 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
@@ -4696,7 +4700,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4706,63 +4710,75 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
+          <t>2021-08-06T11:34:26+00:00</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2021-08-06T11:36:33+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>logo del mercatino</t>
+        </is>
+      </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr"/>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr"/>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
+        </is>
+      </c>
       <c r="V41" t="b">
         <v>0</v>
       </c>
@@ -4771,7 +4787,7 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
@@ -4793,7 +4809,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Iniziative per bambini</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4803,67 +4819,59 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ingresso da corso Cavour, 2</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:00+00:00</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Laboratorio per bambini 6-10 anni</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-16T11:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-06-16T12:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 17.00</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
-        </is>
-      </c>
+      <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>Un percorso ad arte: il mio giardino blu</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
@@ -4876,7 +4884,7 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
@@ -4898,7 +4906,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4908,63 +4916,67 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ingresso da corso Cavour, 2</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2022-06-03T15:42:40+00:00</t>
+          <t>2022-05-30T11:14:00+00:00</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Il ricavato sarà devoluto allassociazione Porta Aperta </t>
+          <t>Laboratorio per bambini 6-10 anni</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2022-06-03T15:43:48+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-16T15:00:00+00:00</t>
+          <t>2022-06-16T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-06-16T16:00:00+00:00</t>
+          <t>2022-06-16T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio/@@images/c0ad8cb1-5f1a-4d1b-83ff-c7132036d15c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-06-04T06:39:39+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Piazza XX Settembre</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 20.30</t>
+          <t xml:space="preserve"> ore 17.00</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
-      <c r="P43" t="inlineStr"/>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
+        </is>
+      </c>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>Cena solidale per i 20 anni di Modenamoremio</t>
+          <t>Un percorso ad arte: il mio giardino blu</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
@@ -4977,7 +4989,7 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -4999,7 +5011,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5009,67 +5021,63 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-06-03T15:42:40+00:00</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Commedia brillante</t>
+          <t xml:space="preserve">Il ricavato sarà devoluto allassociazione Porta Aperta </t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-06-03T15:43:48+00:00</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-16T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-16T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio/@@images/c0ad8cb1-5f1a-4d1b-83ff-c7132036d15c.jpeg</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-06-04T06:39:39+00:00</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> ore 20.30</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Cena solidale per i 20 anni di Modenamoremio</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
@@ -5082,7 +5090,7 @@
       </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
@@ -5104,7 +5112,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5114,79 +5122,71 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr"/>
+          <t>2022-03-19T09:15:00+00:00</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Commedia brillante</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-03-19T09:19:36+00:00</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-05-30T11:00:13+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>FMAV - Museo della Figurina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr">
-        <is>
-          <t>www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U45" t="inlineStr"/>
       <c r="V45" t="b">
         <v>0</v>
       </c>
@@ -5195,7 +5195,7 @@
       </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
@@ -5217,7 +5217,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5258,13 +5258,13 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
         </is>
       </c>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-05-30T11:06:40+00:00</t>
+          <t>2022-05-30T11:00:13+00:00</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
@@ -5274,13 +5274,13 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
         </is>
       </c>
       <c r="Q46" t="inlineStr"/>
@@ -5291,7 +5291,7 @@
       </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
+          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
@@ -5308,7 +5308,7 @@
       </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
@@ -5330,7 +5330,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5340,96 +5340,110 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-30T10:57:49+00:00</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr"/>
+          <t>2022-05-30T11:06:40+00:00</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>FMAV - Museo della Figurina</t>
+        </is>
+      </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr"/>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+        </is>
+      </c>
       <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr"/>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S47" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>www.fmav.org</t>
         </is>
       </c>
       <c r="V47" t="b">
         <v>0</v>
       </c>
-      <c r="W47" t="inlineStr"/>
+      <c r="W47" t="n">
+        <v>41123</v>
+      </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA47" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5439,54 +5453,50 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr"/>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
@@ -5495,42 +5505,44 @@
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr"/>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V48" t="b">
         <v>0</v>
       </c>
-      <c r="W48" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA48" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5540,67 +5552,63 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
@@ -5613,7 +5621,7 @@
       </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
@@ -5635,7 +5643,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5645,67 +5653,67 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr"/>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q50" t="inlineStr"/>
       <c r="R50" t="inlineStr"/>
       <c r="S50" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
@@ -5718,7 +5726,7 @@
       </c>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
@@ -5740,7 +5748,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5750,83 +5758,71 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-02-25T14:15:33+00:00</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-02-28T15:13:23+00:00</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
-      <c r="R51" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
-      <c r="U51" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U51" t="inlineStr"/>
       <c r="V51" t="b">
         <v>0</v>
       </c>
@@ -5835,7 +5831,7 @@
       </c>
       <c r="X51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y51" t="inlineStr">
@@ -5857,7 +5853,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5867,96 +5863,114 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr"/>
+          <t>2022-05-06T10:18:45+00:00</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+        </is>
+      </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr"/>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V52" t="b">
         <v>0</v>
       </c>
-      <c r="W52" t="inlineStr"/>
+      <c r="W52" t="n">
+        <v>41123</v>
+      </c>
       <c r="X52" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Concerti,Musica,Spettacoli</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5966,111 +5980,89 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>ingresso da Corso Cavour, 2</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:21+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>mundus@ater.emr.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2022-07-26T08:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2022-07-26T09:00:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>Grupo Compay Segundo</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>Giardini Ducali</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:24:06+00:00</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.30</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
-        </is>
-      </c>
+      <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>059 340221</t>
-        </is>
-      </c>
+      <c r="R53" t="inlineStr"/>
       <c r="S53" t="inlineStr">
         <is>
-          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr">
         <is>
-          <t>https://www.ater.emr.it/it</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V53" t="b">
         <v>0</v>
       </c>
-      <c r="W53" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W53" t="inlineStr"/>
       <c r="X53" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y53" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA53" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
@@ -6112,27 +6104,27 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2022-08-03T08:00:00+00:00</t>
+          <t>2022-07-26T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2022-08-03T09:00:00+00:00</t>
+          <t>2022-07-26T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Mauro Ottolini</t>
+          <t>Grupo Compay Segundo</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2022-06-01T09:48:07+00:00</t>
+          <t>2022-06-01T09:27:29+00:00</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
@@ -6159,7 +6151,7 @@
       </c>
       <c r="S54" t="inlineStr">
         <is>
-          <t>Nada màs fuerte</t>
+          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
         </is>
       </c>
       <c r="T54" t="inlineStr"/>
@@ -6176,7 +6168,7 @@
       </c>
       <c r="X54" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
@@ -6198,7 +6190,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -6208,96 +6200,118 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-06-01T09:27:21+00:00</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr"/>
+          <t>2022-06-01T09:27:29+00:00</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>mundus@ater.emr.it</t>
+        </is>
+      </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-08-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-08-03T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Mauro Ottolini</t>
+        </is>
+      </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr"/>
+          <t>2022-06-01T09:48:07+00:00</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>Giardini Ducali</t>
+        </is>
+      </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O55" t="inlineStr"/>
-      <c r="P55" t="inlineStr"/>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr"/>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>059 340221</t>
+        </is>
+      </c>
       <c r="S55" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Nada màs fuerte</t>
         </is>
       </c>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V55" t="b">
         <v>0</v>
       </c>
-      <c r="W55" t="inlineStr"/>
+      <c r="W55" t="n">
+        <v>41123</v>
+      </c>
       <c r="X55" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA55" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -6307,106 +6321,96 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:10+00:00</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr"/>
       <c r="N56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="inlineStr"/>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R56" t="inlineStr"/>
       <c r="S56" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V56" t="b">
         <v>0</v>
       </c>
-      <c r="W56" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W56" t="inlineStr"/>
       <c r="X56" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y56" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z56" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA56" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -6416,89 +6420,99 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O57" t="inlineStr"/>
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr"/>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S57" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V57" t="b">
         <v>0</v>
       </c>
-      <c r="W57" t="inlineStr"/>
+      <c r="W57" t="n">
+        <v>41123</v>
+      </c>
       <c r="X57" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y57" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z57" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA57" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -6536,23 +6550,23 @@
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M58" t="inlineStr"/>
@@ -6582,7 +6596,7 @@
       <c r="W58" t="inlineStr"/>
       <c r="X58" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y58" t="inlineStr">
@@ -6635,23 +6649,23 @@
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:27:35+00:00</t>
         </is>
       </c>
       <c r="M59" t="inlineStr"/>
@@ -6681,20 +6695,119 @@
       <c r="W59" t="inlineStr"/>
       <c r="X59" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z59" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA59" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="inlineStr"/>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T60" t="inlineStr"/>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V60" t="b">
+        <v>0</v>
+      </c>
+      <c r="W60" t="inlineStr"/>
+      <c r="X60" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y59" t="inlineStr">
+      <c r="Y60" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z59" t="inlineStr">
+      <c r="Z60" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA59" t="inlineStr">
+      <c r="AA60" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Mon Jun  6 08:17:22 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA51"/>
+  <dimension ref="A1:AA52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1478,7 +1478,7 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2022-03-15T11:11:12+00:00</t>
+          <t>2022-06-06T07:38:50+00:00</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 31 maggio e 1 giugno, 3 giugno e dal 7 al 10 giugno ore 20.30  2, 4, 5, 11 e 12 giugno ore 19.00</t>
+          <t xml:space="preserve"> 31 maggio e 1 giugno ore 20.30  repliche dal 2 al 12 giugno ore 21.15</t>
         </is>
       </c>
       <c r="O10" t="inlineStr"/>
@@ -2055,7 +2055,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2065,110 +2065,112 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Corso Vittorio Emanuele, 59</t>
+          <t>Viale Caduti in Guerra, 196</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2022-06-04T07:59:44+00:00</t>
+          <t>2020-09-17T12:45:54+00:00</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Presentazione del libro</t>
+          <t>A cura delle allieve attrici e degli allievi attori di ERT / Teatro Nazionale</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2022-06-04T07:59:52+00:00</t>
+          <t>2014-09-30T12:50:00+00:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>​info@accademiasla-mo.it</t>
+          <t>info@emiliaromagnateatro.com</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2022-06-08T07:00:00+00:00</t>
+          <t>2022-06-07T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2022-06-08T08:00:00+00:00</t>
+          <t>2022-06-11T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione/@@images/1a4df534-f8d8-4ac6-87d4-3d9176cd882c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/hereafter-episodi-teatrali/@@images/59c6e256-ecc2-48df-912f-b171b831bd83.jpeg</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2022-06-04T07:59:52+00:00</t>
+          <t>2022-06-06T07:48:28+00:00</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Accademia Nazionale di Scienze Lettere e Arti di Modena</t>
+          <t>Teatro Tempio</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.30</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
+        </is>
+      </c>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
         <is>
-          <t>059 225566</t>
+          <t>059/2163021</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>"Delitti in prima pagina. La giustizia nella società dell’informazione"</t>
+          <t>HEREAFTER. Episodi teatrali</t>
         </is>
       </c>
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr">
         <is>
-          <t>www.accademiasla-mo.it</t>
+          <t>http://www.emiliaromagnateatro.com</t>
         </is>
       </c>
       <c r="V16" t="b">
         <v>0</v>
       </c>
-      <c r="W16" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/hereafter-episodi-teatrali</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,64381951149482</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,93139345085676</t>
         </is>
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.93139345085676 44.64381951149482)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2178,67 +2180,79 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Strada Vaciglio Nord, 6</t>
+          <t>Corso Vittorio Emanuele, 59</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2022-06-04T08:30:34+00:00</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>2022-06-04T07:59:44+00:00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2022-06-04T08:30:59+00:00</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr"/>
+          <t>2022-06-04T07:59:52+00:00</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>​info@accademiasla-mo.it</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr">
         <is>
+          <t>2022-06-08T07:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
           <t>2022-06-08T08:00:00+00:00</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>2022-07-08T09:00:00+00:00</t>
-        </is>
-      </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo/@@images/04c6eef6-5450-4d2e-a11b-c353a7bdb6b0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione/@@images/1a4df534-f8d8-4ac6-87d4-3d9176cd882c.jpeg</t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2022-06-04T08:30:59+00:00</t>
+          <t>2022-06-04T07:59:52+00:00</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Sala Renata Bergonzoni della Casa delle Donne</t>
+          <t>Accademia Nazionale di Scienze Lettere e Arti di Modena</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Inaugurazione mercoledì 8 giugno ore 18.30  mostra aperta dal 10 giugno nei seguenti orari:  venerdì e sabato dalle 10 alle 13 (ad esclusione di venerdì 17 giugno) </t>
+          <t xml:space="preserve"> ore 15.30</t>
         </is>
       </c>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ingresso libero</t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>059 225566</t>
+        </is>
+      </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Oro rosso. Fragole, pomodori, molestie e sfruttamento nel Mediterraneo</t>
+          <t>"Delitti in prima pagina. La giustizia nella società dell’informazione"</t>
         </is>
       </c>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>www.accademiasla-mo.it</t>
+        </is>
+      </c>
       <c r="V17" t="b">
         <v>0</v>
       </c>
@@ -2247,7 +2261,7 @@
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
@@ -2269,7 +2283,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Altri eventi,Musica</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2279,63 +2293,63 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Strada Vaciglio Nord, 6</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:04+00:00</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
-        </is>
-      </c>
+          <t>2022-06-04T08:30:34+00:00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-06-04T08:30:59+00:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2022-05-12T09:00:00+00:00</t>
+          <t>2022-06-08T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2022-06-30T10:00:00+00:00</t>
+          <t>2022-07-08T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo/@@images/04c6eef6-5450-4d2e-a11b-c353a7bdb6b0.jpeg</t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-06-04T08:30:59+00:00</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Piazzetta Pomposa</t>
+          <t>Sala Renata Bergonzoni della Casa delle Donne</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
+          <t xml:space="preserve"> Inaugurazione mercoledì 8 giugno ore 18.30  mostra aperta dal 10 giugno nei seguenti orari:  venerdì e sabato dalle 10 alle 13 (ad esclusione di venerdì 17 giugno) </t>
         </is>
       </c>
       <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ingresso libero</t>
+        </is>
+      </c>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr">
         <is>
-          <t>Serate in Pomposa - 1° edizione</t>
+          <t>Oro rosso. Fragole, pomodori, molestie e sfruttamento nel Mediterraneo</t>
         </is>
       </c>
       <c r="T18" t="inlineStr"/>
@@ -2348,7 +2362,7 @@
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
@@ -2370,7 +2384,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi,Musica</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2380,90 +2394,76 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
+          <t>2022-05-20T10:02:04+00:00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-05-20T10:02:34+00:00</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-05-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-30T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazzetta Pomposa</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
         </is>
       </c>
       <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
-        </is>
-      </c>
+      <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Serate in Pomposa - 1° edizione</t>
         </is>
       </c>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>https://www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U19" t="inlineStr"/>
       <c r="V19" t="b">
         <v>0</v>
       </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W19" t="n">
+        <v>41123</v>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
@@ -2485,7 +2485,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2495,76 +2495,90 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
+          <t>2021-09-09T10:12:02+00:00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr"/>
+          <t>2021-09-09T10:12:26+00:00</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2022-05-26T07:16:41+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
         </is>
       </c>
       <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>059 2033166</t>
+        </is>
+      </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>https://www.fmav.org</t>
+        </is>
+      </c>
       <c r="V20" t="b">
         <v>0</v>
       </c>
-      <c r="W20" t="n">
-        <v>41123</v>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
@@ -2586,7 +2600,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2596,63 +2610,63 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Strada Vaciglio Nord, 6</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2022-06-04T08:30:34+00:00</t>
+          <t>2022-05-17T07:24:22+00:00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2022-06-04T08:30:59+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
+          <t>2022-06-10T07:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
           <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>2022-06-10T09:00:00+00:00</t>
-        </is>
-      </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie/@@images/9a9f2a19-02f6-4cd6-a272-5cac5ae7adbd.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2022-06-04T08:52:51+00:00</t>
+          <t>2022-05-26T07:16:41+00:00</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Sala Renata Bergonzoni della Casa delle Donne</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 18.30</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ingresso libero</t>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
         </is>
       </c>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr">
         <is>
-          <t>Da suddite a cittadine. Gabriella Degli Esposti e le partigiane modenesi nelle fonti documentarie e nelle memorie</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T21" t="inlineStr"/>
@@ -2665,7 +2679,7 @@
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
@@ -2687,7 +2701,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2697,67 +2711,63 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>centro storico</t>
+          <t>Strada Vaciglio Nord, 6</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2022-04-29T10:05:46+00:00</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
-        </is>
-      </c>
+          <t>2022-06-04T08:30:34+00:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-06-04T08:30:59+00:00</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2022-05-01T09:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2022-07-17T10:00:00+00:00</t>
+          <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie/@@images/9a9f2a19-02f6-4cd6-a272-5cac5ae7adbd.jpeg</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-06-04T08:52:51+00:00</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Piazza Torre</t>
+          <t>Sala Renata Bergonzoni della Casa delle Donne</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
+          <t xml:space="preserve"> ore 18.30</t>
         </is>
       </c>
       <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ingresso libero</t>
+        </is>
+      </c>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, aperture serali</t>
+          <t>Da suddite a cittadine. Gabriella Degli Esposti e le partigiane modenesi nelle fonti documentarie e nelle memorie</t>
         </is>
       </c>
       <c r="T22" t="inlineStr"/>
@@ -2770,7 +2780,7 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
@@ -2792,7 +2802,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Visite guidate,Altri eventi,Spettacoli</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2800,65 +2810,69 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>centro storico</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2022-05-30T09:56:40+00:00</t>
+          <t>2022-04-29T10:05:46+00:00</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
+          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2022-06-10T09:00:00+00:00</t>
+          <t>2022-05-01T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2022-06-10T10:00:00+00:00</t>
+          <t>2022-07-17T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Duomo di Modena</t>
+          <t>Piazza Torre</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 20.30</t>
+          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
         </is>
       </c>
       <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Gratuito</t>
-        </is>
-      </c>
+      <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr">
         <is>
-          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
+          <t>Torre Ghirlandina, aperture serali</t>
         </is>
       </c>
       <c r="T23" t="inlineStr"/>
@@ -2871,7 +2885,7 @@
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
@@ -2893,7 +2907,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Altri eventi</t>
+          <t>Visite guidate,Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2901,65 +2915,65 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>corso Canalgrande, 85</t>
-        </is>
-      </c>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
+          <t>2022-05-30T09:56:40+00:00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
+          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2022-06-10T11:00:00+00:00</t>
+          <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2022-06-10T12:00:00+00:00</t>
+          <t>2022-06-10T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
         </is>
       </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2022-05-30T11:42:41+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Duomo di Modena</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> dalle ore 20.30</t>
         </is>
       </c>
       <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gratuito</t>
+        </is>
+      </c>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr">
         <is>
-          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
+          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
         </is>
       </c>
       <c r="T24" t="inlineStr"/>
@@ -2972,7 +2986,7 @@
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
@@ -2994,7 +3008,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Concerti</t>
+          <t>Concerti,Spettacoli,Altri eventi</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3004,112 +3018,98 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Strada Pomposiana 292</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2022-05-30T09:03:14+00:00</t>
+          <t>2022-05-30T11:40:24+00:00</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:41:23+00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2022-06-10T19:00:00+00:00</t>
+          <t>2022-06-10T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2022-06-10T21:00:00+00:00</t>
+          <t>2022-06-10T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
         </is>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2022-05-30T11:42:41+00:00</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Fattoria Centofiori</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ore 21.00</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
-        </is>
-      </c>
+      <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>Whatsapp 3293357131</t>
-        </is>
-      </c>
+      <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>Marco Ferri Quartet</t>
+          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>www.fattoriacentofiori.it</t>
-        </is>
-      </c>
+      <c r="U25" t="inlineStr"/>
       <c r="V25" t="b">
         <v>0</v>
       </c>
-      <c r="W25" t="inlineStr">
-        <is>
-          <t>41123</t>
-        </is>
+      <c r="W25" t="n">
+        <v>41123</v>
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>44,63693000592147</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>10,81076003183179</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>POINT (10.81076003183179 44.63693000592147)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Concerti</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3119,98 +3119,112 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>Strada Pomposiana 292</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
+          <t>2022-05-30T09:03:14+00:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-06-10T19:00:00+00:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-06-10T21:00:00+00:00</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2022-05-26T07:20:15+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Fattoria Centofiori</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> Ore 21.00</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
         </is>
       </c>
       <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr"/>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Whatsapp 3293357131</t>
+        </is>
+      </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Marco Ferri Quartet</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr"/>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>www.fattoriacentofiori.it</t>
+        </is>
+      </c>
       <c r="V26" t="b">
         <v>0</v>
       </c>
-      <c r="W26" t="n">
-        <v>41123</v>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>41123</t>
+        </is>
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,63693000592147</t>
         </is>
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,81076003183179</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.81076003183179 44.63693000592147)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3220,79 +3234,67 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Largo Porta Sant’Agostino, 228</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2022-06-04T09:45:49+00:00</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>mostra fotografica di Francesco Jodice</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:24:22+00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2022-06-04T09:46:06+00:00</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>info@agomodena.it</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:25:56+00:00</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2022-06-11T09:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2022-08-28T10:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/ritratti-di-classe/@@images/3dba106b-6f95-4190-991d-b13abf85501a.jpeg</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>Ritratti di classe</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-06-04T09:47:46+00:00</t>
+          <t>2022-05-26T07:20:15+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>AGO Modena Fabbriche culturali</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> vedi sul sito dell'evento</t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Ritratti di Classe</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>www.agomodena.it</t>
-        </is>
-      </c>
+      <c r="U27" t="inlineStr"/>
       <c r="V27" t="b">
         <v>0</v>
       </c>
@@ -3301,7 +3303,7 @@
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/ritratti-di-classe</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3323,7 +3325,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3333,50 +3335,62 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Largo Porta Sant’Agostino, 228</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr"/>
+          <t>2022-06-04T09:45:49+00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>mostra fotografica di Francesco Jodice</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr"/>
+          <t>2022-06-04T09:46:06+00:00</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>info@agomodena.it</t>
+        </is>
+      </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-06-11T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-08-28T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/ritratti-di-classe/@@images/3dba106b-6f95-4190-991d-b13abf85501a.jpeg</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Ritratti di classe</t>
+        </is>
+      </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-06-04T09:47:46+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>AGO Modena Fabbriche culturali</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> vedi sul sito dell'evento</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
@@ -3385,11 +3399,15 @@
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Ritratti di Classe</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr"/>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>www.agomodena.it</t>
+        </is>
+      </c>
       <c r="V28" t="b">
         <v>0</v>
       </c>
@@ -3398,7 +3416,7 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/ritratti-di-classe</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3420,7 +3438,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3430,50 +3448,50 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr"/>
+          <t>2022-05-21T10:36:00+00:00</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Piazza Matteotti</t>
+        </is>
+      </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
@@ -3482,44 +3500,42 @@
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.it/</t>
-        </is>
-      </c>
+      <c r="U29" t="inlineStr"/>
       <c r="V29" t="b">
         <v>0</v>
       </c>
-      <c r="W29" t="inlineStr"/>
+      <c r="W29" t="n">
+        <v>41123</v>
+      </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3529,54 +3545,50 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>via S.Pietro, 1</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:38+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Presentazione del libro</t>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-06-12T09:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-06-12T10:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>Chiostro di San Pietro</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.00</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
@@ -3585,42 +3597,44 @@
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Contro la guerra</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V30" t="b">
         <v>0</v>
       </c>
-      <c r="W30" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W30" t="inlineStr"/>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3630,75 +3644,67 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>via S.Pietro, 1</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
+          <t>2022-05-30T10:02:38+00:00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-12T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>logo del mercatino</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-02-08T10:09:23+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Polisportiva Madonnina</t>
+          <t>Chiostro di San Pietro</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9 alle 13</t>
+          <t xml:space="preserve"> ore 15.00</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>340 2607164 Luisa</t>
-        </is>
-      </c>
+      <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Mercatino della Polisportiva Madonnina</t>
+          <t>Contro la guerra</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
-        </is>
-      </c>
+      <c r="U31" t="inlineStr"/>
       <c r="V31" t="b">
         <v>0</v>
       </c>
@@ -3707,7 +3713,7 @@
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
@@ -3729,108 +3735,94 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Montale Rangone</t>
+          <t>Modena</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2021-04-26T15:03:43+00:00</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
-        </is>
-      </c>
+          <t>2021-08-06T11:34:26+00:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2021-04-26T15:06:06+00:00</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>museo@parcomontale.it</t>
-        </is>
-      </c>
+          <t>2021-08-06T11:36:33+00:00</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-04-03T14:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-06-19T15:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>logo del mercatino</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2022-03-28T14:43:35+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
-        </is>
-      </c>
+      <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr">
         <is>
-          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+          <t>340 2607164 Luisa</t>
         </is>
       </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>Parco archeologico della Terramara di Montale</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr">
         <is>
-          <t>http://www.parcomontale.it/it</t>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
         </is>
       </c>
       <c r="V32" t="b">
         <v>0</v>
       </c>
-      <c r="W32" t="inlineStr">
-        <is>
-          <t>41050</t>
-        </is>
+      <c r="W32" t="n">
+        <v>41123</v>
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
@@ -3852,82 +3844,108 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Modena</t>
+          <t>Montale Rangone</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:13+00:00</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
+          <t>2021-04-26T15:03:43+00:00</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr"/>
+          <t>2021-04-26T15:06:06+00:00</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>museo@parcomontale.it</t>
+        </is>
+      </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2022-06-16T09:00:00+00:00</t>
+          <t>2022-04-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2022-06-16T10:00:00+00:00</t>
+          <t>2022-06-19T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Parco archeologico della Terramara di Montale</t>
+        </is>
+      </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2022-05-06T09:12:25+00:00</t>
+          <t>2022-03-28T14:43:35+00:00</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Piazza Roma</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
+          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
         </is>
       </c>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
+        </is>
+      </c>
       <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+        </is>
+      </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>Rosse e non solo di sera</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr"/>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>http://www.parcomontale.it/it</t>
+        </is>
+      </c>
       <c r="V33" t="b">
         <v>0</v>
       </c>
-      <c r="W33" t="n">
-        <v>41123</v>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>41050</t>
+        </is>
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
@@ -3949,7 +3967,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Iniziative per bambini</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3959,67 +3977,59 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ingresso da corso Cavour, 2</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:00+00:00</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Laboratorio per bambini 6-10 anni</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2022-06-16T11:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2022-06-16T12:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2022-05-30T11:14:22+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 17.00</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
-        </is>
-      </c>
+      <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>Un percorso ad arte: il mio giardino blu</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
@@ -4032,7 +4042,7 @@
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
@@ -4054,7 +4064,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4064,63 +4074,67 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ingresso da corso Cavour, 2</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2022-06-03T15:42:40+00:00</t>
+          <t>2022-05-30T11:14:00+00:00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Il ricavato sarà devoluto allassociazione Porta Aperta </t>
+          <t>Laboratorio per bambini 6-10 anni</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2022-06-03T15:43:48+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2022-06-16T15:00:00+00:00</t>
+          <t>2022-06-16T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2022-06-16T16:00:00+00:00</t>
+          <t>2022-06-16T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio/@@images/c0ad8cb1-5f1a-4d1b-83ff-c7132036d15c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu/@@images/5f9e3da7-9a4f-4468-82bb-e27c6d07e19c.jpeg</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2022-06-04T06:39:39+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>Piazza XX Settembre</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 20.30</t>
+          <t xml:space="preserve"> ore 17.00</t>
         </is>
       </c>
       <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr"/>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso gratuito, prenotazione obbligatoria tramite form online.Iscrizioni valide fino a martedì 14 giugno </t>
+        </is>
+      </c>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Cena solidale per i 20 anni di Modenamoremio</t>
+          <t>Un percorso ad arte: il mio giardino blu</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
@@ -4133,7 +4147,7 @@
       </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/un-percorso-ad-arte-il-mio-giardino-blu</t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
@@ -4155,7 +4169,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4165,67 +4179,63 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-06-03T15:42:40+00:00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Commedia brillante</t>
+          <t xml:space="preserve">Il ricavato sarà devoluto allassociazione Porta Aperta </t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-06-03T15:43:48+00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2022-06-17T08:00:00+00:00</t>
+          <t>2022-06-16T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-16T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio/@@images/c0ad8cb1-5f1a-4d1b-83ff-c7132036d15c.jpeg</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2022-03-19T09:32:45+00:00</t>
+          <t>2022-06-04T06:39:39+00:00</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
+          <t xml:space="preserve"> ore 20.30</t>
         </is>
       </c>
       <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>Il Penitenziere</t>
+          <t>Cena solidale per i 20 anni di Modenamoremio</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
@@ -4238,7 +4248,7 @@
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/cena-solidale-per-i-20-anni-di-modenamoremio</t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
@@ -4260,7 +4270,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4270,79 +4280,71 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 103</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:49+00:00</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr"/>
+          <t>2022-03-19T09:15:00+00:00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Commedia brillante</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2022-05-30T10:57:57+00:00</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-03-19T09:19:36+00:00</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2022-06-18T10:00:00+00:00</t>
+          <t>2022-06-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/il-penitenziere/@@images/0f3e995d-acc4-4d2c-b85c-a01d54e19020.jpeg</t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2022-05-30T11:00:13+00:00</t>
+          <t>2022-03-19T09:32:45+00:00</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>FMAV - Museo della Figurina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
+          <t xml:space="preserve"> Venerdì 17 e Sabato 18 giugno ore 21 - Domenica 19 giugno ore 17 </t>
         </is>
       </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>059 203 2919</t>
-        </is>
-      </c>
+      <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
+          <t>Il Penitenziere</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U37" t="inlineStr"/>
       <c r="V37" t="b">
         <v>0</v>
       </c>
@@ -4351,7 +4353,7 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/il-penitenziere</t>
         </is>
       </c>
       <c r="Y37" t="inlineStr">
@@ -4373,7 +4375,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4414,13 +4416,13 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/8928faa9-26c8-48f5-92df-c9765d7f6f2c.jpeg</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2022-05-30T11:06:40+00:00</t>
+          <t>2022-05-30T11:00:13+00:00</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
@@ -4430,13 +4432,13 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica ore 15-19</t>
         </is>
       </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+          <t xml:space="preserve"> biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
         </is>
       </c>
       <c r="Q38" t="inlineStr"/>
@@ -4447,7 +4449,7 @@
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
+          <t>Non ci prendono più. 40 anni dal Mundial '82</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
@@ -4464,7 +4466,7 @@
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
@@ -4486,7 +4488,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -4496,96 +4498,110 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>corso Canalgrande, 103</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-05-30T10:57:49+00:00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr"/>
+          <t>2022-05-30T10:57:57+00:00</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>biglietteria@fmav.org</t>
+        </is>
+      </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2022-06-18T22:00:00+00:00</t>
+          <t>2022-06-18T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2022-06-19T21:55:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82/@@images/9166f15e-06ad-4213-9a4c-965fc62bc41f.jpeg</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2022-05-10T08:23:02+00:00</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr"/>
+          <t>2022-05-30T11:06:40+00:00</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>FMAV - Museo della Figurina</t>
+        </is>
+      </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ogni sabato alle ore 16 (eccetto i sabati del mese di agosto)</t>
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> La visita è inclusa nel costo del biglietto di ingresso alla mostra: biglietto intero 6 € / ridotto 4 € (Circuito Vivaticket)   Biglietto  cumulativo: Non ci prendono più + Never ending stories: 8 €   ingresso libero ogni mercoledì  </t>
+        </is>
+      </c>
       <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="inlineStr"/>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>059 203 2919</t>
+        </is>
+      </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Visite guidate alla mostra "Non ci prendono più. 40 anni dal Mundial '82"</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>www.fmav.org</t>
         </is>
       </c>
       <c r="V39" t="b">
         <v>0</v>
       </c>
-      <c r="W39" t="inlineStr"/>
+      <c r="W39" t="n">
+        <v>41123</v>
+      </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/visite-guidate-alla-mostra-non-ci-prendono-piu-40-anni-dal-mundial-82</t>
         </is>
       </c>
       <c r="Y39" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA39" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Visite guidate,Iniziative per bambini</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4595,54 +4611,50 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Via Canaletto Sud, 17/A</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-03-31T08:53:45+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2022-03-31T08:55:39+00:00</t>
+          <t>2010-11-03T10:00:00+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2022-06-19T08:00:00+00:00</t>
+          <t>2022-06-18T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2022-06-19T09:00:00+00:00</t>
+          <t>2022-06-19T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti/@@images/856dda7b-b783-4f0a-b0a3-a4e50c9ea91b.jpeg</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr">
         <is>
-          <t>2022-03-31T08:57:09+00:00</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:23:02+00:00</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O40" t="inlineStr"/>
@@ -4651,42 +4663,44 @@
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Quale percussione? - Museolaboratorio</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr"/>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
       <c r="V40" t="b">
         <v>0</v>
       </c>
-      <c r="W40" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W40" t="inlineStr"/>
       <c r="X40" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy15_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y40" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA40" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Visite guidate,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4696,67 +4710,63 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Piazza della Cittadella, 11</t>
+          <t>Via Canaletto Sud, 17/A</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-03-19T09:15:00+00:00</t>
+          <t>2022-03-31T08:53:45+00:00</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Spettacolo teatrale</t>
+          <t>Visita guidata al museolaboratorio per adulti e bambini dai 3 anni in su</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2022-03-19T09:19:36+00:00</t>
+          <t>2022-03-31T08:55:39+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2022-06-25T08:00:00+00:00</t>
+          <t>2022-06-19T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2022-06-25T09:00:00+00:00</t>
+          <t>2022-06-19T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio/@@images/d596fabd-4e8d-410e-b649-5ff01fc72d71.jpeg</t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2022-03-19T09:28:51+00:00</t>
+          <t>2022-03-31T08:57:09+00:00</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Teatro Cittadella</t>
+          <t>Museolaboratorio Quale percussione? presso Condominio ErreNord</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21</t>
+          <t xml:space="preserve"> La visita si svolge nei seguenti orari a scelta: dalle 15 alle 16.30 oppure dalle 17 alle 18.30  </t>
         </is>
       </c>
       <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
-        </is>
-      </c>
+      <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>L'uomo dal fiore in bocca</t>
+          <t>Quale percussione? - Museolaboratorio</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
@@ -4769,7 +4779,7 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_quale-percussione-museolaboratorio</t>
         </is>
       </c>
       <c r="Y41" t="inlineStr">
@@ -4791,7 +4801,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4801,67 +4811,67 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
+          <t>Piazza della Cittadella, 11</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:15+00:00</t>
+          <t>2022-03-19T09:15:00+00:00</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, visite guidate a tema</t>
+          <t>Spettacolo teatrale</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2022-02-25T14:15:33+00:00</t>
+          <t>2022-03-19T09:19:36+00:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2022-06-25T13:00:00+00:00</t>
+          <t>2022-06-25T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2022-06-25T14:00:00+00:00</t>
+          <t>2022-06-25T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/luomo-dal-fiore-in-bocca/@@images/45e6dab9-6388-4246-9a70-62f43619a8ea.jpeg</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2022-02-28T15:13:23+00:00</t>
+          <t>2022-03-19T09:28:51+00:00</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina</t>
+          <t>Teatro Cittadella</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> ore 21</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr"/>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ingresso unico € 10,00 Prenotazioni al 338.2434005 oppure e-mail a: compagnia.andreaferrari@gmail.com</t>
+        </is>
+      </c>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>La pendenza della Ghirlandina tra passato e presente</t>
+          <t>L'uomo dal fiore in bocca</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
@@ -4874,7 +4884,7 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/luomo-dal-fiore-in-bocca</t>
         </is>
       </c>
       <c r="Y42" t="inlineStr">
@@ -4896,7 +4906,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4906,83 +4916,71 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>ritrovo presso la biglietteria della Torre, piazza Torre</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2021-06-10T16:47:55+00:00</t>
+          <t>2022-02-25T14:15:15+00:00</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manifestazione di antiquariato </t>
+          <t>Torre Ghirlandina, visite guidate a tema</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2021-06-10T16:48:45+00:00</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>anticoinpiazzagrande@gmail.com</t>
-        </is>
-      </c>
+          <t>2022-02-25T14:15:33+00:00</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2022-06-25T16:00:00+00:00</t>
+          <t>2022-06-25T13:00:00+00:00</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2022-06-26T17:00:00+00:00</t>
+          <t>2022-06-25T14:00:00+00:00</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente/@@images/146dc964-6d6d-40d4-9297-562ff9a981d1.jpeg</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2022-05-06T10:18:45+00:00</t>
+          <t>2022-02-28T15:13:23+00:00</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+          <t>Torre Ghirlandina</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
+          <t xml:space="preserve"> ore 19.00</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>340 6059686 oppure 338 2098995</t>
-        </is>
-      </c>
+      <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>L'antico in Piazza Grande</t>
+          <t>La pendenza della Ghirlandina tra passato e presente</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>https://www.anticoinpiazzagrande.com/</t>
-        </is>
-      </c>
+      <c r="U43" t="inlineStr"/>
       <c r="V43" t="b">
         <v>0</v>
       </c>
@@ -4991,7 +4989,7 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/la-pendenza-della-ghirlandina-tra-passato-e-presente</t>
         </is>
       </c>
       <c r="Y43" t="inlineStr">
@@ -5013,7 +5011,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5023,96 +5021,114 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2021-06-10T16:47:55+00:00</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Manifestazione di antiquariato </t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr"/>
+          <t>2021-06-10T16:48:45+00:00</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>anticoinpiazzagrande@gmail.com</t>
+        </is>
+      </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2022-07-16T22:00:00+00:00</t>
+          <t>2022-06-25T16:00:00+00:00</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2022-07-17T21:55:00+00:00</t>
+          <t>2022-06-26T17:00:00+00:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy9_of_lantico-in-piazza-grande/@@images/8020db9a-8111-42d3-8b00-6e0ed882ce5e.jpeg</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Immagine presa dal sito della manifestazione L'antico in Piazza Grande</t>
+        </is>
+      </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2022-05-10T08:24:06+00:00</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr"/>
+          <t>2022-05-06T10:18:45+00:00</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>Piazza Grande, Corso Duomo, Piazza Torre, Piazza XX Settembre</t>
+        </is>
+      </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> dalle ore 9.00 alle 19.00</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr"/>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>340 6059686 oppure 338 2098995</t>
+        </is>
+      </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>L'antico in Piazza Grande</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.anticoinpiazzagrande.com/</t>
         </is>
       </c>
       <c r="V44" t="b">
         <v>0</v>
       </c>
-      <c r="W44" t="inlineStr"/>
+      <c r="W44" t="n">
+        <v>41123</v>
+      </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy9_of_lantico-in-piazza-grande</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA44" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Concerti,Musica,Spettacoli</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5122,111 +5138,89 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ingresso da Corso Cavour, 2</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:21+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>mundus@ater.emr.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2022-07-26T08:00:00+00:00</t>
+          <t>2022-07-16T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2022-07-26T09:00:00+00:00</t>
+          <t>2022-07-17T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>Grupo Compay Segundo</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti/@@images/4c8dcfd3-0d26-4d2d-b808-8ca772fa748f.jpeg</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2022-06-01T09:27:29+00:00</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>Giardini Ducali</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:24:06+00:00</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.30</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
-      <c r="P45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
-        </is>
-      </c>
+      <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>059 340221</t>
-        </is>
-      </c>
+      <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr">
         <is>
-          <t>https://www.ater.emr.it/it</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V45" t="b">
         <v>0</v>
       </c>
-      <c r="W45" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W45" t="inlineStr"/>
       <c r="X45" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy16_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y45" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA45" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
@@ -5268,27 +5262,27 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2022-08-03T08:00:00+00:00</t>
+          <t>2022-07-26T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2022-08-03T09:00:00+00:00</t>
+          <t>2022-07-26T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club/@@images/158b60cb-2165-4b16-b232-9ca9b7768911.jpeg</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Mauro Ottolini</t>
+          <t>Grupo Compay Segundo</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>2022-06-01T09:48:07+00:00</t>
+          <t>2022-06-01T09:27:29+00:00</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
@@ -5315,7 +5309,7 @@
       </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>Nada màs fuerte</t>
+          <t>Grupo Compay Segundo de Buena Vista Social Club</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
@@ -5332,7 +5326,7 @@
       </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/grupo-compay-segundo-de-buena-vista-social-club</t>
         </is>
       </c>
       <c r="Y46" t="inlineStr">
@@ -5354,7 +5348,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Concerti,Musica,Spettacoli</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5364,96 +5358,118 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>ingresso da Corso Cavour, 2</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
+          <t>2022-06-01T09:27:21+00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+          <t xml:space="preserve">Concerto della rassegna "Festival Mundus" </t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr"/>
+          <t>2022-06-01T09:27:29+00:00</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>mundus@ater.emr.it</t>
+        </is>
+      </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2022-08-20T22:00:00+00:00</t>
+          <t>2022-08-03T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2022-08-21T21:55:00+00:00</t>
+          <t>2022-08-03T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nada-mas-fuerte/@@images/16dac61f-5ac6-4e42-b262-f9b2fceced5f.jpeg</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Mauro Ottolini</t>
+        </is>
+      </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:10+00:00</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr"/>
+          <t>2022-06-01T09:48:07+00:00</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Giardini Ducali</t>
+        </is>
+      </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 21.30</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr"/>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> biglietto € 10 -  I biglietti sono in vendita online su www.vivaticket.com </t>
+        </is>
+      </c>
       <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr"/>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>059 340221</t>
+        </is>
+      </c>
       <c r="S47" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Nada màs fuerte</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.ater.emr.it/it</t>
         </is>
       </c>
       <c r="V47" t="b">
         <v>0</v>
       </c>
-      <c r="W47" t="inlineStr"/>
+      <c r="W47" t="n">
+        <v>41123</v>
+      </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nada-mas-fuerte</t>
         </is>
       </c>
       <c r="Y47" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA47" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5463,106 +5479,96 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Via Sant'Eufemia e Via Carteria</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2022-04-07T09:03:31+00:00</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr"/>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2022-04-07T09:06:38+00:00</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>traborghiecontrade@libero.it</t>
-        </is>
-      </c>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2022-09-17T08:00:00+00:00</t>
+          <t>2022-08-20T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2022-09-18T09:00:00+00:00</t>
+          <t>2022-08-21T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti/@@images/0dc1bec3-7921-4d86-90bb-66d72dad6173.jpeg</t>
         </is>
       </c>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2022-04-07T09:10:43+00:00</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
-        </is>
-      </c>
+          <t>2022-05-10T08:26:10+00:00</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr"/>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 9.00-19.00</t>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>333/9103351</t>
-        </is>
-      </c>
+      <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
+          <t>Mercato straordinario degli ambulanti</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
       <c r="U48" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/TraBorghieContrade</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V48" t="b">
         <v>0</v>
       </c>
-      <c r="W48" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy17_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA48" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Fiere, Esposizioni e Mostre Mercato,Mercati</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5572,89 +5578,99 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Via Sant'Eufemia e Via Carteria</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:03:31+00:00</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2010-11-03T10:00:00+00:00</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr"/>
+          <t>2022-04-07T09:06:38+00:00</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>traborghiecontrade@libero.it</t>
+        </is>
+      </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2022-09-17T22:00:00+00:00</t>
+          <t>2022-09-17T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2022-09-18T21:55:00+00:00</t>
+          <t>2022-09-18T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade/@@images/2a3356d9-21c8-424c-b3e6-b8a8a93a1725.jpeg</t>
         </is>
       </c>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2022-05-10T08:26:55+00:00</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr"/>
+          <t>2022-04-07T09:10:43+00:00</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>Centro storico - Borgo Sant'Eufemia e Contrada Carteria</t>
+        </is>
+      </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+          <t xml:space="preserve"> ore 9.00-19.00</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
-      <c r="R49" t="inlineStr"/>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>333/9103351</t>
+        </is>
+      </c>
       <c r="S49" t="inlineStr">
         <is>
-          <t>Mercato straordinario degli ambulanti</t>
+          <t>Mercatino artigianato artistico "Tra borghi e contrade"</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>https://www.facebook.com/TraBorghieContrade</t>
         </is>
       </c>
       <c r="V49" t="b">
         <v>0</v>
       </c>
-      <c r="W49" t="inlineStr"/>
+      <c r="W49" t="n">
+        <v>41123</v>
+      </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy2_of_mercatino-artigianato-artistico-tra-borghi-e-contrade</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
@@ -5692,23 +5708,23 @@
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2022-10-15T22:00:00+00:00</t>
+          <t>2022-09-17T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2022-10-16T21:55:00+00:00</t>
+          <t>2022-09-18T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti/@@images/45738906-5f84-43cd-9f29-05f592db26cc.jpeg</t>
         </is>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr">
         <is>
-          <t>2022-05-10T08:27:35+00:00</t>
+          <t>2022-05-10T08:26:55+00:00</t>
         </is>
       </c>
       <c r="M50" t="inlineStr"/>
@@ -5738,7 +5754,7 @@
       <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy18_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
@@ -5791,23 +5807,23 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2022-11-19T23:00:00+00:00</t>
+          <t>2022-10-15T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2022-11-20T22:55:00+00:00</t>
+          <t>2022-10-16T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti/@@images/3d77bfdf-b2a2-4126-b1e5-4ed073129898.jpeg</t>
         </is>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2022-05-10T08:28:15+00:00</t>
+          <t>2022-05-10T08:27:35+00:00</t>
         </is>
       </c>
       <c r="M51" t="inlineStr"/>
@@ -5837,20 +5853,119 @@
       <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr">
         <is>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy19_of_mercato-straordinario-degli-ambulanti</t>
+        </is>
+      </c>
+      <c r="Y51" t="inlineStr">
+        <is>
+          <t>44,65137034620577</t>
+        </is>
+      </c>
+      <c r="Z51" t="inlineStr">
+        <is>
+          <t>10,921029194828652</t>
+        </is>
+      </c>
+      <c r="AA51" t="inlineStr">
+        <is>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Mercati</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Modena</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2019-12-10T09:34:45+00:00</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Bancarelle di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2010-11-03T10:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2022-11-19T23:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>2022-11-20T22:55:00+00:00</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti/@@images/585b45ab-f03a-4650-91cb-e9f754e22d94.jpeg</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>2022-05-10T08:28:15+00:00</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> dalle ore 8.00 alle 14.00</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>Mercato straordinario degli ambulanti</t>
+        </is>
+      </c>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>http://www.consorzioilmercato.it/</t>
+        </is>
+      </c>
+      <c r="V52" t="b">
+        <v>0</v>
+      </c>
+      <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr">
+        <is>
           <t>https://www.comune.modena.it/novita/eventi/2022/copy20_of_mercato-straordinario-degli-ambulanti</t>
         </is>
       </c>
-      <c r="Y51" t="inlineStr">
+      <c r="Y52" t="inlineStr">
         <is>
           <t>44,65137034620577</t>
         </is>
       </c>
-      <c r="Z51" t="inlineStr">
+      <c r="Z52" t="inlineStr">
         <is>
           <t>10,921029194828652</t>
         </is>
       </c>
-      <c r="AA51" t="inlineStr">
+      <c r="AA52" t="inlineStr">
         <is>
           <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>

</xml_diff>

<commit_message>
Latest data: Tue Jun  7 01:08:59 UTC 2022
</commit_message>
<xml_diff>
--- a/docs/eventi/eventi_modena.xlsx
+++ b/docs/eventi/eventi_modena.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA52"/>
+  <dimension ref="A1:AA49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1542,7 +1542,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Concerti,Musica</t>
+          <t>Altri eventi,Spettacoli,Musica,Libri</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1552,90 +1552,76 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>viale Monte Kosica, amgolo viale Molza</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2021-06-24T13:52:45+00:00</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
+          <t>2022-06-03T15:42:40+00:00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Rassegna di eventi culturali in Piazza XX Settembre</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2021-06-24T13:52:57+00:00</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>latenda@comune.modena.it</t>
-        </is>
-      </c>
+          <t>2022-06-03T15:43:48+00:00</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2022-06-06T07:00:00+00:00</t>
+          <t>2022-06-07T15:00:00+00:00</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2022-06-06T14:00:00+00:00</t>
+          <t>2022-06-28T16:00:00+00:00</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/a-la-tenda-il-rock-dei-delta/@@images/e89ce1ee-1337-48c0-8eeb-d60c0b9187d9.jpeg</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Delta Sleep</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/note-di-stelle/@@images/78120e75-8036-4a4c-b46e-10cc1ff7fe4c.jpeg</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2022-06-04T09:03:06+00:00</t>
+          <t>2022-06-04T06:35:10+00:00</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>La Tenda</t>
+          <t>Piazza XX Settembre</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> 7, 14, 21 e 28 giugno alle ore 19 presentazione di libri  alle ore 21 spettacoli</t>
         </is>
       </c>
       <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
+      <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr">
         <is>
-          <t>A La Tenda, il rock dei Delta</t>
+          <t>Note di Stelle</t>
         </is>
       </c>
       <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/latenda</t>
-        </is>
-      </c>
+      <c r="U11" t="inlineStr"/>
       <c r="V11" t="b">
         <v>0</v>
       </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W11" t="n">
+        <v>41123</v>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/a-la-tenda-il-rock-dei-delta</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/note-di-stelle</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
@@ -1657,7 +1643,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Altri eventi</t>
+          <t>Spettacoli,Teatro</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1665,88 +1651,114 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Viale Caduti in Guerra, 196</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2022-05-26T09:12:46+00:00</t>
+          <t>2020-09-17T12:45:54+00:00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Giovedì 2 giugno, celebrazioni con alzabandiera e sfilata della banda cittadina. Iniziative in programma già dal 30 maggio</t>
+          <t>A cura delle allieve attrici e degli allievi attori di ERT / Teatro Nazionale</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2022-05-30T09:29:45+00:00</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr"/>
+          <t>2014-09-30T12:50:00+00:00</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>info@emiliaromagnateatro.com</t>
+        </is>
+      </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2022-05-30T09:00:00+00:00</t>
+          <t>2022-06-07T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2022-06-02T10:00:00+00:00</t>
+          <t>2022-06-11T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/festa-della-repubblica/@@images/0031a2b2-623b-4b21-8316-cfd065155db6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/hereafter-episodi-teatrali/@@images/59c6e256-ecc2-48df-912f-b171b831bd83.jpeg</t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2022-05-30T09:29:45+00:00</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
+          <t>2022-06-06T07:48:28+00:00</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Teatro Tempio</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ore 19.00</t>
+        </is>
+      </c>
       <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
+        </is>
+      </c>
       <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>059/2163021</t>
+        </is>
+      </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>Festa della Repubblica</t>
+          <t>HEREAFTER. Episodi teatrali</t>
         </is>
       </c>
       <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>http://www.emiliaromagnateatro.com</t>
+        </is>
+      </c>
       <c r="V12" t="b">
         <v>0</v>
       </c>
-      <c r="W12" t="n">
-        <v>41123</v>
-      </c>
+      <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/festa-della-repubblica</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/hereafter-episodi-teatrali</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,64381951149482</t>
         </is>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,93139345085676</t>
         </is>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.93139345085676 44.64381951149482)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Musica</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1756,71 +1768,79 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 85</t>
+          <t>Corso Vittorio Emanuele, 59</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+          <t>2022-06-04T07:59:44+00:00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
+          <t>2022-06-04T07:59:52+00:00</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>​info@accademiasla-mo.it</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2022-06-06T11:00:00+00:00</t>
+          <t>2022-06-08T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2022-06-06T12:00:00+00:00</t>
+          <t>2022-06-08T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/concerto-inaugurale-della-nuova-filarmonica-del-teatro-comunale/@@images/bd0aa52a-489c-4715-b957-8a4551ed5f95.jpeg</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Dmitry Masleev</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione/@@images/1a4df534-f8d8-4ac6-87d4-3d9176cd882c.jpeg</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2022-06-01T12:46:07+00:00</t>
+          <t>2022-06-04T07:59:52+00:00</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Accademia Nazionale di Scienze Lettere e Arti di Modena</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> ore 15.30</t>
         </is>
       </c>
       <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ingressio con biglietto gratuito. I biglietti sono disponibili presso la biglietteria del Teatro o telefonando allo 059  2033010</t>
-        </is>
-      </c>
+      <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>059 225566</t>
+        </is>
+      </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>Concerto inaugurale della nuova Filarmonica del Teatro comunale</t>
+          <t>"Delitti in prima pagina. La giustizia nella società dell’informazione"</t>
         </is>
       </c>
       <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>www.accademiasla-mo.it</t>
+        </is>
+      </c>
       <c r="V13" t="b">
         <v>0</v>
       </c>
@@ -1829,7 +1849,7 @@
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/concerto-inaugurale-della-nuova-filarmonica-del-teatro-comunale</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
@@ -1851,7 +1871,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Altri eventi,Mercati</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1861,78 +1881,76 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Ingresso da viale Berengario</t>
+          <t>Strada Vaciglio Nord, 6</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2020-12-29T15:02:32+00:00</t>
+          <t>2022-06-04T08:30:34+00:00</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2020-12-29T15:05:00+00:00</t>
+          <t>2022-06-04T08:30:59+00:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2022-01-03T14:00:00+00:00</t>
+          <t>2022-06-08T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2022-12-26T14:59:00+00:00</t>
+          <t>2022-07-08T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo/@@images/04c6eef6-5450-4d2e-a11b-c353a7bdb6b0.jpeg</t>
         </is>
       </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2021-12-28T10:39:07+00:00</t>
+          <t>2022-06-06T10:06:47+00:00</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Parco Novi Sad</t>
+          <t>Sala Renata Bergonzoni della Casa delle Donne</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
+          <t xml:space="preserve"> Inaugurazione mercoledì 8 giugno ore 18.30  mostra aperta dal 10 giugno nei seguenti orari:  venerdì e sabato dalle 10 alle 13 (ad esclusione di venerdì 17 giugno) </t>
         </is>
       </c>
       <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ingresso libero</t>
+        </is>
+      </c>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr">
         <is>
-          <t>Mercato settimanale del lunedì</t>
+          <t>Oro rosso. Fragole, pomodori, molestie e sfruttamento nel Mediterraneo</t>
         </is>
       </c>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>http://www.consorzioilmercato.com/</t>
-        </is>
-      </c>
+      <c r="U14" t="inlineStr"/>
       <c r="V14" t="b">
         <v>0</v>
       </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W14" t="n">
+        <v>41123</v>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
@@ -1954,7 +1972,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Altri eventi,Spettacoli,Musica,Libri</t>
+          <t>Altri eventi,Musica</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1969,49 +1987,49 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2022-06-03T15:42:40+00:00</t>
+          <t>2022-05-20T10:02:04+00:00</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Rassegna di eventi culturali in Piazza XX Settembre</t>
+          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2022-06-03T15:43:48+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2022-06-07T15:00:00+00:00</t>
+          <t>2022-05-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2022-06-28T16:00:00+00:00</t>
+          <t>2022-06-30T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/note-di-stelle/@@images/78120e75-8036-4a4c-b46e-10cc1ff7fe4c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2022-06-04T06:35:10+00:00</t>
+          <t>2022-05-20T10:02:34+00:00</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Piazza XX Settembre</t>
+          <t>Piazzetta Pomposa</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 7, 14, 21 e 28 giugno alle ore 19 presentazione di libri  alle ore 21 spettacoli</t>
+          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
         </is>
       </c>
       <c r="O15" t="inlineStr"/>
@@ -2020,7 +2038,7 @@
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr">
         <is>
-          <t>Note di Stelle</t>
+          <t>Serate in Pomposa - 1° edizione</t>
         </is>
       </c>
       <c r="T15" t="inlineStr"/>
@@ -2033,7 +2051,7 @@
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/note-di-stelle</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
@@ -2055,7 +2073,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Spettacoli,Teatro</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2065,112 +2083,112 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Viale Caduti in Guerra, 196</t>
+          <t>Corso Cavour, angolo corso Canalgrnde</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2020-09-17T12:45:54+00:00</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>A cura delle allieve attrici e degli allievi attori di ERT / Teatro Nazionale</t>
-        </is>
-      </c>
+          <t>2021-09-09T10:12:02+00:00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2014-09-30T12:50:00+00:00</t>
+          <t>2021-09-09T10:12:26+00:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>info@emiliaromagnateatro.com</t>
+          <t>info@fmav.org - biglietteria@fmav.org</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2022-06-07T22:00:00+00:00</t>
+          <t>2022-06-08T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2022-06-11T21:55:00+00:00</t>
+          <t>2022-09-18T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/hereafter-episodi-teatrali/@@images/59c6e256-ecc2-48df-912f-b171b831bd83.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2022-06-06T07:48:28+00:00</t>
+          <t>2022-05-21T09:18:35+00:00</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Teatro Tempio</t>
+          <t>FMAV - Palazzina dei Giardini</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 19.00</t>
+          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
         </is>
       </c>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A pagamento, vedi nel testo le info per l'acquisto dei biglietti.</t>
+          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
         </is>
       </c>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
         <is>
-          <t>059/2163021</t>
+          <t>059 2033166</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>HEREAFTER. Episodi teatrali</t>
+          <t>Candice Breitz: Never Ending Stories</t>
         </is>
       </c>
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr">
         <is>
-          <t>http://www.emiliaromagnateatro.com</t>
+          <t>https://www.fmav.org</t>
         </is>
       </c>
       <c r="V16" t="b">
         <v>0</v>
       </c>
-      <c r="W16" t="inlineStr"/>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
+      </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/hereafter-episodi-teatrali</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>44,64381951149482</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>10,93139345085676</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>POINT (10.93139345085676 44.64381951149482)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2180,79 +2198,67 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Corso Vittorio Emanuele, 59</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2022-06-04T07:59:44+00:00</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Presentazione del libro</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:24:22+00:00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2022-06-04T07:59:52+00:00</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>​info@accademiasla-mo.it</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:25:56+00:00</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2022-06-08T07:00:00+00:00</t>
+          <t>2022-06-10T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2022-06-08T08:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione/@@images/1a4df534-f8d8-4ac6-87d4-3d9176cd882c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2022-06-04T07:59:52+00:00</t>
+          <t>2022-05-26T07:16:41+00:00</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Accademia Nazionale di Scienze Lettere e Arti di Modena</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.30</t>
+          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
         </is>
       </c>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>059 225566</t>
-        </is>
-      </c>
+      <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr">
         <is>
-          <t>"Delitti in prima pagina. La giustizia nella società dell’informazione"</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>www.accademiasla-mo.it</t>
-        </is>
-      </c>
+      <c r="U17" t="inlineStr"/>
       <c r="V17" t="b">
         <v>0</v>
       </c>
@@ -2261,7 +2267,7 @@
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/delitti-in-prima-pagina-la-giustizia-nella-societa-dell2019informazione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
@@ -2283,7 +2289,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2310,23 +2316,23 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2022-06-08T08:00:00+00:00</t>
+          <t>2022-06-10T08:00:00+00:00</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2022-07-08T09:00:00+00:00</t>
+          <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo/@@images/04c6eef6-5450-4d2e-a11b-c353a7bdb6b0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie/@@images/9a9f2a19-02f6-4cd6-a272-5cac5ae7adbd.jpeg</t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2022-06-06T10:06:47+00:00</t>
+          <t>2022-06-04T08:52:51+00:00</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -2336,7 +2342,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Inaugurazione mercoledì 8 giugno ore 18.30  mostra aperta dal 10 giugno nei seguenti orari:  venerdì e sabato dalle 10 alle 13 (ad esclusione di venerdì 17 giugno) </t>
+          <t xml:space="preserve"> ore 18.30</t>
         </is>
       </c>
       <c r="O18" t="inlineStr"/>
@@ -2349,7 +2355,7 @@
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr">
         <is>
-          <t>Oro rosso. Fragole, pomodori, molestie e sfruttamento nel Mediterraneo</t>
+          <t>Da suddite a cittadine. Gabriella Degli Esposti e le partigiane modenesi nelle fonti documentarie e nelle memorie</t>
         </is>
       </c>
       <c r="T18" t="inlineStr"/>
@@ -2362,7 +2368,7 @@
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/oro-rosso-fragole-pomodori-molestie-e-sfruttamento-nel-mediterraneo</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
@@ -2384,7 +2390,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Altri eventi,Musica</t>
+          <t>Visite guidate</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2394,54 +2400,58 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>centro storico</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:04+00:00</t>
+          <t>2022-04-29T10:05:46+00:00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Rassegna musicale nella suggestiva piazzetta della Pomposa</t>
+          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2022-05-12T09:00:00+00:00</t>
+          <t>2022-05-01T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2022-06-30T10:00:00+00:00</t>
+          <t>2022-07-17T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/serate-in-pomposa-1deg-edizione/@@images/90c7f1e5-b97b-4472-866b-68e21ff4b305.jpeg</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Torre Ghirlandina</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2022-05-20T10:02:34+00:00</t>
+          <t>2022-04-29T10:06:04+00:00</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Piazzetta Pomposa</t>
+          <t>Piazza Torre</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tutti i mercoledì e giovedì, dalle ore 18.30</t>
+          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
         </is>
       </c>
       <c r="O19" t="inlineStr"/>
@@ -2450,7 +2460,7 @@
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr">
         <is>
-          <t>Serate in Pomposa - 1° edizione</t>
+          <t>Torre Ghirlandina, aperture serali</t>
         </is>
       </c>
       <c r="T19" t="inlineStr"/>
@@ -2463,7 +2473,7 @@
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/serate-in-pomposa-1deg-edizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
@@ -2485,7 +2495,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Visite guidate,Altri eventi,Spettacoli</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2493,92 +2503,78 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Corso Cavour, angolo corso Canalgrnde</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:02+00:00</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
+          <t>2022-05-30T09:56:40+00:00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2021-09-09T10:12:26+00:00</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>info@fmav.org - biglietteria@fmav.org</t>
-        </is>
-      </c>
+          <t>2022-05-30T09:57:07+00:00</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2022-06-08T10:00:00+00:00</t>
+          <t>2022-06-10T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2022-09-18T11:00:00+00:00</t>
+          <t>2022-06-10T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/candice-breitz-never-ending-stories/@@images/d5ebf4a4-66cb-44cb-9e8c-79f9fcfc72ea.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2022-05-21T09:18:35+00:00</t>
+          <t>2022-05-30T09:57:07+00:00</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>FMAV - Palazzina dei Giardini</t>
+          <t>Duomo di Modena</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dal mercoledì alla domenica dalle 15 alle 19 </t>
+          <t xml:space="preserve"> dalle ore 20.30</t>
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ingresso 6 € / riduzioni 4 € (Circuito Vivaticket) Ingresso libero: ogni mercoledì </t>
+          <t xml:space="preserve"> Gratuito</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>059 2033166</t>
-        </is>
-      </c>
+      <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr">
         <is>
-          <t>Candice Breitz: Never Ending Stories</t>
+          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>https://www.fmav.org</t>
-        </is>
-      </c>
+      <c r="U20" t="inlineStr"/>
       <c r="V20" t="b">
         <v>0</v>
       </c>
-      <c r="W20" t="inlineStr">
-        <is>
-          <t>41121</t>
-        </is>
+      <c r="W20" t="n">
+        <v>41123</v>
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/candice-breitz-never-ending-stories</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
@@ -2600,7 +2596,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Concerti,Spettacoli,Altri eventi</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2610,63 +2606,63 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>corso Canalgrande, 85</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr"/>
+          <t>2022-05-30T11:40:24+00:00</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-30T11:41:23+00:00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2022-06-10T07:00:00+00:00</t>
+          <t>2022-06-10T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-06-10T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/c62a264a-bdfb-469d-85eb-8d034a4afbbc.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2022-05-26T07:16:41+00:00</t>
+          <t>2022-05-30T11:42:41+00:00</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Teatro comunale Pavarotti-Freni</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 17 alle 18.30</t>
+          <t xml:space="preserve"> ore 21.00</t>
         </is>
       </c>
       <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
-        </is>
-      </c>
+      <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
         </is>
       </c>
       <c r="T21" t="inlineStr"/>
@@ -2679,7 +2675,7 @@
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
         </is>
       </c>
       <c r="Y21" t="inlineStr">
@@ -2701,7 +2697,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni</t>
+          <t>Concerti</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2711,98 +2707,112 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Strada Vaciglio Nord, 6</t>
+          <t>Strada Pomposiana 292</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2022-06-04T08:30:34+00:00</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
+          <t>2022-05-30T09:03:14+00:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+        </is>
+      </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2022-06-04T08:30:59+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2022-06-10T08:00:00+00:00</t>
+          <t>2022-06-10T19:00:00+00:00</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2022-06-10T09:00:00+00:00</t>
+          <t>2022-06-10T21:00:00+00:00</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie/@@images/9a9f2a19-02f6-4cd6-a272-5cac5ae7adbd.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2022-06-04T08:52:51+00:00</t>
+          <t>2022-05-30T09:33:45+00:00</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Sala Renata Bergonzoni della Casa delle Donne</t>
+          <t>Fattoria Centofiori</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 18.30</t>
+          <t xml:space="preserve"> Ore 21.00</t>
         </is>
       </c>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ingresso libero</t>
+          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
         </is>
       </c>
       <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="inlineStr"/>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Whatsapp 3293357131</t>
+        </is>
+      </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>Da suddite a cittadine. Gabriella Degli Esposti e le partigiane modenesi nelle fonti documentarie e nelle memorie</t>
+          <t>Marco Ferri Quartet</t>
         </is>
       </c>
       <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>www.fattoriacentofiori.it</t>
+        </is>
+      </c>
       <c r="V22" t="b">
         <v>0</v>
       </c>
-      <c r="W22" t="n">
-        <v>41123</v>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>41123</t>
+        </is>
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/da-suddite-a-cittadine-gabriella-degli-esposti-e-le-partigiane-modenesi-nelle-fonti-documentarie-e-nelle-memorie</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>44,64582</t>
+          <t>44,63693000592147</t>
         </is>
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>10,92572</t>
+          <t>10,81076003183179</t>
         </is>
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>POINT (10.92572 44.64582)</t>
+          <t>POINT (10.81076003183179 44.63693000592147)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Visite guidate</t>
+          <t>Altri eventi,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2812,67 +2822,63 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>centro storico</t>
+          <t>via Selmi, 63</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2022-04-29T10:05:46+00:00</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Visite straordinarie, dalle 19 alle 22, il venerdì, sabato e domenica, dal 1 maggio al 17 luglio.</t>
-        </is>
-      </c>
+          <t>2022-05-17T07:24:22+00:00</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-05-17T07:25:56+00:00</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2022-05-01T09:00:00+00:00</t>
+          <t>2022-05-28T07:00:00+00:00</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2022-07-17T10:00:00+00:00</t>
+          <t>2022-06-11T08:00:00+00:00</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/torre-ghirlandina-aperture-serali/@@images/bfdf71f9-ed36-4565-8549-0084dd664317.jpeg</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>Torre Ghirlandina</t>
-        </is>
-      </c>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2022-04-29T10:06:04+00:00</t>
+          <t>2022-05-26T07:20:15+00:00</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Piazza Torre</t>
+          <t>Complesso San Paolo</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dal 1 maggio al 17 luglio: tutti i venerdì, sabato e domenica dalle 19 alle 22 </t>
+          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
         </is>
       </c>
       <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
+        </is>
+      </c>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr">
         <is>
-          <t>Torre Ghirlandina, aperture serali</t>
+          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
         </is>
       </c>
       <c r="T23" t="inlineStr"/>
@@ -2885,7 +2891,7 @@
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/torre-ghirlandina-aperture-serali</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
@@ -2907,7 +2913,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Visite guidate,Altri eventi,Spettacoli</t>
+          <t>Mostre</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2915,69 +2921,81 @@
           <t>Modena</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Largo Porta Sant’Agostino, 228</t>
+        </is>
+      </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2022-05-30T09:56:40+00:00</t>
+          <t>2022-06-04T09:45:49+00:00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Una serata speciale incentrata intorno e dentro al Duomo di Modena</t>
+          <t>mostra fotografica di Francesco Jodice</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
+          <t>2022-06-04T09:46:06+00:00</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>info@agomodena.it</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2022-06-10T09:00:00+00:00</t>
+          <t>2022-06-11T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2022-06-10T10:00:00+00:00</t>
+          <t>2022-08-28T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione/@@images/5d98cc67-ebaa-4fc2-a6f2-fbd81bef52b2.jpeg</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/ritratti-di-classe/@@images/3dba106b-6f95-4190-991d-b13abf85501a.jpeg</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Ritratti di classe</t>
+        </is>
+      </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2022-05-30T09:57:07+00:00</t>
+          <t>2022-06-04T09:47:46+00:00</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Duomo di Modena</t>
+          <t>AGO Modena Fabbriche culturali</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle ore 20.30</t>
+          <t xml:space="preserve"> vedi sul sito dell'evento</t>
         </is>
       </c>
       <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Gratuito</t>
-        </is>
-      </c>
+      <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr">
         <is>
-          <t>Creature e custodi. La lunga notte delle Chiese - 7°edizione</t>
+          <t>Ritratti di Classe</t>
         </is>
       </c>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr"/>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>www.agomodena.it</t>
+        </is>
+      </c>
       <c r="V24" t="b">
         <v>0</v>
       </c>
@@ -2986,7 +3004,7 @@
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/creature-e-custodi-la-lunga-notte-delle-chiese-7degedizione</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/ritratti-di-classe</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
@@ -3008,7 +3026,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Concerti,Spettacoli,Altri eventi</t>
+          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3018,54 +3036,50 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>corso Canalgrande, 85</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2022-05-30T11:40:24+00:00</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Spettacolo di beneficenza per la Croce rossa internazionale, a favore dei profughi e dei feriti dell’Ucraina</t>
-        </is>
-      </c>
+          <t>2022-05-21T10:32:36+00:00</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2022-05-30T11:41:23+00:00</t>
+          <t>2022-05-21T10:32:42+00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2022-06-10T11:00:00+00:00</t>
+          <t>2022-06-11T10:00:00+00:00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2022-06-10T12:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925/@@images/cbb45c4a-6948-4f24-a365-a1c1a9b8cd7c.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
         </is>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2022-05-30T11:42:41+00:00</t>
+          <t>2022-05-21T10:36:00+00:00</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Teatro comunale Pavarotti-Freni</t>
+          <t>Piazza Matteotti</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 21.00</t>
+          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
         </is>
       </c>
       <c r="O25" t="inlineStr"/>
@@ -3074,7 +3088,7 @@
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>Dolce époque. Classical Crossover Concert in stile 1880-1925</t>
+          <t>Nocinopoli - La città del nocino</t>
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
@@ -3087,7 +3101,7 @@
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/dolce-epoque-classical-crossover-concert-in-stile-1880-1925</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
@@ -3109,7 +3123,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Concerti</t>
+          <t>Mercati</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3119,112 +3133,96 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Strada Pomposiana 292</t>
+          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2022-05-30T09:03:14+00:00</t>
+          <t>2019-12-10T09:34:45+00:00</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Serate musicali nel polo ambientale di Marzaglia </t>
+          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
+          <t>2021-10-09T08:00:00+00:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2022-06-10T19:00:00+00:00</t>
+          <t>2022-06-11T22:00:00+00:00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2022-06-10T21:00:00+00:00</t>
+          <t>2022-06-12T21:55:00+00:00</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/marco-ferri-quartet/@@images/85be16b4-09b5-4d77-958a-0d5460201cf0.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2022-05-30T09:33:45+00:00</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>Fattoria Centofiori</t>
-        </is>
-      </c>
+          <t>2022-04-07T09:39:39+00:00</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ore 21.00</t>
+          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Per informazione sui costi contattare tramite  Whatsapp il numero 3293357131 </t>
-        </is>
-      </c>
+      <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>Whatsapp 3293357131</t>
-        </is>
-      </c>
+      <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr">
         <is>
-          <t>Marco Ferri Quartet</t>
+          <t>Fatto in Italia</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr">
         <is>
-          <t>www.fattoriacentofiori.it</t>
+          <t>http://www.consorzioilmercato.it/</t>
         </is>
       </c>
       <c r="V26" t="b">
         <v>0</v>
       </c>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>41123</t>
-        </is>
-      </c>
+      <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/marco-ferri-quartet</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>44,63693000592147</t>
+          <t>44,65137034620577</t>
         </is>
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>10,81076003183179</t>
+          <t>10,921029194828652</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>POINT (10.81076003183179 44.63693000592147)</t>
+          <t>POINT (10.921029194828652 44.65137034620577)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Altri eventi,Iniziative per bambini</t>
+          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3234,63 +3232,63 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>via Selmi, 63</t>
+          <t>via S.Pietro, 1</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2022-05-17T07:24:22+00:00</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
+          <t>2022-05-30T10:02:38+00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Presentazione del libro</t>
+        </is>
+      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2022-05-17T07:25:56+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2022-05-28T07:00:00+00:00</t>
+          <t>2022-06-12T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2022-06-11T08:00:00+00:00</t>
+          <t>2022-06-12T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi/@@images/faf8f0b5-e078-4310-9f19-8f71719228e5.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2022-05-26T07:20:15+00:00</t>
+          <t>2022-05-30T10:02:53+00:00</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>Complesso San Paolo</t>
+          <t>Chiostro di San Pietro</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato 28 maggio e sabato 11 giugno dalle ore 10 alle 12.30</t>
+          <t xml:space="preserve"> ore 15.00</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Iscrizione su prenotazione, è richiesto un contributo di 3€ a partecipante.  </t>
-        </is>
-      </c>
+      <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr">
         <is>
-          <t>Laboratori artistici in occasione della mostra dedicata a Gianni Valbonesi</t>
+          <t>Contro la guerra</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
@@ -3303,7 +3301,7 @@
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy_of_laboratori-artistici-in-occasione-della-mostra-dedicata-a-gianni-valbonesi</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
@@ -3325,7 +3323,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Mostre</t>
+          <t>Mercati,Iniziative per bambini</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3335,77 +3333,73 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Largo Porta Sant’Agostino, 228</t>
+          <t>via Don Pasquino Fiorenzi, 134</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2022-06-04T09:45:49+00:00</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>mostra fotografica di Francesco Jodice</t>
-        </is>
-      </c>
+          <t>2021-08-06T11:34:26+00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2022-06-04T09:46:06+00:00</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>info@agomodena.it</t>
-        </is>
-      </c>
+          <t>2021-08-06T11:36:33+00:00</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2022-06-11T09:00:00+00:00</t>
+          <t>2022-06-12T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2022-08-28T10:00:00+00:00</t>
+          <t>2022-06-12T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/ritratti-di-classe/@@images/3dba106b-6f95-4190-991d-b13abf85501a.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina/@@images/7fbd75c5-a620-4574-9c40-f012be16941a.jpeg</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Ritratti di classe</t>
+          <t>logo del mercatino</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2022-06-04T09:47:46+00:00</t>
+          <t>2022-02-08T10:09:23+00:00</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>AGO Modena Fabbriche culturali</t>
+          <t>Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> vedi sul sito dell'evento</t>
+          <t xml:space="preserve"> dalle ore 9 alle 13</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr"/>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>340 2607164 Luisa</t>
+        </is>
+      </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>Ritratti di Classe</t>
+          <t>Mercatino della Polisportiva Madonnina</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr">
         <is>
-          <t>www.agomodena.it</t>
+          <t>https://www.facebook.com/mercatinopolisportivamadonnina/</t>
         </is>
       </c>
       <c r="V28" t="b">
@@ -3416,7 +3410,7 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/ritratti-di-classe</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_mercatino-della-polisportiva-madonnina</t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
@@ -3438,82 +3432,108 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Altri eventi,Fiere, Esposizioni e Mostre Mercato</t>
+          <t>Altri eventi,Iniziative per bambini,Visite guidate</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Modena</t>
+          <t>Montale Rangone</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Centro storico</t>
+          <t>Via Vandelli (Statale 12 – Nuova Estense)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:36+00:00</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
+          <t>2021-04-26T15:03:43+00:00</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Riapertura al pubblico tutte le domeniche e festivi dal 3 aprile al 19 giugno 2022</t>
+        </is>
+      </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2022-05-21T10:32:42+00:00</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr"/>
+          <t>2021-04-26T15:06:06+00:00</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>museo@parcomontale.it</t>
+        </is>
+      </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2022-06-11T10:00:00+00:00</t>
+          <t>2022-04-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-19T15:00:00+00:00</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/nocinopoli-la-citta-del-nocino/@@images/0c419aa8-b36d-411f-ae54-b60ae09f6bd7.jpeg</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr"/>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/parco-archeologico-della-terramara-di-montale/@@images/f7d0a110-c97e-4787-b356-c6a2116576e3.jpeg</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Parco archeologico della Terramara di Montale</t>
+        </is>
+      </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2022-05-21T10:36:00+00:00</t>
+          <t>2022-03-28T14:43:35+00:00</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Piazza Matteotti</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sabato dalle ore 11 alle 21  domenica dalle ore 10.30 alle 21</t>
+          <t xml:space="preserve"> Il Parco è aperto dal 3 aprile al 19 giugno, tutte le domeniche e nei giorni festivi di lunedì 18 aprile, lunedì 25 aprile e giovedì 2 giugno</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7 euro intero, ridotto 5 euro dai 6 ai 13 anni,  gratuito fino a 5 anni e dai 65 anni  riduzione del 50% ai possessori della fidelity card del Parco</t>
+        </is>
+      </c>
       <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr"/>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>Per informazioni e prenotazioni: tel. 335 8136948 dalle 9 alle 13 oppure 059 532020 negli orari di apertura del Parco</t>
+        </is>
+      </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Nocinopoli - La città del nocino</t>
+          <t>Parco archeologico della Terramara di Montale</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>http://www.parcomontale.it/it</t>
+        </is>
+      </c>
       <c r="V29" t="b">
         <v>0</v>
       </c>
-      <c r="W29" t="n">
-        <v>41123</v>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>41050</t>
+        </is>
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/nocinopoli-la-citta-del-nocino</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/parco-archeologico-della-terramara-di-montale</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
@@ -3535,7 +3555,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Mercati</t>
+          <t>Altri eventi,Mercati</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3545,50 +3565,50 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>parco Novi Sad (ex - Piazza d'Armi)</t>
+          <t>Ingresso da viale Berengario</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2019-12-10T09:34:45+00:00</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Mercato di ambulanti che propongono prodotti sia alimentari che extralimentari</t>
-        </is>
-      </c>
+          <t>2020-12-29T15:02:32+00:00</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2021-10-09T08:00:00+00:00</t>
+          <t>2020-12-29T15:05:00+00:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2022-06-11T22:00:00+00:00</t>
+          <t>2022-01-03T14:00:00+00:00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2022-06-12T21:55:00+00:00</t>
+          <t>2022-12-26T14:59:00+00:00</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/copy4_of_fatto-in-italia/@@images/b8f32f6a-f0bd-4736-bb21-b49871c73eec.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/mercato-settimanale-del-lunedi-1/@@images/44cdb524-15a5-405b-89af-f9e36f3adeb6.jpeg</t>
         </is>
       </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2022-04-07T09:39:39+00:00</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr"/>
+          <t>2021-12-28T10:39:07+00:00</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>Parco Novi Sad</t>
+        </is>
+      </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> dalle 7.00 alle 14.30</t>
+          <t xml:space="preserve"> il lunedì dalle ore 8 alle 14</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
@@ -3597,44 +3617,48 @@
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr">
         <is>
-          <t>Fatto in Italia</t>
+          <t>Mercato settimanale del lunedì</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr">
         <is>
-          <t>http://www.consorzioilmercato.it/</t>
+          <t>http://www.consorzioilmercato.com/</t>
         </is>
       </c>
       <c r="V30" t="b">
         <v>0</v>
       </c>
-      <c r="W30" t="inlineStr"/>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>41121</t>
+        </is>
+      </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/copy4_of_fatto-in-italia</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/mercato-settimanale-del-lunedi-1</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>44,65137034620577</t>
+          <t>44,64582</t>
         </is>
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>10,921029194828652</t>
+          <t>10,92572</t>
         </is>
       </c>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>POINT (10.921029194828652 44.65137034620577)</t>
+          <t>POINT (10.92572 44.64582)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Conferenze, Seminari, Incontri e Lezioni,Libri</t>
+          <t>Altri eventi</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3644,54 +3668,50 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>via S.Pietro, 1</t>
+          <t>Centro storico</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:38+00:00</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Presentazione del libro</t>
-        </is>
-      </c>
+          <t>2022-05-06T09:12:13+00:00</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2022-06-12T09:00:00+00:00</t>
+          <t>2022-06-16T09:00:00+00:00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2022-06-12T10:00:00+00:00</t>
+          <t>2022-06-16T10:00:00+00:00</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/api/novita/eventi/2022/contro-la-guerra/@@images/9575eb12-02b7-4af0-8868-9cf74809a77f.jpeg</t>
+          <t>https://www.comune.modena.it/api/novita/eventi/2022/rosse-e-non-solo-di-sera/@@images/9d3d995c-a7e0-4621-9ce7-58d692875e1c.jpeg</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2022-05-30T10:02:53+00:00</t>
+          <t>2022-05-06T09:12:25+00:00</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Chiostro di San Pietro</t>
+          <t>Piazza Roma</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ore 15.00</t>
+          <t xml:space="preserve"> Dalle ore 18.30 alle 24.00</t>
         </is>
       </c>
       <c r="O31" t="inlineStr"/>
@@ -3700,7 +3720,7 @@
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>Contro la guerra</t>
+          <t>Rosse e non solo di sera</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
@@ -3713,7 +3733,7 @@
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>https://www.comune.modena.it/novita/eventi/2022/contro-la-guerra</t>
+          <t>https://www.comune.modena.it/novita/eventi/2022/rosse-e-non-solo-di-sera</t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
@@ -3735,7 +3755,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Mercati,Iniziative per bambini</t>
+          <t>Iniziative per bambini</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3745,75 +3765,71 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>via Don Pasquino Fiorenzi, 134</t>
+          <t>ingresso da corso Cavour, 2</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2021-08-06T11:34:26+00:00</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>2022-05-30T11:14:00+00:00</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Laboratorio per bambini 6-10 anni</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2021-08-06T11:36:33+00:00</t>
+          <t>2022-05-30T11:14:22+00:00</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2022-06-12T11:00:00+00:00</t>
+          <t>2022-06-16T11:00:00+00:00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2022-06-12T12:00:00+00:00</t>
+          <t>2022-06-16T12:00:00+00:00</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>https:/